<commit_message>
Change demand growth and availability factor for LDVs
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
+++ b/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{212B4E07-CD8B-4604-B0E1-53933D997E7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B34B3F5-8BE8-4AAC-9F18-693C0BA89863}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commoditties" sheetId="6" r:id="rId1"/>
@@ -1278,13 +1278,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="0.000"/>
-    <numFmt numFmtId="179" formatCode="0.0"/>
-    <numFmt numFmtId="199" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="\Te\x\t"/>
   </numFmts>
   <fonts count="27" x14ac:knownFonts="1">
     <font>
@@ -1569,7 +1569,7 @@
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
@@ -1579,15 +1579,15 @@
   <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="199" fontId="3" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="199" fontId="4" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="199" fontId="5" fillId="2" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="5" fillId="2" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="199" fontId="5" fillId="2" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="2" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="199" fontId="16" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="16" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
@@ -1597,7 +1597,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="199" fontId="14" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="14" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1622,7 +1622,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="178" fontId="14" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1631,7 +1631,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="199" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1644,11 +1644,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="199" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="199" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1667,20 +1667,20 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="199" fontId="22" fillId="8" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="22" fillId="8" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="199" fontId="22" fillId="8" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="22" fillId="8" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="199" fontId="22" fillId="8" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="22" fillId="8" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1703,11 +1703,11 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="199" fontId="22" fillId="8" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="22" fillId="8" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="26" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1716,10 +1716,10 @@
     <cellStyle name="20% - Accent5" xfId="1" builtinId="46"/>
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="3"/>
-    <cellStyle name="Normal 2" xfId="4"/>
-    <cellStyle name="Normal 4" xfId="5"/>
-    <cellStyle name="Normale_B2020" xfId="6"/>
+    <cellStyle name="Normal 10" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Normal 4" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Normale_B2020" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Percent" xfId="7" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2316,7 +2316,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L162"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3667,11 +3667,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:V245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C183" sqref="C183"/>
+    <sheetView tabSelected="1" topLeftCell="A211" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E235" sqref="E235"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -13827,7 +13827,7 @@
       <c r="U216" s="48"/>
       <c r="V216" s="48"/>
     </row>
-    <row r="217" spans="2:22" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="217" spans="2:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B217" s="1" t="str">
         <f t="shared" si="59"/>
         <v>TLRAIL_ELC_51</v>
@@ -15725,7 +15725,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L96"/>
   <sheetViews>
     <sheetView topLeftCell="A73" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">

</xml_diff>

<commit_message>
Modify freight demand (from mtkm to btkm)
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
+++ b/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B34B3F5-8BE8-4AAC-9F18-693C0BA89863}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7087A4F-1CBA-45C7-8138-0F5F58FAF2C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
   <definedNames>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1" iterateCount="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -3670,8 +3670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:V245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A211" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E235" sqref="E235"/>
+    <sheetView tabSelected="1" topLeftCell="A162" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F237" sqref="F237:H240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -13455,7 +13455,7 @@
     </row>
     <row r="212" spans="2:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B212" s="1" t="str">
-        <f t="shared" ref="B212:E231" si="59">B133</f>
+        <f t="shared" ref="B212:H231" si="59">B133</f>
         <v>TBUS_ICE_DST_41</v>
       </c>
       <c r="C212" s="1" t="str">
@@ -13993,11 +13993,11 @@
         <v>2019</v>
       </c>
       <c r="F219" s="44">
-        <f t="shared" ref="F219:N219" si="68">F140/1000</f>
+        <f>F140/1000</f>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="G219" s="44">
-        <f t="shared" si="68"/>
+        <f t="shared" ref="F219:N219" si="68">G140/1000</f>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="H219" s="44">
@@ -14067,7 +14067,7 @@
         <v>2019</v>
       </c>
       <c r="F220" s="44">
-        <f t="shared" ref="F220:N220" si="69">F141/1000</f>
+        <f t="shared" ref="F220:H220" si="69">F141/1000</f>
         <v>0.2789926277445503</v>
       </c>
       <c r="G220" s="44">
@@ -14079,27 +14079,27 @@
         <v>0.29940672245756628</v>
       </c>
       <c r="I220" s="61">
-        <f t="shared" si="69"/>
+        <f t="shared" ref="I220:N220" si="70">I141/1000</f>
         <v>9.5765005696129197</v>
       </c>
       <c r="J220" s="61">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>9.7582754878242248</v>
       </c>
       <c r="K220" s="61">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>9.7582754878242248</v>
       </c>
       <c r="L220" s="61">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.47882502848064601</v>
       </c>
       <c r="M220" s="61">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.48791377439121131</v>
       </c>
       <c r="N220" s="61">
-        <f t="shared" si="69"/>
+        <f t="shared" si="70"/>
         <v>0.48791377439121131</v>
       </c>
       <c r="O220" s="61">
@@ -14143,39 +14143,39 @@
         <v>2019</v>
       </c>
       <c r="F221" s="44">
-        <f t="shared" ref="F221:N221" si="70">F142/1000</f>
+        <f t="shared" ref="F221:H221" si="71">F142/1000</f>
         <v>0.32958068295525367</v>
       </c>
       <c r="G221" s="44">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.32958068295525367</v>
       </c>
       <c r="H221" s="44">
-        <f t="shared" si="70"/>
+        <f t="shared" si="71"/>
         <v>0.35369634268368688</v>
       </c>
       <c r="I221" s="61">
-        <f t="shared" si="70"/>
+        <f t="shared" ref="I221:N221" si="72">I142/1000</f>
         <v>10.096922826294074</v>
       </c>
       <c r="J221" s="61">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>10.351034840162802</v>
       </c>
       <c r="K221" s="61">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>10.351034840162802</v>
       </c>
       <c r="L221" s="61">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>0.50484614131470373</v>
       </c>
       <c r="M221" s="61">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>0.51755174200814014</v>
       </c>
       <c r="N221" s="61">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>0.51755174200814014</v>
       </c>
       <c r="O221" s="61">
@@ -14219,39 +14219,39 @@
         <v>2019</v>
       </c>
       <c r="F222" s="44">
-        <f t="shared" ref="F222:N222" si="71">F143/1000</f>
+        <f t="shared" ref="F222:H222" si="73">F143/1000</f>
         <v>0.398560896777929</v>
       </c>
       <c r="G222" s="44">
-        <f t="shared" si="71"/>
+        <f t="shared" si="73"/>
         <v>0.398560896777929</v>
       </c>
       <c r="H222" s="44">
-        <f t="shared" si="71"/>
+        <f t="shared" si="73"/>
         <v>0.42772388922509469</v>
       </c>
       <c r="I222" s="61">
-        <f t="shared" si="71"/>
+        <f t="shared" ref="I222:N222" si="74">I143/1000</f>
         <v>10.145722351623276</v>
       </c>
       <c r="J222" s="61">
-        <f t="shared" si="71"/>
+        <f t="shared" si="74"/>
         <v>10.150434697371828</v>
       </c>
       <c r="K222" s="61">
-        <f t="shared" si="71"/>
+        <f t="shared" si="74"/>
         <v>9.9035101452376217</v>
       </c>
       <c r="L222" s="61">
-        <f t="shared" si="71"/>
+        <f t="shared" si="74"/>
         <v>0.50728611758116382</v>
       </c>
       <c r="M222" s="61">
-        <f t="shared" si="71"/>
+        <f t="shared" si="74"/>
         <v>0.50752173486859142</v>
       </c>
       <c r="N222" s="61">
-        <f t="shared" si="71"/>
+        <f t="shared" si="74"/>
         <v>0.49517550726188114</v>
       </c>
       <c r="O222" s="61">
@@ -14295,39 +14295,39 @@
         <v>2019</v>
       </c>
       <c r="F223" s="44">
-        <f t="shared" ref="F223:N223" si="72">F144/1000</f>
+        <f t="shared" ref="F223:H223" si="75">F144/1000</f>
         <v>0.41376149075428847</v>
       </c>
       <c r="G223" s="44">
-        <f t="shared" si="72"/>
+        <f t="shared" si="75"/>
         <v>0.41376149075428847</v>
       </c>
       <c r="H223" s="44">
-        <f t="shared" si="72"/>
+        <f t="shared" si="75"/>
         <v>0.44403672178508996</v>
       </c>
       <c r="I223" s="61">
-        <f t="shared" si="72"/>
+        <f t="shared" ref="I223:N223" si="76">I144/1000</f>
         <v>10.40583270384842</v>
       </c>
       <c r="J223" s="61">
-        <f t="shared" si="72"/>
+        <f t="shared" si="76"/>
         <v>10.471237465116175</v>
       </c>
       <c r="K223" s="61">
-        <f t="shared" si="72"/>
+        <f t="shared" si="76"/>
         <v>10.224312912981967</v>
       </c>
       <c r="L223" s="61">
-        <f t="shared" si="72"/>
+        <f t="shared" si="76"/>
         <v>0.52029163519242105</v>
       </c>
       <c r="M223" s="61">
-        <f t="shared" si="72"/>
+        <f t="shared" si="76"/>
         <v>0.52356187325580883</v>
       </c>
       <c r="N223" s="61">
-        <f t="shared" si="72"/>
+        <f t="shared" si="76"/>
         <v>0.51121564564909838</v>
       </c>
       <c r="O223" s="61">
@@ -14371,39 +14371,39 @@
         <v>2019</v>
       </c>
       <c r="F224" s="44">
-        <f t="shared" ref="F224:N224" si="73">F145/1000</f>
+        <f t="shared" ref="F224:H224" si="77">F145/1000</f>
         <v>0.67414282041722684</v>
       </c>
       <c r="G224" s="44">
-        <f t="shared" si="73"/>
+        <f t="shared" si="77"/>
         <v>0.72205409077519145</v>
       </c>
       <c r="H224" s="44">
-        <f t="shared" si="73"/>
+        <f t="shared" si="77"/>
         <v>0.77497952151263994</v>
       </c>
       <c r="I224" s="61">
-        <f t="shared" si="73"/>
+        <f t="shared" ref="I224:N224" si="78">I145/1000</f>
         <v>12.047947602157109</v>
       </c>
       <c r="J224" s="61">
-        <f t="shared" si="73"/>
+        <f t="shared" si="78"/>
         <v>11.721622328338229</v>
       </c>
       <c r="K224" s="61">
-        <f t="shared" si="73"/>
+        <f t="shared" si="78"/>
         <v>11.029755355596377</v>
       </c>
       <c r="L224" s="61">
-        <f t="shared" si="73"/>
+        <f t="shared" si="78"/>
         <v>0.60239738010785537</v>
       </c>
       <c r="M224" s="61">
-        <f t="shared" si="73"/>
+        <f t="shared" si="78"/>
         <v>0.58608111641691152</v>
       </c>
       <c r="N224" s="61">
-        <f t="shared" si="73"/>
+        <f t="shared" si="78"/>
         <v>0.55148776777981889</v>
       </c>
       <c r="O224" s="61">
@@ -14446,39 +14446,39 @@
         <v>2019</v>
       </c>
       <c r="F225" s="44">
-        <f t="shared" ref="F225:N225" si="74">F146/1000</f>
+        <f t="shared" ref="F225:H225" si="79">F146/1000</f>
         <v>0.69985375036063702</v>
       </c>
       <c r="G225" s="44">
-        <f t="shared" si="74"/>
+        <f t="shared" si="79"/>
         <v>0.74959229422558771</v>
       </c>
       <c r="H225" s="44">
-        <f t="shared" si="74"/>
+        <f t="shared" si="79"/>
         <v>0.80453623202222746</v>
       </c>
       <c r="I225" s="61">
-        <f t="shared" si="74"/>
+        <f t="shared" ref="I225:N225" si="80">I146/1000</f>
         <v>12.322245791776353</v>
       </c>
       <c r="J225" s="61">
-        <f t="shared" si="74"/>
+        <f t="shared" si="80"/>
         <v>12.059923428868629</v>
       </c>
       <c r="K225" s="61">
-        <f t="shared" si="74"/>
+        <f t="shared" si="80"/>
         <v>11.368056456126777</v>
       </c>
       <c r="L225" s="61">
-        <f t="shared" si="74"/>
+        <f t="shared" si="80"/>
         <v>0.6161122895888177</v>
       </c>
       <c r="M225" s="61">
-        <f t="shared" si="74"/>
+        <f t="shared" si="80"/>
         <v>0.60299617144343154</v>
       </c>
       <c r="N225" s="61">
-        <f t="shared" si="74"/>
+        <f t="shared" si="80"/>
         <v>0.5684028228063388</v>
       </c>
       <c r="O225" s="61">
@@ -14521,39 +14521,39 @@
         <v>2019</v>
       </c>
       <c r="F226" s="44">
-        <f t="shared" ref="F226:N226" si="75">F147/1000</f>
+        <f t="shared" ref="F226:H226" si="81">F147/1000</f>
         <v>0.2789926277445503</v>
       </c>
       <c r="G226" s="44">
-        <f t="shared" si="75"/>
+        <f t="shared" si="81"/>
         <v>0.2789926277445503</v>
       </c>
       <c r="H226" s="44">
-        <f t="shared" si="75"/>
+        <f t="shared" si="81"/>
         <v>0.29940672245756628</v>
       </c>
       <c r="I226" s="61">
-        <f t="shared" si="75"/>
+        <f t="shared" ref="I226:N226" si="82">I147/1000</f>
         <v>9.6711959582822224</v>
       </c>
       <c r="J226" s="61">
-        <f t="shared" si="75"/>
+        <f t="shared" si="82"/>
         <v>9.8529708764935258</v>
       </c>
       <c r="K226" s="61">
-        <f t="shared" si="75"/>
+        <f t="shared" si="82"/>
         <v>9.8529708764935258</v>
       </c>
       <c r="L226" s="61">
-        <f t="shared" si="75"/>
+        <f t="shared" si="82"/>
         <v>0.48355979791411113</v>
       </c>
       <c r="M226" s="61">
-        <f t="shared" si="75"/>
+        <f t="shared" si="82"/>
         <v>0.49264854382467632</v>
       </c>
       <c r="N226" s="61">
-        <f t="shared" si="75"/>
+        <f t="shared" si="82"/>
         <v>0.49264854382467632</v>
       </c>
       <c r="O226" s="61">
@@ -14597,39 +14597,39 @@
         <v>2019</v>
       </c>
       <c r="F227" s="44">
-        <f t="shared" ref="F227:N227" si="76">F148/1000</f>
+        <f t="shared" ref="F227:H227" si="83">F148/1000</f>
         <v>0.31969326246659607</v>
       </c>
       <c r="G227" s="44">
-        <f t="shared" si="76"/>
+        <f t="shared" si="83"/>
         <v>0.31969326246659607</v>
       </c>
       <c r="H227" s="44">
-        <f t="shared" si="76"/>
+        <f t="shared" si="83"/>
         <v>0.34308545240317628</v>
       </c>
       <c r="I227" s="61">
-        <f t="shared" si="76"/>
+        <f t="shared" ref="I227:N227" si="84">I148/1000</f>
         <v>10.096922826294074</v>
       </c>
       <c r="J227" s="61">
-        <f t="shared" si="76"/>
+        <f t="shared" si="84"/>
         <v>10.351034840162802</v>
       </c>
       <c r="K227" s="61">
-        <f t="shared" si="76"/>
+        <f t="shared" si="84"/>
         <v>10.351034840162802</v>
       </c>
       <c r="L227" s="61">
-        <f t="shared" si="76"/>
+        <f t="shared" si="84"/>
         <v>0.50484614131470373</v>
       </c>
       <c r="M227" s="61">
-        <f t="shared" si="76"/>
+        <f t="shared" si="84"/>
         <v>0.51755174200814014</v>
       </c>
       <c r="N227" s="61">
-        <f t="shared" si="76"/>
+        <f t="shared" si="84"/>
         <v>0.51755174200814014</v>
       </c>
       <c r="O227" s="61">
@@ -14673,39 +14673,39 @@
         <v>2019</v>
       </c>
       <c r="F228" s="44">
-        <f t="shared" ref="F228:N228" si="77">F149/1000</f>
+        <f t="shared" ref="F228:H228" si="85">F149/1000</f>
         <v>0.2789926277445503</v>
       </c>
       <c r="G228" s="44">
-        <f t="shared" si="77"/>
+        <f t="shared" si="85"/>
         <v>0.2789926277445503</v>
       </c>
       <c r="H228" s="44">
-        <f t="shared" si="77"/>
+        <f t="shared" si="85"/>
         <v>0.29940672245756628</v>
       </c>
       <c r="I228" s="61">
-        <f t="shared" si="77"/>
+        <f t="shared" ref="I228:N228" si="86">I149/1000</f>
         <v>10.534150626574213</v>
       </c>
       <c r="J228" s="61">
-        <f t="shared" si="77"/>
+        <f t="shared" si="86"/>
         <v>10.734103036606648</v>
       </c>
       <c r="K228" s="61">
-        <f t="shared" si="77"/>
+        <f t="shared" si="86"/>
         <v>10.734103036606648</v>
       </c>
       <c r="L228" s="61">
-        <f t="shared" si="77"/>
+        <f t="shared" si="86"/>
         <v>0.52670753132871073</v>
       </c>
       <c r="M228" s="61">
-        <f t="shared" si="77"/>
+        <f t="shared" si="86"/>
         <v>0.53670515183033241</v>
       </c>
       <c r="N228" s="61">
-        <f t="shared" si="77"/>
+        <f t="shared" si="86"/>
         <v>0.53670515183033241</v>
       </c>
       <c r="O228" s="61">
@@ -14747,39 +14747,39 @@
         <v>2019</v>
       </c>
       <c r="F229" s="44">
-        <f t="shared" ref="F229:N229" si="78">F150/1000</f>
+        <f t="shared" ref="F229:H229" si="87">F150/1000</f>
         <v>0.2789926277445503</v>
       </c>
       <c r="G229" s="44">
-        <f t="shared" si="78"/>
+        <f t="shared" si="87"/>
         <v>0.2789926277445503</v>
       </c>
       <c r="H229" s="44">
-        <f t="shared" si="78"/>
+        <f t="shared" si="87"/>
         <v>0.29940672245756628</v>
       </c>
       <c r="I229" s="61">
-        <f t="shared" si="78"/>
+        <f t="shared" ref="I229:N229" si="88">I150/1000</f>
         <v>11.105497087871228</v>
       </c>
       <c r="J229" s="61">
-        <f t="shared" si="78"/>
+        <f t="shared" si="88"/>
         <v>10.869164632408763</v>
       </c>
       <c r="K229" s="61">
-        <f t="shared" si="78"/>
+        <f t="shared" si="88"/>
         <v>10.140150477852512</v>
       </c>
       <c r="L229" s="61">
-        <f t="shared" si="78"/>
+        <f t="shared" si="88"/>
         <v>0.55527485439356139</v>
       </c>
       <c r="M229" s="61">
-        <f t="shared" si="78"/>
+        <f t="shared" si="88"/>
         <v>0.54345823162043816</v>
       </c>
       <c r="N229" s="61">
-        <f t="shared" si="78"/>
+        <f t="shared" si="88"/>
         <v>0.5070075238926256</v>
       </c>
       <c r="O229" s="61">
@@ -14821,39 +14821,39 @@
         <v>2019</v>
       </c>
       <c r="F230" s="44">
-        <f t="shared" ref="F230:N230" si="79">F151/1000</f>
+        <f t="shared" ref="F230:H230" si="89">F151/1000</f>
         <v>0.41376149075428847</v>
       </c>
       <c r="G230" s="44">
-        <f t="shared" si="79"/>
+        <f t="shared" si="89"/>
         <v>0.41376149075428847</v>
       </c>
       <c r="H230" s="44">
-        <f t="shared" si="79"/>
+        <f t="shared" si="89"/>
         <v>0.44403672178508996</v>
       </c>
       <c r="I230" s="61">
-        <f t="shared" si="79"/>
+        <f t="shared" ref="I230:N230" si="90">I151/1000</f>
         <v>11.105497087871228</v>
       </c>
       <c r="J230" s="61">
-        <f t="shared" si="79"/>
+        <f t="shared" si="90"/>
         <v>10.869164632408763</v>
       </c>
       <c r="K230" s="61">
-        <f t="shared" si="79"/>
+        <f t="shared" si="90"/>
         <v>10.140150477852512</v>
       </c>
       <c r="L230" s="61">
-        <f t="shared" si="79"/>
+        <f t="shared" si="90"/>
         <v>0.55527485439356139</v>
       </c>
       <c r="M230" s="61">
-        <f t="shared" si="79"/>
+        <f t="shared" si="90"/>
         <v>0.54345823162043816</v>
       </c>
       <c r="N230" s="61">
-        <f t="shared" si="79"/>
+        <f t="shared" si="90"/>
         <v>0.5070075238926256</v>
       </c>
       <c r="O230" s="61">
@@ -14895,39 +14895,39 @@
         <v>2019</v>
       </c>
       <c r="F231" s="44">
-        <f t="shared" ref="F231:N231" si="80">F152/1000</f>
+        <f t="shared" ref="F231:H231" si="91">F152/1000</f>
         <v>0.51915586851518869</v>
       </c>
       <c r="G231" s="44">
-        <f t="shared" si="80"/>
+        <f t="shared" si="91"/>
         <v>0.56725205251932043</v>
       </c>
       <c r="H231" s="44">
-        <f t="shared" si="80"/>
+        <f t="shared" si="91"/>
         <v>0.63917635582918664</v>
       </c>
       <c r="I231" s="61">
-        <f t="shared" si="80"/>
+        <f t="shared" ref="I231:N231" si="92">I152/1000</f>
         <v>14.291462874665452</v>
       </c>
       <c r="J231" s="61">
-        <f t="shared" si="80"/>
+        <f t="shared" si="92"/>
         <v>13.280673962531228</v>
       </c>
       <c r="K231" s="61">
-        <f t="shared" si="80"/>
+        <f t="shared" si="92"/>
         <v>11.259096138262775</v>
       </c>
       <c r="L231" s="61">
-        <f t="shared" si="80"/>
+        <f t="shared" si="92"/>
         <v>0.71457314373327263</v>
       </c>
       <c r="M231" s="61">
-        <f t="shared" si="80"/>
+        <f t="shared" si="92"/>
         <v>0.66403369812656132</v>
       </c>
       <c r="N231" s="61">
-        <f t="shared" si="80"/>
+        <f t="shared" si="92"/>
         <v>0.56295480691313882</v>
       </c>
       <c r="O231" s="61">
@@ -14953,55 +14953,55 @@
     </row>
     <row r="232" spans="2:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B232" s="1" t="str">
-        <f t="shared" ref="B232:E240" si="81">B153</f>
+        <f t="shared" ref="B232:H240" si="93">B153</f>
         <v>TFLGV_BEV_ELE_61</v>
       </c>
       <c r="C232" s="1" t="str">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>TRAELC</v>
       </c>
       <c r="D232" s="1" t="str">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>TFGV</v>
       </c>
       <c r="E232" s="1">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>2019</v>
       </c>
       <c r="F232" s="44">
-        <f t="shared" ref="F232:N232" si="82">F153/1000</f>
+        <f t="shared" ref="F232:H232" si="94">F153/1000</f>
         <v>1.0137796002761721</v>
       </c>
       <c r="G232" s="44">
-        <f t="shared" si="82"/>
+        <f t="shared" si="94"/>
         <v>1.0910199507734044</v>
       </c>
       <c r="H232" s="44">
-        <f t="shared" si="82"/>
+        <f t="shared" si="94"/>
         <v>1.1779688726992128</v>
       </c>
       <c r="I232" s="61">
-        <f t="shared" si="82"/>
+        <f t="shared" ref="I232:N232" si="95">I153/1000</f>
         <v>14.167345509515204</v>
       </c>
       <c r="J232" s="61">
-        <f t="shared" si="82"/>
+        <f t="shared" si="95"/>
         <v>13.282158626969251</v>
       </c>
       <c r="K232" s="61">
-        <f t="shared" si="82"/>
+        <f t="shared" si="95"/>
         <v>11.511784861877349</v>
       </c>
       <c r="L232" s="61">
-        <f t="shared" si="82"/>
+        <f t="shared" si="95"/>
         <v>0.70836727547576028</v>
       </c>
       <c r="M232" s="61">
-        <f t="shared" si="82"/>
+        <f t="shared" si="95"/>
         <v>0.66410793134846258</v>
       </c>
       <c r="N232" s="61">
-        <f t="shared" si="82"/>
+        <f t="shared" si="95"/>
         <v>0.57558924309386739</v>
       </c>
       <c r="O232" s="61">
@@ -15027,55 +15027,55 @@
     </row>
     <row r="233" spans="2:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B233" s="1" t="str">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>TFHGV_ICE_DST_71</v>
       </c>
       <c r="C233" s="1" t="str">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>TRADST,TRABDL</v>
       </c>
       <c r="D233" s="1" t="str">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>TFGV</v>
       </c>
       <c r="E233" s="1">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>2019</v>
       </c>
       <c r="F233" s="44">
-        <f t="shared" ref="F233:N233" si="83">F154/1000</f>
+        <f t="shared" ref="F233:H233" si="96">F154/1000</f>
         <v>0.11165882530460597</v>
       </c>
       <c r="G233" s="44">
-        <f t="shared" si="83"/>
+        <f t="shared" si="96"/>
         <v>0.11165882530460597</v>
       </c>
       <c r="H233" s="44">
-        <f t="shared" si="83"/>
+        <f t="shared" si="96"/>
         <v>0.1198289832537235</v>
       </c>
       <c r="I233" s="61">
-        <f t="shared" si="83"/>
+        <f t="shared" ref="I233:N233" si="97">I154/1000</f>
         <v>42.314084948424728</v>
       </c>
       <c r="J233" s="61">
-        <f t="shared" si="83"/>
+        <f t="shared" si="97"/>
         <v>43.379015078746733</v>
       </c>
       <c r="K233" s="61">
-        <f t="shared" si="83"/>
+        <f t="shared" si="97"/>
         <v>43.379015078746733</v>
       </c>
       <c r="L233" s="61">
-        <f t="shared" si="83"/>
+        <f t="shared" si="97"/>
         <v>2.1157042474212369</v>
       </c>
       <c r="M233" s="61">
-        <f t="shared" si="83"/>
+        <f t="shared" si="97"/>
         <v>2.1689507539373367</v>
       </c>
       <c r="N233" s="61">
-        <f t="shared" si="83"/>
+        <f t="shared" si="97"/>
         <v>2.1689507539373367</v>
       </c>
       <c r="O233" s="61">
@@ -15083,15 +15083,15 @@
         <v>57.43</v>
       </c>
       <c r="P233" s="61">
-        <f t="shared" ref="P233:R240" si="84">P154</f>
+        <f t="shared" ref="P233:R240" si="98">P154</f>
         <v>4.9794387824114352</v>
       </c>
       <c r="Q233" s="47">
-        <f t="shared" si="84"/>
+        <f t="shared" si="98"/>
         <v>15</v>
       </c>
       <c r="R233" s="62">
-        <f t="shared" si="84"/>
+        <f t="shared" si="98"/>
         <v>1E-3</v>
       </c>
       <c r="S233" s="48"/>
@@ -15103,55 +15103,55 @@
     </row>
     <row r="234" spans="2:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B234" s="1" t="str">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>TFHGV_HEV_DST_71</v>
       </c>
       <c r="C234" s="1" t="str">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>TRADST,TRABDL</v>
       </c>
       <c r="D234" s="1" t="str">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>TFGV</v>
       </c>
       <c r="E234" s="1">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>2019</v>
       </c>
       <c r="F234" s="44">
-        <f t="shared" ref="F234:N234" si="85">F155/1000</f>
+        <f t="shared" ref="F234:H234" si="99">F155/1000</f>
         <v>0.1401784886166369</v>
       </c>
       <c r="G234" s="44">
-        <f t="shared" si="85"/>
+        <f t="shared" si="99"/>
         <v>0.1401784886166369</v>
       </c>
       <c r="H234" s="44">
-        <f t="shared" si="85"/>
+        <f t="shared" si="99"/>
         <v>0.15043545119834201</v>
       </c>
       <c r="I234" s="61">
-        <f t="shared" si="85"/>
+        <f t="shared" ref="I234:N234" si="100">I155/1000</f>
         <v>71.442144518076645</v>
       </c>
       <c r="J234" s="61">
-        <f t="shared" si="85"/>
+        <f t="shared" si="100"/>
         <v>61.236123872637116</v>
       </c>
       <c r="K234" s="61">
-        <f t="shared" si="85"/>
+        <f t="shared" si="100"/>
         <v>47.716916586621402</v>
       </c>
       <c r="L234" s="61">
-        <f t="shared" si="85"/>
+        <f t="shared" si="100"/>
         <v>3.5721072259038325</v>
       </c>
       <c r="M234" s="61">
-        <f t="shared" si="85"/>
+        <f t="shared" si="100"/>
         <v>3.0618061936318557</v>
       </c>
       <c r="N234" s="61">
-        <f t="shared" si="85"/>
+        <f t="shared" si="100"/>
         <v>2.3858458293310703</v>
       </c>
       <c r="O234" s="61">
@@ -15159,15 +15159,15 @@
         <v>57.43</v>
       </c>
       <c r="P234" s="61">
-        <f t="shared" si="84"/>
+        <f t="shared" si="98"/>
         <v>4.9794387824114352</v>
       </c>
       <c r="Q234" s="47">
-        <f t="shared" si="84"/>
+        <f t="shared" si="98"/>
         <v>15</v>
       </c>
       <c r="R234" s="62">
-        <f t="shared" si="84"/>
+        <f t="shared" si="98"/>
         <v>1E-3</v>
       </c>
       <c r="S234" s="48"/>
@@ -15179,55 +15179,55 @@
     </row>
     <row r="235" spans="2:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B235" s="1" t="str">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>TFHGV_ICE_B100_71</v>
       </c>
       <c r="C235" s="1" t="str">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>TRADST,TRABDL</v>
       </c>
       <c r="D235" s="1" t="str">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>TFGV</v>
       </c>
       <c r="E235" s="1">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>2019</v>
       </c>
       <c r="F235" s="44">
-        <f t="shared" ref="F235:N235" si="86">F156/1000</f>
+        <f t="shared" ref="F235:H235" si="101">F156/1000</f>
         <v>0.10830906054546778</v>
       </c>
       <c r="G235" s="44">
-        <f t="shared" si="86"/>
+        <f t="shared" si="101"/>
         <v>0.10830906054546778</v>
       </c>
       <c r="H235" s="44">
-        <f t="shared" si="86"/>
+        <f t="shared" si="101"/>
         <v>0.1162341137561118</v>
       </c>
       <c r="I235" s="61">
-        <f t="shared" si="86"/>
+        <f t="shared" ref="I235:N235" si="102">I156/1000</f>
         <v>42.314084948424728</v>
       </c>
       <c r="J235" s="61">
-        <f t="shared" si="86"/>
+        <f t="shared" si="102"/>
         <v>43.379015078746733</v>
       </c>
       <c r="K235" s="61">
-        <f t="shared" si="86"/>
+        <f t="shared" si="102"/>
         <v>43.379015078746733</v>
       </c>
       <c r="L235" s="61">
-        <f t="shared" si="86"/>
+        <f t="shared" si="102"/>
         <v>2.1157042474212369</v>
       </c>
       <c r="M235" s="61">
-        <f t="shared" si="86"/>
+        <f t="shared" si="102"/>
         <v>2.1689507539373367</v>
       </c>
       <c r="N235" s="61">
-        <f t="shared" si="86"/>
+        <f t="shared" si="102"/>
         <v>2.1689507539373367</v>
       </c>
       <c r="O235" s="61">
@@ -15235,15 +15235,15 @@
         <v>57.43</v>
       </c>
       <c r="P235" s="61">
-        <f t="shared" si="84"/>
+        <f t="shared" si="98"/>
         <v>4.9794387824114352</v>
       </c>
       <c r="Q235" s="47">
-        <f t="shared" si="84"/>
+        <f t="shared" si="98"/>
         <v>15</v>
       </c>
       <c r="R235" s="62">
-        <f t="shared" si="84"/>
+        <f t="shared" si="98"/>
         <v>1E-3</v>
       </c>
       <c r="S235" s="48"/>
@@ -15255,55 +15255,55 @@
     </row>
     <row r="236" spans="2:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B236" s="1" t="str">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>TFHGV_FCV_H2_71</v>
       </c>
       <c r="C236" s="1" t="str">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>TRAH2</v>
       </c>
       <c r="D236" s="1" t="str">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>TFGV</v>
       </c>
       <c r="E236" s="1">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>2019</v>
       </c>
       <c r="F236" s="44">
-        <f t="shared" ref="F236:N236" si="87">F157/1000</f>
+        <f t="shared" ref="F236:H236" si="103">F157/1000</f>
         <v>0.19238045705949228</v>
       </c>
       <c r="G236" s="44">
-        <f t="shared" si="87"/>
+        <f t="shared" si="103"/>
         <v>0.21020316970260602</v>
       </c>
       <c r="H236" s="44">
-        <f t="shared" si="87"/>
+        <f t="shared" si="103"/>
         <v>0.23685572471274502</v>
       </c>
       <c r="I236" s="61">
-        <f t="shared" si="87"/>
+        <f t="shared" ref="I236:N236" si="104">I157/1000</f>
         <v>71.442144518076645</v>
       </c>
       <c r="J236" s="61">
-        <f t="shared" si="87"/>
+        <f t="shared" si="104"/>
         <v>61.236123872637116</v>
       </c>
       <c r="K236" s="61">
-        <f t="shared" si="87"/>
+        <f t="shared" si="104"/>
         <v>47.716916586621402</v>
       </c>
       <c r="L236" s="61">
-        <f t="shared" si="87"/>
+        <f t="shared" si="104"/>
         <v>3.5721072259038325</v>
       </c>
       <c r="M236" s="61">
-        <f t="shared" si="87"/>
+        <f t="shared" si="104"/>
         <v>3.0618061936318557</v>
       </c>
       <c r="N236" s="61">
-        <f t="shared" si="87"/>
+        <f t="shared" si="104"/>
         <v>2.3858458293310703</v>
       </c>
       <c r="O236" s="61">
@@ -15311,15 +15311,15 @@
         <v>57.43</v>
       </c>
       <c r="P236" s="61">
-        <f t="shared" si="84"/>
+        <f t="shared" si="98"/>
         <v>4.9794387824114352</v>
       </c>
       <c r="Q236" s="47">
-        <f t="shared" si="84"/>
+        <f t="shared" si="98"/>
         <v>15</v>
       </c>
       <c r="R236" s="62">
-        <f t="shared" si="84"/>
+        <f t="shared" si="98"/>
         <v>1E-3</v>
       </c>
       <c r="S236" s="48"/>
@@ -15329,55 +15329,55 @@
     </row>
     <row r="237" spans="2:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B237" s="1" t="str">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>TFHGV_ICE_BCNG_71</v>
       </c>
       <c r="C237" s="1" t="str">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>TRABNG</v>
       </c>
       <c r="D237" s="1" t="str">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>TFGV</v>
       </c>
       <c r="E237" s="1">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>2019</v>
       </c>
       <c r="F237" s="44">
-        <f t="shared" ref="F237:N237" si="88">F158/1000</f>
+        <f t="shared" ref="F237:H237" si="105">F158/1000</f>
         <v>0.10607588403937566</v>
       </c>
       <c r="G237" s="44">
-        <f t="shared" si="88"/>
+        <f t="shared" si="105"/>
         <v>0.10607588403937566</v>
       </c>
       <c r="H237" s="44">
-        <f t="shared" si="88"/>
+        <f t="shared" si="105"/>
         <v>0.11383753409103732</v>
       </c>
       <c r="I237" s="61">
-        <f t="shared" si="88"/>
+        <f t="shared" ref="I237:N237" si="106">I158/1000</f>
         <v>101.97964125149409</v>
       </c>
       <c r="J237" s="61">
-        <f t="shared" si="88"/>
+        <f t="shared" si="106"/>
         <v>71.077643780739507</v>
       </c>
       <c r="K237" s="61">
-        <f t="shared" si="88"/>
+        <f t="shared" si="106"/>
         <v>46.584490473656707</v>
       </c>
       <c r="L237" s="61">
-        <f t="shared" si="88"/>
+        <f t="shared" si="106"/>
         <v>5.0989820625747049</v>
       </c>
       <c r="M237" s="61">
-        <f t="shared" si="88"/>
+        <f t="shared" si="106"/>
         <v>3.5538821890369761</v>
       </c>
       <c r="N237" s="61">
-        <f t="shared" si="88"/>
+        <f t="shared" si="106"/>
         <v>2.3292245236828353</v>
       </c>
       <c r="O237" s="61">
@@ -15385,15 +15385,15 @@
         <v>57.43</v>
       </c>
       <c r="P237" s="61">
-        <f t="shared" si="84"/>
+        <f t="shared" si="98"/>
         <v>4.9794387824114352</v>
       </c>
       <c r="Q237" s="47">
-        <f t="shared" si="84"/>
+        <f t="shared" si="98"/>
         <v>15</v>
       </c>
       <c r="R237" s="62">
-        <f t="shared" si="84"/>
+        <f t="shared" si="98"/>
         <v>1E-3</v>
       </c>
       <c r="S237" s="48"/>
@@ -15403,55 +15403,55 @@
     </row>
     <row r="238" spans="2:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B238" s="1" t="str">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>TFGV_RAIL_DST_81</v>
       </c>
       <c r="C238" s="1" t="str">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>TRADST</v>
       </c>
       <c r="D238" s="1" t="str">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>TFRAIL</v>
       </c>
       <c r="E238" s="1">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>2019</v>
       </c>
       <c r="F238" s="44">
-        <f t="shared" ref="F238:N238" si="89">F159/1000</f>
+        <f t="shared" ref="F238:H238" si="107">F159/1000</f>
         <v>7.4999999999999997E-3</v>
       </c>
       <c r="G238" s="44">
-        <f t="shared" si="89"/>
+        <f t="shared" si="107"/>
         <v>7.7000000000000002E-3</v>
       </c>
       <c r="H238" s="44">
-        <f t="shared" si="89"/>
+        <f t="shared" si="107"/>
         <v>7.7999999999999996E-3</v>
       </c>
       <c r="I238" s="61">
-        <f t="shared" si="89"/>
+        <f t="shared" ref="I238:N238" si="108">I159/1000</f>
         <v>469.60386878903267</v>
       </c>
       <c r="J238" s="61">
-        <f t="shared" si="89"/>
+        <f t="shared" si="108"/>
         <v>469.60386878903267</v>
       </c>
       <c r="K238" s="61">
-        <f t="shared" si="89"/>
+        <f t="shared" si="108"/>
         <v>469.60386878903267</v>
       </c>
       <c r="L238" s="61">
-        <f t="shared" si="89"/>
+        <f t="shared" si="108"/>
         <v>23.480193439451636</v>
       </c>
       <c r="M238" s="61">
-        <f t="shared" si="89"/>
+        <f t="shared" si="108"/>
         <v>23.480193439451636</v>
       </c>
       <c r="N238" s="61">
-        <f t="shared" si="89"/>
+        <f t="shared" si="108"/>
         <v>23.480193439451636</v>
       </c>
       <c r="O238" s="61">
@@ -15459,15 +15459,15 @@
         <v>39.363999999999997</v>
       </c>
       <c r="P238" s="61">
-        <f t="shared" si="84"/>
+        <f t="shared" si="98"/>
         <v>164.83335026928157</v>
       </c>
       <c r="Q238" s="47">
-        <f t="shared" si="84"/>
+        <f t="shared" si="98"/>
         <v>15</v>
       </c>
       <c r="R238" s="62">
-        <f t="shared" si="84"/>
+        <f t="shared" si="98"/>
         <v>1E-3</v>
       </c>
       <c r="S238" s="48"/>
@@ -15477,55 +15477,55 @@
     </row>
     <row r="239" spans="2:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B239" s="1" t="str">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>TFGV_RAIL_ELE_81</v>
       </c>
       <c r="C239" s="1" t="str">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>TRAELC</v>
       </c>
       <c r="D239" s="1" t="str">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>TFRAIL</v>
       </c>
       <c r="E239" s="1">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>2019</v>
       </c>
       <c r="F239" s="44">
-        <f t="shared" ref="F239:N239" si="90">F160/1000</f>
+        <f t="shared" ref="F239:H239" si="109">F160/1000</f>
         <v>1.9800000000000002E-2</v>
       </c>
       <c r="G239" s="44">
-        <f t="shared" si="90"/>
+        <f t="shared" si="109"/>
         <v>2.0299999999999999E-2</v>
       </c>
       <c r="H239" s="44">
-        <f t="shared" si="90"/>
+        <f t="shared" si="109"/>
         <v>2.0500000000000001E-2</v>
       </c>
       <c r="I239" s="61">
-        <f t="shared" si="90"/>
+        <f t="shared" ref="I239:N239" si="110">I160/1000</f>
         <v>438.88212036358203</v>
       </c>
       <c r="J239" s="61">
-        <f t="shared" si="90"/>
+        <f t="shared" si="110"/>
         <v>438.88212036358203</v>
       </c>
       <c r="K239" s="61">
-        <f t="shared" si="90"/>
+        <f t="shared" si="110"/>
         <v>438.88212036358203</v>
       </c>
       <c r="L239" s="61">
-        <f t="shared" si="90"/>
+        <f t="shared" si="110"/>
         <v>21.944106018179102</v>
       </c>
       <c r="M239" s="61">
-        <f t="shared" si="90"/>
+        <f t="shared" si="110"/>
         <v>21.944106018179102</v>
       </c>
       <c r="N239" s="61">
-        <f t="shared" si="90"/>
+        <f t="shared" si="110"/>
         <v>21.944106018179102</v>
       </c>
       <c r="O239" s="61">
@@ -15533,15 +15533,15 @@
         <v>39.363999999999997</v>
       </c>
       <c r="P239" s="61">
-        <f t="shared" si="84"/>
+        <f t="shared" si="98"/>
         <v>164.83335026928157</v>
       </c>
       <c r="Q239" s="47">
-        <f t="shared" si="84"/>
+        <f t="shared" si="98"/>
         <v>15</v>
       </c>
       <c r="R239" s="62">
-        <f t="shared" si="84"/>
+        <f t="shared" si="98"/>
         <v>1E-3</v>
       </c>
       <c r="S239" s="48"/>
@@ -15551,55 +15551,55 @@
     </row>
     <row r="240" spans="2:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B240" s="1" t="str">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>TFGV_RAIL_H2_81</v>
       </c>
       <c r="C240" s="1" t="str">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>TRAH2</v>
       </c>
       <c r="D240" s="1" t="str">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>TFRAIL</v>
       </c>
       <c r="E240" s="1">
-        <f t="shared" si="81"/>
+        <f t="shared" si="93"/>
         <v>2019</v>
       </c>
       <c r="F240" s="44">
-        <f t="shared" ref="F240:N240" si="91">F161/1000</f>
+        <f t="shared" ref="F240:H240" si="111">F161/1000</f>
         <v>1.1393475951168699E-2</v>
       </c>
       <c r="G240" s="44">
-        <f t="shared" si="91"/>
+        <f t="shared" si="111"/>
         <v>1.17796954749371E-2</v>
       </c>
       <c r="H240" s="44">
-        <f t="shared" si="91"/>
+        <f t="shared" si="111"/>
         <v>1.26364006003871E-2</v>
       </c>
       <c r="I240" s="61">
-        <f t="shared" si="91"/>
+        <f t="shared" ref="I240:N240" si="112">I161/1000</f>
         <v>582.10068176688731</v>
       </c>
       <c r="J240" s="61">
-        <f t="shared" si="91"/>
+        <f t="shared" si="112"/>
         <v>525.06724769825223</v>
       </c>
       <c r="K240" s="61">
-        <f t="shared" si="91"/>
+        <f t="shared" si="112"/>
         <v>494.7324684497766</v>
       </c>
       <c r="L240" s="61">
-        <f t="shared" si="91"/>
+        <f t="shared" si="112"/>
         <v>29.105034088344368</v>
       </c>
       <c r="M240" s="61">
-        <f t="shared" si="91"/>
+        <f t="shared" si="112"/>
         <v>26.253362384912613</v>
       </c>
       <c r="N240" s="61">
-        <f t="shared" si="91"/>
+        <f t="shared" si="112"/>
         <v>24.736623422488833</v>
       </c>
       <c r="O240" s="61">
@@ -15607,15 +15607,15 @@
         <v>39.363999999999997</v>
       </c>
       <c r="P240" s="61">
-        <f t="shared" si="84"/>
+        <f t="shared" si="98"/>
         <v>164.83335026928157</v>
       </c>
       <c r="Q240" s="47">
-        <f t="shared" si="84"/>
+        <f t="shared" si="98"/>
         <v>15</v>
       </c>
       <c r="R240" s="62">
-        <f t="shared" si="84"/>
+        <f t="shared" si="98"/>
         <v>1E-3</v>
       </c>
       <c r="S240" s="48"/>

</xml_diff>

<commit_message>
Remove names from name manager
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
+++ b/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EA23D25-C068-42F0-B5B0-BFF4431376DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EC9ECF1-886F-492D-BA30-A91B40BF43BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,11 +19,7 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
-    <externalReference r:id="rId5"/>
   </externalReferences>
-  <definedNames>
-    <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -1280,11 +1276,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
-    <numFmt numFmtId="167" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="\Te\x\t"/>
   </numFmts>
   <fonts count="26" x14ac:knownFonts="1">
     <font>
@@ -1564,21 +1560,21 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="15" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="15" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1588,7 +1584,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1613,7 +1609,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1622,7 +1618,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1635,11 +1631,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1658,20 +1654,20 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="21" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="21" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="21" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="21" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="21" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="21" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1680,11 +1676,11 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="9" fontId="11" fillId="9" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="41" fontId="22" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="22" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1694,11 +1690,11 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="21" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="21" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="25" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1802,141 +1798,6 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="IEA Data"/>
-      <sheetName val="E&amp;D Drivers"/>
-      <sheetName val="AGR_Fuels"/>
-      <sheetName val="AGR"/>
-      <sheetName val="RES_Fuels"/>
-      <sheetName val="RH1"/>
-      <sheetName val="RH2"/>
-      <sheetName val="RH3"/>
-      <sheetName val="RH4"/>
-      <sheetName val="RC1"/>
-      <sheetName val="RC2"/>
-      <sheetName val="RC3"/>
-      <sheetName val="RC4"/>
-      <sheetName val="RHW"/>
-      <sheetName val="RRF"/>
-      <sheetName val="RCW"/>
-      <sheetName val="RCD"/>
-      <sheetName val="RK1"/>
-      <sheetName val="RK2"/>
-      <sheetName val="RK3"/>
-      <sheetName val="RK4"/>
-      <sheetName val="RDW"/>
-      <sheetName val="RME"/>
-      <sheetName val="RL1"/>
-      <sheetName val="RL2"/>
-      <sheetName val="RL3"/>
-      <sheetName val="RL4"/>
-      <sheetName val="COM_Fuels"/>
-      <sheetName val="CH1"/>
-      <sheetName val="CH2"/>
-      <sheetName val="CH3"/>
-      <sheetName val="CH4"/>
-      <sheetName val="CC1"/>
-      <sheetName val="CC2"/>
-      <sheetName val="CC3"/>
-      <sheetName val="CC4"/>
-      <sheetName val="CHW"/>
-      <sheetName val="CAA"/>
-      <sheetName val="CLA"/>
-      <sheetName val="ElastPar"/>
-      <sheetName val="Conversion Factors"/>
-      <sheetName val="Intro"/>
-      <sheetName val="TechRep"/>
-      <sheetName val="Other_HYDRO"/>
-      <sheetName val="Other_NUCL"/>
-      <sheetName val="Other_THERM"/>
-      <sheetName val="Other_CHP"/>
-      <sheetName val="Other_RENEW"/>
-      <sheetName val="Other_HEAT"/>
-      <sheetName val="ELC_FUELS"/>
-      <sheetName val="ELC"/>
-      <sheetName val="HEAT"/>
-      <sheetName val="CHP"/>
-      <sheetName val="ELC_EMI"/>
-      <sheetName val="Constant Table"/>
-      <sheetName val="ANS_ITEMS_DEL"/>
-      <sheetName val="ANS_ITEMS"/>
-      <sheetName val="ANS_TIDDATA"/>
-      <sheetName val="ANS_TSDATA"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1">
-        <row r="2">
-          <cell r="A2" t="str">
-            <v>^FI_ST: TCH, PRC</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
-      <sheetData sheetId="34"/>
-      <sheetData sheetId="35"/>
-      <sheetData sheetId="36"/>
-      <sheetData sheetId="37"/>
-      <sheetData sheetId="38"/>
-      <sheetData sheetId="39" refreshError="1"/>
-      <sheetData sheetId="40" refreshError="1"/>
-      <sheetData sheetId="41"/>
-      <sheetData sheetId="42"/>
-      <sheetData sheetId="43"/>
-      <sheetData sheetId="44"/>
-      <sheetData sheetId="45"/>
-      <sheetData sheetId="46"/>
-      <sheetData sheetId="47"/>
-      <sheetData sheetId="48"/>
-      <sheetData sheetId="49"/>
-      <sheetData sheetId="50"/>
-      <sheetData sheetId="51"/>
-      <sheetData sheetId="52"/>
-      <sheetData sheetId="53"/>
-      <sheetData sheetId="54"/>
-      <sheetData sheetId="55"/>
-      <sheetData sheetId="56"/>
-      <sheetData sheetId="57"/>
-      <sheetData sheetId="58"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
@@ -3532,7 +3393,7 @@
         <v>227</v>
       </c>
       <c r="L144" s="23" t="e">
-        <f>'[2]FREH Capital Costs'!#REF!</f>
+        <f>'[1]FREH Capital Costs'!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -3541,7 +3402,7 @@
         <v>228</v>
       </c>
       <c r="L145" s="23" t="e">
-        <f>'[2]FREH Capital Costs'!#REF!</f>
+        <f>'[1]FREH Capital Costs'!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -3550,7 +3411,7 @@
         <v>229</v>
       </c>
       <c r="L146" s="23" t="e">
-        <f>'[2]FREH Capital Costs'!#REF!</f>
+        <f>'[1]FREH Capital Costs'!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -3559,7 +3420,7 @@
         <v>230</v>
       </c>
       <c r="L147" s="23" t="e">
-        <f>'[2]FREH Capital Costs'!#REF!</f>
+        <f>'[1]FREH Capital Costs'!#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
@@ -3659,8 +3520,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B3:V245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F237" sqref="F237:H240"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E251" sqref="E251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Modify limit type for dual-fuel technologies
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
+++ b/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_Irish-TIMES-model\VA_Transport\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797F9894-BF40-46C2-AB58-94B5F3DC3770}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584973B6-A854-4387-A24C-9878845FE6C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1423,7 +1423,7 @@
     <t xml:space="preserve"> Share-I~0</t>
   </si>
   <si>
-    <t>LO</t>
+    <t>UP</t>
   </si>
 </sst>
 </file>
@@ -1751,7 +1751,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1898,7 +1898,6 @@
     <xf numFmtId="0" fontId="27" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="20% - Accent5" xfId="1" builtinId="46"/>
@@ -3906,8 +3905,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B3:AL232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A113" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AJ182" sqref="AJ182"/>
+    <sheetView tabSelected="1" topLeftCell="Q149" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AK181" sqref="AK181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -9646,7 +9645,7 @@
       <c r="D163" s="60" t="s">
         <v>381</v>
       </c>
-      <c r="E163" s="76" t="s">
+      <c r="E163" s="60" t="s">
         <v>383</v>
       </c>
       <c r="F163" s="61">
@@ -9731,14 +9730,14 @@
         <v>0.5</v>
       </c>
       <c r="AI163" s="1" t="str">
-        <f>B163</f>
+        <f t="shared" ref="AI163:AI178" si="5">B163</f>
         <v>TCAR_ICE_DF_21</v>
       </c>
       <c r="AJ163" s="1" t="str">
-        <f>C163</f>
+        <f t="shared" ref="AJ163:AJ178" si="6">C163</f>
         <v>TRACNG</v>
       </c>
-      <c r="AK163" s="1" t="s">
+      <c r="AK163" s="60" t="s">
         <v>383</v>
       </c>
       <c r="AL163" s="1">
@@ -9757,7 +9756,7 @@
       <c r="D164" s="60" t="s">
         <v>381</v>
       </c>
-      <c r="E164" s="66" t="s">
+      <c r="E164" s="60" t="s">
         <v>383</v>
       </c>
       <c r="F164" s="61">
@@ -9842,14 +9841,14 @@
         <v>0.3</v>
       </c>
       <c r="AI164" s="1" t="str">
-        <f>B164</f>
+        <f t="shared" si="5"/>
         <v>TCAR_PHEV10_GSL_21</v>
       </c>
       <c r="AJ164" s="1" t="str">
-        <f>C164</f>
+        <f t="shared" si="6"/>
         <v>TRAELC</v>
       </c>
-      <c r="AK164" s="1" t="s">
+      <c r="AK164" s="60" t="s">
         <v>383</v>
       </c>
       <c r="AL164" s="1">
@@ -9858,7 +9857,7 @@
     </row>
     <row r="165" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B165" s="59" t="str">
-        <f t="shared" ref="B165:B169" si="5">B100</f>
+        <f t="shared" ref="B165:B169" si="7">B100</f>
         <v>TCAR_PHEV20_GSL_21</v>
       </c>
       <c r="C165" s="59" t="str">
@@ -9868,7 +9867,7 @@
       <c r="D165" s="60" t="s">
         <v>381</v>
       </c>
-      <c r="E165" s="66" t="s">
+      <c r="E165" s="60" t="s">
         <v>383</v>
       </c>
       <c r="F165" s="61">
@@ -9953,14 +9952,14 @@
         <v>0.4</v>
       </c>
       <c r="AI165" s="1" t="str">
-        <f>B165</f>
+        <f t="shared" si="5"/>
         <v>TCAR_PHEV20_GSL_21</v>
       </c>
       <c r="AJ165" s="1" t="str">
-        <f>C165</f>
+        <f t="shared" si="6"/>
         <v>TRAELC</v>
       </c>
-      <c r="AK165" s="1" t="s">
+      <c r="AK165" s="60" t="s">
         <v>383</v>
       </c>
       <c r="AL165" s="1">
@@ -9969,7 +9968,7 @@
     </row>
     <row r="166" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B166" s="59" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>TCAR_PHEV40_GSL_21</v>
       </c>
       <c r="C166" s="1" t="str">
@@ -9979,7 +9978,7 @@
       <c r="D166" s="60" t="s">
         <v>381</v>
       </c>
-      <c r="E166" s="66" t="s">
+      <c r="E166" s="60" t="s">
         <v>383</v>
       </c>
       <c r="F166" s="61">
@@ -10064,14 +10063,14 @@
         <v>0.5</v>
       </c>
       <c r="AI166" s="1" t="str">
-        <f>B166</f>
+        <f t="shared" si="5"/>
         <v>TCAR_PHEV40_GSL_21</v>
       </c>
       <c r="AJ166" s="1" t="str">
-        <f>C166</f>
+        <f t="shared" si="6"/>
         <v>TRAELC</v>
       </c>
-      <c r="AK166" s="1" t="s">
+      <c r="AK166" s="60" t="s">
         <v>383</v>
       </c>
       <c r="AL166" s="1">
@@ -10080,7 +10079,7 @@
     </row>
     <row r="167" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B167" s="59" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>TCAR_PHEV10_DST_21</v>
       </c>
       <c r="C167" s="1" t="str">
@@ -10090,7 +10089,7 @@
       <c r="D167" s="60" t="s">
         <v>381</v>
       </c>
-      <c r="E167" s="66" t="s">
+      <c r="E167" s="60" t="s">
         <v>383</v>
       </c>
       <c r="F167" s="61">
@@ -10175,14 +10174,14 @@
         <v>0.3</v>
       </c>
       <c r="AI167" s="1" t="str">
-        <f>B167</f>
+        <f t="shared" si="5"/>
         <v>TCAR_PHEV10_DST_21</v>
       </c>
       <c r="AJ167" s="1" t="str">
-        <f>C167</f>
+        <f t="shared" si="6"/>
         <v>TRAELC</v>
       </c>
-      <c r="AK167" s="1" t="s">
+      <c r="AK167" s="60" t="s">
         <v>383</v>
       </c>
       <c r="AL167" s="1">
@@ -10191,7 +10190,7 @@
     </row>
     <row r="168" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B168" s="59" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>TCAR_PHEV20_DST_21</v>
       </c>
       <c r="C168" s="1" t="str">
@@ -10201,7 +10200,7 @@
       <c r="D168" s="60" t="s">
         <v>381</v>
       </c>
-      <c r="E168" s="66" t="s">
+      <c r="E168" s="60" t="s">
         <v>383</v>
       </c>
       <c r="F168" s="61">
@@ -10286,14 +10285,14 @@
         <v>0.4</v>
       </c>
       <c r="AI168" s="1" t="str">
-        <f>B168</f>
+        <f t="shared" si="5"/>
         <v>TCAR_PHEV20_DST_21</v>
       </c>
       <c r="AJ168" s="1" t="str">
-        <f>C168</f>
+        <f t="shared" si="6"/>
         <v>TRAELC</v>
       </c>
-      <c r="AK168" s="1" t="s">
+      <c r="AK168" s="60" t="s">
         <v>383</v>
       </c>
       <c r="AL168" s="1">
@@ -10302,7 +10301,7 @@
     </row>
     <row r="169" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B169" s="59" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>TCAR_PHEV40_DST_21</v>
       </c>
       <c r="C169" s="1" t="str">
@@ -10312,7 +10311,7 @@
       <c r="D169" s="60" t="s">
         <v>381</v>
       </c>
-      <c r="E169" s="66" t="s">
+      <c r="E169" s="60" t="s">
         <v>383</v>
       </c>
       <c r="F169" s="61">
@@ -10397,14 +10396,14 @@
         <v>0.5</v>
       </c>
       <c r="AI169" s="1" t="str">
-        <f>B169</f>
+        <f t="shared" si="5"/>
         <v>TCAR_PHEV40_DST_21</v>
       </c>
       <c r="AJ169" s="1" t="str">
-        <f>C169</f>
+        <f t="shared" si="6"/>
         <v>TRAELC</v>
       </c>
-      <c r="AK169" s="1" t="s">
+      <c r="AK169" s="60" t="s">
         <v>383</v>
       </c>
       <c r="AL169" s="1">
@@ -10423,7 +10422,7 @@
       <c r="D170" s="60" t="s">
         <v>381</v>
       </c>
-      <c r="E170" s="66" t="s">
+      <c r="E170" s="60" t="s">
         <v>383</v>
       </c>
       <c r="F170" s="53">
@@ -10508,14 +10507,14 @@
         <v>0.5</v>
       </c>
       <c r="AI170" s="1" t="str">
-        <f>B170</f>
+        <f t="shared" si="5"/>
         <v>TTAXI_ICE_DF_31</v>
       </c>
       <c r="AJ170" s="1" t="str">
-        <f>C170</f>
+        <f t="shared" si="6"/>
         <v>TRACNG</v>
       </c>
-      <c r="AK170" s="1" t="s">
+      <c r="AK170" s="60" t="s">
         <v>383</v>
       </c>
       <c r="AL170" s="1">
@@ -10534,7 +10533,7 @@
       <c r="D171" s="60" t="s">
         <v>381</v>
       </c>
-      <c r="E171" s="66" t="s">
+      <c r="E171" s="60" t="s">
         <v>383</v>
       </c>
       <c r="F171" s="61">
@@ -10619,14 +10618,14 @@
         <v>0.3</v>
       </c>
       <c r="AI171" s="1" t="str">
-        <f>B171</f>
+        <f t="shared" si="5"/>
         <v>TTAXI_PHEV10_GSL_31</v>
       </c>
       <c r="AJ171" s="1" t="str">
-        <f>C171</f>
+        <f t="shared" si="6"/>
         <v>TRAELC</v>
       </c>
-      <c r="AK171" s="1" t="s">
+      <c r="AK171" s="60" t="s">
         <v>383</v>
       </c>
       <c r="AL171" s="1">
@@ -10635,7 +10634,7 @@
     </row>
     <row r="172" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B172" s="59" t="str">
-        <f t="shared" ref="B172:B176" si="6">B119</f>
+        <f t="shared" ref="B172:B176" si="8">B119</f>
         <v>TTAXI_PHEV20_GSL_31</v>
       </c>
       <c r="C172" s="1" t="str">
@@ -10645,7 +10644,7 @@
       <c r="D172" s="60" t="s">
         <v>381</v>
       </c>
-      <c r="E172" s="66" t="s">
+      <c r="E172" s="60" t="s">
         <v>383</v>
       </c>
       <c r="F172" s="61">
@@ -10730,14 +10729,14 @@
         <v>0.4</v>
       </c>
       <c r="AI172" s="1" t="str">
-        <f>B172</f>
+        <f t="shared" si="5"/>
         <v>TTAXI_PHEV20_GSL_31</v>
       </c>
       <c r="AJ172" s="1" t="str">
-        <f>C172</f>
+        <f t="shared" si="6"/>
         <v>TRAELC</v>
       </c>
-      <c r="AK172" s="1" t="s">
+      <c r="AK172" s="60" t="s">
         <v>383</v>
       </c>
       <c r="AL172" s="1">
@@ -10746,7 +10745,7 @@
     </row>
     <row r="173" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B173" s="59" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>TTAXI_PHEV40_GSL_31</v>
       </c>
       <c r="C173" s="1" t="str">
@@ -10756,7 +10755,7 @@
       <c r="D173" s="60" t="s">
         <v>381</v>
       </c>
-      <c r="E173" s="66" t="s">
+      <c r="E173" s="60" t="s">
         <v>383</v>
       </c>
       <c r="F173" s="61">
@@ -10841,14 +10840,14 @@
         <v>0.5</v>
       </c>
       <c r="AI173" s="1" t="str">
-        <f>B173</f>
+        <f t="shared" si="5"/>
         <v>TTAXI_PHEV40_GSL_31</v>
       </c>
       <c r="AJ173" s="1" t="str">
-        <f>C173</f>
+        <f t="shared" si="6"/>
         <v>TRAELC</v>
       </c>
-      <c r="AK173" s="1" t="s">
+      <c r="AK173" s="60" t="s">
         <v>383</v>
       </c>
       <c r="AL173" s="1">
@@ -10857,7 +10856,7 @@
     </row>
     <row r="174" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B174" s="59" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>TTAXI_PHEV10_DST_31</v>
       </c>
       <c r="C174" s="1" t="str">
@@ -10867,7 +10866,7 @@
       <c r="D174" s="60" t="s">
         <v>381</v>
       </c>
-      <c r="E174" s="66" t="s">
+      <c r="E174" s="60" t="s">
         <v>383</v>
       </c>
       <c r="F174" s="61">
@@ -10952,14 +10951,14 @@
         <v>0.3</v>
       </c>
       <c r="AI174" s="1" t="str">
-        <f>B174</f>
+        <f t="shared" si="5"/>
         <v>TTAXI_PHEV10_DST_31</v>
       </c>
       <c r="AJ174" s="1" t="str">
-        <f>C174</f>
+        <f t="shared" si="6"/>
         <v>TRAELC</v>
       </c>
-      <c r="AK174" s="1" t="s">
+      <c r="AK174" s="60" t="s">
         <v>383</v>
       </c>
       <c r="AL174" s="1">
@@ -10968,7 +10967,7 @@
     </row>
     <row r="175" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B175" s="59" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>TTAXI_PHEV20_DST_31</v>
       </c>
       <c r="C175" s="1" t="str">
@@ -10978,7 +10977,7 @@
       <c r="D175" s="60" t="s">
         <v>381</v>
       </c>
-      <c r="E175" s="66" t="s">
+      <c r="E175" s="60" t="s">
         <v>383</v>
       </c>
       <c r="F175" s="61">
@@ -11063,14 +11062,14 @@
         <v>0.4</v>
       </c>
       <c r="AI175" s="1" t="str">
-        <f>B175</f>
+        <f t="shared" si="5"/>
         <v>TTAXI_PHEV20_DST_31</v>
       </c>
       <c r="AJ175" s="1" t="str">
-        <f>C175</f>
+        <f t="shared" si="6"/>
         <v>TRAELC</v>
       </c>
-      <c r="AK175" s="1" t="s">
+      <c r="AK175" s="60" t="s">
         <v>383</v>
       </c>
       <c r="AL175" s="1">
@@ -11079,7 +11078,7 @@
     </row>
     <row r="176" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B176" s="59" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>TTAXI_PHEV40_DST_31</v>
       </c>
       <c r="C176" s="1" t="str">
@@ -11089,7 +11088,7 @@
       <c r="D176" s="60" t="s">
         <v>381</v>
       </c>
-      <c r="E176" s="66" t="s">
+      <c r="E176" s="60" t="s">
         <v>383</v>
       </c>
       <c r="F176" s="61">
@@ -11174,14 +11173,14 @@
         <v>0.5</v>
       </c>
       <c r="AI176" s="1" t="str">
-        <f>B176</f>
+        <f t="shared" si="5"/>
         <v>TTAXI_PHEV40_DST_31</v>
       </c>
       <c r="AJ176" s="1" t="str">
-        <f>C176</f>
+        <f t="shared" si="6"/>
         <v>TRAELC</v>
       </c>
-      <c r="AK176" s="1" t="s">
+      <c r="AK176" s="60" t="s">
         <v>383</v>
       </c>
       <c r="AL176" s="1">
@@ -11200,7 +11199,7 @@
       <c r="D177" s="60" t="s">
         <v>381</v>
       </c>
-      <c r="E177" s="66" t="s">
+      <c r="E177" s="60" t="s">
         <v>383</v>
       </c>
       <c r="F177" s="61">
@@ -11285,14 +11284,14 @@
         <v>0.5</v>
       </c>
       <c r="AI177" s="1" t="str">
-        <f>B177</f>
+        <f t="shared" si="5"/>
         <v>TFLGV_PHEV_DST_61</v>
       </c>
       <c r="AJ177" s="1" t="str">
-        <f>C177</f>
+        <f t="shared" si="6"/>
         <v>TRAELC</v>
       </c>
-      <c r="AK177" s="1" t="s">
+      <c r="AK177" s="60" t="s">
         <v>383</v>
       </c>
       <c r="AL177" s="1">
@@ -11396,14 +11395,14 @@
         <v>0.5</v>
       </c>
       <c r="AI178" s="30" t="str">
-        <f>B178</f>
+        <f t="shared" si="5"/>
         <v>TFLGV_PHEV_BCNG_61</v>
       </c>
       <c r="AJ178" s="30" t="str">
-        <f>C178</f>
+        <f t="shared" si="6"/>
         <v>TRAELC</v>
       </c>
-      <c r="AK178" s="30" t="s">
+      <c r="AK178" s="69" t="s">
         <v>383</v>
       </c>
       <c r="AL178" s="30">

</xml_diff>

<commit_message>
Remove white space from technology name
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
+++ b/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_Irish-TIMES-model\VA_Transport\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0376C76-CA56-406A-A688-D4D420D07898}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E63E08-C828-47E9-9852-9B8AFD5F4F44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commodities" sheetId="6" r:id="rId1"/>
@@ -1147,111 +1147,57 @@
     <t>TRA Taxis:  Gasoline ICEs - New</t>
   </si>
   <si>
-    <t>T- TAX-ICE_DST31</t>
-  </si>
-  <si>
     <t>TRA Taxis: Diesel ICEs - New</t>
   </si>
   <si>
-    <t>T- TAX-ICE_DF31</t>
-  </si>
-  <si>
     <t>TRA Taxis: Dual fuel ICEs (CNG/BCNG &amp; Gasoline) - New</t>
   </si>
   <si>
-    <t>T- TAX-ICE_NGB31</t>
-  </si>
-  <si>
     <t>TRA Taxis: BioCNG and CNG ICEs - New</t>
   </si>
   <si>
-    <t>T- TAX-ICE_E8531</t>
-  </si>
-  <si>
     <t>TRA Taxis: Flex fuel ICEs - New</t>
   </si>
   <si>
-    <t>T- TAX-ICE_B10031</t>
-  </si>
-  <si>
     <t>TRA Taxis: Biodiesel ICEs - New</t>
   </si>
   <si>
-    <t>T- TAX-HEV_GSL31</t>
-  </si>
-  <si>
     <t>TRA Taxis: Gasoline HEVs - New</t>
   </si>
   <si>
-    <t>T- TAX-HEV_DST31</t>
-  </si>
-  <si>
     <t>TRA Taxis: Diesel HEV - New</t>
   </si>
   <si>
-    <t>T- TAX-PHEV10_GSL31</t>
-  </si>
-  <si>
     <t>TRA Taxis: Gasoline PHEV, 10-mile all-electric range - New</t>
   </si>
   <si>
-    <t>T- TAX-PHEV20_GSL31</t>
-  </si>
-  <si>
     <t>TRA Taxis: Gasoline PHEV, 20-mile all-electric range - New</t>
   </si>
   <si>
-    <t>T- TAX-PHEV40_GSL31</t>
-  </si>
-  <si>
     <t>TRA Taxis: Gasoline PHEV, 40-mile all-electric range - New</t>
   </si>
   <si>
-    <t>T- TAX-PHEV10_DST31</t>
-  </si>
-  <si>
     <t>TRA Taxis: Diesel PHEV, 10-mile all-electric range - New</t>
   </si>
   <si>
-    <t>T- TAX-PHEV20_DST31</t>
-  </si>
-  <si>
     <t>TRA Taxis: Diesel PHEV, 20-mile all-electric range - New</t>
   </si>
   <si>
-    <t>T- TAX-PHEV40_DST31</t>
-  </si>
-  <si>
     <t>TRA Taxis: Diesel PHEV, 40-mile all-electric range - New</t>
   </si>
   <si>
-    <t>T- TAX-EV100_ELC31</t>
-  </si>
-  <si>
     <t>TRA Taxis: BEV 100 mile (160 km) all-electric range - New</t>
   </si>
   <si>
-    <t>T- TAX-EV150_ELC31</t>
-  </si>
-  <si>
     <t>TRA Taxis: BEV 150 mile (240 km) all-electric range - New</t>
   </si>
   <si>
-    <t>T- TAX-EV250_ELC31</t>
-  </si>
-  <si>
     <t>TRA Taxis: BEV 250 mile (400 km) all-electric range - New</t>
   </si>
   <si>
-    <t>T- TAX-ICE_HYD31</t>
-  </si>
-  <si>
     <t>TRA Taxis: Hydrogen ICEs - New</t>
   </si>
   <si>
-    <t>T- TAX-FCV_HYD31</t>
-  </si>
-  <si>
     <t>TRA Taxis: Fuel cell vehicles - New</t>
   </si>
   <si>
@@ -1418,6 +1364,60 @@
   </si>
   <si>
     <t>TRA Goods Train: Hydrogen Fuel Cell Train - New</t>
+  </si>
+  <si>
+    <t>T-TAX-ICE_DF31</t>
+  </si>
+  <si>
+    <t>T-TAX-ICE_NGB31</t>
+  </si>
+  <si>
+    <t>T-TAX-ICE_E8531</t>
+  </si>
+  <si>
+    <t>T-TAX-ICE_B10031</t>
+  </si>
+  <si>
+    <t>T-TAX-HEV_GSL31</t>
+  </si>
+  <si>
+    <t>T-TAX-HEV_DST31</t>
+  </si>
+  <si>
+    <t>T-TAX-PHEV10_GSL31</t>
+  </si>
+  <si>
+    <t>T-TAX-PHEV20_GSL31</t>
+  </si>
+  <si>
+    <t>T-TAX-PHEV40_GSL31</t>
+  </si>
+  <si>
+    <t>T-TAX-PHEV10_DST31</t>
+  </si>
+  <si>
+    <t>T-TAX-PHEV20_DST31</t>
+  </si>
+  <si>
+    <t>T-TAX-PHEV40_DST31</t>
+  </si>
+  <si>
+    <t>T-TAX-EV100_ELC31</t>
+  </si>
+  <si>
+    <t>T-TAX-EV150_ELC31</t>
+  </si>
+  <si>
+    <t>T-TAX-EV250_ELC31</t>
+  </si>
+  <si>
+    <t>T-TAX-ICE_HYD31</t>
+  </si>
+  <si>
+    <t>T-TAX-FCV_HYD31</t>
+  </si>
+  <si>
+    <t>T-TAX-ICE_DST31</t>
   </si>
 </sst>
 </file>
@@ -1425,11 +1425,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="165" formatCode="\Te\x\t"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="32" x14ac:knownFonts="1">
     <font>
@@ -1777,22 +1777,22 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="18" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1802,7 +1802,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1835,7 +1835,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1848,7 +1848,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1867,44 +1867,44 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="24" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="24" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="24" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="24" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="24" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="24" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="9" fontId="14" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="41" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="41" fontId="25" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="25" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="24" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="24" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="3" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2576,30 +2576,30 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L162"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="60.6640625" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" width="60.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.42578125" customWidth="1"/>
     <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="60.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" customWidth="1"/>
+    <col min="12" max="12" width="60.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>41</v>
       </c>
       <c r="B1" s="20"/>
     </row>
-    <row r="3" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="21"/>
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
@@ -2609,7 +2609,7 @@
       <c r="G3" s="22"/>
       <c r="H3" s="22"/>
     </row>
-    <row r="4" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="21"/>
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
@@ -2619,7 +2619,7 @@
       <c r="G4" s="22"/>
       <c r="H4" s="22"/>
     </row>
-    <row r="5" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
         <v>42</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>50</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
         <v>59</v>
       </c>
@@ -2689,7 +2689,7 @@
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="22"/>
       <c r="B8" s="74" t="s">
         <v>62</v>
@@ -2705,7 +2705,7 @@
       <c r="G8" s="22"/>
       <c r="H8" s="22"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="74" t="s">
         <v>63</v>
@@ -2721,7 +2721,7 @@
       <c r="G9" s="22"/>
       <c r="H9" s="22"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="22"/>
       <c r="B10" s="74" t="s">
         <v>64</v>
@@ -2737,7 +2737,7 @@
       <c r="G10" s="22"/>
       <c r="H10" s="22"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="22"/>
       <c r="B11" s="74" t="s">
         <v>66</v>
@@ -2753,7 +2753,7 @@
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="22"/>
       <c r="B12" s="74" t="s">
         <v>67</v>
@@ -2769,7 +2769,7 @@
       <c r="G12" s="22"/>
       <c r="H12" s="22"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="22"/>
       <c r="B13" s="74" t="s">
         <v>68</v>
@@ -2785,7 +2785,7 @@
       <c r="G13" s="22"/>
       <c r="H13" s="22"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="22"/>
       <c r="B14" s="74" t="s">
         <v>70</v>
@@ -2801,7 +2801,7 @@
       <c r="G14" s="22"/>
       <c r="H14" s="22"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="22"/>
       <c r="B15" s="74" t="s">
         <v>40</v>
@@ -2821,7 +2821,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="74" t="s">
         <v>144</v>
@@ -2835,7 +2835,7 @@
       <c r="E16" s="22"/>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="74" t="s">
         <v>234</v>
@@ -2849,7 +2849,7 @@
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="74" t="s">
         <v>73</v>
@@ -2866,7 +2866,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B19" s="74" t="s">
         <v>237</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="22"/>
       <c r="B20" s="74" t="s">
         <v>239</v>
@@ -2893,7 +2893,7 @@
       <c r="G20" s="69"/>
       <c r="H20" s="69"/>
     </row>
-    <row r="21" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="22"/>
       <c r="B21" s="74" t="s">
         <v>219</v>
@@ -2909,7 +2909,7 @@
       <c r="G21" s="69"/>
       <c r="H21" s="69"/>
     </row>
-    <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="29"/>
       <c r="B22" s="75" t="s">
         <v>242</v>
@@ -2925,7 +2925,7 @@
       <c r="G22" s="29"/>
       <c r="H22" s="29"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="22" t="s">
         <v>74</v>
       </c>
@@ -2943,7 +2943,7 @@
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="22"/>
       <c r="B24" s="22" t="s">
         <v>213</v>
@@ -2960,7 +2960,7 @@
       <c r="H24" s="22"/>
       <c r="I24" s="22"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="22"/>
       <c r="B25" s="22" t="s">
         <v>215</v>
@@ -2977,7 +2977,7 @@
       <c r="H25" s="22"/>
       <c r="I25" s="22"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B26" s="22" t="s">
         <v>75</v>
       </c>
@@ -2993,7 +2993,7 @@
       <c r="H26" s="22"/>
       <c r="I26" s="22"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B27" s="22" t="s">
         <v>78</v>
       </c>
@@ -3009,7 +3009,7 @@
       <c r="H27" s="22"/>
       <c r="I27" s="22"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B28" s="22" t="s">
         <v>80</v>
       </c>
@@ -3024,7 +3024,7 @@
       <c r="G28" s="22"/>
       <c r="H28" s="22"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>82</v>
       </c>
@@ -3039,7 +3039,7 @@
       <c r="G29" s="22"/>
       <c r="H29" s="22"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>84</v>
       </c>
@@ -3054,7 +3054,7 @@
       <c r="G30" s="22"/>
       <c r="H30" s="22"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>86</v>
       </c>
@@ -3069,7 +3069,7 @@
       <c r="G31" s="22"/>
       <c r="H31" s="22"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="30"/>
       <c r="B32" s="30" t="s">
         <v>88</v>
@@ -3085,7 +3085,7 @@
       <c r="G32" s="29"/>
       <c r="H32" s="29"/>
     </row>
-    <row r="33" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -3103,7 +3103,7 @@
       <c r="G33" s="22"/>
       <c r="H33" s="22"/>
     </row>
-    <row r="34" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B34" s="31" t="s">
         <v>94</v>
       </c>
@@ -3118,7 +3118,7 @@
       <c r="G34" s="22"/>
       <c r="H34" s="22"/>
     </row>
-    <row r="35" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B35" s="31" t="s">
         <v>96</v>
       </c>
@@ -3133,7 +3133,7 @@
       <c r="G35" s="22"/>
       <c r="H35" s="22"/>
     </row>
-    <row r="36" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="B36" s="31" t="s">
         <v>98</v>
       </c>
@@ -3148,7 +3148,7 @@
       <c r="G36" s="22"/>
       <c r="H36" s="22"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B37" s="22" t="s">
         <v>100</v>
       </c>
@@ -3163,7 +3163,7 @@
       <c r="G37" s="22"/>
       <c r="H37" s="22"/>
     </row>
-    <row r="38" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="32"/>
       <c r="B38" s="33" t="s">
         <v>102</v>
@@ -3179,7 +3179,7 @@
       <c r="G38" s="33"/>
       <c r="H38" s="33"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B39" s="22"/>
       <c r="C39" s="22"/>
       <c r="D39" s="22"/>
@@ -3188,7 +3188,7 @@
       <c r="G39" s="22"/>
       <c r="H39" s="22"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B40" s="22"/>
       <c r="C40" s="22"/>
       <c r="E40" s="22"/>
@@ -3196,13 +3196,13 @@
       <c r="G40" s="22"/>
       <c r="H40" s="22"/>
     </row>
-    <row r="43" spans="1:8" ht="21" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B43" s="84" t="s">
         <v>104</v>
       </c>
       <c r="C43" s="84"/>
     </row>
-    <row r="44" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B44" s="26" t="s">
         <v>57</v>
       </c>
@@ -3210,19 +3210,19 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B45" s="76" t="s">
         <v>244</v>
       </c>
       <c r="C45" s="77"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B46" s="78" t="s">
         <v>245</v>
       </c>
       <c r="C46" s="78"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B47" s="79" t="s">
         <v>246</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B48" s="79" t="s">
         <v>248</v>
       </c>
@@ -3238,13 +3238,13 @@
         <v>249</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B49" s="78" t="s">
         <v>69</v>
       </c>
       <c r="C49" s="78"/>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B50" s="79" t="s">
         <v>250</v>
       </c>
@@ -3253,7 +3253,7 @@
       </c>
       <c r="I50" s="22"/>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B51" s="79" t="s">
         <v>252</v>
       </c>
@@ -3262,7 +3262,7 @@
       </c>
       <c r="I51" s="22"/>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B52" s="79" t="s">
         <v>254</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B53" s="79" t="s">
         <v>256</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B54" s="79" t="s">
         <v>258</v>
       </c>
@@ -3286,7 +3286,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B55" s="79" t="s">
         <v>260</v>
       </c>
@@ -3294,7 +3294,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B56" s="79" t="s">
         <v>262</v>
       </c>
@@ -3302,7 +3302,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B57" s="79" t="s">
         <v>264</v>
       </c>
@@ -3310,7 +3310,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B58" s="79" t="s">
         <v>266</v>
       </c>
@@ -3318,7 +3318,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B59" s="79" t="s">
         <v>268</v>
       </c>
@@ -3326,7 +3326,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B60" s="79" t="s">
         <v>270</v>
       </c>
@@ -3334,7 +3334,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B61" s="79" t="s">
         <v>272</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B62" s="79" t="s">
         <v>274</v>
       </c>
@@ -3350,7 +3350,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B63" s="79" t="s">
         <v>276</v>
       </c>
@@ -3358,7 +3358,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B64" s="79" t="s">
         <v>278</v>
       </c>
@@ -3366,7 +3366,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B65" s="79" t="s">
         <v>280</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B66" s="79" t="s">
         <v>282</v>
       </c>
@@ -3382,7 +3382,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B67" s="79" t="s">
         <v>284</v>
       </c>
@@ -3390,7 +3390,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B68" s="79" t="s">
         <v>286</v>
       </c>
@@ -3398,13 +3398,13 @@
         <v>287</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B69" s="78" t="s">
         <v>288</v>
       </c>
       <c r="C69" s="78"/>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B70" s="79" t="s">
         <v>289</v>
       </c>
@@ -3412,418 +3412,418 @@
         <v>290</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B71" s="79" t="s">
+        <v>381</v>
+      </c>
+      <c r="C71" s="79" t="s">
         <v>291</v>
       </c>
-      <c r="C71" s="79" t="s">
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B72" s="79" t="s">
+        <v>364</v>
+      </c>
+      <c r="C72" s="79" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B72" s="79" t="s">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B73" s="79" t="s">
+        <v>365</v>
+      </c>
+      <c r="C73" s="79" t="s">
         <v>293</v>
       </c>
-      <c r="C72" s="79" t="s">
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B74" s="79" t="s">
+        <v>366</v>
+      </c>
+      <c r="C74" s="79" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B73" s="79" t="s">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B75" s="79" t="s">
+        <v>367</v>
+      </c>
+      <c r="C75" s="79" t="s">
         <v>295</v>
       </c>
-      <c r="C73" s="79" t="s">
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B76" s="79" t="s">
+        <v>368</v>
+      </c>
+      <c r="C76" s="79" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B74" s="79" t="s">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B77" s="79" t="s">
+        <v>369</v>
+      </c>
+      <c r="C77" s="79" t="s">
         <v>297</v>
       </c>
-      <c r="C74" s="79" t="s">
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B78" s="79" t="s">
+        <v>370</v>
+      </c>
+      <c r="C78" s="79" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B75" s="79" t="s">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B79" s="79" t="s">
+        <v>371</v>
+      </c>
+      <c r="C79" s="79" t="s">
         <v>299</v>
       </c>
-      <c r="C75" s="79" t="s">
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B80" s="79" t="s">
+        <v>372</v>
+      </c>
+      <c r="C80" s="79" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B76" s="79" t="s">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B81" s="79" t="s">
+        <v>373</v>
+      </c>
+      <c r="C81" s="79" t="s">
         <v>301</v>
       </c>
-      <c r="C76" s="79" t="s">
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B82" s="79" t="s">
+        <v>374</v>
+      </c>
+      <c r="C82" s="79" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B77" s="79" t="s">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B83" s="79" t="s">
+        <v>375</v>
+      </c>
+      <c r="C83" s="79" t="s">
         <v>303</v>
       </c>
-      <c r="C77" s="79" t="s">
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B84" s="79" t="s">
+        <v>376</v>
+      </c>
+      <c r="C84" s="79" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B78" s="79" t="s">
+    <row r="85" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B85" s="79" t="s">
+        <v>377</v>
+      </c>
+      <c r="C85" s="79" t="s">
         <v>305</v>
       </c>
-      <c r="C78" s="79" t="s">
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B86" s="79" t="s">
+        <v>378</v>
+      </c>
+      <c r="C86" s="79" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B79" s="79" t="s">
+    <row r="87" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B87" s="79" t="s">
+        <v>379</v>
+      </c>
+      <c r="C87" s="79" t="s">
         <v>307</v>
       </c>
-      <c r="C79" s="79" t="s">
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B88" s="79" t="s">
+        <v>380</v>
+      </c>
+      <c r="C88" s="79" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B80" s="79" t="s">
+    <row r="89" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B89" s="78" t="s">
         <v>309</v>
       </c>
-      <c r="C80" s="79" t="s">
+      <c r="C89" s="78"/>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B90" s="79" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B81" s="79" t="s">
+      <c r="C90" s="79" t="s">
         <v>311</v>
       </c>
-      <c r="C81" s="79" t="s">
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B91" s="79" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B82" s="79" t="s">
+      <c r="C91" s="79" t="s">
         <v>313</v>
       </c>
-      <c r="C82" s="79" t="s">
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B92" s="79" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B83" s="79" t="s">
+      <c r="C92" s="79" t="s">
         <v>315</v>
       </c>
-      <c r="C83" s="79" t="s">
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B93" s="79" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B84" s="79" t="s">
+      <c r="C93" s="79" t="s">
         <v>317</v>
       </c>
-      <c r="C84" s="79" t="s">
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B94" s="79" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B85" s="79" t="s">
+      <c r="C94" s="79" t="s">
         <v>319</v>
       </c>
-      <c r="C85" s="79" t="s">
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B95" s="78" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B86" s="79" t="s">
+      <c r="C95" s="78"/>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B96" s="79" t="s">
         <v>321</v>
       </c>
-      <c r="C86" s="79" t="s">
+      <c r="C96" s="79" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B87" s="79" t="s">
+    <row r="97" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B97" s="79" t="s">
         <v>323</v>
       </c>
-      <c r="C87" s="79" t="s">
+      <c r="C97" s="79" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B88" s="79" t="s">
+    <row r="98" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B98" s="79" t="s">
         <v>325</v>
       </c>
-      <c r="C88" s="79" t="s">
+      <c r="C98" s="79" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B89" s="78" t="s">
-        <v>327</v>
-      </c>
-      <c r="C89" s="78"/>
-    </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B90" s="79" t="s">
-        <v>328</v>
-      </c>
-      <c r="C90" s="79" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B91" s="79" t="s">
-        <v>330</v>
-      </c>
-      <c r="C91" s="79" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B92" s="79" t="s">
-        <v>332</v>
-      </c>
-      <c r="C92" s="79" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B93" s="79" t="s">
-        <v>334</v>
-      </c>
-      <c r="C93" s="79" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B94" s="79" t="s">
-        <v>336</v>
-      </c>
-      <c r="C94" s="79" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B95" s="78" t="s">
-        <v>338</v>
-      </c>
-      <c r="C95" s="78"/>
-    </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B96" s="79" t="s">
-        <v>339</v>
-      </c>
-      <c r="C96" s="79" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="97" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B97" s="79" t="s">
-        <v>341</v>
-      </c>
-      <c r="C97" s="79" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B98" s="79" t="s">
-        <v>343</v>
-      </c>
-      <c r="C98" s="79" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="99" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B99" s="80" t="s">
         <v>77</v>
       </c>
       <c r="C99" s="81"/>
     </row>
-    <row r="100" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B100" s="78" t="s">
+        <v>327</v>
+      </c>
+      <c r="C100" s="78"/>
+    </row>
+    <row r="101" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B101" s="79" t="s">
+        <v>328</v>
+      </c>
+      <c r="C101" s="79" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="102" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B102" s="79" t="s">
+        <v>330</v>
+      </c>
+      <c r="C102" s="79" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="103" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B103" s="79" t="s">
+        <v>332</v>
+      </c>
+      <c r="C103" s="79" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="104" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B104" s="79" t="s">
+        <v>334</v>
+      </c>
+      <c r="C104" s="79" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="105" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B105" s="79" t="s">
+        <v>336</v>
+      </c>
+      <c r="C105" s="79" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="106" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B106" s="79" t="s">
+        <v>338</v>
+      </c>
+      <c r="C106" s="79" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="107" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B107" s="79" t="s">
+        <v>340</v>
+      </c>
+      <c r="C107" s="79" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="108" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B108" s="78" t="s">
+        <v>342</v>
+      </c>
+      <c r="C108" s="78"/>
+    </row>
+    <row r="109" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B109" s="79" t="s">
+        <v>343</v>
+      </c>
+      <c r="C109" s="79" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="110" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B110" s="79" t="s">
         <v>345</v>
       </c>
-      <c r="C100" s="78"/>
-    </row>
-    <row r="101" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B101" s="79" t="s">
+      <c r="C110" s="79" t="s">
         <v>346</v>
       </c>
-      <c r="C101" s="79" t="s">
+      <c r="J110" s="22"/>
+    </row>
+    <row r="111" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B111" s="79" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="102" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B102" s="79" t="s">
+      <c r="C111" s="79" t="s">
         <v>348</v>
       </c>
-      <c r="C102" s="79" t="s">
+      <c r="J111" s="22"/>
+    </row>
+    <row r="112" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B112" s="79" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="103" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B103" s="79" t="s">
+      <c r="C112" s="79" t="s">
         <v>350</v>
       </c>
-      <c r="C103" s="79" t="s">
+      <c r="J112" s="22"/>
+    </row>
+    <row r="113" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B113" s="79" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="104" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B104" s="79" t="s">
+      <c r="C113" s="79" t="s">
         <v>352</v>
       </c>
-      <c r="C104" s="79" t="s">
+      <c r="J113" s="22"/>
+    </row>
+    <row r="114" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B114" s="79" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="105" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B105" s="79" t="s">
+      <c r="C114" s="79" t="s">
         <v>354</v>
       </c>
-      <c r="C105" s="79" t="s">
+      <c r="J114" s="22"/>
+    </row>
+    <row r="115" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B115" s="79" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="106" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B106" s="79" t="s">
+      <c r="C115" s="79" t="s">
         <v>356</v>
       </c>
-      <c r="C106" s="79" t="s">
+      <c r="J115" s="22"/>
+    </row>
+    <row r="116" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B116" s="78" t="s">
         <v>357</v>
-      </c>
-    </row>
-    <row r="107" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B107" s="79" t="s">
-        <v>358</v>
-      </c>
-      <c r="C107" s="79" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="108" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B108" s="78" t="s">
-        <v>360</v>
-      </c>
-      <c r="C108" s="78"/>
-    </row>
-    <row r="109" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B109" s="79" t="s">
-        <v>361</v>
-      </c>
-      <c r="C109" s="79" t="s">
-        <v>362</v>
-      </c>
-    </row>
-    <row r="110" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B110" s="79" t="s">
-        <v>363</v>
-      </c>
-      <c r="C110" s="79" t="s">
-        <v>364</v>
-      </c>
-      <c r="J110" s="22"/>
-    </row>
-    <row r="111" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B111" s="79" t="s">
-        <v>365</v>
-      </c>
-      <c r="C111" s="79" t="s">
-        <v>366</v>
-      </c>
-      <c r="J111" s="22"/>
-    </row>
-    <row r="112" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B112" s="79" t="s">
-        <v>367</v>
-      </c>
-      <c r="C112" s="79" t="s">
-        <v>368</v>
-      </c>
-      <c r="J112" s="22"/>
-    </row>
-    <row r="113" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B113" s="79" t="s">
-        <v>369</v>
-      </c>
-      <c r="C113" s="79" t="s">
-        <v>370</v>
-      </c>
-      <c r="J113" s="22"/>
-    </row>
-    <row r="114" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B114" s="79" t="s">
-        <v>371</v>
-      </c>
-      <c r="C114" s="79" t="s">
-        <v>372</v>
-      </c>
-      <c r="J114" s="22"/>
-    </row>
-    <row r="115" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B115" s="79" t="s">
-        <v>373</v>
-      </c>
-      <c r="C115" s="79" t="s">
-        <v>374</v>
-      </c>
-      <c r="J115" s="22"/>
-    </row>
-    <row r="116" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B116" s="78" t="s">
-        <v>375</v>
       </c>
       <c r="C116" s="78"/>
       <c r="J116" s="22"/>
     </row>
-    <row r="117" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B117" s="79" t="s">
-        <v>376</v>
+        <v>358</v>
       </c>
       <c r="C117" s="79" t="s">
-        <v>377</v>
+        <v>359</v>
       </c>
       <c r="J117" s="22"/>
     </row>
-    <row r="118" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B118" s="79" t="s">
-        <v>378</v>
+        <v>360</v>
       </c>
       <c r="C118" s="79" t="s">
-        <v>379</v>
+        <v>361</v>
       </c>
       <c r="J118" s="22"/>
     </row>
-    <row r="119" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B119" s="79" t="s">
-        <v>380</v>
+        <v>362</v>
       </c>
       <c r="C119" s="79" t="s">
-        <v>381</v>
+        <v>363</v>
       </c>
       <c r="J119" s="22"/>
     </row>
-    <row r="120" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:10" x14ac:dyDescent="0.2">
       <c r="J120" s="22"/>
     </row>
-    <row r="121" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:10" x14ac:dyDescent="0.2">
       <c r="J121" s="22"/>
     </row>
-    <row r="122" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:10" x14ac:dyDescent="0.2">
       <c r="J122" s="22"/>
     </row>
-    <row r="123" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:10" x14ac:dyDescent="0.2">
       <c r="J123" s="22"/>
     </row>
-    <row r="124" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:10" x14ac:dyDescent="0.2">
       <c r="J124" s="22"/>
     </row>
-    <row r="143" spans="11:12" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="143" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K143" s="34" t="s">
         <v>116</v>
       </c>
       <c r="L143" s="35"/>
     </row>
-    <row r="144" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K144" s="22" t="s">
         <v>117</v>
       </c>
@@ -3832,7 +3832,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="145" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K145" s="22" t="s">
         <v>118</v>
       </c>
@@ -3841,7 +3841,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="146" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="146" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K146" s="22" t="s">
         <v>119</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="147" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K147" s="22" t="s">
         <v>120</v>
       </c>
@@ -3859,12 +3859,12 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="152" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K152" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="153" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="153" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K153" t="s">
         <v>106</v>
       </c>
@@ -3872,7 +3872,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="154" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="154" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K154" t="s">
         <v>108</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="155" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K155" t="s">
         <v>110</v>
       </c>
@@ -3888,7 +3888,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="156" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K156" t="s">
         <v>112</v>
       </c>
@@ -3896,7 +3896,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="157" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="157" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K157" t="s">
         <v>114</v>
       </c>
@@ -3904,12 +3904,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="158" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="158" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K158" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="159" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="159" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K159" t="s">
         <v>117</v>
       </c>
@@ -3917,7 +3917,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="160" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="160" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K160" t="s">
         <v>118</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="161" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="161" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K161" t="s">
         <v>119</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="162" spans="11:12" x14ac:dyDescent="0.25">
+    <row r="162" spans="11:12" x14ac:dyDescent="0.2">
       <c r="K162" t="s">
         <v>120</v>
       </c>
@@ -3959,30 +3959,30 @@
       <selection activeCell="B174" sqref="B174"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.21875" customWidth="1"/>
-    <col min="2" max="2" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" customWidth="1"/>
-    <col min="4" max="4" width="26.109375" customWidth="1"/>
-    <col min="5" max="5" width="25.88671875" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" customWidth="1"/>
-    <col min="9" max="11" width="18.109375" customWidth="1"/>
-    <col min="12" max="14" width="19.88671875" customWidth="1"/>
-    <col min="16" max="16" width="16.33203125" customWidth="1"/>
-    <col min="17" max="17" width="12.33203125" customWidth="1"/>
-    <col min="18" max="18" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="11" width="18.140625" customWidth="1"/>
+    <col min="12" max="14" width="19.85546875" customWidth="1"/>
+    <col min="16" max="16" width="16.28515625" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" customWidth="1"/>
+    <col min="18" max="18" width="11.140625" customWidth="1"/>
     <col min="19" max="19" width="14" customWidth="1"/>
-    <col min="20" max="20" width="14.109375" customWidth="1"/>
-    <col min="21" max="21" width="13.5546875" customWidth="1"/>
-    <col min="22" max="22" width="13.88671875" customWidth="1"/>
-    <col min="34" max="34" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.6640625" customWidth="1"/>
+    <col min="20" max="20" width="14.140625" customWidth="1"/>
+    <col min="21" max="21" width="13.5703125" customWidth="1"/>
+    <col min="22" max="22" width="13.85546875" customWidth="1"/>
+    <col min="34" max="34" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
@@ -3998,7 +3998,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
@@ -4030,7 +4030,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="2:13" ht="28.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" ht="28.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>25</v>
       </c>
@@ -4062,7 +4062,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
         <v>136</v>
       </c>
@@ -4077,7 +4077,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
         <v>29</v>
       </c>
@@ -4103,7 +4103,7 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
@@ -4129,7 +4129,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="2:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" ht="15" x14ac:dyDescent="0.25">
       <c r="B9" s="27" t="s">
         <v>137</v>
       </c>
@@ -4145,7 +4145,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
         <v>29</v>
       </c>
@@ -4165,7 +4165,7 @@
       </c>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
         <v>29</v>
       </c>
@@ -4186,7 +4186,7 @@
       <c r="I11" s="10"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
         <v>29</v>
       </c>
@@ -4207,7 +4207,7 @@
       <c r="I12" s="10"/>
       <c r="M12" s="14"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
         <v>29</v>
       </c>
@@ -4228,7 +4228,7 @@
       <c r="I13" s="10"/>
       <c r="M13" s="18"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
         <v>29</v>
       </c>
@@ -4249,7 +4249,7 @@
       <c r="I14" s="10"/>
       <c r="M14" s="18"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
@@ -4270,7 +4270,7 @@
       <c r="I15" s="10"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
         <v>29</v>
       </c>
@@ -4290,7 +4290,7 @@
       </c>
       <c r="I16" s="10"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
         <v>29</v>
       </c>
@@ -4316,7 +4316,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
         <v>29</v>
       </c>
@@ -4336,7 +4336,7 @@
       </c>
       <c r="I18" s="10"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
         <v>29</v>
       </c>
@@ -4356,7 +4356,7 @@
       </c>
       <c r="I19" s="10"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
         <v>29</v>
       </c>
@@ -4376,7 +4376,7 @@
       </c>
       <c r="I20" s="10"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
         <v>29</v>
       </c>
@@ -4396,7 +4396,7 @@
       </c>
       <c r="I21" s="10"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
         <v>29</v>
       </c>
@@ -4416,7 +4416,7 @@
       </c>
       <c r="I22" s="10"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
         <v>29</v>
       </c>
@@ -4436,7 +4436,7 @@
       </c>
       <c r="I23" s="10"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
         <v>29</v>
       </c>
@@ -4456,7 +4456,7 @@
       </c>
       <c r="I24" s="10"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
         <v>29</v>
       </c>
@@ -4476,7 +4476,7 @@
       </c>
       <c r="I25" s="10"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
         <v>29</v>
       </c>
@@ -4496,7 +4496,7 @@
       </c>
       <c r="I26" s="10"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
         <v>29</v>
       </c>
@@ -4516,7 +4516,7 @@
       </c>
       <c r="I27" s="10"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B28" s="3" t="s">
         <v>29</v>
       </c>
@@ -4536,7 +4536,7 @@
       </c>
       <c r="I28" s="10"/>
     </row>
-    <row r="29" spans="2:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:13" ht="15" x14ac:dyDescent="0.25">
       <c r="B29" s="27" t="s">
         <v>138</v>
       </c>
@@ -4549,7 +4549,7 @@
       <c r="I29" s="27"/>
       <c r="J29" s="27"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B30" s="3" t="s">
         <v>29</v>
       </c>
@@ -4569,13 +4569,13 @@
       </c>
       <c r="I30" s="10"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B31" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D31" s="1" t="str">
         <f>Commodities!B71</f>
-        <v>T- TAX-ICE_DST31</v>
+        <v>T-TAX-ICE_DST31</v>
       </c>
       <c r="E31" s="1" t="str">
         <f>Commodities!C71</f>
@@ -4589,13 +4589,13 @@
       </c>
       <c r="I31" s="10"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B32" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D32" s="1" t="str">
         <f>Commodities!B72</f>
-        <v>T- TAX-ICE_DF31</v>
+        <v>T-TAX-ICE_DF31</v>
       </c>
       <c r="E32" s="1" t="str">
         <f>Commodities!C72</f>
@@ -4609,13 +4609,13 @@
       </c>
       <c r="I32" s="10"/>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B33" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D33" s="1" t="str">
         <f>Commodities!B73</f>
-        <v>T- TAX-ICE_NGB31</v>
+        <v>T-TAX-ICE_NGB31</v>
       </c>
       <c r="E33" s="1" t="str">
         <f>Commodities!C73</f>
@@ -4629,13 +4629,13 @@
       </c>
       <c r="I33" s="10"/>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B34" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D34" s="1" t="str">
         <f>Commodities!B74</f>
-        <v>T- TAX-ICE_E8531</v>
+        <v>T-TAX-ICE_E8531</v>
       </c>
       <c r="E34" s="1" t="str">
         <f>Commodities!C74</f>
@@ -4649,13 +4649,13 @@
       </c>
       <c r="I34" s="10"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B35" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D35" s="1" t="str">
         <f>Commodities!B75</f>
-        <v>T- TAX-ICE_B10031</v>
+        <v>T-TAX-ICE_B10031</v>
       </c>
       <c r="E35" s="1" t="str">
         <f>Commodities!C75</f>
@@ -4669,13 +4669,13 @@
       </c>
       <c r="I35" s="10"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B36" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D36" s="1" t="str">
         <f>Commodities!B76</f>
-        <v>T- TAX-HEV_GSL31</v>
+        <v>T-TAX-HEV_GSL31</v>
       </c>
       <c r="E36" s="1" t="str">
         <f>Commodities!C76</f>
@@ -4689,13 +4689,13 @@
       </c>
       <c r="I36" s="10"/>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B37" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D37" s="1" t="str">
         <f>Commodities!B77</f>
-        <v>T- TAX-HEV_DST31</v>
+        <v>T-TAX-HEV_DST31</v>
       </c>
       <c r="E37" s="1" t="str">
         <f>Commodities!C77</f>
@@ -4709,13 +4709,13 @@
       </c>
       <c r="I37" s="10"/>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B38" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D38" s="1" t="str">
         <f>Commodities!B78</f>
-        <v>T- TAX-PHEV10_GSL31</v>
+        <v>T-TAX-PHEV10_GSL31</v>
       </c>
       <c r="E38" s="1" t="str">
         <f>Commodities!C78</f>
@@ -4729,13 +4729,13 @@
       </c>
       <c r="I38" s="10"/>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B39" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D39" s="1" t="str">
         <f>Commodities!B79</f>
-        <v>T- TAX-PHEV20_GSL31</v>
+        <v>T-TAX-PHEV20_GSL31</v>
       </c>
       <c r="E39" s="1" t="str">
         <f>Commodities!C79</f>
@@ -4749,13 +4749,13 @@
       </c>
       <c r="I39" s="10"/>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B40" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D40" s="1" t="str">
         <f>Commodities!B80</f>
-        <v>T- TAX-PHEV40_GSL31</v>
+        <v>T-TAX-PHEV40_GSL31</v>
       </c>
       <c r="E40" s="1" t="str">
         <f>Commodities!C80</f>
@@ -4769,13 +4769,13 @@
       </c>
       <c r="I40" s="10"/>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B41" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D41" s="1" t="str">
         <f>Commodities!B81</f>
-        <v>T- TAX-PHEV10_DST31</v>
+        <v>T-TAX-PHEV10_DST31</v>
       </c>
       <c r="E41" s="1" t="str">
         <f>Commodities!C81</f>
@@ -4789,13 +4789,13 @@
       </c>
       <c r="I41" s="10"/>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B42" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D42" s="1" t="str">
         <f>Commodities!B82</f>
-        <v>T- TAX-PHEV20_DST31</v>
+        <v>T-TAX-PHEV20_DST31</v>
       </c>
       <c r="E42" s="1" t="str">
         <f>Commodities!C82</f>
@@ -4809,13 +4809,13 @@
       </c>
       <c r="I42" s="10"/>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B43" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D43" s="1" t="str">
         <f>Commodities!B83</f>
-        <v>T- TAX-PHEV40_DST31</v>
+        <v>T-TAX-PHEV40_DST31</v>
       </c>
       <c r="E43" s="1" t="str">
         <f>Commodities!C83</f>
@@ -4829,13 +4829,13 @@
       </c>
       <c r="I43" s="10"/>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B44" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D44" s="1" t="str">
         <f>Commodities!B84</f>
-        <v>T- TAX-EV100_ELC31</v>
+        <v>T-TAX-EV100_ELC31</v>
       </c>
       <c r="E44" s="1" t="str">
         <f>Commodities!C84</f>
@@ -4849,13 +4849,13 @@
       </c>
       <c r="I44" s="10"/>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B45" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D45" s="1" t="str">
         <f>Commodities!B85</f>
-        <v>T- TAX-EV150_ELC31</v>
+        <v>T-TAX-EV150_ELC31</v>
       </c>
       <c r="E45" s="1" t="str">
         <f>Commodities!C85</f>
@@ -4869,13 +4869,13 @@
       </c>
       <c r="I45" s="10"/>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B46" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D46" s="1" t="str">
         <f>Commodities!B86</f>
-        <v>T- TAX-EV250_ELC31</v>
+        <v>T-TAX-EV250_ELC31</v>
       </c>
       <c r="E46" s="1" t="str">
         <f>Commodities!C86</f>
@@ -4889,13 +4889,13 @@
       </c>
       <c r="I46" s="10"/>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B47" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D47" s="1" t="str">
         <f>Commodities!B87</f>
-        <v>T- TAX-ICE_HYD31</v>
+        <v>T-TAX-ICE_HYD31</v>
       </c>
       <c r="E47" s="1" t="str">
         <f>Commodities!C87</f>
@@ -4909,13 +4909,13 @@
       </c>
       <c r="I47" s="10"/>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B48" s="3" t="s">
         <v>29</v>
       </c>
       <c r="D48" s="1" t="str">
         <f>Commodities!B88</f>
-        <v>T- TAX-FCV_HYD31</v>
+        <v>T-TAX-FCV_HYD31</v>
       </c>
       <c r="E48" s="1" t="str">
         <f>Commodities!C88</f>
@@ -4929,7 +4929,7 @@
       </c>
       <c r="I48" s="10"/>
     </row>
-    <row r="49" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B49" s="27" t="s">
         <v>139</v>
       </c>
@@ -4942,7 +4942,7 @@
       <c r="I49" s="27"/>
       <c r="J49" s="27"/>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B50" s="3" t="s">
         <v>29</v>
       </c>
@@ -4962,7 +4962,7 @@
       </c>
       <c r="I50" s="10"/>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B51" s="3" t="s">
         <v>29</v>
       </c>
@@ -4982,7 +4982,7 @@
       </c>
       <c r="I51" s="10"/>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B52" s="3" t="s">
         <v>29</v>
       </c>
@@ -5002,7 +5002,7 @@
       </c>
       <c r="I52" s="10"/>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B53" s="3" t="s">
         <v>29</v>
       </c>
@@ -5022,7 +5022,7 @@
       </c>
       <c r="I53" s="10"/>
     </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B54" s="3" t="s">
         <v>29</v>
       </c>
@@ -5042,7 +5042,7 @@
       </c>
       <c r="I54" s="10"/>
     </row>
-    <row r="55" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B55" s="27" t="s">
         <v>140</v>
       </c>
@@ -5055,7 +5055,7 @@
       <c r="I55" s="27"/>
       <c r="J55" s="27"/>
     </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B56" s="3" t="s">
         <v>29</v>
       </c>
@@ -5075,7 +5075,7 @@
       </c>
       <c r="I56" s="10"/>
     </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B57" s="3" t="s">
         <v>29</v>
       </c>
@@ -5095,7 +5095,7 @@
       </c>
       <c r="I57" s="10"/>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B58" s="3" t="s">
         <v>29</v>
       </c>
@@ -5115,7 +5115,7 @@
       </c>
       <c r="I58" s="10"/>
     </row>
-    <row r="59" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B59" s="27" t="s">
         <v>141</v>
       </c>
@@ -5128,7 +5128,7 @@
       <c r="I59" s="27"/>
       <c r="J59" s="27"/>
     </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B60" s="3" t="s">
         <v>29</v>
       </c>
@@ -5148,7 +5148,7 @@
       </c>
       <c r="I60" s="10"/>
     </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B61" s="3" t="s">
         <v>29</v>
       </c>
@@ -5168,7 +5168,7 @@
       </c>
       <c r="I61" s="10"/>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B62" s="3" t="s">
         <v>29</v>
       </c>
@@ -5188,7 +5188,7 @@
       </c>
       <c r="I62" s="10"/>
     </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B63" s="3" t="s">
         <v>29</v>
       </c>
@@ -5208,7 +5208,7 @@
       </c>
       <c r="I63" s="10"/>
     </row>
-    <row r="64" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B64" s="3" t="s">
         <v>29</v>
       </c>
@@ -5228,7 +5228,7 @@
       </c>
       <c r="I64" s="28"/>
     </row>
-    <row r="65" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B65" s="3" t="s">
         <v>29</v>
       </c>
@@ -5248,7 +5248,7 @@
       </c>
       <c r="I65" s="10"/>
     </row>
-    <row r="66" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B66" s="3" t="s">
         <v>29</v>
       </c>
@@ -5268,7 +5268,7 @@
       </c>
       <c r="I66" s="10"/>
     </row>
-    <row r="67" spans="2:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:16" ht="15" x14ac:dyDescent="0.25">
       <c r="B67" s="27" t="s">
         <v>142</v>
       </c>
@@ -5281,7 +5281,7 @@
       <c r="I67" s="27"/>
       <c r="J67" s="27"/>
     </row>
-    <row r="68" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B68" s="3" t="s">
         <v>29</v>
       </c>
@@ -5301,7 +5301,7 @@
       </c>
       <c r="I68" s="10"/>
     </row>
-    <row r="69" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B69" s="3" t="s">
         <v>29</v>
       </c>
@@ -5321,7 +5321,7 @@
       </c>
       <c r="I69" s="10"/>
     </row>
-    <row r="70" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B70" s="3" t="s">
         <v>29</v>
       </c>
@@ -5341,7 +5341,7 @@
       </c>
       <c r="I70" s="10"/>
     </row>
-    <row r="71" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B71" s="3" t="s">
         <v>29</v>
       </c>
@@ -5361,7 +5361,7 @@
       </c>
       <c r="I71" s="10"/>
     </row>
-    <row r="72" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B72" s="3" t="s">
         <v>29</v>
       </c>
@@ -5381,7 +5381,7 @@
       </c>
       <c r="I72" s="28"/>
     </row>
-    <row r="73" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B73" s="3" t="s">
         <v>29</v>
       </c>
@@ -5401,7 +5401,7 @@
       </c>
       <c r="I73" s="28"/>
     </row>
-    <row r="74" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B74" s="3" t="s">
         <v>29</v>
       </c>
@@ -5421,7 +5421,7 @@
       </c>
       <c r="I74" s="28"/>
     </row>
-    <row r="75" spans="2:16" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:16" ht="15" x14ac:dyDescent="0.25">
       <c r="B75" s="27" t="s">
         <v>143</v>
       </c>
@@ -5434,7 +5434,7 @@
       <c r="I75" s="27"/>
       <c r="J75" s="27"/>
     </row>
-    <row r="76" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B76" s="3" t="s">
         <v>29</v>
       </c>
@@ -5454,7 +5454,7 @@
       </c>
       <c r="I76" s="10"/>
     </row>
-    <row r="77" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B77" s="3" t="s">
         <v>29</v>
       </c>
@@ -5474,7 +5474,7 @@
       </c>
       <c r="I77" s="10"/>
     </row>
-    <row r="78" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B78" s="3" t="s">
         <v>29</v>
       </c>
@@ -5494,26 +5494,26 @@
       </c>
       <c r="I78" s="10"/>
     </row>
-    <row r="79" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:16" x14ac:dyDescent="0.2">
       <c r="D79" s="1"/>
       <c r="P79" s="22"/>
     </row>
-    <row r="80" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:16" x14ac:dyDescent="0.2">
       <c r="P80" s="22"/>
     </row>
-    <row r="81" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:18" x14ac:dyDescent="0.2">
       <c r="P81" s="22"/>
     </row>
-    <row r="82" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:18" x14ac:dyDescent="0.2">
       <c r="P82" s="22"/>
     </row>
-    <row r="83" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:18" x14ac:dyDescent="0.2">
       <c r="P83" s="22"/>
     </row>
-    <row r="84" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:18" x14ac:dyDescent="0.2">
       <c r="P84" s="22"/>
     </row>
-    <row r="85" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="7" t="s">
@@ -5528,7 +5528,7 @@
       <c r="K85" s="9"/>
       <c r="L85" s="1"/>
     </row>
-    <row r="86" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B86" s="11" t="s">
         <v>1</v>
       </c>
@@ -5581,7 +5581,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="87" spans="2:18" ht="21" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:18" ht="33.75" x14ac:dyDescent="0.2">
       <c r="B87" s="40" t="s">
         <v>32</v>
       </c>
@@ -5632,7 +5632,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="88" spans="2:18" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:18" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B88" s="39" t="s">
         <v>36</v>
       </c>
@@ -5679,7 +5679,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="89" spans="2:18" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B89" s="27" t="s">
         <v>136</v>
       </c>
@@ -5700,7 +5700,7 @@
       <c r="Q89" s="27"/>
       <c r="R89" s="27"/>
     </row>
-    <row r="90" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B90" s="53" t="str">
         <f>D7</f>
         <v>T-MOT-ICE_GSL01</v>
@@ -5756,7 +5756,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="91" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B91" s="53" t="str">
         <f>D8</f>
         <v>T-MOT-EV_ELC01</v>
@@ -5812,7 +5812,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="92" spans="2:18" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B92" s="27" t="s">
         <v>137</v>
       </c>
@@ -5833,7 +5833,7 @@
       <c r="Q92" s="27"/>
       <c r="R92" s="27"/>
     </row>
-    <row r="93" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B93" s="53" t="str">
         <f t="shared" ref="B93:B111" si="0">D10</f>
         <v>T-CAR-ICE_GSL21</v>
@@ -5889,7 +5889,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="94" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B94" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-ICE_DST21</v>
@@ -5945,7 +5945,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="95" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B95" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-ICE_DF21</v>
@@ -6001,7 +6001,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="96" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B96" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-ICE_NGB21</v>
@@ -6057,7 +6057,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="97" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B97" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-ICE_E8521</v>
@@ -6113,7 +6113,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="98" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B98" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-ICE_B10021</v>
@@ -6169,7 +6169,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="99" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B99" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-HEV_GSL21</v>
@@ -6225,7 +6225,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="100" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B100" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-HEV_DST21</v>
@@ -6281,7 +6281,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="101" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B101" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-PHEV10_GSL21</v>
@@ -6337,7 +6337,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="102" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B102" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-PHEV20_GSL21</v>
@@ -6393,7 +6393,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="103" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B103" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-PHEV40_GSL21</v>
@@ -6449,7 +6449,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="104" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B104" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-PHEV10_DST21</v>
@@ -6505,7 +6505,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="105" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B105" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-PHEV20_DST21</v>
@@ -6561,7 +6561,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="106" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B106" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-PHEV40_DST21</v>
@@ -6617,7 +6617,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="107" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B107" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-BEV100_ELC21</v>
@@ -6673,7 +6673,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="108" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B108" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-EV150_ELC21</v>
@@ -6729,7 +6729,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="109" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B109" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-EV250_ELC21</v>
@@ -6785,7 +6785,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="110" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B110" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-ICE_HYD21</v>
@@ -6841,7 +6841,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="111" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B111" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-FCV_HYD21</v>
@@ -6897,7 +6897,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="112" spans="2:18" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B112" s="27" t="s">
         <v>138</v>
       </c>
@@ -6918,7 +6918,7 @@
       <c r="Q112" s="27"/>
       <c r="R112" s="27"/>
     </row>
-    <row r="113" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B113" s="53" t="str">
         <f t="shared" ref="B113:B131" si="1">D30</f>
         <v>T-TAX-ICE_GSL31</v>
@@ -6974,10 +6974,10 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="114" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B114" s="53" t="str">
         <f t="shared" si="1"/>
-        <v>T- TAX-ICE_DST31</v>
+        <v>T-TAX-ICE_DST31</v>
       </c>
       <c r="C114" s="1" t="str">
         <f>Commodities!B20</f>
@@ -7030,10 +7030,10 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="115" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B115" s="53" t="str">
         <f t="shared" si="1"/>
-        <v>T- TAX-ICE_DF31</v>
+        <v>T-TAX-ICE_DF31</v>
       </c>
       <c r="C115" s="1" t="str">
         <f>Commodities!B9&amp;","&amp;Commodities!B13</f>
@@ -7086,10 +7086,10 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="116" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B116" s="53" t="str">
         <f t="shared" si="1"/>
-        <v>T- TAX-ICE_NGB31</v>
+        <v>T-TAX-ICE_NGB31</v>
       </c>
       <c r="C116" s="1" t="str">
         <f>Commodities!B22</f>
@@ -7142,10 +7142,10 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="117" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B117" s="53" t="str">
         <f t="shared" si="1"/>
-        <v>T- TAX-ICE_E8531</v>
+        <v>T-TAX-ICE_E8531</v>
       </c>
       <c r="C117" s="1" t="str">
         <f>Commodities!B21</f>
@@ -7198,10 +7198,10 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="118" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B118" s="53" t="str">
         <f t="shared" si="1"/>
-        <v>T- TAX-ICE_B10031</v>
+        <v>T-TAX-ICE_B10031</v>
       </c>
       <c r="C118" s="1" t="str">
         <f>Commodities!B12</f>
@@ -7254,10 +7254,10 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="119" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B119" s="53" t="str">
         <f t="shared" si="1"/>
-        <v>T- TAX-HEV_GSL31</v>
+        <v>T-TAX-HEV_GSL31</v>
       </c>
       <c r="C119" s="1" t="str">
         <f>Commodities!B19</f>
@@ -7310,10 +7310,10 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="120" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B120" s="53" t="str">
         <f t="shared" si="1"/>
-        <v>T- TAX-HEV_DST31</v>
+        <v>T-TAX-HEV_DST31</v>
       </c>
       <c r="C120" s="1" t="str">
         <f>Commodities!B20</f>
@@ -7366,10 +7366,10 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="121" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B121" s="53" t="str">
         <f t="shared" si="1"/>
-        <v>T- TAX-PHEV10_GSL31</v>
+        <v>T-TAX-PHEV10_GSL31</v>
       </c>
       <c r="C121" s="1" t="str">
         <f>Commodities!B19&amp;","&amp;Commodities!B15</f>
@@ -7422,10 +7422,10 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="122" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B122" s="53" t="str">
         <f t="shared" si="1"/>
-        <v>T- TAX-PHEV20_GSL31</v>
+        <v>T-TAX-PHEV20_GSL31</v>
       </c>
       <c r="C122" s="1" t="str">
         <f>Commodities!B19&amp;","&amp;Commodities!B15</f>
@@ -7478,10 +7478,10 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="123" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B123" s="53" t="str">
         <f t="shared" si="1"/>
-        <v>T- TAX-PHEV40_GSL31</v>
+        <v>T-TAX-PHEV40_GSL31</v>
       </c>
       <c r="C123" s="1" t="str">
         <f>Commodities!B19&amp;","&amp;Commodities!B15</f>
@@ -7534,10 +7534,10 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="124" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B124" s="53" t="str">
         <f t="shared" si="1"/>
-        <v>T- TAX-PHEV10_DST31</v>
+        <v>T-TAX-PHEV10_DST31</v>
       </c>
       <c r="C124" s="1" t="str">
         <f>Commodities!B20&amp;","&amp;Commodities!B15</f>
@@ -7590,10 +7590,10 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="125" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B125" s="53" t="str">
         <f t="shared" si="1"/>
-        <v>T- TAX-PHEV20_DST31</v>
+        <v>T-TAX-PHEV20_DST31</v>
       </c>
       <c r="C125" s="1" t="str">
         <f>Commodities!B20&amp;","&amp;Commodities!B15</f>
@@ -7646,10 +7646,10 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="126" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B126" s="53" t="str">
         <f t="shared" si="1"/>
-        <v>T- TAX-PHEV40_DST31</v>
+        <v>T-TAX-PHEV40_DST31</v>
       </c>
       <c r="C126" s="1" t="str">
         <f>Commodities!B20&amp;","&amp;Commodities!B15</f>
@@ -7702,10 +7702,10 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="127" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B127" s="53" t="str">
         <f t="shared" si="1"/>
-        <v>T- TAX-EV100_ELC31</v>
+        <v>T-TAX-EV100_ELC31</v>
       </c>
       <c r="C127" s="1" t="str">
         <f>Commodities!B15</f>
@@ -7758,10 +7758,10 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="128" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B128" s="53" t="str">
         <f t="shared" si="1"/>
-        <v>T- TAX-EV150_ELC31</v>
+        <v>T-TAX-EV150_ELC31</v>
       </c>
       <c r="C128" s="1" t="str">
         <f>Commodities!B15</f>
@@ -7814,10 +7814,10 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="129" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B129" s="53" t="str">
         <f t="shared" si="1"/>
-        <v>T- TAX-EV250_ELC31</v>
+        <v>T-TAX-EV250_ELC31</v>
       </c>
       <c r="C129" s="1" t="str">
         <f>Commodities!B15</f>
@@ -7870,10 +7870,10 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="130" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B130" s="53" t="str">
         <f t="shared" si="1"/>
-        <v>T- TAX-ICE_HYD31</v>
+        <v>T-TAX-ICE_HYD31</v>
       </c>
       <c r="C130" s="1" t="str">
         <f>Commodities!B17</f>
@@ -7926,10 +7926,10 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="131" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B131" s="53" t="str">
         <f t="shared" si="1"/>
-        <v>T- TAX-FCV_HYD31</v>
+        <v>T-TAX-FCV_HYD31</v>
       </c>
       <c r="C131" s="1" t="str">
         <f>Commodities!B17</f>
@@ -7982,7 +7982,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="132" spans="2:18" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B132" s="27" t="s">
         <v>139</v>
       </c>
@@ -8003,7 +8003,7 @@
       <c r="Q132" s="27"/>
       <c r="R132" s="27"/>
     </row>
-    <row r="133" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B133" s="53" t="str">
         <f>D50</f>
         <v>T-BUS-ICE_DST41</v>
@@ -8059,7 +8059,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="134" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B134" s="53" t="str">
         <f>D51</f>
         <v>T-BUS-ICE_B10041</v>
@@ -8115,7 +8115,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="135" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B135" s="53" t="str">
         <f>D52</f>
         <v>T-BUS-ICE_NGB41</v>
@@ -8171,7 +8171,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="136" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B136" s="53" t="str">
         <f>D53</f>
         <v>T-BUS-BEV_ELC41</v>
@@ -8227,7 +8227,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="137" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B137" s="53" t="str">
         <f>D54</f>
         <v>T-BUS-FCV_HYD41</v>
@@ -8283,7 +8283,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="138" spans="2:18" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B138" s="27" t="s">
         <v>140</v>
       </c>
@@ -8304,7 +8304,7 @@
       <c r="Q138" s="27"/>
       <c r="R138" s="27"/>
     </row>
-    <row r="139" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B139" s="53" t="str">
         <f>D56</f>
         <v>T-LPT-EV_ELC51</v>
@@ -8360,7 +8360,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="140" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B140" s="53" t="str">
         <f>D57</f>
         <v>T-HPT-EV_ELC51</v>
@@ -8416,7 +8416,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="141" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B141" s="53" t="str">
         <f>D58</f>
         <v>T-HPT-ICE_DST51</v>
@@ -8472,7 +8472,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="142" spans="2:18" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B142" s="27" t="s">
         <v>141</v>
       </c>
@@ -8493,7 +8493,7 @@
       <c r="Q142" s="27"/>
       <c r="R142" s="27"/>
     </row>
-    <row r="143" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B143" s="54" t="str">
         <f t="shared" ref="B143:B149" si="2">D60</f>
         <v>T-LGT-ICE_DST61</v>
@@ -8549,7 +8549,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="144" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B144" s="54" t="str">
         <f t="shared" si="2"/>
         <v>T-LGT-HEV_DST61</v>
@@ -8605,7 +8605,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="145" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B145" s="54" t="str">
         <f t="shared" si="2"/>
         <v>T-LGT-PHEV_DST61</v>
@@ -8661,7 +8661,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="146" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B146" s="54" t="str">
         <f t="shared" si="2"/>
         <v>T-LGT-ICE_NBG61</v>
@@ -8717,7 +8717,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="147" spans="2:18" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B147" s="54" t="str">
         <f t="shared" si="2"/>
         <v>T-LGT-PHEV_NGB61</v>
@@ -8773,7 +8773,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="148" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B148" s="54" t="str">
         <f t="shared" si="2"/>
         <v>T-LGT-FCV_HYD61</v>
@@ -8829,7 +8829,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="149" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B149" s="54" t="str">
         <f t="shared" si="2"/>
         <v>T-LGT-BEV_ELC61</v>
@@ -8885,7 +8885,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="150" spans="2:18" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B150" s="27" t="s">
         <v>142</v>
       </c>
@@ -8906,7 +8906,7 @@
       <c r="Q150" s="27"/>
       <c r="R150" s="27"/>
     </row>
-    <row r="151" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B151" s="54" t="str">
         <f t="shared" ref="B151:B157" si="3">D68</f>
         <v>T-HGT-ICE_DST71</v>
@@ -8962,7 +8962,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="152" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B152" s="54" t="str">
         <f t="shared" si="3"/>
         <v>T-HGT-HEV_DST71</v>
@@ -9018,7 +9018,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="153" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B153" s="54" t="str">
         <f t="shared" si="3"/>
         <v>T-HGT-FCV_HYD71</v>
@@ -9074,7 +9074,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="154" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B154" s="54" t="str">
         <f t="shared" si="3"/>
         <v>T-HGT-ICE_NGB71</v>
@@ -9130,7 +9130,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="155" spans="2:18" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B155" s="54" t="str">
         <f t="shared" si="3"/>
         <v>T-HGT-HEV_NGB71</v>
@@ -9186,7 +9186,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="156" spans="2:18" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B156" s="54" t="str">
         <f t="shared" si="3"/>
         <v>T-HGT-ICE_LNG71</v>
@@ -9242,7 +9242,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="157" spans="2:18" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B157" s="54" t="str">
         <f t="shared" si="3"/>
         <v>T-HGT-BEV_ELC71</v>
@@ -9298,7 +9298,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="158" spans="2:18" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="B158" s="27" t="s">
         <v>143</v>
       </c>
@@ -9319,7 +9319,7 @@
       <c r="Q158" s="27"/>
       <c r="R158" s="27"/>
     </row>
-    <row r="159" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B159" s="53" t="str">
         <f>D76</f>
         <v>T-GTR-ICE_DST81</v>
@@ -9375,7 +9375,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="160" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:18" ht="15" x14ac:dyDescent="0.25">
       <c r="B160" s="53" t="str">
         <f>D77</f>
         <v>T-GTR-EV_ELC81</v>
@@ -9431,7 +9431,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="161" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B161" s="61" t="str">
         <f>D78</f>
         <v>T-GTR-FCV_HYD81</v>
@@ -9487,13 +9487,13 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="162" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:38" x14ac:dyDescent="0.2">
       <c r="B162" s="1"/>
     </row>
-    <row r="163" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:38" x14ac:dyDescent="0.2">
       <c r="B163" s="1"/>
     </row>
-    <row r="167" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:38" x14ac:dyDescent="0.2">
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
       <c r="D167" s="1"/>
@@ -9520,7 +9520,7 @@
       <c r="Y167" s="1"/>
       <c r="Z167" s="1"/>
     </row>
-    <row r="168" spans="2:38" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:38" x14ac:dyDescent="0.2">
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
       <c r="D168" s="1"/>
@@ -9547,7 +9547,7 @@
       <c r="Y168" s="1"/>
       <c r="Z168" s="1"/>
     </row>
-    <row r="169" spans="2:38" ht="21" x14ac:dyDescent="0.4">
+    <row r="169" spans="2:38" ht="21" x14ac:dyDescent="0.35">
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
       <c r="D169" s="1"/>
@@ -9587,7 +9587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="2:38" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:38" ht="15" x14ac:dyDescent="0.2">
       <c r="B170" s="24" t="s">
         <v>1</v>
       </c>
@@ -9721,7 +9721,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="171" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B171" s="58" t="str">
         <f>B95</f>
         <v>T-CAR-ICE_DF21</v>
@@ -9832,7 +9832,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="172" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B172" s="58" t="str">
         <f t="shared" ref="B172:B177" si="6">B101</f>
         <v>T-CAR-PHEV10_GSL21</v>
@@ -9943,7 +9943,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="173" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B173" s="58" t="str">
         <f t="shared" si="6"/>
         <v>T-CAR-PHEV20_GSL21</v>
@@ -10054,7 +10054,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="174" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B174" s="58" t="str">
         <f t="shared" si="6"/>
         <v>T-CAR-PHEV40_GSL21</v>
@@ -10165,7 +10165,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="175" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B175" s="58" t="str">
         <f t="shared" si="6"/>
         <v>T-CAR-PHEV10_DST21</v>
@@ -10276,7 +10276,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="176" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B176" s="58" t="str">
         <f t="shared" si="6"/>
         <v>T-CAR-PHEV20_DST21</v>
@@ -10387,7 +10387,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="177" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B177" s="58" t="str">
         <f t="shared" si="6"/>
         <v>T-CAR-PHEV40_DST21</v>
@@ -10498,10 +10498,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="178" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B178" s="58" t="str">
         <f>B115</f>
-        <v>T- TAX-ICE_DF31</v>
+        <v>T-TAX-ICE_DF31</v>
       </c>
       <c r="C178" s="1" t="str">
         <f>Commodities!B13</f>
@@ -10596,7 +10596,7 @@
       </c>
       <c r="AI178" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>T- TAX-ICE_DF31</v>
+        <v>T-TAX-ICE_DF31</v>
       </c>
       <c r="AJ178" s="1" t="str">
         <f t="shared" si="5"/>
@@ -10609,10 +10609,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="179" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B179" s="58" t="str">
         <f>B121</f>
-        <v>T- TAX-PHEV10_GSL31</v>
+        <v>T-TAX-PHEV10_GSL31</v>
       </c>
       <c r="C179" s="1" t="str">
         <f>Commodities!B15</f>
@@ -10707,7 +10707,7 @@
       </c>
       <c r="AI179" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>T- TAX-PHEV10_GSL31</v>
+        <v>T-TAX-PHEV10_GSL31</v>
       </c>
       <c r="AJ179" s="1" t="str">
         <f t="shared" si="5"/>
@@ -10720,10 +10720,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="180" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B180" s="58" t="str">
         <f t="shared" ref="B180:B184" si="7">B122</f>
-        <v>T- TAX-PHEV20_GSL31</v>
+        <v>T-TAX-PHEV20_GSL31</v>
       </c>
       <c r="C180" s="1" t="str">
         <f>Commodities!B15</f>
@@ -10818,7 +10818,7 @@
       </c>
       <c r="AI180" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>T- TAX-PHEV20_GSL31</v>
+        <v>T-TAX-PHEV20_GSL31</v>
       </c>
       <c r="AJ180" s="1" t="str">
         <f t="shared" si="5"/>
@@ -10831,10 +10831,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="181" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B181" s="58" t="str">
         <f t="shared" si="7"/>
-        <v>T- TAX-PHEV40_GSL31</v>
+        <v>T-TAX-PHEV40_GSL31</v>
       </c>
       <c r="C181" s="1" t="str">
         <f>Commodities!B15</f>
@@ -10929,7 +10929,7 @@
       </c>
       <c r="AI181" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>T- TAX-PHEV40_GSL31</v>
+        <v>T-TAX-PHEV40_GSL31</v>
       </c>
       <c r="AJ181" s="1" t="str">
         <f t="shared" si="5"/>
@@ -10942,10 +10942,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="182" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B182" s="58" t="str">
         <f t="shared" si="7"/>
-        <v>T- TAX-PHEV10_DST31</v>
+        <v>T-TAX-PHEV10_DST31</v>
       </c>
       <c r="C182" s="1" t="str">
         <f>Commodities!B15</f>
@@ -11040,7 +11040,7 @@
       </c>
       <c r="AI182" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>T- TAX-PHEV10_DST31</v>
+        <v>T-TAX-PHEV10_DST31</v>
       </c>
       <c r="AJ182" s="1" t="str">
         <f t="shared" si="5"/>
@@ -11053,10 +11053,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="183" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B183" s="58" t="str">
         <f t="shared" si="7"/>
-        <v>T- TAX-PHEV20_DST31</v>
+        <v>T-TAX-PHEV20_DST31</v>
       </c>
       <c r="C183" s="1" t="str">
         <f>Commodities!B15</f>
@@ -11151,7 +11151,7 @@
       </c>
       <c r="AI183" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>T- TAX-PHEV20_DST31</v>
+        <v>T-TAX-PHEV20_DST31</v>
       </c>
       <c r="AJ183" s="1" t="str">
         <f t="shared" si="5"/>
@@ -11164,10 +11164,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="184" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B184" s="58" t="str">
         <f t="shared" si="7"/>
-        <v>T- TAX-PHEV40_DST31</v>
+        <v>T-TAX-PHEV40_DST31</v>
       </c>
       <c r="C184" s="1" t="str">
         <f>Commodities!B15</f>
@@ -11262,7 +11262,7 @@
       </c>
       <c r="AI184" s="1" t="str">
         <f t="shared" si="4"/>
-        <v>T- TAX-PHEV40_DST31</v>
+        <v>T-TAX-PHEV40_DST31</v>
       </c>
       <c r="AJ184" s="1" t="str">
         <f t="shared" si="5"/>
@@ -11275,7 +11275,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="185" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B185" s="58" t="str">
         <f>B145</f>
         <v>T-LGT-PHEV_DST61</v>
@@ -11386,7 +11386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B186" s="71" t="str">
         <f>B147</f>
         <v>T-LGT-PHEV_NGB61</v>
@@ -11497,7 +11497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="187" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B187" s="58"/>
       <c r="C187" s="1"/>
       <c r="D187" s="59"/>
@@ -11529,7 +11529,7 @@
       <c r="AE187" s="60"/>
       <c r="AF187" s="60"/>
     </row>
-    <row r="188" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B188" s="58"/>
       <c r="C188" s="1"/>
       <c r="D188" s="59"/>
@@ -11561,7 +11561,7 @@
       <c r="AE188" s="60"/>
       <c r="AF188" s="60"/>
     </row>
-    <row r="189" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B189" s="58"/>
       <c r="C189" s="1"/>
       <c r="D189" s="59"/>
@@ -11593,7 +11593,7 @@
       <c r="AD189" s="42"/>
       <c r="AE189" s="42"/>
     </row>
-    <row r="190" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B190" s="58"/>
       <c r="C190" s="1"/>
       <c r="D190" s="59"/>
@@ -11625,7 +11625,7 @@
       <c r="AD190" s="42"/>
       <c r="AE190" s="42"/>
     </row>
-    <row r="191" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B191" s="63"/>
       <c r="C191" s="64"/>
       <c r="D191" s="65"/>
@@ -11657,7 +11657,7 @@
       <c r="AD191" s="66"/>
       <c r="AE191" s="66"/>
     </row>
-    <row r="192" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:38" ht="15" x14ac:dyDescent="0.25">
       <c r="B192" s="63"/>
       <c r="C192" s="64"/>
       <c r="D192" s="65"/>
@@ -11689,7 +11689,7 @@
       <c r="AD192" s="66"/>
       <c r="AE192" s="66"/>
     </row>
-    <row r="193" spans="2:32" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:32" ht="15" x14ac:dyDescent="0.25">
       <c r="B193" s="63"/>
       <c r="C193" s="64"/>
       <c r="D193" s="65"/>
@@ -11721,7 +11721,7 @@
       <c r="AD193" s="66"/>
       <c r="AE193" s="66"/>
     </row>
-    <row r="194" spans="2:32" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:32" ht="15" x14ac:dyDescent="0.25">
       <c r="B194" s="63"/>
       <c r="C194" s="64"/>
       <c r="D194" s="65"/>
@@ -11753,7 +11753,7 @@
       <c r="AD194" s="66"/>
       <c r="AE194" s="66"/>
     </row>
-    <row r="195" spans="2:32" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:32" ht="15" x14ac:dyDescent="0.25">
       <c r="B195" s="63"/>
       <c r="C195" s="64"/>
       <c r="D195" s="65"/>
@@ -11785,7 +11785,7 @@
       <c r="AD195" s="66"/>
       <c r="AE195" s="66"/>
     </row>
-    <row r="196" spans="2:32" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:32" ht="15" x14ac:dyDescent="0.25">
       <c r="B196" s="63"/>
       <c r="C196" s="64"/>
       <c r="D196" s="65"/>
@@ -11817,7 +11817,7 @@
       <c r="AD196" s="66"/>
       <c r="AE196" s="66"/>
     </row>
-    <row r="197" spans="2:32" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:32" ht="15" x14ac:dyDescent="0.25">
       <c r="B197" s="63"/>
       <c r="C197" s="64"/>
       <c r="D197" s="65"/>
@@ -11849,7 +11849,7 @@
       <c r="AD197" s="67"/>
       <c r="AE197" s="67"/>
     </row>
-    <row r="198" spans="2:32" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:32" ht="15" x14ac:dyDescent="0.25">
       <c r="B198" s="63"/>
       <c r="C198" s="64"/>
       <c r="D198" s="65"/>
@@ -11881,7 +11881,7 @@
       <c r="AD198" s="67"/>
       <c r="AE198" s="67"/>
     </row>
-    <row r="199" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B199" s="64"/>
       <c r="C199" s="64"/>
       <c r="D199" s="65"/>
@@ -11913,7 +11913,7 @@
       <c r="AD199" s="67"/>
       <c r="AE199" s="67"/>
     </row>
-    <row r="200" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B200" s="64"/>
       <c r="C200" s="64"/>
       <c r="D200" s="65"/>
@@ -11945,7 +11945,7 @@
       <c r="AD200" s="67"/>
       <c r="AE200" s="67"/>
     </row>
-    <row r="201" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
       <c r="D201" s="1"/>
@@ -11978,8 +11978,8 @@
       <c r="AE201" s="1"/>
       <c r="AF201" s="1"/>
     </row>
-    <row r="202" spans="2:32" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="203" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:32" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="203" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
       <c r="D203" s="1"/>
@@ -12012,7 +12012,7 @@
       <c r="AE203" s="1"/>
       <c r="AF203" s="1"/>
     </row>
-    <row r="204" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
       <c r="D204" s="1"/>
@@ -12045,7 +12045,7 @@
       <c r="AE204" s="1"/>
       <c r="AF204" s="1"/>
     </row>
-    <row r="205" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
       <c r="D205" s="1"/>
@@ -12078,7 +12078,7 @@
       <c r="AE205" s="1"/>
       <c r="AF205" s="1"/>
     </row>
-    <row r="206" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
       <c r="D206" s="1"/>
@@ -12111,7 +12111,7 @@
       <c r="AE206" s="1"/>
       <c r="AF206" s="1"/>
     </row>
-    <row r="207" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
       <c r="D207" s="1"/>
@@ -12144,7 +12144,7 @@
       <c r="AE207" s="1"/>
       <c r="AF207" s="1"/>
     </row>
-    <row r="208" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
       <c r="D208" s="1"/>
@@ -12177,7 +12177,7 @@
       <c r="AE208" s="1"/>
       <c r="AF208" s="1"/>
     </row>
-    <row r="209" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
       <c r="D209" s="1"/>
@@ -12210,7 +12210,7 @@
       <c r="AE209" s="1"/>
       <c r="AF209" s="1"/>
     </row>
-    <row r="210" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
       <c r="D210" s="1"/>
@@ -12243,7 +12243,7 @@
       <c r="AE210" s="1"/>
       <c r="AF210" s="1"/>
     </row>
-    <row r="211" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
       <c r="D211" s="1"/>
@@ -12276,7 +12276,7 @@
       <c r="AE211" s="1"/>
       <c r="AF211" s="1"/>
     </row>
-    <row r="212" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
       <c r="D212" s="1"/>
@@ -12309,7 +12309,7 @@
       <c r="AE212" s="1"/>
       <c r="AF212" s="1"/>
     </row>
-    <row r="213" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
       <c r="D213" s="1"/>
@@ -12336,7 +12336,7 @@
       <c r="Y213" s="1"/>
       <c r="Z213" s="1"/>
     </row>
-    <row r="214" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
       <c r="D214" s="1"/>
@@ -12363,7 +12363,7 @@
       <c r="Y214" s="1"/>
       <c r="Z214" s="1"/>
     </row>
-    <row r="215" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
       <c r="D215" s="1"/>
@@ -12390,7 +12390,7 @@
       <c r="Y215" s="1"/>
       <c r="Z215" s="1"/>
     </row>
-    <row r="216" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
       <c r="D216" s="1"/>
@@ -12417,7 +12417,7 @@
       <c r="Y216" s="1"/>
       <c r="Z216" s="1"/>
     </row>
-    <row r="217" spans="2:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:32" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
       <c r="D217" s="1"/>
@@ -12444,7 +12444,7 @@
       <c r="Y217" s="1"/>
       <c r="Z217" s="1"/>
     </row>
-    <row r="218" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
       <c r="D218" s="1"/>
@@ -12471,7 +12471,7 @@
       <c r="Y218" s="1"/>
       <c r="Z218" s="1"/>
     </row>
-    <row r="219" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B219" s="1"/>
       <c r="C219" s="1"/>
       <c r="D219" s="1"/>
@@ -12498,7 +12498,7 @@
       <c r="Y219" s="1"/>
       <c r="Z219" s="1"/>
     </row>
-    <row r="220" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B220" s="1"/>
       <c r="C220" s="1"/>
       <c r="D220" s="1"/>
@@ -12525,7 +12525,7 @@
       <c r="Y220" s="1"/>
       <c r="Z220" s="1"/>
     </row>
-    <row r="221" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B221" s="1"/>
       <c r="C221" s="1"/>
       <c r="D221" s="1"/>
@@ -12552,7 +12552,7 @@
       <c r="Y221" s="1"/>
       <c r="Z221" s="1"/>
     </row>
-    <row r="222" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>
       <c r="D222" s="1"/>
@@ -12579,7 +12579,7 @@
       <c r="Y222" s="1"/>
       <c r="Z222" s="1"/>
     </row>
-    <row r="223" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
       <c r="D223" s="1"/>
@@ -12606,7 +12606,7 @@
       <c r="Y223" s="1"/>
       <c r="Z223" s="1"/>
     </row>
-    <row r="224" spans="2:32" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B224" s="1"/>
       <c r="C224" s="1"/>
       <c r="D224" s="1"/>
@@ -12633,7 +12633,7 @@
       <c r="Y224" s="1"/>
       <c r="Z224" s="1"/>
     </row>
-    <row r="225" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>
       <c r="D225" s="1"/>
@@ -12660,7 +12660,7 @@
       <c r="Y225" s="1"/>
       <c r="Z225" s="1"/>
     </row>
-    <row r="226" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B226" s="1"/>
       <c r="C226" s="1"/>
       <c r="D226" s="1"/>
@@ -12687,7 +12687,7 @@
       <c r="Y226" s="1"/>
       <c r="Z226" s="1"/>
     </row>
-    <row r="227" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B227" s="1"/>
       <c r="C227" s="1"/>
       <c r="D227" s="1"/>
@@ -12714,7 +12714,7 @@
       <c r="Y227" s="1"/>
       <c r="Z227" s="1"/>
     </row>
-    <row r="228" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B228" s="1"/>
       <c r="C228" s="1"/>
       <c r="D228" s="1"/>
@@ -12741,7 +12741,7 @@
       <c r="Y228" s="1"/>
       <c r="Z228" s="1"/>
     </row>
-    <row r="229" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B229" s="1"/>
       <c r="C229" s="1"/>
       <c r="D229" s="1"/>
@@ -12768,10 +12768,10 @@
       <c r="Y229" s="1"/>
       <c r="Z229" s="1"/>
     </row>
-    <row r="230" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="231" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="232" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="233" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="231" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="232" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="233" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B233" s="1"/>
       <c r="C233" s="1"/>
       <c r="D233" s="1"/>
@@ -12798,7 +12798,7 @@
       <c r="Y233" s="1"/>
       <c r="Z233" s="1"/>
     </row>
-    <row r="234" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B234" s="1"/>
       <c r="C234" s="1"/>
       <c r="D234" s="1"/>
@@ -12825,7 +12825,7 @@
       <c r="Y234" s="1"/>
       <c r="Z234" s="1"/>
     </row>
-    <row r="235" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B235" s="1"/>
       <c r="C235" s="1"/>
       <c r="D235" s="1"/>
@@ -12852,7 +12852,7 @@
       <c r="Y235" s="1"/>
       <c r="Z235" s="1"/>
     </row>
-    <row r="236" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B236" s="1"/>
       <c r="C236" s="1"/>
       <c r="D236" s="1"/>
@@ -12879,7 +12879,7 @@
       <c r="Y236" s="1"/>
       <c r="Z236" s="1"/>
     </row>
-    <row r="237" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B237" s="1"/>
       <c r="C237" s="1"/>
       <c r="D237" s="1"/>
@@ -12906,7 +12906,7 @@
       <c r="Y237" s="1"/>
       <c r="Z237" s="1"/>
     </row>
-    <row r="238" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B238" s="1"/>
       <c r="C238" s="1"/>
       <c r="D238" s="1"/>
@@ -12933,7 +12933,7 @@
       <c r="Y238" s="1"/>
       <c r="Z238" s="1"/>
     </row>
-    <row r="239" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B239" s="1"/>
       <c r="C239" s="1"/>
       <c r="D239" s="1"/>
@@ -12960,7 +12960,7 @@
       <c r="Y239" s="1"/>
       <c r="Z239" s="1"/>
     </row>
-    <row r="240" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:26" x14ac:dyDescent="0.2">
       <c r="B240" s="1"/>
       <c r="C240" s="1"/>
       <c r="D240" s="1"/>
@@ -13003,19 +13003,19 @@
       <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.21875" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" customWidth="1"/>
-    <col min="3" max="11" width="14.109375" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="11" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>146</v>
       </c>
@@ -13050,7 +13050,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>157</v>
       </c>
@@ -13085,7 +13085,7 @@
         <v>2574</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>158</v>
       </c>
@@ -13124,7 +13124,7 @@
         <v>4.044339163234481E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>159</v>
       </c>
@@ -13163,7 +13163,7 @@
         <v>7.0982279191462321E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>160</v>
       </c>
@@ -13202,7 +13202,7 @@
         <v>3.9667538813275338E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>161</v>
       </c>
@@ -13241,7 +13241,7 @@
         <v>3.4071494011901911E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>162</v>
       </c>
@@ -13280,7 +13280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>163</v>
       </c>
@@ -13319,7 +13319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>164</v>
       </c>
@@ -13358,7 +13358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>165</v>
       </c>
@@ -13397,7 +13397,7 @@
         <v>9.7889515257063141E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>166</v>
       </c>
@@ -13436,7 +13436,7 @@
         <v>2.81535528281486E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>167</v>
       </c>
@@ -13475,7 +13475,7 @@
         <v>5.7611198692605467E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>168</v>
       </c>
@@ -13514,7 +13514,7 @@
         <v>8.8694833975750467E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>169</v>
       </c>
@@ -13553,7 +13553,7 @@
         <v>1.0399729276888665E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>170</v>
       </c>
@@ -13592,7 +13592,7 @@
         <v>9.0378599668199111E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>171</v>
       </c>
@@ -13631,7 +13631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>172</v>
       </c>
@@ -13670,7 +13670,7 @@
         <v>4.9027295162475133E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>173</v>
       </c>
@@ -13709,7 +13709,7 @@
         <v>7.5934531228075966E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>174</v>
       </c>
@@ -13748,7 +13748,7 @@
         <v>5.7817542527464363E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>175</v>
       </c>
@@ -13787,7 +13787,7 @@
         <v>8.2620071477504387E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>176</v>
       </c>
@@ -13826,7 +13826,7 @@
         <v>3.8875178487417154E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>177</v>
       </c>
@@ -13865,7 +13865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>178</v>
       </c>
@@ -13904,7 +13904,7 @@
         <v>1.7844614838597853E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>179</v>
       </c>
@@ -13943,7 +13943,7 @@
         <v>3.2627087167889597E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>180</v>
       </c>
@@ -13982,7 +13982,7 @@
         <v>4.7624157085434599E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>181</v>
       </c>
@@ -14021,7 +14021,7 @@
         <v>6.1160312652178582E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>182</v>
       </c>
@@ -14060,7 +14060,7 @@
         <v>7.6570070239441387E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>183</v>
       </c>
@@ -14099,7 +14099,7 @@
         <v>4.0385615358584315E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>184</v>
       </c>
@@ -14138,7 +14138,7 @@
         <v>4.4355670741269594E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>185</v>
       </c>
@@ -14177,7 +14177,7 @@
         <v>6.0252399778799404E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>186</v>
       </c>
@@ -14216,7 +14216,7 @@
         <v>5.8395305265069287E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>187</v>
       </c>
@@ -14255,7 +14255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>188</v>
       </c>
@@ -14294,7 +14294,7 @@
         <v>2.9713512219681899E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>189</v>
       </c>
@@ -14333,7 +14333,7 @@
         <v>7.1543534422278537E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>190</v>
       </c>
@@ -14372,7 +14372,7 @@
         <v>8.253753394356084E-6</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>191</v>
       </c>
@@ -14411,7 +14411,7 @@
         <v>6.1077775118235022E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>192</v>
       </c>
@@ -14450,7 +14450,7 @@
         <v>1.5434518847445876E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>193</v>
       </c>
@@ -14489,7 +14489,7 @@
         <v>1.0143862921663627E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>194</v>
       </c>
@@ -14528,7 +14528,7 @@
         <v>9.9045040732272994E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>195</v>
       </c>
@@ -14567,7 +14567,7 @@
         <v>9.4786103980785269E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>196</v>
       </c>
@@ -14606,7 +14606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>197</v>
       </c>
@@ -14645,7 +14645,7 @@
         <v>0.1113926558102297</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>198</v>
       </c>
@@ -14684,17 +14684,17 @@
         <v>1.3948843236461781E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>147</v>
       </c>
@@ -14726,7 +14726,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>168</v>
       </c>
@@ -14758,7 +14758,7 @@
         <v>61500</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>170</v>
       </c>
@@ -14790,7 +14790,7 @@
         <v>43995</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>174</v>
       </c>
@@ -14822,7 +14822,7 @@
         <v>41670</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>182</v>
       </c>
@@ -14854,7 +14854,7 @@
         <v>37720</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>186</v>
       </c>
@@ -14886,7 +14886,7 @@
         <v>37990</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>189</v>
       </c>
@@ -14918,7 +14918,7 @@
         <v>42025</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>195</v>
       </c>
@@ -14950,7 +14950,7 @@
         <v>40395</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>197</v>
       </c>
@@ -14982,17 +14982,17 @@
         <v>73975</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="36" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>147</v>
       </c>
@@ -15024,7 +15024,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>168</v>
       </c>
@@ -15069,7 +15069,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>170</v>
       </c>
@@ -15114,7 +15114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>174</v>
       </c>
@@ -15159,7 +15159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>182</v>
       </c>
@@ -15204,7 +15204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>186</v>
       </c>
@@ -15249,7 +15249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>189</v>
       </c>
@@ -15294,7 +15294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>195</v>
       </c>
@@ -15339,7 +15339,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>197</v>
       </c>
@@ -15384,7 +15384,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="45" t="s">
         <v>201</v>
       </c>
@@ -15429,12 +15429,12 @@
         <v>931</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
         <v>147</v>
       </c>
@@ -15466,7 +15466,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>168</v>
       </c>
@@ -15511,7 +15511,7 @@
         <v>2.5412637704730561E-5</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>170</v>
       </c>
@@ -15556,7 +15556,7 @@
         <v>1.270631885236528E-5</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>174</v>
       </c>
@@ -15601,7 +15601,7 @@
         <v>2.5412637704730561E-5</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>182</v>
       </c>
@@ -15646,7 +15646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>186</v>
       </c>
@@ -15691,7 +15691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>189</v>
       </c>
@@ -15736,7 +15736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>195</v>
       </c>
@@ -15781,7 +15781,7 @@
         <v>1.1003672126148334E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>197</v>
       </c>
@@ -15826,7 +15826,7 @@
         <v>7.6237913114191687E-4</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="45" t="s">
         <v>201</v>
       </c>
@@ -15871,7 +15871,7 @@
         <v>1.1829582851552077E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A90" s="48" t="s">
         <v>65</v>
       </c>
@@ -15880,7 +15880,7 @@
         <v>21831.587082756254</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A91" s="48" t="s">
         <v>203</v>
       </c>
@@ -15889,12 +15889,12 @@
         <v>20290.14478354996</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="49" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D95" s="42"/>
       <c r="E95" s="42"/>
       <c r="F95" s="42"/>
@@ -15904,7 +15904,7 @@
       <c r="J95" s="42"/>
       <c r="K95" s="42"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B96" s="42"/>
       <c r="C96" s="42"/>
       <c r="D96" s="42"/>

</xml_diff>

<commit_message>
Modify the purchase price for heavy-duty goods vehicle
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
+++ b/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E63E08-C828-47E9-9852-9B8AFD5F4F44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A547D4BC-84C2-409A-9E0C-F3DF006A9F6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commodities" sheetId="6" r:id="rId1"/>
@@ -1425,11 +1425,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="\Te\x\t"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="\Te\x\t"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="32" x14ac:knownFonts="1">
     <font>
@@ -1777,22 +1777,22 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="18" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1802,7 +1802,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1835,7 +1835,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1848,7 +1848,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1867,44 +1867,44 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="24" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="24" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="24" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="24" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="24" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="24" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="9" fontId="14" fillId="9" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="41" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="164" fontId="25" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="41" fontId="25" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="167" fontId="24" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="24" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="3" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2576,30 +2576,30 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L162"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
       <selection activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
     <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="60.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="60.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" customWidth="1"/>
     <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="60.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" customWidth="1"/>
+    <col min="12" max="12" width="60.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="19" t="s">
         <v>41</v>
       </c>
       <c r="B1" s="20"/>
     </row>
-    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A3" s="21"/>
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
@@ -2609,7 +2609,7 @@
       <c r="G3" s="22"/>
       <c r="H3" s="22"/>
     </row>
-    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A4" s="21"/>
       <c r="B4" s="22"/>
       <c r="C4" s="22"/>
@@ -2619,7 +2619,7 @@
       <c r="G4" s="22"/>
       <c r="H4" s="22"/>
     </row>
-    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>42</v>
       </c>
@@ -2645,7 +2645,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="25" t="s">
         <v>50</v>
       </c>
@@ -2671,7 +2671,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>59</v>
       </c>
@@ -2689,7 +2689,7 @@
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="22"/>
       <c r="B8" s="74" t="s">
         <v>62</v>
@@ -2705,7 +2705,7 @@
       <c r="G8" s="22"/>
       <c r="H8" s="22"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="74" t="s">
         <v>63</v>
@@ -2721,7 +2721,7 @@
       <c r="G9" s="22"/>
       <c r="H9" s="22"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="74" t="s">
         <v>64</v>
@@ -2737,7 +2737,7 @@
       <c r="G10" s="22"/>
       <c r="H10" s="22"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="74" t="s">
         <v>66</v>
@@ -2753,7 +2753,7 @@
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
       <c r="B12" s="74" t="s">
         <v>67</v>
@@ -2769,7 +2769,7 @@
       <c r="G12" s="22"/>
       <c r="H12" s="22"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
       <c r="B13" s="74" t="s">
         <v>68</v>
@@ -2785,7 +2785,7 @@
       <c r="G13" s="22"/>
       <c r="H13" s="22"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
       <c r="B14" s="74" t="s">
         <v>70</v>
@@ -2801,7 +2801,7 @@
       <c r="G14" s="22"/>
       <c r="H14" s="22"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
       <c r="B15" s="74" t="s">
         <v>40</v>
@@ -2821,7 +2821,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="74" t="s">
         <v>144</v>
@@ -2835,7 +2835,7 @@
       <c r="E16" s="22"/>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="74" t="s">
         <v>234</v>
@@ -2849,7 +2849,7 @@
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="74" t="s">
         <v>73</v>
@@ -2866,7 +2866,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="74" t="s">
         <v>237</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="22"/>
       <c r="B20" s="74" t="s">
         <v>239</v>
@@ -2893,7 +2893,7 @@
       <c r="G20" s="69"/>
       <c r="H20" s="69"/>
     </row>
-    <row r="21" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="22"/>
       <c r="B21" s="74" t="s">
         <v>219</v>
@@ -2909,7 +2909,7 @@
       <c r="G21" s="69"/>
       <c r="H21" s="69"/>
     </row>
-    <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="29"/>
       <c r="B22" s="75" t="s">
         <v>242</v>
@@ -2925,7 +2925,7 @@
       <c r="G22" s="29"/>
       <c r="H22" s="29"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>74</v>
       </c>
@@ -2943,7 +2943,7 @@
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="22"/>
       <c r="B24" s="22" t="s">
         <v>213</v>
@@ -2960,7 +2960,7 @@
       <c r="H24" s="22"/>
       <c r="I24" s="22"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="22"/>
       <c r="B25" s="22" t="s">
         <v>215</v>
@@ -2977,7 +2977,7 @@
       <c r="H25" s="22"/>
       <c r="I25" s="22"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B26" s="22" t="s">
         <v>75</v>
       </c>
@@ -2993,7 +2993,7 @@
       <c r="H26" s="22"/>
       <c r="I26" s="22"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B27" s="22" t="s">
         <v>78</v>
       </c>
@@ -3009,7 +3009,7 @@
       <c r="H27" s="22"/>
       <c r="I27" s="22"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B28" s="22" t="s">
         <v>80</v>
       </c>
@@ -3024,7 +3024,7 @@
       <c r="G28" s="22"/>
       <c r="H28" s="22"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>82</v>
       </c>
@@ -3039,7 +3039,7 @@
       <c r="G29" s="22"/>
       <c r="H29" s="22"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>84</v>
       </c>
@@ -3054,7 +3054,7 @@
       <c r="G30" s="22"/>
       <c r="H30" s="22"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>86</v>
       </c>
@@ -3069,7 +3069,7 @@
       <c r="G31" s="22"/>
       <c r="H31" s="22"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="30"/>
       <c r="B32" s="30" t="s">
         <v>88</v>
@@ -3085,7 +3085,7 @@
       <c r="G32" s="29"/>
       <c r="H32" s="29"/>
     </row>
-    <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -3103,7 +3103,7 @@
       <c r="G33" s="22"/>
       <c r="H33" s="22"/>
     </row>
-    <row r="34" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B34" s="31" t="s">
         <v>94</v>
       </c>
@@ -3118,7 +3118,7 @@
       <c r="G34" s="22"/>
       <c r="H34" s="22"/>
     </row>
-    <row r="35" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B35" s="31" t="s">
         <v>96</v>
       </c>
@@ -3133,7 +3133,7 @@
       <c r="G35" s="22"/>
       <c r="H35" s="22"/>
     </row>
-    <row r="36" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B36" s="31" t="s">
         <v>98</v>
       </c>
@@ -3148,7 +3148,7 @@
       <c r="G36" s="22"/>
       <c r="H36" s="22"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" s="22" t="s">
         <v>100</v>
       </c>
@@ -3163,7 +3163,7 @@
       <c r="G37" s="22"/>
       <c r="H37" s="22"/>
     </row>
-    <row r="38" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="32"/>
       <c r="B38" s="33" t="s">
         <v>102</v>
@@ -3179,7 +3179,7 @@
       <c r="G38" s="33"/>
       <c r="H38" s="33"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B39" s="22"/>
       <c r="C39" s="22"/>
       <c r="D39" s="22"/>
@@ -3188,7 +3188,7 @@
       <c r="G39" s="22"/>
       <c r="H39" s="22"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B40" s="22"/>
       <c r="C40" s="22"/>
       <c r="E40" s="22"/>
@@ -3196,13 +3196,13 @@
       <c r="G40" s="22"/>
       <c r="H40" s="22"/>
     </row>
-    <row r="43" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" ht="21" x14ac:dyDescent="0.4">
       <c r="B43" s="84" t="s">
         <v>104</v>
       </c>
       <c r="C43" s="84"/>
     </row>
-    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="26" t="s">
         <v>57</v>
       </c>
@@ -3210,19 +3210,19 @@
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="76" t="s">
         <v>244</v>
       </c>
       <c r="C45" s="77"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B46" s="78" t="s">
         <v>245</v>
       </c>
       <c r="C46" s="78"/>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B47" s="79" t="s">
         <v>246</v>
       </c>
@@ -3230,7 +3230,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B48" s="79" t="s">
         <v>248</v>
       </c>
@@ -3238,13 +3238,13 @@
         <v>249</v>
       </c>
     </row>
-    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B49" s="78" t="s">
         <v>69</v>
       </c>
       <c r="C49" s="78"/>
     </row>
-    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B50" s="79" t="s">
         <v>250</v>
       </c>
@@ -3253,7 +3253,7 @@
       </c>
       <c r="I50" s="22"/>
     </row>
-    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B51" s="79" t="s">
         <v>252</v>
       </c>
@@ -3262,7 +3262,7 @@
       </c>
       <c r="I51" s="22"/>
     </row>
-    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B52" s="79" t="s">
         <v>254</v>
       </c>
@@ -3270,7 +3270,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B53" s="79" t="s">
         <v>256</v>
       </c>
@@ -3278,7 +3278,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B54" s="79" t="s">
         <v>258</v>
       </c>
@@ -3286,7 +3286,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B55" s="79" t="s">
         <v>260</v>
       </c>
@@ -3294,7 +3294,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="56" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B56" s="79" t="s">
         <v>262</v>
       </c>
@@ -3302,7 +3302,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="57" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B57" s="79" t="s">
         <v>264</v>
       </c>
@@ -3310,7 +3310,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B58" s="79" t="s">
         <v>266</v>
       </c>
@@ -3318,7 +3318,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="59" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B59" s="79" t="s">
         <v>268</v>
       </c>
@@ -3326,7 +3326,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="60" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B60" s="79" t="s">
         <v>270</v>
       </c>
@@ -3334,7 +3334,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B61" s="79" t="s">
         <v>272</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="62" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B62" s="79" t="s">
         <v>274</v>
       </c>
@@ -3350,7 +3350,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="63" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B63" s="79" t="s">
         <v>276</v>
       </c>
@@ -3358,7 +3358,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="64" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B64" s="79" t="s">
         <v>278</v>
       </c>
@@ -3366,7 +3366,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" s="79" t="s">
         <v>280</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" s="79" t="s">
         <v>282</v>
       </c>
@@ -3382,7 +3382,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" s="79" t="s">
         <v>284</v>
       </c>
@@ -3390,7 +3390,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" s="79" t="s">
         <v>286</v>
       </c>
@@ -3398,13 +3398,13 @@
         <v>287</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" s="78" t="s">
         <v>288</v>
       </c>
       <c r="C69" s="78"/>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" s="79" t="s">
         <v>289</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" s="79" t="s">
         <v>381</v>
       </c>
@@ -3420,7 +3420,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" s="79" t="s">
         <v>364</v>
       </c>
@@ -3428,7 +3428,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" s="79" t="s">
         <v>365</v>
       </c>
@@ -3436,7 +3436,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" s="79" t="s">
         <v>366</v>
       </c>
@@ -3444,7 +3444,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" s="79" t="s">
         <v>367</v>
       </c>
@@ -3452,7 +3452,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" s="79" t="s">
         <v>368</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" s="79" t="s">
         <v>369</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" s="79" t="s">
         <v>370</v>
       </c>
@@ -3476,7 +3476,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" s="79" t="s">
         <v>371</v>
       </c>
@@ -3484,7 +3484,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" s="79" t="s">
         <v>372</v>
       </c>
@@ -3492,7 +3492,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" s="79" t="s">
         <v>373</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" s="79" t="s">
         <v>374</v>
       </c>
@@ -3508,7 +3508,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" s="79" t="s">
         <v>375</v>
       </c>
@@ -3516,7 +3516,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" s="79" t="s">
         <v>376</v>
       </c>
@@ -3524,7 +3524,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" s="79" t="s">
         <v>377</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" s="79" t="s">
         <v>378</v>
       </c>
@@ -3540,7 +3540,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" s="79" t="s">
         <v>379</v>
       </c>
@@ -3548,7 +3548,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" s="79" t="s">
         <v>380</v>
       </c>
@@ -3556,13 +3556,13 @@
         <v>308</v>
       </c>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" s="78" t="s">
         <v>309</v>
       </c>
       <c r="C89" s="78"/>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" s="79" t="s">
         <v>310</v>
       </c>
@@ -3570,7 +3570,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" s="79" t="s">
         <v>312</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" s="79" t="s">
         <v>314</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" s="79" t="s">
         <v>316</v>
       </c>
@@ -3594,7 +3594,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" s="79" t="s">
         <v>318</v>
       </c>
@@ -3602,13 +3602,13 @@
         <v>319</v>
       </c>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" s="78" t="s">
         <v>320</v>
       </c>
       <c r="C95" s="78"/>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" s="79" t="s">
         <v>321</v>
       </c>
@@ -3616,7 +3616,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="97" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B97" s="79" t="s">
         <v>323</v>
       </c>
@@ -3624,7 +3624,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B98" s="79" t="s">
         <v>325</v>
       </c>
@@ -3632,19 +3632,19 @@
         <v>326</v>
       </c>
     </row>
-    <row r="99" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B99" s="80" t="s">
         <v>77</v>
       </c>
       <c r="C99" s="81"/>
     </row>
-    <row r="100" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B100" s="78" t="s">
         <v>327</v>
       </c>
       <c r="C100" s="78"/>
     </row>
-    <row r="101" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B101" s="79" t="s">
         <v>328</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="102" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B102" s="79" t="s">
         <v>330</v>
       </c>
@@ -3660,7 +3660,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="103" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B103" s="79" t="s">
         <v>332</v>
       </c>
@@ -3668,7 +3668,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="104" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B104" s="79" t="s">
         <v>334</v>
       </c>
@@ -3676,7 +3676,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="105" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B105" s="79" t="s">
         <v>336</v>
       </c>
@@ -3684,7 +3684,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="106" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B106" s="79" t="s">
         <v>338</v>
       </c>
@@ -3692,7 +3692,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="107" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B107" s="79" t="s">
         <v>340</v>
       </c>
@@ -3700,13 +3700,13 @@
         <v>341</v>
       </c>
     </row>
-    <row r="108" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B108" s="78" t="s">
         <v>342</v>
       </c>
       <c r="C108" s="78"/>
     </row>
-    <row r="109" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B109" s="79" t="s">
         <v>343</v>
       </c>
@@ -3714,7 +3714,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="110" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B110" s="79" t="s">
         <v>345</v>
       </c>
@@ -3723,7 +3723,7 @@
       </c>
       <c r="J110" s="22"/>
     </row>
-    <row r="111" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B111" s="79" t="s">
         <v>347</v>
       </c>
@@ -3732,7 +3732,7 @@
       </c>
       <c r="J111" s="22"/>
     </row>
-    <row r="112" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B112" s="79" t="s">
         <v>349</v>
       </c>
@@ -3741,7 +3741,7 @@
       </c>
       <c r="J112" s="22"/>
     </row>
-    <row r="113" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B113" s="79" t="s">
         <v>351</v>
       </c>
@@ -3750,7 +3750,7 @@
       </c>
       <c r="J113" s="22"/>
     </row>
-    <row r="114" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B114" s="79" t="s">
         <v>353</v>
       </c>
@@ -3759,7 +3759,7 @@
       </c>
       <c r="J114" s="22"/>
     </row>
-    <row r="115" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B115" s="79" t="s">
         <v>355</v>
       </c>
@@ -3768,14 +3768,14 @@
       </c>
       <c r="J115" s="22"/>
     </row>
-    <row r="116" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B116" s="78" t="s">
         <v>357</v>
       </c>
       <c r="C116" s="78"/>
       <c r="J116" s="22"/>
     </row>
-    <row r="117" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B117" s="79" t="s">
         <v>358</v>
       </c>
@@ -3784,7 +3784,7 @@
       </c>
       <c r="J117" s="22"/>
     </row>
-    <row r="118" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B118" s="79" t="s">
         <v>360</v>
       </c>
@@ -3793,7 +3793,7 @@
       </c>
       <c r="J118" s="22"/>
     </row>
-    <row r="119" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B119" s="79" t="s">
         <v>362</v>
       </c>
@@ -3802,28 +3802,28 @@
       </c>
       <c r="J119" s="22"/>
     </row>
-    <row r="120" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J120" s="22"/>
     </row>
-    <row r="121" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J121" s="22"/>
     </row>
-    <row r="122" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J122" s="22"/>
     </row>
-    <row r="123" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J123" s="22"/>
     </row>
-    <row r="124" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:10" x14ac:dyDescent="0.25">
       <c r="J124" s="22"/>
     </row>
-    <row r="143" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="143" spans="11:12" ht="13.8" x14ac:dyDescent="0.25">
       <c r="K143" s="34" t="s">
         <v>116</v>
       </c>
       <c r="L143" s="35"/>
     </row>
-    <row r="144" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="144" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K144" s="22" t="s">
         <v>117</v>
       </c>
@@ -3832,7 +3832,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="145" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="145" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K145" s="22" t="s">
         <v>118</v>
       </c>
@@ -3841,7 +3841,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="146" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="146" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K146" s="22" t="s">
         <v>119</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="147" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="147" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K147" s="22" t="s">
         <v>120</v>
       </c>
@@ -3859,12 +3859,12 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="152" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="152" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K152" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="153" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="153" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K153" t="s">
         <v>106</v>
       </c>
@@ -3872,7 +3872,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="154" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="154" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K154" t="s">
         <v>108</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="155" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="155" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K155" t="s">
         <v>110</v>
       </c>
@@ -3888,7 +3888,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="156" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="156" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K156" t="s">
         <v>112</v>
       </c>
@@ -3896,7 +3896,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="157" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="157" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K157" t="s">
         <v>114</v>
       </c>
@@ -3904,12 +3904,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="158" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="158" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K158" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="159" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="159" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K159" t="s">
         <v>117</v>
       </c>
@@ -3917,7 +3917,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="160" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="160" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K160" t="s">
         <v>118</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="161" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="161" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K161" t="s">
         <v>119</v>
       </c>
@@ -3933,7 +3933,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="162" spans="11:12" x14ac:dyDescent="0.2">
+    <row r="162" spans="11:12" x14ac:dyDescent="0.25">
       <c r="K162" t="s">
         <v>120</v>
       </c>
@@ -3955,34 +3955,34 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B3:AL240"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B174" sqref="B174"/>
+    <sheetView tabSelected="1" topLeftCell="A149" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D165" sqref="D165"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
-    <col min="5" max="5" width="25.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" customWidth="1"/>
-    <col min="9" max="11" width="18.140625" customWidth="1"/>
-    <col min="12" max="14" width="19.85546875" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" customWidth="1"/>
-    <col min="17" max="17" width="12.28515625" customWidth="1"/>
-    <col min="18" max="18" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" customWidth="1"/>
+    <col min="4" max="4" width="26.109375" customWidth="1"/>
+    <col min="5" max="5" width="25.88671875" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" customWidth="1"/>
+    <col min="7" max="7" width="10.109375" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="9" max="11" width="18.109375" customWidth="1"/>
+    <col min="12" max="14" width="19.88671875" customWidth="1"/>
+    <col min="16" max="16" width="16.33203125" customWidth="1"/>
+    <col min="17" max="17" width="12.33203125" customWidth="1"/>
+    <col min="18" max="18" width="11.109375" customWidth="1"/>
     <col min="19" max="19" width="14" customWidth="1"/>
-    <col min="20" max="20" width="14.140625" customWidth="1"/>
-    <col min="21" max="21" width="13.5703125" customWidth="1"/>
-    <col min="22" max="22" width="13.85546875" customWidth="1"/>
-    <col min="34" max="34" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.7109375" customWidth="1"/>
+    <col min="20" max="20" width="14.109375" customWidth="1"/>
+    <col min="21" max="21" width="13.5546875" customWidth="1"/>
+    <col min="22" max="22" width="13.88671875" customWidth="1"/>
+    <col min="34" max="34" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
@@ -3998,7 +3998,7 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
@@ -4030,7 +4030,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
     </row>
-    <row r="5" spans="2:13" ht="28.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
         <v>25</v>
       </c>
@@ -4062,7 +4062,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
     </row>
-    <row r="6" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="27" t="s">
         <v>136</v>
       </c>
@@ -4077,7 +4077,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>29</v>
       </c>
@@ -4103,7 +4103,7 @@
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
         <v>29</v>
       </c>
@@ -4129,7 +4129,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
     </row>
-    <row r="9" spans="2:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B9" s="27" t="s">
         <v>137</v>
       </c>
@@ -4145,7 +4145,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>29</v>
       </c>
@@ -4165,7 +4165,7 @@
       </c>
       <c r="I10" s="10"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
         <v>29</v>
       </c>
@@ -4186,7 +4186,7 @@
       <c r="I11" s="10"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>29</v>
       </c>
@@ -4207,7 +4207,7 @@
       <c r="I12" s="10"/>
       <c r="M12" s="14"/>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
         <v>29</v>
       </c>
@@ -4228,7 +4228,7 @@
       <c r="I13" s="10"/>
       <c r="M13" s="18"/>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
         <v>29</v>
       </c>
@@ -4249,7 +4249,7 @@
       <c r="I14" s="10"/>
       <c r="M14" s="18"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
         <v>29</v>
       </c>
@@ -4270,7 +4270,7 @@
       <c r="I15" s="10"/>
       <c r="M15" s="1"/>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
         <v>29</v>
       </c>
@@ -4290,7 +4290,7 @@
       </c>
       <c r="I16" s="10"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
         <v>29</v>
       </c>
@@ -4316,7 +4316,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>29</v>
       </c>
@@ -4336,7 +4336,7 @@
       </c>
       <c r="I18" s="10"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>29</v>
       </c>
@@ -4356,7 +4356,7 @@
       </c>
       <c r="I19" s="10"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
         <v>29</v>
       </c>
@@ -4376,7 +4376,7 @@
       </c>
       <c r="I20" s="10"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
         <v>29</v>
       </c>
@@ -4396,7 +4396,7 @@
       </c>
       <c r="I21" s="10"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
         <v>29</v>
       </c>
@@ -4416,7 +4416,7 @@
       </c>
       <c r="I22" s="10"/>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>29</v>
       </c>
@@ -4436,7 +4436,7 @@
       </c>
       <c r="I23" s="10"/>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>29</v>
       </c>
@@ -4456,7 +4456,7 @@
       </c>
       <c r="I24" s="10"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>29</v>
       </c>
@@ -4476,7 +4476,7 @@
       </c>
       <c r="I25" s="10"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>29</v>
       </c>
@@ -4496,7 +4496,7 @@
       </c>
       <c r="I26" s="10"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>29</v>
       </c>
@@ -4516,7 +4516,7 @@
       </c>
       <c r="I27" s="10"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>29</v>
       </c>
@@ -4536,7 +4536,7 @@
       </c>
       <c r="I28" s="10"/>
     </row>
-    <row r="29" spans="2:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B29" s="27" t="s">
         <v>138</v>
       </c>
@@ -4549,7 +4549,7 @@
       <c r="I29" s="27"/>
       <c r="J29" s="27"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
         <v>29</v>
       </c>
@@ -4569,7 +4569,7 @@
       </c>
       <c r="I30" s="10"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
         <v>29</v>
       </c>
@@ -4589,7 +4589,7 @@
       </c>
       <c r="I31" s="10"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
         <v>29</v>
       </c>
@@ -4609,7 +4609,7 @@
       </c>
       <c r="I32" s="10"/>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
         <v>29</v>
       </c>
@@ -4629,7 +4629,7 @@
       </c>
       <c r="I33" s="10"/>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
         <v>29</v>
       </c>
@@ -4649,7 +4649,7 @@
       </c>
       <c r="I34" s="10"/>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B35" s="3" t="s">
         <v>29</v>
       </c>
@@ -4669,7 +4669,7 @@
       </c>
       <c r="I35" s="10"/>
     </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B36" s="3" t="s">
         <v>29</v>
       </c>
@@ -4689,7 +4689,7 @@
       </c>
       <c r="I36" s="10"/>
     </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
         <v>29</v>
       </c>
@@ -4709,7 +4709,7 @@
       </c>
       <c r="I37" s="10"/>
     </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B38" s="3" t="s">
         <v>29</v>
       </c>
@@ -4729,7 +4729,7 @@
       </c>
       <c r="I38" s="10"/>
     </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B39" s="3" t="s">
         <v>29</v>
       </c>
@@ -4749,7 +4749,7 @@
       </c>
       <c r="I39" s="10"/>
     </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B40" s="3" t="s">
         <v>29</v>
       </c>
@@ -4769,7 +4769,7 @@
       </c>
       <c r="I40" s="10"/>
     </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B41" s="3" t="s">
         <v>29</v>
       </c>
@@ -4789,7 +4789,7 @@
       </c>
       <c r="I41" s="10"/>
     </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B42" s="3" t="s">
         <v>29</v>
       </c>
@@ -4809,7 +4809,7 @@
       </c>
       <c r="I42" s="10"/>
     </row>
-    <row r="43" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B43" s="3" t="s">
         <v>29</v>
       </c>
@@ -4829,7 +4829,7 @@
       </c>
       <c r="I43" s="10"/>
     </row>
-    <row r="44" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B44" s="3" t="s">
         <v>29</v>
       </c>
@@ -4849,7 +4849,7 @@
       </c>
       <c r="I44" s="10"/>
     </row>
-    <row r="45" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B45" s="3" t="s">
         <v>29</v>
       </c>
@@ -4869,7 +4869,7 @@
       </c>
       <c r="I45" s="10"/>
     </row>
-    <row r="46" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" s="3" t="s">
         <v>29</v>
       </c>
@@ -4889,7 +4889,7 @@
       </c>
       <c r="I46" s="10"/>
     </row>
-    <row r="47" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B47" s="3" t="s">
         <v>29</v>
       </c>
@@ -4909,7 +4909,7 @@
       </c>
       <c r="I47" s="10"/>
     </row>
-    <row r="48" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
         <v>29</v>
       </c>
@@ -4929,7 +4929,7 @@
       </c>
       <c r="I48" s="10"/>
     </row>
-    <row r="49" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B49" s="27" t="s">
         <v>139</v>
       </c>
@@ -4942,7 +4942,7 @@
       <c r="I49" s="27"/>
       <c r="J49" s="27"/>
     </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B50" s="3" t="s">
         <v>29</v>
       </c>
@@ -4962,7 +4962,7 @@
       </c>
       <c r="I50" s="10"/>
     </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B51" s="3" t="s">
         <v>29</v>
       </c>
@@ -4982,7 +4982,7 @@
       </c>
       <c r="I51" s="10"/>
     </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B52" s="3" t="s">
         <v>29</v>
       </c>
@@ -5002,7 +5002,7 @@
       </c>
       <c r="I52" s="10"/>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B53" s="3" t="s">
         <v>29</v>
       </c>
@@ -5022,7 +5022,7 @@
       </c>
       <c r="I53" s="10"/>
     </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B54" s="3" t="s">
         <v>29</v>
       </c>
@@ -5042,7 +5042,7 @@
       </c>
       <c r="I54" s="10"/>
     </row>
-    <row r="55" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B55" s="27" t="s">
         <v>140</v>
       </c>
@@ -5055,7 +5055,7 @@
       <c r="I55" s="27"/>
       <c r="J55" s="27"/>
     </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B56" s="3" t="s">
         <v>29</v>
       </c>
@@ -5075,7 +5075,7 @@
       </c>
       <c r="I56" s="10"/>
     </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B57" s="3" t="s">
         <v>29</v>
       </c>
@@ -5095,7 +5095,7 @@
       </c>
       <c r="I57" s="10"/>
     </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B58" s="3" t="s">
         <v>29</v>
       </c>
@@ -5115,7 +5115,7 @@
       </c>
       <c r="I58" s="10"/>
     </row>
-    <row r="59" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:10" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B59" s="27" t="s">
         <v>141</v>
       </c>
@@ -5128,7 +5128,7 @@
       <c r="I59" s="27"/>
       <c r="J59" s="27"/>
     </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B60" s="3" t="s">
         <v>29</v>
       </c>
@@ -5148,7 +5148,7 @@
       </c>
       <c r="I60" s="10"/>
     </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B61" s="3" t="s">
         <v>29</v>
       </c>
@@ -5168,7 +5168,7 @@
       </c>
       <c r="I61" s="10"/>
     </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B62" s="3" t="s">
         <v>29</v>
       </c>
@@ -5188,7 +5188,7 @@
       </c>
       <c r="I62" s="10"/>
     </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B63" s="3" t="s">
         <v>29</v>
       </c>
@@ -5208,7 +5208,7 @@
       </c>
       <c r="I63" s="10"/>
     </row>
-    <row r="64" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B64" s="3" t="s">
         <v>29</v>
       </c>
@@ -5228,7 +5228,7 @@
       </c>
       <c r="I64" s="28"/>
     </row>
-    <row r="65" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B65" s="3" t="s">
         <v>29</v>
       </c>
@@ -5248,7 +5248,7 @@
       </c>
       <c r="I65" s="10"/>
     </row>
-    <row r="66" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B66" s="3" t="s">
         <v>29</v>
       </c>
@@ -5268,7 +5268,7 @@
       </c>
       <c r="I66" s="10"/>
     </row>
-    <row r="67" spans="2:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B67" s="27" t="s">
         <v>142</v>
       </c>
@@ -5281,7 +5281,7 @@
       <c r="I67" s="27"/>
       <c r="J67" s="27"/>
     </row>
-    <row r="68" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B68" s="3" t="s">
         <v>29</v>
       </c>
@@ -5301,7 +5301,7 @@
       </c>
       <c r="I68" s="10"/>
     </row>
-    <row r="69" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B69" s="3" t="s">
         <v>29</v>
       </c>
@@ -5321,7 +5321,7 @@
       </c>
       <c r="I69" s="10"/>
     </row>
-    <row r="70" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B70" s="3" t="s">
         <v>29</v>
       </c>
@@ -5341,7 +5341,7 @@
       </c>
       <c r="I70" s="10"/>
     </row>
-    <row r="71" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B71" s="3" t="s">
         <v>29</v>
       </c>
@@ -5361,7 +5361,7 @@
       </c>
       <c r="I71" s="10"/>
     </row>
-    <row r="72" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B72" s="3" t="s">
         <v>29</v>
       </c>
@@ -5381,7 +5381,7 @@
       </c>
       <c r="I72" s="28"/>
     </row>
-    <row r="73" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B73" s="3" t="s">
         <v>29</v>
       </c>
@@ -5401,7 +5401,7 @@
       </c>
       <c r="I73" s="28"/>
     </row>
-    <row r="74" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B74" s="3" t="s">
         <v>29</v>
       </c>
@@ -5421,7 +5421,7 @@
       </c>
       <c r="I74" s="28"/>
     </row>
-    <row r="75" spans="2:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B75" s="27" t="s">
         <v>143</v>
       </c>
@@ -5434,7 +5434,7 @@
       <c r="I75" s="27"/>
       <c r="J75" s="27"/>
     </row>
-    <row r="76" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B76" s="3" t="s">
         <v>29</v>
       </c>
@@ -5454,7 +5454,7 @@
       </c>
       <c r="I76" s="10"/>
     </row>
-    <row r="77" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B77" s="3" t="s">
         <v>29</v>
       </c>
@@ -5474,7 +5474,7 @@
       </c>
       <c r="I77" s="10"/>
     </row>
-    <row r="78" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B78" s="3" t="s">
         <v>29</v>
       </c>
@@ -5494,26 +5494,26 @@
       </c>
       <c r="I78" s="10"/>
     </row>
-    <row r="79" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:16" x14ac:dyDescent="0.25">
       <c r="D79" s="1"/>
       <c r="P79" s="22"/>
     </row>
-    <row r="80" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:16" x14ac:dyDescent="0.25">
       <c r="P80" s="22"/>
     </row>
-    <row r="81" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:18" x14ac:dyDescent="0.25">
       <c r="P81" s="22"/>
     </row>
-    <row r="82" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:18" x14ac:dyDescent="0.25">
       <c r="P82" s="22"/>
     </row>
-    <row r="83" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:18" x14ac:dyDescent="0.25">
       <c r="P83" s="22"/>
     </row>
-    <row r="84" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:18" x14ac:dyDescent="0.25">
       <c r="P84" s="22"/>
     </row>
-    <row r="85" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="7" t="s">
@@ -5528,7 +5528,7 @@
       <c r="K85" s="9"/>
       <c r="L85" s="1"/>
     </row>
-    <row r="86" spans="2:18" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B86" s="11" t="s">
         <v>1</v>
       </c>
@@ -5581,7 +5581,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="87" spans="2:18" ht="33.75" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:18" ht="21" x14ac:dyDescent="0.25">
       <c r="B87" s="40" t="s">
         <v>32</v>
       </c>
@@ -5632,7 +5632,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="88" spans="2:18" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:18" ht="28.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B88" s="39" t="s">
         <v>36</v>
       </c>
@@ -5679,7 +5679,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="89" spans="2:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:18" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B89" s="27" t="s">
         <v>136</v>
       </c>
@@ -5700,7 +5700,7 @@
       <c r="Q89" s="27"/>
       <c r="R89" s="27"/>
     </row>
-    <row r="90" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B90" s="53" t="str">
         <f>D7</f>
         <v>T-MOT-ICE_GSL01</v>
@@ -5756,7 +5756,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="91" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B91" s="53" t="str">
         <f>D8</f>
         <v>T-MOT-EV_ELC01</v>
@@ -5812,7 +5812,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="92" spans="2:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:18" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B92" s="27" t="s">
         <v>137</v>
       </c>
@@ -5833,7 +5833,7 @@
       <c r="Q92" s="27"/>
       <c r="R92" s="27"/>
     </row>
-    <row r="93" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B93" s="53" t="str">
         <f t="shared" ref="B93:B111" si="0">D10</f>
         <v>T-CAR-ICE_GSL21</v>
@@ -5889,7 +5889,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="94" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B94" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-ICE_DST21</v>
@@ -5945,7 +5945,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="95" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B95" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-ICE_DF21</v>
@@ -6001,7 +6001,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="96" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B96" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-ICE_NGB21</v>
@@ -6057,7 +6057,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="97" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B97" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-ICE_E8521</v>
@@ -6113,7 +6113,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="98" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B98" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-ICE_B10021</v>
@@ -6169,7 +6169,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="99" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B99" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-HEV_GSL21</v>
@@ -6225,7 +6225,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="100" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B100" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-HEV_DST21</v>
@@ -6281,7 +6281,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="101" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B101" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-PHEV10_GSL21</v>
@@ -6337,7 +6337,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="102" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B102" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-PHEV20_GSL21</v>
@@ -6393,7 +6393,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="103" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B103" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-PHEV40_GSL21</v>
@@ -6449,7 +6449,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="104" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B104" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-PHEV10_DST21</v>
@@ -6505,7 +6505,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="105" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B105" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-PHEV20_DST21</v>
@@ -6561,7 +6561,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="106" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B106" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-PHEV40_DST21</v>
@@ -6617,7 +6617,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="107" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B107" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-BEV100_ELC21</v>
@@ -6673,7 +6673,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="108" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B108" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-EV150_ELC21</v>
@@ -6729,7 +6729,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="109" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B109" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-EV250_ELC21</v>
@@ -6785,7 +6785,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="110" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B110" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-ICE_HYD21</v>
@@ -6841,7 +6841,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="111" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B111" s="53" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-FCV_HYD21</v>
@@ -6897,7 +6897,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="112" spans="2:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:18" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B112" s="27" t="s">
         <v>138</v>
       </c>
@@ -6918,7 +6918,7 @@
       <c r="Q112" s="27"/>
       <c r="R112" s="27"/>
     </row>
-    <row r="113" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B113" s="53" t="str">
         <f t="shared" ref="B113:B131" si="1">D30</f>
         <v>T-TAX-ICE_GSL31</v>
@@ -6974,7 +6974,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="114" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B114" s="53" t="str">
         <f t="shared" si="1"/>
         <v>T-TAX-ICE_DST31</v>
@@ -7030,7 +7030,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="115" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B115" s="53" t="str">
         <f t="shared" si="1"/>
         <v>T-TAX-ICE_DF31</v>
@@ -7086,7 +7086,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="116" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B116" s="53" t="str">
         <f t="shared" si="1"/>
         <v>T-TAX-ICE_NGB31</v>
@@ -7142,7 +7142,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="117" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B117" s="53" t="str">
         <f t="shared" si="1"/>
         <v>T-TAX-ICE_E8531</v>
@@ -7198,7 +7198,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="118" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B118" s="53" t="str">
         <f t="shared" si="1"/>
         <v>T-TAX-ICE_B10031</v>
@@ -7254,7 +7254,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="119" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B119" s="53" t="str">
         <f t="shared" si="1"/>
         <v>T-TAX-HEV_GSL31</v>
@@ -7310,7 +7310,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="120" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B120" s="53" t="str">
         <f t="shared" si="1"/>
         <v>T-TAX-HEV_DST31</v>
@@ -7366,7 +7366,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="121" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B121" s="53" t="str">
         <f t="shared" si="1"/>
         <v>T-TAX-PHEV10_GSL31</v>
@@ -7422,7 +7422,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="122" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B122" s="53" t="str">
         <f t="shared" si="1"/>
         <v>T-TAX-PHEV20_GSL31</v>
@@ -7478,7 +7478,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="123" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B123" s="53" t="str">
         <f t="shared" si="1"/>
         <v>T-TAX-PHEV40_GSL31</v>
@@ -7534,7 +7534,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="124" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B124" s="53" t="str">
         <f t="shared" si="1"/>
         <v>T-TAX-PHEV10_DST31</v>
@@ -7590,7 +7590,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="125" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B125" s="53" t="str">
         <f t="shared" si="1"/>
         <v>T-TAX-PHEV20_DST31</v>
@@ -7646,7 +7646,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="126" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B126" s="53" t="str">
         <f t="shared" si="1"/>
         <v>T-TAX-PHEV40_DST31</v>
@@ -7702,7 +7702,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="127" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B127" s="53" t="str">
         <f t="shared" si="1"/>
         <v>T-TAX-EV100_ELC31</v>
@@ -7758,7 +7758,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="128" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B128" s="53" t="str">
         <f t="shared" si="1"/>
         <v>T-TAX-EV150_ELC31</v>
@@ -7814,7 +7814,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="129" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B129" s="53" t="str">
         <f t="shared" si="1"/>
         <v>T-TAX-EV250_ELC31</v>
@@ -7870,7 +7870,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="130" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B130" s="53" t="str">
         <f t="shared" si="1"/>
         <v>T-TAX-ICE_HYD31</v>
@@ -7926,7 +7926,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="131" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B131" s="53" t="str">
         <f t="shared" si="1"/>
         <v>T-TAX-FCV_HYD31</v>
@@ -7982,7 +7982,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="132" spans="2:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:18" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B132" s="27" t="s">
         <v>139</v>
       </c>
@@ -8003,7 +8003,7 @@
       <c r="Q132" s="27"/>
       <c r="R132" s="27"/>
     </row>
-    <row r="133" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B133" s="53" t="str">
         <f>D50</f>
         <v>T-BUS-ICE_DST41</v>
@@ -8059,7 +8059,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="134" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B134" s="53" t="str">
         <f>D51</f>
         <v>T-BUS-ICE_B10041</v>
@@ -8115,7 +8115,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="135" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B135" s="53" t="str">
         <f>D52</f>
         <v>T-BUS-ICE_NGB41</v>
@@ -8171,7 +8171,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="136" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B136" s="53" t="str">
         <f>D53</f>
         <v>T-BUS-BEV_ELC41</v>
@@ -8227,7 +8227,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="137" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B137" s="53" t="str">
         <f>D54</f>
         <v>T-BUS-FCV_HYD41</v>
@@ -8283,7 +8283,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="138" spans="2:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:18" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B138" s="27" t="s">
         <v>140</v>
       </c>
@@ -8304,7 +8304,7 @@
       <c r="Q138" s="27"/>
       <c r="R138" s="27"/>
     </row>
-    <row r="139" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B139" s="53" t="str">
         <f>D56</f>
         <v>T-LPT-EV_ELC51</v>
@@ -8360,7 +8360,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="140" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B140" s="53" t="str">
         <f>D57</f>
         <v>T-HPT-EV_ELC51</v>
@@ -8416,7 +8416,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="141" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B141" s="53" t="str">
         <f>D58</f>
         <v>T-HPT-ICE_DST51</v>
@@ -8472,7 +8472,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="142" spans="2:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:18" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B142" s="27" t="s">
         <v>141</v>
       </c>
@@ -8493,7 +8493,7 @@
       <c r="Q142" s="27"/>
       <c r="R142" s="27"/>
     </row>
-    <row r="143" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B143" s="54" t="str">
         <f t="shared" ref="B143:B149" si="2">D60</f>
         <v>T-LGT-ICE_DST61</v>
@@ -8549,7 +8549,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="144" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B144" s="54" t="str">
         <f t="shared" si="2"/>
         <v>T-LGT-HEV_DST61</v>
@@ -8605,7 +8605,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="145" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B145" s="54" t="str">
         <f t="shared" si="2"/>
         <v>T-LGT-PHEV_DST61</v>
@@ -8661,7 +8661,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="146" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B146" s="54" t="str">
         <f t="shared" si="2"/>
         <v>T-LGT-ICE_NBG61</v>
@@ -8717,7 +8717,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="147" spans="2:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:18" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B147" s="54" t="str">
         <f t="shared" si="2"/>
         <v>T-LGT-PHEV_NGB61</v>
@@ -8773,7 +8773,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="148" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B148" s="54" t="str">
         <f t="shared" si="2"/>
         <v>T-LGT-FCV_HYD61</v>
@@ -8829,7 +8829,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="149" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B149" s="54" t="str">
         <f t="shared" si="2"/>
         <v>T-LGT-BEV_ELC61</v>
@@ -8885,7 +8885,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="150" spans="2:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:18" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B150" s="27" t="s">
         <v>142</v>
       </c>
@@ -8906,7 +8906,7 @@
       <c r="Q150" s="27"/>
       <c r="R150" s="27"/>
     </row>
-    <row r="151" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B151" s="54" t="str">
         <f t="shared" ref="B151:B157" si="3">D68</f>
         <v>T-HGT-ICE_DST71</v>
@@ -8962,7 +8962,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="152" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B152" s="54" t="str">
         <f t="shared" si="3"/>
         <v>T-HGT-HEV_DST71</v>
@@ -9018,7 +9018,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="153" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B153" s="54" t="str">
         <f t="shared" si="3"/>
         <v>T-HGT-FCV_HYD71</v>
@@ -9074,7 +9074,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="154" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B154" s="54" t="str">
         <f t="shared" si="3"/>
         <v>T-HGT-ICE_NGB71</v>
@@ -9130,7 +9130,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="155" spans="2:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:18" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B155" s="54" t="str">
         <f t="shared" si="3"/>
         <v>T-HGT-HEV_NGB71</v>
@@ -9186,7 +9186,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="156" spans="2:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:18" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B156" s="54" t="str">
         <f t="shared" si="3"/>
         <v>T-HGT-ICE_LNG71</v>
@@ -9212,13 +9212,13 @@
         <v>0.155</v>
       </c>
       <c r="I156" s="56">
-        <v>113.17</v>
+        <v>130.68600000000001</v>
       </c>
       <c r="J156" s="56">
-        <v>114.45</v>
+        <v>128.75800000000001</v>
       </c>
       <c r="K156" s="56">
-        <v>112.16</v>
+        <v>126.18300000000001</v>
       </c>
       <c r="L156" s="56">
         <v>5.0989820625747049</v>
@@ -9242,7 +9242,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="157" spans="2:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:18" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B157" s="54" t="str">
         <f t="shared" si="3"/>
         <v>T-HGT-BEV_ELC71</v>
@@ -9298,7 +9298,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="158" spans="2:18" s="1" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:18" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B158" s="27" t="s">
         <v>143</v>
       </c>
@@ -9319,7 +9319,7 @@
       <c r="Q158" s="27"/>
       <c r="R158" s="27"/>
     </row>
-    <row r="159" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B159" s="53" t="str">
         <f>D76</f>
         <v>T-GTR-ICE_DST81</v>
@@ -9375,7 +9375,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="160" spans="2:18" ht="15" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:18" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B160" s="53" t="str">
         <f>D77</f>
         <v>T-GTR-EV_ELC81</v>
@@ -9431,7 +9431,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="161" spans="2:38" ht="15" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B161" s="61" t="str">
         <f>D78</f>
         <v>T-GTR-FCV_HYD81</v>
@@ -9487,13 +9487,13 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="162" spans="2:38" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B162" s="1"/>
     </row>
-    <row r="163" spans="2:38" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B163" s="1"/>
     </row>
-    <row r="167" spans="2:38" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
       <c r="D167" s="1"/>
@@ -9520,7 +9520,7 @@
       <c r="Y167" s="1"/>
       <c r="Z167" s="1"/>
     </row>
-    <row r="168" spans="2:38" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:38" x14ac:dyDescent="0.25">
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
       <c r="D168" s="1"/>
@@ -9547,7 +9547,7 @@
       <c r="Y168" s="1"/>
       <c r="Z168" s="1"/>
     </row>
-    <row r="169" spans="2:38" ht="21" x14ac:dyDescent="0.35">
+    <row r="169" spans="2:38" ht="21" x14ac:dyDescent="0.4">
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
       <c r="D169" s="1"/>
@@ -9587,7 +9587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="2:38" ht="15" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:38" ht="14.4" x14ac:dyDescent="0.25">
       <c r="B170" s="24" t="s">
         <v>1</v>
       </c>
@@ -9721,7 +9721,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="171" spans="2:38" ht="15" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B171" s="58" t="str">
         <f>B95</f>
         <v>T-CAR-ICE_DF21</v>
@@ -9832,7 +9832,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="172" spans="2:38" ht="15" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B172" s="58" t="str">
         <f t="shared" ref="B172:B177" si="6">B101</f>
         <v>T-CAR-PHEV10_GSL21</v>
@@ -9943,7 +9943,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="173" spans="2:38" ht="15" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B173" s="58" t="str">
         <f t="shared" si="6"/>
         <v>T-CAR-PHEV20_GSL21</v>
@@ -10054,7 +10054,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="174" spans="2:38" ht="15" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B174" s="58" t="str">
         <f t="shared" si="6"/>
         <v>T-CAR-PHEV40_GSL21</v>
@@ -10165,7 +10165,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="175" spans="2:38" ht="15" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B175" s="58" t="str">
         <f t="shared" si="6"/>
         <v>T-CAR-PHEV10_DST21</v>
@@ -10276,7 +10276,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="176" spans="2:38" ht="15" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B176" s="58" t="str">
         <f t="shared" si="6"/>
         <v>T-CAR-PHEV20_DST21</v>
@@ -10387,7 +10387,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="177" spans="2:38" ht="15" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B177" s="58" t="str">
         <f t="shared" si="6"/>
         <v>T-CAR-PHEV40_DST21</v>
@@ -10498,7 +10498,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="178" spans="2:38" ht="15" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B178" s="58" t="str">
         <f>B115</f>
         <v>T-TAX-ICE_DF31</v>
@@ -10609,7 +10609,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="179" spans="2:38" ht="15" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B179" s="58" t="str">
         <f>B121</f>
         <v>T-TAX-PHEV10_GSL31</v>
@@ -10720,7 +10720,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="180" spans="2:38" ht="15" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B180" s="58" t="str">
         <f t="shared" ref="B180:B184" si="7">B122</f>
         <v>T-TAX-PHEV20_GSL31</v>
@@ -10831,7 +10831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="181" spans="2:38" ht="15" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B181" s="58" t="str">
         <f t="shared" si="7"/>
         <v>T-TAX-PHEV40_GSL31</v>
@@ -10942,7 +10942,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="182" spans="2:38" ht="15" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B182" s="58" t="str">
         <f t="shared" si="7"/>
         <v>T-TAX-PHEV10_DST31</v>
@@ -11053,7 +11053,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="183" spans="2:38" ht="15" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B183" s="58" t="str">
         <f t="shared" si="7"/>
         <v>T-TAX-PHEV20_DST31</v>
@@ -11164,7 +11164,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="184" spans="2:38" ht="15" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B184" s="58" t="str">
         <f t="shared" si="7"/>
         <v>T-TAX-PHEV40_DST31</v>
@@ -11275,7 +11275,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="185" spans="2:38" ht="15" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B185" s="58" t="str">
         <f>B145</f>
         <v>T-LGT-PHEV_DST61</v>
@@ -11386,7 +11386,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="186" spans="2:38" ht="15" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B186" s="71" t="str">
         <f>B147</f>
         <v>T-LGT-PHEV_NGB61</v>
@@ -11497,7 +11497,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="187" spans="2:38" ht="15" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B187" s="58"/>
       <c r="C187" s="1"/>
       <c r="D187" s="59"/>
@@ -11529,7 +11529,7 @@
       <c r="AE187" s="60"/>
       <c r="AF187" s="60"/>
     </row>
-    <row r="188" spans="2:38" ht="15" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B188" s="58"/>
       <c r="C188" s="1"/>
       <c r="D188" s="59"/>
@@ -11561,7 +11561,7 @@
       <c r="AE188" s="60"/>
       <c r="AF188" s="60"/>
     </row>
-    <row r="189" spans="2:38" ht="15" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B189" s="58"/>
       <c r="C189" s="1"/>
       <c r="D189" s="59"/>
@@ -11593,7 +11593,7 @@
       <c r="AD189" s="42"/>
       <c r="AE189" s="42"/>
     </row>
-    <row r="190" spans="2:38" ht="15" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B190" s="58"/>
       <c r="C190" s="1"/>
       <c r="D190" s="59"/>
@@ -11625,7 +11625,7 @@
       <c r="AD190" s="42"/>
       <c r="AE190" s="42"/>
     </row>
-    <row r="191" spans="2:38" ht="15" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B191" s="63"/>
       <c r="C191" s="64"/>
       <c r="D191" s="65"/>
@@ -11657,7 +11657,7 @@
       <c r="AD191" s="66"/>
       <c r="AE191" s="66"/>
     </row>
-    <row r="192" spans="2:38" ht="15" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:38" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B192" s="63"/>
       <c r="C192" s="64"/>
       <c r="D192" s="65"/>
@@ -11689,7 +11689,7 @@
       <c r="AD192" s="66"/>
       <c r="AE192" s="66"/>
     </row>
-    <row r="193" spans="2:32" ht="15" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:32" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B193" s="63"/>
       <c r="C193" s="64"/>
       <c r="D193" s="65"/>
@@ -11721,7 +11721,7 @@
       <c r="AD193" s="66"/>
       <c r="AE193" s="66"/>
     </row>
-    <row r="194" spans="2:32" ht="15" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:32" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B194" s="63"/>
       <c r="C194" s="64"/>
       <c r="D194" s="65"/>
@@ -11753,7 +11753,7 @@
       <c r="AD194" s="66"/>
       <c r="AE194" s="66"/>
     </row>
-    <row r="195" spans="2:32" ht="15" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:32" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B195" s="63"/>
       <c r="C195" s="64"/>
       <c r="D195" s="65"/>
@@ -11785,7 +11785,7 @@
       <c r="AD195" s="66"/>
       <c r="AE195" s="66"/>
     </row>
-    <row r="196" spans="2:32" ht="15" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:32" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B196" s="63"/>
       <c r="C196" s="64"/>
       <c r="D196" s="65"/>
@@ -11817,7 +11817,7 @@
       <c r="AD196" s="66"/>
       <c r="AE196" s="66"/>
     </row>
-    <row r="197" spans="2:32" ht="15" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:32" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B197" s="63"/>
       <c r="C197" s="64"/>
       <c r="D197" s="65"/>
@@ -11849,7 +11849,7 @@
       <c r="AD197" s="67"/>
       <c r="AE197" s="67"/>
     </row>
-    <row r="198" spans="2:32" ht="15" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:32" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B198" s="63"/>
       <c r="C198" s="64"/>
       <c r="D198" s="65"/>
@@ -11881,7 +11881,7 @@
       <c r="AD198" s="67"/>
       <c r="AE198" s="67"/>
     </row>
-    <row r="199" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B199" s="64"/>
       <c r="C199" s="64"/>
       <c r="D199" s="65"/>
@@ -11913,7 +11913,7 @@
       <c r="AD199" s="67"/>
       <c r="AE199" s="67"/>
     </row>
-    <row r="200" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B200" s="64"/>
       <c r="C200" s="64"/>
       <c r="D200" s="65"/>
@@ -11945,7 +11945,7 @@
       <c r="AD200" s="67"/>
       <c r="AE200" s="67"/>
     </row>
-    <row r="201" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
       <c r="D201" s="1"/>
@@ -11978,8 +11978,8 @@
       <c r="AE201" s="1"/>
       <c r="AF201" s="1"/>
     </row>
-    <row r="202" spans="2:32" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="203" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:32" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="203" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
       <c r="D203" s="1"/>
@@ -12012,7 +12012,7 @@
       <c r="AE203" s="1"/>
       <c r="AF203" s="1"/>
     </row>
-    <row r="204" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
       <c r="D204" s="1"/>
@@ -12045,7 +12045,7 @@
       <c r="AE204" s="1"/>
       <c r="AF204" s="1"/>
     </row>
-    <row r="205" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
       <c r="D205" s="1"/>
@@ -12078,7 +12078,7 @@
       <c r="AE205" s="1"/>
       <c r="AF205" s="1"/>
     </row>
-    <row r="206" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="206" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
       <c r="D206" s="1"/>
@@ -12111,7 +12111,7 @@
       <c r="AE206" s="1"/>
       <c r="AF206" s="1"/>
     </row>
-    <row r="207" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="207" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
       <c r="D207" s="1"/>
@@ -12144,7 +12144,7 @@
       <c r="AE207" s="1"/>
       <c r="AF207" s="1"/>
     </row>
-    <row r="208" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="208" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
       <c r="D208" s="1"/>
@@ -12177,7 +12177,7 @@
       <c r="AE208" s="1"/>
       <c r="AF208" s="1"/>
     </row>
-    <row r="209" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="209" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
       <c r="D209" s="1"/>
@@ -12210,7 +12210,7 @@
       <c r="AE209" s="1"/>
       <c r="AF209" s="1"/>
     </row>
-    <row r="210" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="210" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
       <c r="D210" s="1"/>
@@ -12243,7 +12243,7 @@
       <c r="AE210" s="1"/>
       <c r="AF210" s="1"/>
     </row>
-    <row r="211" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="211" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
       <c r="D211" s="1"/>
@@ -12276,7 +12276,7 @@
       <c r="AE211" s="1"/>
       <c r="AF211" s="1"/>
     </row>
-    <row r="212" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="212" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
       <c r="D212" s="1"/>
@@ -12309,7 +12309,7 @@
       <c r="AE212" s="1"/>
       <c r="AF212" s="1"/>
     </row>
-    <row r="213" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="213" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
       <c r="D213" s="1"/>
@@ -12336,7 +12336,7 @@
       <c r="Y213" s="1"/>
       <c r="Z213" s="1"/>
     </row>
-    <row r="214" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="214" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
       <c r="D214" s="1"/>
@@ -12363,7 +12363,7 @@
       <c r="Y214" s="1"/>
       <c r="Z214" s="1"/>
     </row>
-    <row r="215" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="215" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
       <c r="D215" s="1"/>
@@ -12390,7 +12390,7 @@
       <c r="Y215" s="1"/>
       <c r="Z215" s="1"/>
     </row>
-    <row r="216" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="216" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
       <c r="D216" s="1"/>
@@ -12417,7 +12417,7 @@
       <c r="Y216" s="1"/>
       <c r="Z216" s="1"/>
     </row>
-    <row r="217" spans="2:32" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="2:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
       <c r="D217" s="1"/>
@@ -12444,7 +12444,7 @@
       <c r="Y217" s="1"/>
       <c r="Z217" s="1"/>
     </row>
-    <row r="218" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="218" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
       <c r="D218" s="1"/>
@@ -12471,7 +12471,7 @@
       <c r="Y218" s="1"/>
       <c r="Z218" s="1"/>
     </row>
-    <row r="219" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="219" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B219" s="1"/>
       <c r="C219" s="1"/>
       <c r="D219" s="1"/>
@@ -12498,7 +12498,7 @@
       <c r="Y219" s="1"/>
       <c r="Z219" s="1"/>
     </row>
-    <row r="220" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="220" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B220" s="1"/>
       <c r="C220" s="1"/>
       <c r="D220" s="1"/>
@@ -12525,7 +12525,7 @@
       <c r="Y220" s="1"/>
       <c r="Z220" s="1"/>
     </row>
-    <row r="221" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="221" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B221" s="1"/>
       <c r="C221" s="1"/>
       <c r="D221" s="1"/>
@@ -12552,7 +12552,7 @@
       <c r="Y221" s="1"/>
       <c r="Z221" s="1"/>
     </row>
-    <row r="222" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="222" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>
       <c r="D222" s="1"/>
@@ -12579,7 +12579,7 @@
       <c r="Y222" s="1"/>
       <c r="Z222" s="1"/>
     </row>
-    <row r="223" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="223" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
       <c r="D223" s="1"/>
@@ -12606,7 +12606,7 @@
       <c r="Y223" s="1"/>
       <c r="Z223" s="1"/>
     </row>
-    <row r="224" spans="2:32" x14ac:dyDescent="0.2">
+    <row r="224" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B224" s="1"/>
       <c r="C224" s="1"/>
       <c r="D224" s="1"/>
@@ -12633,7 +12633,7 @@
       <c r="Y224" s="1"/>
       <c r="Z224" s="1"/>
     </row>
-    <row r="225" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="225" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>
       <c r="D225" s="1"/>
@@ -12660,7 +12660,7 @@
       <c r="Y225" s="1"/>
       <c r="Z225" s="1"/>
     </row>
-    <row r="226" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="226" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B226" s="1"/>
       <c r="C226" s="1"/>
       <c r="D226" s="1"/>
@@ -12687,7 +12687,7 @@
       <c r="Y226" s="1"/>
       <c r="Z226" s="1"/>
     </row>
-    <row r="227" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="227" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B227" s="1"/>
       <c r="C227" s="1"/>
       <c r="D227" s="1"/>
@@ -12714,7 +12714,7 @@
       <c r="Y227" s="1"/>
       <c r="Z227" s="1"/>
     </row>
-    <row r="228" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="228" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B228" s="1"/>
       <c r="C228" s="1"/>
       <c r="D228" s="1"/>
@@ -12741,7 +12741,7 @@
       <c r="Y228" s="1"/>
       <c r="Z228" s="1"/>
     </row>
-    <row r="229" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="229" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B229" s="1"/>
       <c r="C229" s="1"/>
       <c r="D229" s="1"/>
@@ -12768,10 +12768,10 @@
       <c r="Y229" s="1"/>
       <c r="Z229" s="1"/>
     </row>
-    <row r="230" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="231" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="232" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="233" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="230" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="231" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="232" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="233" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B233" s="1"/>
       <c r="C233" s="1"/>
       <c r="D233" s="1"/>
@@ -12798,7 +12798,7 @@
       <c r="Y233" s="1"/>
       <c r="Z233" s="1"/>
     </row>
-    <row r="234" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="234" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B234" s="1"/>
       <c r="C234" s="1"/>
       <c r="D234" s="1"/>
@@ -12825,7 +12825,7 @@
       <c r="Y234" s="1"/>
       <c r="Z234" s="1"/>
     </row>
-    <row r="235" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="235" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B235" s="1"/>
       <c r="C235" s="1"/>
       <c r="D235" s="1"/>
@@ -12852,7 +12852,7 @@
       <c r="Y235" s="1"/>
       <c r="Z235" s="1"/>
     </row>
-    <row r="236" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="236" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B236" s="1"/>
       <c r="C236" s="1"/>
       <c r="D236" s="1"/>
@@ -12879,7 +12879,7 @@
       <c r="Y236" s="1"/>
       <c r="Z236" s="1"/>
     </row>
-    <row r="237" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="237" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B237" s="1"/>
       <c r="C237" s="1"/>
       <c r="D237" s="1"/>
@@ -12906,7 +12906,7 @@
       <c r="Y237" s="1"/>
       <c r="Z237" s="1"/>
     </row>
-    <row r="238" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="238" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B238" s="1"/>
       <c r="C238" s="1"/>
       <c r="D238" s="1"/>
@@ -12933,7 +12933,7 @@
       <c r="Y238" s="1"/>
       <c r="Z238" s="1"/>
     </row>
-    <row r="239" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="239" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B239" s="1"/>
       <c r="C239" s="1"/>
       <c r="D239" s="1"/>
@@ -12960,7 +12960,7 @@
       <c r="Y239" s="1"/>
       <c r="Z239" s="1"/>
     </row>
-    <row r="240" spans="2:26" x14ac:dyDescent="0.2">
+    <row r="240" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B240" s="1"/>
       <c r="C240" s="1"/>
       <c r="D240" s="1"/>
@@ -13003,19 +13003,19 @@
       <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
-    <col min="3" max="11" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+    <col min="3" max="11" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>146</v>
       </c>
@@ -13050,7 +13050,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>157</v>
       </c>
@@ -13085,7 +13085,7 @@
         <v>2574</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>158</v>
       </c>
@@ -13124,7 +13124,7 @@
         <v>4.044339163234481E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>159</v>
       </c>
@@ -13163,7 +13163,7 @@
         <v>7.0982279191462321E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>160</v>
       </c>
@@ -13202,7 +13202,7 @@
         <v>3.9667538813275338E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>161</v>
       </c>
@@ -13241,7 +13241,7 @@
         <v>3.4071494011901911E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>162</v>
       </c>
@@ -13280,7 +13280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>163</v>
       </c>
@@ -13319,7 +13319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>164</v>
       </c>
@@ -13358,7 +13358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>165</v>
       </c>
@@ -13397,7 +13397,7 @@
         <v>9.7889515257063141E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>166</v>
       </c>
@@ -13436,7 +13436,7 @@
         <v>2.81535528281486E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>167</v>
       </c>
@@ -13475,7 +13475,7 @@
         <v>5.7611198692605467E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>168</v>
       </c>
@@ -13514,7 +13514,7 @@
         <v>8.8694833975750467E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>169</v>
       </c>
@@ -13553,7 +13553,7 @@
         <v>1.0399729276888665E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>170</v>
       </c>
@@ -13592,7 +13592,7 @@
         <v>9.0378599668199111E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>171</v>
       </c>
@@ -13631,7 +13631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>172</v>
       </c>
@@ -13670,7 +13670,7 @@
         <v>4.9027295162475133E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>173</v>
       </c>
@@ -13709,7 +13709,7 @@
         <v>7.5934531228075966E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>174</v>
       </c>
@@ -13748,7 +13748,7 @@
         <v>5.7817542527464363E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>175</v>
       </c>
@@ -13787,7 +13787,7 @@
         <v>8.2620071477504387E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>176</v>
       </c>
@@ -13826,7 +13826,7 @@
         <v>3.8875178487417154E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>177</v>
       </c>
@@ -13865,7 +13865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>178</v>
       </c>
@@ -13904,7 +13904,7 @@
         <v>1.7844614838597853E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>179</v>
       </c>
@@ -13943,7 +13943,7 @@
         <v>3.2627087167889597E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>180</v>
       </c>
@@ -13982,7 +13982,7 @@
         <v>4.7624157085434599E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>181</v>
       </c>
@@ -14021,7 +14021,7 @@
         <v>6.1160312652178582E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>182</v>
       </c>
@@ -14060,7 +14060,7 @@
         <v>7.6570070239441387E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>183</v>
       </c>
@@ -14099,7 +14099,7 @@
         <v>4.0385615358584315E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>184</v>
       </c>
@@ -14138,7 +14138,7 @@
         <v>4.4355670741269594E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>185</v>
       </c>
@@ -14177,7 +14177,7 @@
         <v>6.0252399778799404E-4</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>186</v>
       </c>
@@ -14216,7 +14216,7 @@
         <v>5.8395305265069287E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>187</v>
       </c>
@@ -14255,7 +14255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>188</v>
       </c>
@@ -14294,7 +14294,7 @@
         <v>2.9713512219681899E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>189</v>
       </c>
@@ -14333,7 +14333,7 @@
         <v>7.1543534422278537E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>190</v>
       </c>
@@ -14372,7 +14372,7 @@
         <v>8.253753394356084E-6</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>191</v>
       </c>
@@ -14411,7 +14411,7 @@
         <v>6.1077775118235022E-4</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>192</v>
       </c>
@@ -14450,7 +14450,7 @@
         <v>1.5434518847445876E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>193</v>
       </c>
@@ -14489,7 +14489,7 @@
         <v>1.0143862921663627E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>194</v>
       </c>
@@ -14528,7 +14528,7 @@
         <v>9.9045040732272994E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>195</v>
       </c>
@@ -14567,7 +14567,7 @@
         <v>9.4786103980785269E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>196</v>
       </c>
@@ -14606,7 +14606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>197</v>
       </c>
@@ -14645,7 +14645,7 @@
         <v>0.1113926558102297</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>198</v>
       </c>
@@ -14684,17 +14684,17 @@
         <v>1.3948843236461781E-2</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>147</v>
       </c>
@@ -14726,7 +14726,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>168</v>
       </c>
@@ -14758,7 +14758,7 @@
         <v>61500</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>170</v>
       </c>
@@ -14790,7 +14790,7 @@
         <v>43995</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>174</v>
       </c>
@@ -14822,7 +14822,7 @@
         <v>41670</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>182</v>
       </c>
@@ -14854,7 +14854,7 @@
         <v>37720</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>186</v>
       </c>
@@ -14886,7 +14886,7 @@
         <v>37990</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>189</v>
       </c>
@@ -14918,7 +14918,7 @@
         <v>42025</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>195</v>
       </c>
@@ -14950,7 +14950,7 @@
         <v>40395</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>197</v>
       </c>
@@ -14982,17 +14982,17 @@
         <v>73975</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="36" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>147</v>
       </c>
@@ -15024,7 +15024,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>168</v>
       </c>
@@ -15069,7 +15069,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>170</v>
       </c>
@@ -15114,7 +15114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>174</v>
       </c>
@@ -15159,7 +15159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>182</v>
       </c>
@@ -15204,7 +15204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>186</v>
       </c>
@@ -15249,7 +15249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>189</v>
       </c>
@@ -15294,7 +15294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>195</v>
       </c>
@@ -15339,7 +15339,7 @@
         <v>866</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>197</v>
       </c>
@@ -15384,7 +15384,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A73" s="45" t="s">
         <v>201</v>
       </c>
@@ -15429,12 +15429,12 @@
         <v>931</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>147</v>
       </c>
@@ -15466,7 +15466,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>168</v>
       </c>
@@ -15511,7 +15511,7 @@
         <v>2.5412637704730561E-5</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>170</v>
       </c>
@@ -15556,7 +15556,7 @@
         <v>1.270631885236528E-5</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>174</v>
       </c>
@@ -15601,7 +15601,7 @@
         <v>2.5412637704730561E-5</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>182</v>
       </c>
@@ -15646,7 +15646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>186</v>
       </c>
@@ -15691,7 +15691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>189</v>
       </c>
@@ -15736,7 +15736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>195</v>
       </c>
@@ -15781,7 +15781,7 @@
         <v>1.1003672126148334E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>197</v>
       </c>
@@ -15826,7 +15826,7 @@
         <v>7.6237913114191687E-4</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A87" s="45" t="s">
         <v>201</v>
       </c>
@@ -15871,7 +15871,7 @@
         <v>1.1829582851552077E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A90" s="48" t="s">
         <v>65</v>
       </c>
@@ -15880,7 +15880,7 @@
         <v>21831.587082756254</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A91" s="48" t="s">
         <v>203</v>
       </c>
@@ -15889,12 +15889,12 @@
         <v>20290.14478354996</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="49" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D95" s="42"/>
       <c r="E95" s="42"/>
       <c r="F95" s="42"/>
@@ -15904,7 +15904,7 @@
       <c r="J95" s="42"/>
       <c r="K95" s="42"/>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B96" s="42"/>
       <c r="C96" s="42"/>
       <c r="D96" s="42"/>

</xml_diff>

<commit_message>
Resolve Dummy Import for Transport Freight and calibrate regional load factor and Modify UC for Freight
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
+++ b/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\VEDA_Models\~g2v_Irish-TIMES-model\tra-updates\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1CE4039-44CE-4D2B-84BB-27332987B9A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D8C714-6EE0-4173-B06D-FC9C8752AC47}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1483,10 +1483,31 @@
     <numFmt numFmtId="165" formatCode="\Te\x\t"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="40" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1705,6 +1726,16 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -1837,69 +1868,110 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="20" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="23" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1908,156 +1980,199 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="24" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="27" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="24" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="27" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="24" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="27" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="9" fontId="16" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="41" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="41" fontId="25" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="24" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="19" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="41" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="41" fontId="28" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="27" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="19" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="35" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="22" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="34" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="9" fontId="34" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="37" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="9" fontId="37" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="34" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="37" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="8" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="8" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="8" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="8" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="8" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="8" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="8" borderId="0" xfId="8" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="8" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="8" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="8" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="39" fillId="0" borderId="0" xfId="12" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="12" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="8" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="8" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="8" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="53">
     <cellStyle name="20% - Accent5" xfId="1" builtinId="46"/>
     <cellStyle name="20% - Accent5 2" xfId="7" xr:uid="{41FADB5D-774C-4581-9E04-795745F45B3A}"/>
+    <cellStyle name="20% - Accent5 2 2" xfId="22" xr:uid="{9D85FBE9-8CBA-4BC4-A23E-71E72F7E6CC9}"/>
+    <cellStyle name="20% - Accent5 2 3" xfId="35" xr:uid="{64A1DEB4-76C7-4D7E-B183-769228520DF6}"/>
+    <cellStyle name="20% - Accent5 2 4" xfId="48" xr:uid="{B6EB5E8B-FCFF-4F4E-8AB6-E3215DFC371B}"/>
     <cellStyle name="20% - Accent5 3" xfId="11" xr:uid="{42C3DA6A-E515-4F68-9D9F-3335D19CEA18}"/>
+    <cellStyle name="20% - Accent5 3 2" xfId="26" xr:uid="{7ABCF359-2591-4C83-A95F-469CD11EC77F}"/>
+    <cellStyle name="20% - Accent5 3 3" xfId="39" xr:uid="{A4C767C1-51C3-47D5-A74C-587D3519900C}"/>
+    <cellStyle name="20% - Accent5 3 4" xfId="52" xr:uid="{C90B685B-F75D-460B-BDFC-7D7533C48C33}"/>
+    <cellStyle name="20% - Accent5 4" xfId="15" xr:uid="{DC1DD871-6B98-4E25-8BE8-6A14C839CFCF}"/>
+    <cellStyle name="20% - Accent5 5" xfId="30" xr:uid="{0FAED7C7-EA67-4CB3-AE34-15128E10EBDD}"/>
+    <cellStyle name="20% - Accent5 6" xfId="43" xr:uid="{AED42CDA-BA61-497A-9B25-6EC421F7DD74}"/>
     <cellStyle name="Comma 2" xfId="5" xr:uid="{ED6C98B7-B2A1-4B47-AF8A-A39872245B39}"/>
+    <cellStyle name="Comma 2 2" xfId="20" xr:uid="{B7AC5FAF-634D-41F9-85B3-9CDBB33D0333}"/>
+    <cellStyle name="Comma 2 3" xfId="33" xr:uid="{9A5060E8-4621-4D2E-8FA3-F2C0D822E9A4}"/>
+    <cellStyle name="Comma 2 4" xfId="46" xr:uid="{640D3F39-7ADA-41F7-A824-1BFD8996D38B}"/>
     <cellStyle name="Comma 3" xfId="9" xr:uid="{9BBE06F6-DF43-4386-A7EA-84770CBB1110}"/>
+    <cellStyle name="Comma 3 2" xfId="24" xr:uid="{AB59C64B-085D-4C79-B275-6709641D5BB7}"/>
+    <cellStyle name="Comma 3 3" xfId="37" xr:uid="{96E677B2-1E39-47F3-B561-DD4F13597381}"/>
+    <cellStyle name="Comma 3 4" xfId="50" xr:uid="{B86C2900-CA03-40CB-895D-AA126B40D038}"/>
+    <cellStyle name="Comma 4" xfId="13" xr:uid="{F10BAA2F-325D-48FE-B4DE-588412CF4783}"/>
+    <cellStyle name="Comma 5" xfId="28" xr:uid="{A96DE9F5-7FB1-4FAB-B94D-B2EF920E5378}"/>
+    <cellStyle name="Comma 6" xfId="41" xr:uid="{F6AC73A4-766F-41AF-8546-1BD92C1A5DC3}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{4F4ED162-C45F-4637-99B9-0DC288E0E26C}"/>
+    <cellStyle name="Normal 2 2" xfId="18" xr:uid="{73520720-7CC8-4636-BEA4-4BA7AD8E3294}"/>
+    <cellStyle name="Normal 2 3" xfId="31" xr:uid="{3DE8F047-C232-4A35-B429-F0537449F260}"/>
+    <cellStyle name="Normal 2 4" xfId="44" xr:uid="{4FF9CFE9-7E21-4A6B-A29A-1180095F3394}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{6F56F0E9-E05C-4C30-B878-F9B9EA162652}"/>
+    <cellStyle name="Normal 3 2" xfId="19" xr:uid="{A32771C3-61B9-4017-BCB7-A8447F558936}"/>
+    <cellStyle name="Normal 3 3" xfId="32" xr:uid="{6D6D7D4C-E015-466A-A2A9-35851197F9B9}"/>
+    <cellStyle name="Normal 3 4" xfId="45" xr:uid="{3F2C4675-A6B6-4303-ADF3-7F5FDBCC1201}"/>
     <cellStyle name="Normal 4" xfId="8" xr:uid="{E0019DBD-0F4A-4352-B357-025C5C0BFAEC}"/>
+    <cellStyle name="Normal 4 2" xfId="23" xr:uid="{10393A82-218B-43FD-AA73-2D1C9788B975}"/>
+    <cellStyle name="Normal 4 3" xfId="36" xr:uid="{62A12A76-EC25-4B9B-9DE7-60E39637AA4D}"/>
+    <cellStyle name="Normal 4 4" xfId="49" xr:uid="{0D81F105-5652-4284-861E-275768C81364}"/>
+    <cellStyle name="Normal 5" xfId="16" xr:uid="{49545144-F3A9-4825-A6BA-5936F162C050}"/>
+    <cellStyle name="Normal 6" xfId="12" xr:uid="{4EF6E554-0085-465F-A330-E88543107D27}"/>
+    <cellStyle name="Normal 7" xfId="27" xr:uid="{2534D22A-6169-4D9A-B012-B7294C0AC758}"/>
+    <cellStyle name="Normal 8" xfId="40" xr:uid="{19F067A3-D80D-48FD-BF06-BF292EC8BB24}"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
     <cellStyle name="Percent 2" xfId="6" xr:uid="{BC0C5A78-644A-4E8A-8133-E61F2E94C271}"/>
+    <cellStyle name="Percent 2 2" xfId="21" xr:uid="{ABEFFD90-1C5B-44F4-94F2-8F5C545B6CE3}"/>
+    <cellStyle name="Percent 2 3" xfId="34" xr:uid="{F1235FEE-D3ED-46E3-8284-249567537760}"/>
+    <cellStyle name="Percent 2 4" xfId="47" xr:uid="{9B5DB1B9-289D-4910-A43A-3BB8D718BF50}"/>
     <cellStyle name="Percent 3" xfId="10" xr:uid="{5A577D97-9D8D-44CD-94BE-F7C4D5E216D4}"/>
+    <cellStyle name="Percent 3 2" xfId="25" xr:uid="{AA877386-D0A2-4CA8-9066-CA902896BC86}"/>
+    <cellStyle name="Percent 3 3" xfId="38" xr:uid="{2C62A5E3-4F5C-4053-B9EE-104D29570544}"/>
+    <cellStyle name="Percent 3 4" xfId="51" xr:uid="{71214003-4755-4936-B69C-71301425DFDB}"/>
+    <cellStyle name="Percent 4" xfId="17" xr:uid="{766E512C-159B-4546-AE75-4E591D8E346F}"/>
+    <cellStyle name="Percent 5" xfId="14" xr:uid="{761C96E9-6829-47E8-ABEF-BAFE0B7B7D1A}"/>
+    <cellStyle name="Percent 6" xfId="29" xr:uid="{3C9E2FB6-4013-4108-851E-44B42960E338}"/>
+    <cellStyle name="Percent 7" xfId="42" xr:uid="{E615D24B-233E-4FC3-8466-3E474BB7156C}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -3235,10 +3350,10 @@
       <c r="H41" s="22"/>
     </row>
     <row r="44" spans="1:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="B44" s="94" t="s">
+      <c r="B44" s="103" t="s">
         <v>101</v>
       </c>
-      <c r="C44" s="94"/>
+      <c r="C44" s="103"/>
     </row>
     <row r="45" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="26" t="s">
@@ -3920,26 +4035,26 @@
       <c r="C130" s="66"/>
     </row>
     <row r="131" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B131" s="98" t="s">
+      <c r="B131" s="97" t="s">
         <v>395</v>
       </c>
-      <c r="C131" s="98" t="s">
+      <c r="C131" s="97" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="132" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B132" s="98" t="s">
+      <c r="B132" s="97" t="s">
         <v>393</v>
       </c>
-      <c r="C132" s="98" t="s">
+      <c r="C132" s="97" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="133" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B133" s="98" t="s">
+      <c r="B133" s="97" t="s">
         <v>394</v>
       </c>
-      <c r="C133" s="98" t="s">
+      <c r="C133" s="97" t="s">
         <v>381</v>
       </c>
     </row>
@@ -3950,18 +4065,18 @@
       <c r="C134" s="66"/>
     </row>
     <row r="135" spans="2:12" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B135" s="99" t="s">
+      <c r="B135" s="98" t="s">
         <v>396</v>
       </c>
-      <c r="C135" s="100" t="s">
+      <c r="C135" s="99" t="s">
         <v>390</v>
       </c>
     </row>
     <row r="136" spans="2:12" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="B136" s="101" t="s">
+      <c r="B136" s="100" t="s">
         <v>397</v>
       </c>
-      <c r="C136" s="101" t="s">
+      <c r="C136" s="100" t="s">
         <v>391</v>
       </c>
     </row>
@@ -4061,7 +4176,7 @@
   <mergeCells count="1">
     <mergeCell ref="B44:C44"/>
   </mergeCells>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4071,8 +4186,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B3:AO265"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C190" sqref="C190"/>
+    <sheetView tabSelected="1" topLeftCell="H140" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q173" sqref="Q173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5872,7 +5987,7 @@
       <c r="P92" s="22"/>
     </row>
     <row r="93" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B93" s="96" t="s">
+      <c r="B93" s="95" t="s">
         <v>29</v>
       </c>
       <c r="C93" s="30"/>
@@ -5884,10 +5999,10 @@
         <f>Commodities!C136</f>
         <v>Aviation international - New</v>
       </c>
-      <c r="F93" s="97" t="s">
+      <c r="F93" s="96" t="s">
         <v>61</v>
       </c>
-      <c r="G93" s="97" t="s">
+      <c r="G93" s="96" t="s">
         <v>383</v>
       </c>
       <c r="H93" s="30"/>
@@ -6342,7 +6457,7 @@
         <v>21.831587082756254</v>
       </c>
       <c r="K105" s="48">
-        <f t="shared" ref="K105:K144" si="1">J105-((J105-L105)/4)</f>
+        <f t="shared" ref="K105:K142" si="1">J105-((J105-L105)/4)</f>
         <v>21.831587082756254</v>
       </c>
       <c r="L105" s="48">
@@ -8671,7 +8786,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="145" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B145" s="1" t="str">
         <f>D51</f>
         <v>T-BUS-ICE_B10041</v>
@@ -8731,7 +8846,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="146" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B146" s="1" t="str">
         <f>D52</f>
         <v>T-BUS-ICE_NGB41</v>
@@ -8791,7 +8906,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="147" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B147" s="1" t="str">
         <f>D53</f>
         <v>T-BUS-BEV_ELC41</v>
@@ -8851,7 +8966,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="148" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B148" s="1" t="str">
         <f>D54</f>
         <v>T-BUS-FCV_HYD41</v>
@@ -8911,7 +9026,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="149" spans="2:19" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:22" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B149" s="27" t="s">
         <v>117</v>
       </c>
@@ -8933,7 +9048,7 @@
       <c r="R149" s="27"/>
       <c r="S149" s="27"/>
     </row>
-    <row r="150" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B150" s="1" t="str">
         <f>D56</f>
         <v>T-LPT-BEV_ELC51</v>
@@ -8993,7 +9108,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="151" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B151" s="1" t="str">
         <f>D57</f>
         <v>T-HPT-BEV_ELC51</v>
@@ -9053,7 +9168,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="152" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B152" s="1" t="str">
         <f>D58</f>
         <v>T-HPT-ICE_DST51</v>
@@ -9113,7 +9228,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="153" spans="2:19" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:22" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B153" s="27" t="s">
         <v>118</v>
       </c>
@@ -9135,7 +9250,7 @@
       <c r="R153" s="27"/>
       <c r="S153" s="27"/>
     </row>
-    <row r="154" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B154" s="1" t="str">
         <f t="shared" ref="B154:B160" si="6">D60</f>
         <v>T-LGT-ICE_DST61</v>
@@ -9183,10 +9298,10 @@
         <v>0.51755174200814014</v>
       </c>
       <c r="P154" s="51">
-        <v>22.277000000000001</v>
+        <v>20.794499999999999</v>
       </c>
       <c r="Q154" s="51">
-        <v>4.5999999999999999E-2</v>
+        <v>4.5493804447819669E-2</v>
       </c>
       <c r="R154" s="50">
         <v>20</v>
@@ -9195,7 +9310,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="155" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B155" s="1" t="str">
         <f t="shared" si="6"/>
         <v>T-LGT-HEV_DST61</v>
@@ -9243,10 +9358,11 @@
         <v>0.51121564564909838</v>
       </c>
       <c r="P155" s="51">
-        <v>22.277000000000001</v>
+        <v>20.794499999999999</v>
       </c>
       <c r="Q155" s="51">
-        <v>4.5999999999999999E-2</v>
+        <f>Q154</f>
+        <v>4.5493804447819669E-2</v>
       </c>
       <c r="R155" s="50">
         <v>20</v>
@@ -9255,7 +9371,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="156" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B156" s="1" t="str">
         <f t="shared" si="6"/>
         <v>T-LGT-PHEV_DST61</v>
@@ -9303,10 +9419,11 @@
         <v>0.5684028228063388</v>
       </c>
       <c r="P156" s="51">
-        <v>22.277000000000001</v>
+        <v>20.794499999999999</v>
       </c>
       <c r="Q156" s="51">
-        <v>4.5999999999999999E-2</v>
+        <f t="shared" ref="Q156:Q160" si="8">Q155</f>
+        <v>4.5493804447819669E-2</v>
       </c>
       <c r="R156" s="50">
         <v>20</v>
@@ -9315,7 +9432,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="157" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B157" s="1" t="str">
         <f t="shared" si="6"/>
         <v>T-LGT-ICE_NBG61</v>
@@ -9363,10 +9480,11 @@
         <v>0.53670515183033241</v>
       </c>
       <c r="P157" s="51">
-        <v>22.277000000000001</v>
+        <v>20.794499999999999</v>
       </c>
       <c r="Q157" s="51">
-        <v>4.5999999999999999E-2</v>
+        <f t="shared" si="8"/>
+        <v>4.5493804447819669E-2</v>
       </c>
       <c r="R157" s="50">
         <v>20</v>
@@ -9375,7 +9493,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="158" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B158" s="1" t="str">
         <f t="shared" si="6"/>
         <v>T-LGT-PHEV_NGB61</v>
@@ -9423,10 +9541,11 @@
         <v>0.5684028228063388</v>
       </c>
       <c r="P158" s="51">
-        <v>22.277000000000001</v>
+        <v>20.794499999999999</v>
       </c>
       <c r="Q158" s="51">
-        <v>4.5999999999999999E-2</v>
+        <f t="shared" si="8"/>
+        <v>4.5493804447819669E-2</v>
       </c>
       <c r="R158" s="50">
         <v>20</v>
@@ -9435,7 +9554,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="159" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B159" s="1" t="str">
         <f t="shared" si="6"/>
         <v>T-LGT-FCV_HYD61</v>
@@ -9483,10 +9602,11 @@
         <v>0.56295480691313882</v>
       </c>
       <c r="P159" s="51">
-        <v>22.277000000000001</v>
+        <v>20.794499999999999</v>
       </c>
       <c r="Q159" s="51">
-        <v>4.5999999999999999E-2</v>
+        <f t="shared" si="8"/>
+        <v>4.5493804447819669E-2</v>
       </c>
       <c r="R159" s="50">
         <v>20</v>
@@ -9494,8 +9614,9 @@
       <c r="S159" s="50">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="160" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="U159" s="101"/>
+    </row>
+    <row r="160" spans="2:22" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B160" s="1" t="str">
         <f t="shared" si="6"/>
         <v>T-LGT-BEV_ELC61</v>
@@ -9543,10 +9664,11 @@
         <v>0.57558924309386739</v>
       </c>
       <c r="P160" s="51">
-        <v>22.277000000000001</v>
+        <v>20.794499999999999</v>
       </c>
       <c r="Q160" s="51">
-        <v>4.5999999999999999E-2</v>
+        <f t="shared" si="8"/>
+        <v>4.5493804447819669E-2</v>
       </c>
       <c r="R160" s="50">
         <v>20</v>
@@ -9554,8 +9676,10 @@
       <c r="S160" s="50">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="161" spans="2:19" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="U160" s="101"/>
+      <c r="V160" s="1"/>
+    </row>
+    <row r="161" spans="2:22" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B161" s="27" t="s">
         <v>342</v>
       </c>
@@ -9576,10 +9700,11 @@
       <c r="Q161" s="27"/>
       <c r="R161" s="27"/>
       <c r="S161" s="27"/>
-    </row>
-    <row r="162" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U161" s="102"/>
+    </row>
+    <row r="162" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B162" s="1" t="str">
-        <f t="shared" ref="B162:B168" si="8">D68</f>
+        <f t="shared" ref="B162:B168" si="9">D68</f>
         <v>T-MGT-ICE_DST71</v>
       </c>
       <c r="C162" s="1" t="str">
@@ -9591,72 +9716,70 @@
         <v>TRAF</v>
       </c>
       <c r="E162" s="1">
-        <f t="shared" ref="E162:R162" si="9">E170</f>
+        <f t="shared" ref="E162:J162" si="10">E170</f>
         <v>2019</v>
       </c>
       <c r="F162" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.121</v>
       </c>
       <c r="G162" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.13200000000000001</v>
       </c>
       <c r="H162" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0.157</v>
       </c>
       <c r="I162" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>95.69</v>
       </c>
       <c r="J162" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>100.95</v>
       </c>
       <c r="K162" s="48">
-        <f t="shared" ref="K162:K168" si="10">J162-((J162-L162)/4)</f>
+        <f t="shared" ref="K162:K168" si="11">J162-((J162-L162)/4)</f>
         <v>100.95</v>
       </c>
       <c r="L162" s="1">
-        <f>L170</f>
+        <f t="shared" ref="L162:O168" si="12">L170</f>
         <v>100.95</v>
       </c>
       <c r="M162" s="48">
-        <f>M170</f>
+        <f t="shared" si="12"/>
         <v>2.1157042474212369</v>
       </c>
       <c r="N162" s="48">
-        <f>N170</f>
+        <f t="shared" si="12"/>
         <v>2.1689507539373367</v>
       </c>
       <c r="O162" s="48">
-        <f>O170</f>
+        <f t="shared" si="12"/>
         <v>2.1689507539373367</v>
       </c>
-      <c r="P162" s="1">
-        <f>P170</f>
-        <v>57.43</v>
-      </c>
-      <c r="Q162" s="1">
-        <f>Q170</f>
-        <v>8.8650000000000002</v>
+      <c r="P162" s="48">
+        <v>29.397500000000001</v>
+      </c>
+      <c r="Q162" s="51">
+        <v>3.592571901094749</v>
       </c>
       <c r="R162" s="1">
         <v>20</v>
       </c>
       <c r="S162" s="1">
-        <f>S170</f>
+        <f t="shared" ref="S162:S168" si="13">S170</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="163" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B163" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>T-MGT-HEV_DST71</v>
       </c>
       <c r="C163" s="1" t="str">
-        <f t="shared" ref="C163:R168" si="11">C171</f>
+        <f t="shared" ref="C163:J168" si="14">C171</f>
         <v>TRADSB</v>
       </c>
       <c r="D163" s="1" t="str">
@@ -9664,27 +9787,27 @@
         <v>TRAF</v>
       </c>
       <c r="E163" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>2019</v>
       </c>
       <c r="F163" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.17299999999999999</v>
       </c>
       <c r="G163" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.189</v>
       </c>
       <c r="H163" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.224</v>
       </c>
       <c r="I163" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>124.73</v>
       </c>
       <c r="J163" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>125.12</v>
       </c>
       <c r="K163" s="48">
@@ -9692,403 +9815,397 @@
         <v>123.88250000000001</v>
       </c>
       <c r="L163" s="1">
-        <f>L171</f>
+        <f t="shared" si="12"/>
         <v>120.17</v>
       </c>
       <c r="M163" s="48">
-        <f>M171</f>
+        <f t="shared" si="12"/>
         <v>3.5721072259038325</v>
       </c>
       <c r="N163" s="48">
-        <f>N171</f>
+        <f t="shared" si="12"/>
         <v>3.0618061936318557</v>
       </c>
       <c r="O163" s="48">
-        <f>O171</f>
+        <f t="shared" si="12"/>
         <v>2.3858458293310703</v>
       </c>
-      <c r="P163" s="1">
-        <f>P171</f>
-        <v>57.43</v>
-      </c>
-      <c r="Q163" s="1">
-        <f>Q171</f>
-        <v>8.8650000000000002</v>
+      <c r="P163" s="48">
+        <v>29.397500000000001</v>
+      </c>
+      <c r="Q163" s="51">
+        <f>Q162</f>
+        <v>3.592571901094749</v>
       </c>
       <c r="R163" s="1">
         <v>20</v>
       </c>
       <c r="S163" s="1">
-        <f>S171</f>
+        <f t="shared" si="13"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="164" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B164" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>T-MGT-FCV_HYD71</v>
       </c>
       <c r="C164" s="1" t="str">
+        <f t="shared" si="14"/>
+        <v>TRAHYD</v>
+      </c>
+      <c r="D164" s="1" t="str">
+        <f t="shared" ref="D164:D168" si="15">D163</f>
+        <v>TRAF</v>
+      </c>
+      <c r="E164" s="1">
+        <f t="shared" si="14"/>
+        <v>2019</v>
+      </c>
+      <c r="F164" s="1">
+        <f t="shared" si="14"/>
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="G164" s="1">
+        <f t="shared" si="14"/>
+        <v>0.22</v>
+      </c>
+      <c r="H164" s="1">
+        <f t="shared" si="14"/>
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="I164" s="1">
+        <f t="shared" si="14"/>
+        <v>345.67</v>
+      </c>
+      <c r="J164" s="1">
+        <f t="shared" si="14"/>
+        <v>222.22</v>
+      </c>
+      <c r="K164" s="48">
         <f t="shared" si="11"/>
-        <v>TRAHYD</v>
-      </c>
-      <c r="D164" s="1" t="str">
-        <f t="shared" ref="D164:D168" si="12">D163</f>
-        <v>TRAF</v>
-      </c>
-      <c r="E164" s="1">
-        <f t="shared" si="11"/>
-        <v>2019</v>
-      </c>
-      <c r="F164" s="1">
-        <f t="shared" si="11"/>
-        <v>0.20100000000000001</v>
-      </c>
-      <c r="G164" s="1">
-        <f t="shared" si="11"/>
-        <v>0.22</v>
-      </c>
-      <c r="H164" s="1">
-        <f t="shared" si="11"/>
-        <v>0.26200000000000001</v>
-      </c>
-      <c r="I164" s="1">
-        <f t="shared" si="11"/>
-        <v>345.67</v>
-      </c>
-      <c r="J164" s="1">
-        <f t="shared" si="11"/>
-        <v>222.22</v>
-      </c>
-      <c r="K164" s="48">
-        <f t="shared" si="10"/>
         <v>195.70750000000001</v>
       </c>
       <c r="L164" s="1">
-        <f>L172</f>
+        <f t="shared" si="12"/>
         <v>116.17</v>
       </c>
       <c r="M164" s="48">
-        <f>M172</f>
+        <f t="shared" si="12"/>
         <v>3.5721072259038325</v>
       </c>
       <c r="N164" s="48">
-        <f>N172</f>
+        <f t="shared" si="12"/>
         <v>3.0618061936318557</v>
       </c>
       <c r="O164" s="48">
-        <f>O172</f>
+        <f t="shared" si="12"/>
         <v>2.3858458293310703</v>
       </c>
-      <c r="P164" s="1">
-        <f>P172</f>
-        <v>57.43</v>
-      </c>
-      <c r="Q164" s="1">
-        <f>Q172</f>
-        <v>8.8650000000000002</v>
+      <c r="P164" s="48">
+        <v>29.397500000000001</v>
+      </c>
+      <c r="Q164" s="51">
+        <f t="shared" ref="Q164:Q168" si="16">Q163</f>
+        <v>3.592571901094749</v>
       </c>
       <c r="R164" s="1">
         <v>20</v>
       </c>
       <c r="S164" s="1">
-        <f>S172</f>
+        <f t="shared" si="13"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="165" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B165" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>T-MGT-ICE_NGB71</v>
       </c>
       <c r="C165" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>TRANGB</v>
       </c>
       <c r="D165" s="1" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>TRAF</v>
       </c>
       <c r="E165" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>2019</v>
       </c>
       <c r="F165" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.11799999999999999</v>
       </c>
       <c r="G165" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.14099999999999999</v>
       </c>
       <c r="H165" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.155</v>
       </c>
       <c r="I165" s="1">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>115.69</v>
       </c>
       <c r="J165" s="1">
+        <f t="shared" si="14"/>
+        <v>120.95</v>
+      </c>
+      <c r="K165" s="48">
         <f t="shared" si="11"/>
         <v>120.95</v>
       </c>
-      <c r="K165" s="48">
-        <f t="shared" si="10"/>
+      <c r="L165" s="1">
+        <f t="shared" si="12"/>
         <v>120.95</v>
       </c>
-      <c r="L165" s="1">
-        <f>L173</f>
-        <v>120.95</v>
-      </c>
       <c r="M165" s="48">
-        <f>M173</f>
+        <f t="shared" si="12"/>
         <v>5.0989820625747049</v>
       </c>
       <c r="N165" s="48">
-        <f>N173</f>
+        <f t="shared" si="12"/>
         <v>3.5538821890369761</v>
       </c>
       <c r="O165" s="48">
-        <f>O173</f>
+        <f t="shared" si="12"/>
         <v>2.3292245236828353</v>
       </c>
-      <c r="P165" s="1">
-        <f>P173</f>
-        <v>57.43</v>
-      </c>
-      <c r="Q165" s="1">
-        <f>Q173</f>
-        <v>8.8650000000000002</v>
+      <c r="P165" s="48">
+        <v>29.397500000000001</v>
+      </c>
+      <c r="Q165" s="51">
+        <f t="shared" si="16"/>
+        <v>3.592571901094749</v>
       </c>
       <c r="R165" s="1">
         <v>20</v>
       </c>
       <c r="S165" s="1">
-        <f>S173</f>
+        <f t="shared" si="13"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="166" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B166" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>T-MGT-HEV_NGB71</v>
       </c>
       <c r="C166" s="1" t="str">
+        <f t="shared" si="14"/>
+        <v>TRANGB</v>
+      </c>
+      <c r="D166" s="1" t="str">
+        <f t="shared" si="15"/>
+        <v>TRAF</v>
+      </c>
+      <c r="E166" s="1">
+        <f t="shared" si="14"/>
+        <v>2019</v>
+      </c>
+      <c r="F166" s="1">
+        <f t="shared" si="14"/>
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="G166" s="1">
+        <f t="shared" si="14"/>
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="H166" s="1">
+        <f t="shared" si="14"/>
+        <v>0.222</v>
+      </c>
+      <c r="I166" s="1">
+        <f t="shared" si="14"/>
+        <v>144.72999999999999</v>
+      </c>
+      <c r="J166" s="1">
+        <f t="shared" si="14"/>
+        <v>145.12</v>
+      </c>
+      <c r="K166" s="48">
         <f t="shared" si="11"/>
-        <v>TRANGB</v>
-      </c>
-      <c r="D166" s="1" t="str">
+        <v>143.88249999999999</v>
+      </c>
+      <c r="L166" s="1">
         <f t="shared" si="12"/>
-        <v>TRAF</v>
-      </c>
-      <c r="E166" s="1">
-        <f t="shared" si="11"/>
-        <v>2019</v>
-      </c>
-      <c r="F166" s="1">
-        <f t="shared" si="11"/>
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="G166" s="1">
-        <f t="shared" si="11"/>
-        <v>0.20100000000000001</v>
-      </c>
-      <c r="H166" s="1">
-        <f t="shared" si="11"/>
-        <v>0.222</v>
-      </c>
-      <c r="I166" s="1">
-        <f t="shared" si="11"/>
-        <v>144.72999999999999</v>
-      </c>
-      <c r="J166" s="1">
-        <f t="shared" si="11"/>
-        <v>145.12</v>
-      </c>
-      <c r="K166" s="48">
-        <f t="shared" si="10"/>
-        <v>143.88249999999999</v>
-      </c>
-      <c r="L166" s="1">
-        <f>L174</f>
         <v>140.16999999999999</v>
       </c>
       <c r="M166" s="48">
-        <f>M174</f>
+        <f t="shared" si="12"/>
         <v>5.0989820625747049</v>
       </c>
       <c r="N166" s="48">
-        <f>N174</f>
+        <f t="shared" si="12"/>
         <v>3.5538821890369761</v>
       </c>
       <c r="O166" s="48">
-        <f>O174</f>
+        <f t="shared" si="12"/>
         <v>2.3292245236828353</v>
       </c>
-      <c r="P166" s="1">
-        <f>P174</f>
-        <v>57.43</v>
-      </c>
-      <c r="Q166" s="1">
-        <f>Q174</f>
-        <v>8.8650000000000002</v>
+      <c r="P166" s="48">
+        <v>29.397500000000001</v>
+      </c>
+      <c r="Q166" s="51">
+        <f t="shared" si="16"/>
+        <v>3.592571901094749</v>
       </c>
       <c r="R166" s="1">
         <v>20</v>
       </c>
       <c r="S166" s="1">
-        <f>S174</f>
+        <f t="shared" si="13"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="167" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B167" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>T-MGT-ICE_LNG71</v>
       </c>
       <c r="C167" s="1" t="str">
+        <f t="shared" si="14"/>
+        <v>TRALNG</v>
+      </c>
+      <c r="D167" s="1" t="str">
+        <f t="shared" si="15"/>
+        <v>TRAF</v>
+      </c>
+      <c r="E167" s="1">
+        <f t="shared" si="14"/>
+        <v>2019</v>
+      </c>
+      <c r="F167" s="1">
+        <f t="shared" si="14"/>
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="G167" s="1">
+        <f t="shared" si="14"/>
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="H167" s="1">
+        <f t="shared" si="14"/>
+        <v>0.155</v>
+      </c>
+      <c r="I167" s="1">
+        <f t="shared" si="14"/>
+        <v>130.68600000000001</v>
+      </c>
+      <c r="J167" s="1">
+        <f t="shared" si="14"/>
+        <v>128.75800000000001</v>
+      </c>
+      <c r="K167" s="48">
         <f t="shared" si="11"/>
-        <v>TRALNG</v>
-      </c>
-      <c r="D167" s="1" t="str">
+        <v>128.11425</v>
+      </c>
+      <c r="L167" s="1">
         <f t="shared" si="12"/>
-        <v>TRAF</v>
-      </c>
-      <c r="E167" s="1">
-        <f t="shared" si="11"/>
-        <v>2019</v>
-      </c>
-      <c r="F167" s="1">
-        <f t="shared" si="11"/>
-        <v>0.11799999999999999</v>
-      </c>
-      <c r="G167" s="1">
-        <f t="shared" si="11"/>
-        <v>0.14099999999999999</v>
-      </c>
-      <c r="H167" s="1">
-        <f t="shared" si="11"/>
-        <v>0.155</v>
-      </c>
-      <c r="I167" s="1">
-        <f t="shared" si="11"/>
-        <v>130.68600000000001</v>
-      </c>
-      <c r="J167" s="1">
-        <f t="shared" si="11"/>
-        <v>128.75800000000001</v>
-      </c>
-      <c r="K167" s="48">
-        <f t="shared" si="10"/>
-        <v>128.11425</v>
-      </c>
-      <c r="L167" s="1">
-        <f>L175</f>
         <v>126.18300000000001</v>
       </c>
       <c r="M167" s="48">
-        <f>M175</f>
+        <f t="shared" si="12"/>
         <v>5.0989820625747049</v>
       </c>
       <c r="N167" s="48">
-        <f>N175</f>
+        <f t="shared" si="12"/>
         <v>3.5538821890369761</v>
       </c>
       <c r="O167" s="48">
-        <f>O175</f>
+        <f t="shared" si="12"/>
         <v>2.3292245236828353</v>
       </c>
-      <c r="P167" s="1">
-        <f>P175</f>
-        <v>57.43</v>
-      </c>
-      <c r="Q167" s="1">
-        <f>Q175</f>
-        <v>8.8650000000000002</v>
+      <c r="P167" s="48">
+        <v>29.397500000000001</v>
+      </c>
+      <c r="Q167" s="51">
+        <f t="shared" si="16"/>
+        <v>3.592571901094749</v>
       </c>
       <c r="R167" s="1">
         <v>20</v>
       </c>
       <c r="S167" s="1">
-        <f>S175</f>
+        <f t="shared" si="13"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="168" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B168" s="1" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>T-MGT-BEV_ELC71</v>
       </c>
       <c r="C168" s="1" t="str">
+        <f t="shared" si="14"/>
+        <v>TRAELC</v>
+      </c>
+      <c r="D168" s="1" t="str">
+        <f t="shared" si="15"/>
+        <v>TRAF</v>
+      </c>
+      <c r="E168" s="1">
+        <f t="shared" si="14"/>
+        <v>2019</v>
+      </c>
+      <c r="F168" s="1">
+        <f t="shared" si="14"/>
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="G168" s="1">
+        <f t="shared" si="14"/>
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="H168" s="1">
+        <f t="shared" si="14"/>
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="I168" s="1">
+        <f t="shared" si="14"/>
+        <v>345.67</v>
+      </c>
+      <c r="J168" s="1">
+        <f t="shared" si="14"/>
+        <v>274.11</v>
+      </c>
+      <c r="K168" s="48">
         <f t="shared" si="11"/>
-        <v>TRAELC</v>
-      </c>
-      <c r="D168" s="1" t="str">
+        <v>234.625</v>
+      </c>
+      <c r="L168" s="1">
         <f t="shared" si="12"/>
-        <v>TRAF</v>
-      </c>
-      <c r="E168" s="1">
-        <f t="shared" si="11"/>
-        <v>2019</v>
-      </c>
-      <c r="F168" s="1">
-        <f t="shared" si="11"/>
-        <v>0.34699999999999998</v>
-      </c>
-      <c r="G168" s="1">
-        <f t="shared" si="11"/>
-        <v>0.34699999999999998</v>
-      </c>
-      <c r="H168" s="1">
-        <f t="shared" si="11"/>
-        <v>0.34699999999999998</v>
-      </c>
-      <c r="I168" s="1">
-        <f t="shared" si="11"/>
-        <v>345.67</v>
-      </c>
-      <c r="J168" s="1">
-        <f t="shared" si="11"/>
-        <v>274.11</v>
-      </c>
-      <c r="K168" s="48">
-        <f t="shared" si="10"/>
-        <v>234.625</v>
-      </c>
-      <c r="L168" s="1">
-        <f>L176</f>
         <v>116.17</v>
       </c>
       <c r="M168" s="48">
-        <f>M176</f>
+        <f t="shared" si="12"/>
         <v>3.5721072259038325</v>
       </c>
       <c r="N168" s="48">
-        <f>N176</f>
+        <f t="shared" si="12"/>
         <v>3.0618061936318557</v>
       </c>
       <c r="O168" s="48">
-        <f>O176</f>
+        <f t="shared" si="12"/>
         <v>2.3858458293310703</v>
       </c>
-      <c r="P168" s="1">
-        <f>P176</f>
-        <v>57.43</v>
-      </c>
-      <c r="Q168" s="1">
-        <f>Q176</f>
-        <v>8.8650000000000002</v>
+      <c r="P168" s="48">
+        <v>29.397500000000001</v>
+      </c>
+      <c r="Q168" s="51">
+        <f t="shared" si="16"/>
+        <v>3.592571901094749</v>
       </c>
       <c r="R168" s="1">
         <v>20</v>
       </c>
       <c r="S168" s="1">
-        <f>S176</f>
+        <f t="shared" si="13"/>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="169" spans="2:19" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:22" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B169" s="27" t="s">
         <v>119</v>
       </c>
@@ -10110,9 +10227,9 @@
       <c r="R169" s="27"/>
       <c r="S169" s="27"/>
     </row>
-    <row r="170" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B170" s="1" t="str">
-        <f t="shared" ref="B170:B176" si="13">D76</f>
+        <f t="shared" ref="B170:B176" si="17">D76</f>
         <v>T-HGT-ICE_DST81</v>
       </c>
       <c r="C170" s="1" t="str">
@@ -10142,7 +10259,7 @@
         <v>100.95</v>
       </c>
       <c r="K170" s="48">
-        <f t="shared" ref="K170:K176" si="14">J170-((J170-L170)/4)</f>
+        <f t="shared" ref="K170:K176" si="18">J170-((J170-L170)/4)</f>
         <v>100.95</v>
       </c>
       <c r="L170" s="51">
@@ -10158,10 +10275,10 @@
         <v>2.1689507539373367</v>
       </c>
       <c r="P170" s="51">
-        <v>57.43</v>
+        <v>50.915999999999997</v>
       </c>
       <c r="Q170" s="51">
-        <v>8.8650000000000002</v>
+        <v>9.2231504438872829</v>
       </c>
       <c r="R170" s="50">
         <v>20</v>
@@ -10169,10 +10286,11 @@
       <c r="S170" s="50">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="171" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V170" s="1"/>
+    </row>
+    <row r="171" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B171" s="1" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>T-HGT-HEV_DST81</v>
       </c>
       <c r="C171" s="1" t="str">
@@ -10202,7 +10320,7 @@
         <v>125.12</v>
       </c>
       <c r="K171" s="48">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>123.88250000000001</v>
       </c>
       <c r="L171" s="51">
@@ -10218,10 +10336,11 @@
         <v>2.3858458293310703</v>
       </c>
       <c r="P171" s="51">
-        <v>57.43</v>
+        <v>50.915999999999997</v>
       </c>
       <c r="Q171" s="51">
-        <v>8.8650000000000002</v>
+        <f>Q170</f>
+        <v>9.2231504438872829</v>
       </c>
       <c r="R171" s="50">
         <v>20</v>
@@ -10229,10 +10348,11 @@
       <c r="S171" s="50">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="172" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V171" s="1"/>
+    </row>
+    <row r="172" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B172" s="1" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>T-HGT-FCV_HYD81</v>
       </c>
       <c r="C172" s="1" t="str">
@@ -10240,7 +10360,7 @@
         <v>TRAHYD</v>
       </c>
       <c r="D172" s="50" t="str">
-        <f t="shared" ref="D172:D176" si="15">D171</f>
+        <f t="shared" ref="D172:D176" si="19">D171</f>
         <v>TRAF</v>
       </c>
       <c r="E172" s="50">
@@ -10262,7 +10382,7 @@
         <v>222.22</v>
       </c>
       <c r="K172" s="48">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>195.70750000000001</v>
       </c>
       <c r="L172" s="51">
@@ -10278,10 +10398,11 @@
         <v>2.3858458293310703</v>
       </c>
       <c r="P172" s="51">
-        <v>57.43</v>
+        <v>50.915999999999997</v>
       </c>
       <c r="Q172" s="51">
-        <v>8.8650000000000002</v>
+        <f t="shared" ref="Q172:Q176" si="20">Q171</f>
+        <v>9.2231504438872829</v>
       </c>
       <c r="R172" s="50">
         <v>20</v>
@@ -10289,10 +10410,11 @@
       <c r="S172" s="50">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="173" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V172" s="1"/>
+    </row>
+    <row r="173" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B173" s="1" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>T-HGT-ICE_NGB81</v>
       </c>
       <c r="C173" s="1" t="str">
@@ -10300,7 +10422,7 @@
         <v>TRANGB</v>
       </c>
       <c r="D173" s="50" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>TRAF</v>
       </c>
       <c r="E173" s="50">
@@ -10322,7 +10444,7 @@
         <v>120.95</v>
       </c>
       <c r="K173" s="48">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>120.95</v>
       </c>
       <c r="L173" s="51">
@@ -10338,10 +10460,11 @@
         <v>2.3292245236828353</v>
       </c>
       <c r="P173" s="51">
-        <v>57.43</v>
+        <v>50.915999999999997</v>
       </c>
       <c r="Q173" s="51">
-        <v>8.8650000000000002</v>
+        <f t="shared" si="20"/>
+        <v>9.2231504438872829</v>
       </c>
       <c r="R173" s="50">
         <v>20</v>
@@ -10349,10 +10472,11 @@
       <c r="S173" s="50">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="174" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V173" s="1"/>
+    </row>
+    <row r="174" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B174" s="1" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>T-HGT-HEV_NGB81</v>
       </c>
       <c r="C174" s="1" t="str">
@@ -10360,7 +10484,7 @@
         <v>TRANGB</v>
       </c>
       <c r="D174" s="50" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>TRAF</v>
       </c>
       <c r="E174" s="50">
@@ -10382,7 +10506,7 @@
         <v>145.12</v>
       </c>
       <c r="K174" s="48">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>143.88249999999999</v>
       </c>
       <c r="L174" s="51">
@@ -10398,10 +10522,11 @@
         <v>2.3292245236828353</v>
       </c>
       <c r="P174" s="51">
-        <v>57.43</v>
+        <v>50.915999999999997</v>
       </c>
       <c r="Q174" s="51">
-        <v>8.8650000000000002</v>
+        <f t="shared" si="20"/>
+        <v>9.2231504438872829</v>
       </c>
       <c r="R174" s="50">
         <v>20</v>
@@ -10410,9 +10535,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="175" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B175" s="1" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>T-HGT-ICE_LNG81</v>
       </c>
       <c r="C175" s="1" t="str">
@@ -10420,7 +10545,7 @@
         <v>TRALNG</v>
       </c>
       <c r="D175" s="50" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>TRAF</v>
       </c>
       <c r="E175" s="50">
@@ -10442,7 +10567,7 @@
         <v>128.75800000000001</v>
       </c>
       <c r="K175" s="48">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>128.11425</v>
       </c>
       <c r="L175" s="51">
@@ -10458,10 +10583,11 @@
         <v>2.3292245236828353</v>
       </c>
       <c r="P175" s="51">
-        <v>57.43</v>
+        <v>50.915999999999997</v>
       </c>
       <c r="Q175" s="51">
-        <v>8.8650000000000002</v>
+        <f t="shared" si="20"/>
+        <v>9.2231504438872829</v>
       </c>
       <c r="R175" s="50">
         <v>20</v>
@@ -10470,9 +10596,9 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="176" spans="2:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B176" s="1" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>T-HGT-BEV_ELC81</v>
       </c>
       <c r="C176" s="1" t="str">
@@ -10480,7 +10606,7 @@
         <v>TRAELC</v>
       </c>
       <c r="D176" s="50" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>TRAF</v>
       </c>
       <c r="E176" s="50">
@@ -10502,7 +10628,7 @@
         <v>274.11</v>
       </c>
       <c r="K176" s="48">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>234.625</v>
       </c>
       <c r="L176" s="51">
@@ -10518,10 +10644,11 @@
         <v>2.3858458293310703</v>
       </c>
       <c r="P176" s="51">
-        <v>57.43</v>
+        <v>50.915999999999997</v>
       </c>
       <c r="Q176" s="51">
-        <v>8.8650000000000002</v>
+        <f t="shared" si="20"/>
+        <v>9.2231504438872829</v>
       </c>
       <c r="R176" s="50">
         <v>20</v>
@@ -10584,7 +10711,7 @@
         <v>469.60386878903267</v>
       </c>
       <c r="K178" s="48">
-        <f t="shared" ref="K178:K180" si="16">J178-((J178-L178)/4)</f>
+        <f t="shared" ref="K178:K179" si="21">J178-((J178-L178)/4)</f>
         <v>469.60386878903267</v>
       </c>
       <c r="L178" s="48">
@@ -10644,7 +10771,7 @@
         <v>438.88212036358203</v>
       </c>
       <c r="K179" s="48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="21"/>
         <v>438.88212036358203</v>
       </c>
       <c r="L179" s="48">
@@ -10698,17 +10825,17 @@
         <v>1.26364006003871E-2</v>
       </c>
       <c r="I180" s="73">
-        <v>582.10068176688731</v>
+        <v>682.10068176688696</v>
       </c>
       <c r="J180" s="73">
-        <v>525.06724769825223</v>
+        <v>625.067247698252</v>
       </c>
       <c r="K180" s="48">
-        <f t="shared" si="16"/>
-        <v>517.48355288613334</v>
+        <f>J180-((J180-L180)/4)</f>
+        <v>617.48355288613323</v>
       </c>
       <c r="L180" s="73">
-        <v>494.7324684497766</v>
+        <v>594.732468449777</v>
       </c>
       <c r="M180" s="73">
         <v>29.105034088344368</v>
@@ -10785,7 +10912,7 @@
     </row>
     <row r="183" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B183" s="1" t="str">
-        <f t="shared" ref="B183:B184" si="17">D89</f>
+        <f t="shared" ref="B183:B184" si="22">D89</f>
         <v>T-NAV_NEW</v>
       </c>
       <c r="C183" s="1" t="str">
@@ -10814,7 +10941,7 @@
     </row>
     <row r="184" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B184" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="22"/>
         <v>T-OTH_NEW</v>
       </c>
       <c r="C184" s="1" t="str">
@@ -10918,13 +11045,13 @@
       <c r="E187" s="80">
         <v>2019</v>
       </c>
-      <c r="F187" s="95">
+      <c r="F187" s="94">
         <v>1</v>
       </c>
-      <c r="G187" s="95">
+      <c r="G187" s="94">
         <v>1.05</v>
       </c>
-      <c r="H187" s="95">
+      <c r="H187" s="94">
         <v>1.1000000000000001</v>
       </c>
       <c r="I187" s="30"/>
@@ -11266,11 +11393,11 @@
         <v>0.5</v>
       </c>
       <c r="AI195" s="75" t="str">
-        <f t="shared" ref="AI195:AI211" si="18">B195</f>
+        <f t="shared" ref="AI195:AI211" si="23">B195</f>
         <v>T-CAR-ICE_DF21</v>
       </c>
       <c r="AJ195" s="75" t="str">
-        <f t="shared" ref="AJ195:AJ211" si="19">C195</f>
+        <f t="shared" ref="AJ195:AJ211" si="24">C195</f>
         <v>TRACNG</v>
       </c>
       <c r="AK195" s="75" t="s">
@@ -11377,11 +11504,11 @@
         <v>0.4</v>
       </c>
       <c r="AI196" s="75" t="str">
-        <f t="shared" ref="AI196" si="20">B196</f>
+        <f t="shared" ref="AI196" si="25">B196</f>
         <v>T-CAR-ICE_DF21</v>
       </c>
       <c r="AJ196" s="75" t="str">
-        <f t="shared" ref="AJ196" si="21">C196</f>
+        <f t="shared" ref="AJ196" si="26">C196</f>
         <v>TRACNG</v>
       </c>
       <c r="AK196" s="75" t="s">
@@ -11393,7 +11520,7 @@
     </row>
     <row r="197" spans="2:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B197" s="1" t="str">
-        <f t="shared" ref="B197:B202" si="22">B112</f>
+        <f t="shared" ref="B197:B202" si="27">B112</f>
         <v>T-CAR-PHEV10_GSL21</v>
       </c>
       <c r="C197" s="1" t="str">
@@ -11488,11 +11615,11 @@
         <v>0.3</v>
       </c>
       <c r="AI197" s="75" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>T-CAR-PHEV10_GSL21</v>
       </c>
       <c r="AJ197" s="75" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>TRAELC</v>
       </c>
       <c r="AK197" s="75" t="s">
@@ -11504,7 +11631,7 @@
     </row>
     <row r="198" spans="2:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B198" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>T-CAR-PHEV20_GSL21</v>
       </c>
       <c r="C198" s="1" t="str">
@@ -11599,11 +11726,11 @@
         <v>0.4</v>
       </c>
       <c r="AI198" s="75" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>T-CAR-PHEV20_GSL21</v>
       </c>
       <c r="AJ198" s="75" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>TRAELC</v>
       </c>
       <c r="AK198" s="75" t="s">
@@ -11615,7 +11742,7 @@
     </row>
     <row r="199" spans="2:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B199" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>T-CAR-PHEV40_GSL21</v>
       </c>
       <c r="C199" s="1" t="str">
@@ -11710,11 +11837,11 @@
         <v>0.5</v>
       </c>
       <c r="AI199" s="75" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>T-CAR-PHEV40_GSL21</v>
       </c>
       <c r="AJ199" s="75" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>TRAELC</v>
       </c>
       <c r="AK199" s="75" t="s">
@@ -11726,7 +11853,7 @@
     </row>
     <row r="200" spans="2:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B200" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>T-CAR-PHEV10_DST21</v>
       </c>
       <c r="C200" s="1" t="str">
@@ -11821,11 +11948,11 @@
         <v>0.3</v>
       </c>
       <c r="AI200" s="75" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>T-CAR-PHEV10_DST21</v>
       </c>
       <c r="AJ200" s="75" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>TRAELC</v>
       </c>
       <c r="AK200" s="75" t="s">
@@ -11837,7 +11964,7 @@
     </row>
     <row r="201" spans="2:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B201" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>T-CAR-PHEV20_DST21</v>
       </c>
       <c r="C201" s="1" t="str">
@@ -11932,11 +12059,11 @@
         <v>0.4</v>
       </c>
       <c r="AI201" s="75" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>T-CAR-PHEV20_DST21</v>
       </c>
       <c r="AJ201" s="75" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>TRAELC</v>
       </c>
       <c r="AK201" s="75" t="s">
@@ -11948,7 +12075,7 @@
     </row>
     <row r="202" spans="2:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B202" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>T-CAR-PHEV40_DST21</v>
       </c>
       <c r="C202" s="1" t="str">
@@ -12043,11 +12170,11 @@
         <v>0.5</v>
       </c>
       <c r="AI202" s="75" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>T-CAR-PHEV40_DST21</v>
       </c>
       <c r="AJ202" s="75" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>TRAELC</v>
       </c>
       <c r="AK202" s="75" t="s">
@@ -12154,11 +12281,11 @@
         <v>0.5</v>
       </c>
       <c r="AI203" s="75" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>T-TAX-ICE_DF31</v>
       </c>
       <c r="AJ203" s="75" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>TRACNG</v>
       </c>
       <c r="AK203" s="75" t="s">
@@ -12265,11 +12392,11 @@
         <v>0.3</v>
       </c>
       <c r="AI204" s="75" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>T-TAX-PHEV10_GSL31</v>
       </c>
       <c r="AJ204" s="75" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>TRAELC</v>
       </c>
       <c r="AK204" s="75" t="s">
@@ -12281,7 +12408,7 @@
     </row>
     <row r="205" spans="2:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B205" s="1" t="str">
-        <f t="shared" ref="B205:B209" si="23">B133</f>
+        <f t="shared" ref="B205:B209" si="28">B133</f>
         <v>T-TAX-PHEV20_GSL31</v>
       </c>
       <c r="C205" s="1" t="str">
@@ -12376,11 +12503,11 @@
         <v>0.4</v>
       </c>
       <c r="AI205" s="75" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>T-TAX-PHEV20_GSL31</v>
       </c>
       <c r="AJ205" s="75" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>TRAELC</v>
       </c>
       <c r="AK205" s="75" t="s">
@@ -12392,7 +12519,7 @@
     </row>
     <row r="206" spans="2:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B206" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>T-TAX-PHEV40_GSL31</v>
       </c>
       <c r="C206" s="1" t="str">
@@ -12487,11 +12614,11 @@
         <v>0.5</v>
       </c>
       <c r="AI206" s="75" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>T-TAX-PHEV40_GSL31</v>
       </c>
       <c r="AJ206" s="75" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>TRAELC</v>
       </c>
       <c r="AK206" s="75" t="s">
@@ -12503,7 +12630,7 @@
     </row>
     <row r="207" spans="2:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B207" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>T-TAX-PHEV10_DST31</v>
       </c>
       <c r="C207" s="1" t="str">
@@ -12598,11 +12725,11 @@
         <v>0.3</v>
       </c>
       <c r="AI207" s="75" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>T-TAX-PHEV10_DST31</v>
       </c>
       <c r="AJ207" s="75" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>TRAELC</v>
       </c>
       <c r="AK207" s="75" t="s">
@@ -12614,7 +12741,7 @@
     </row>
     <row r="208" spans="2:38" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B208" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>T-TAX-PHEV20_DST31</v>
       </c>
       <c r="C208" s="1" t="str">
@@ -12709,11 +12836,11 @@
         <v>0.4</v>
       </c>
       <c r="AI208" s="75" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>T-TAX-PHEV20_DST31</v>
       </c>
       <c r="AJ208" s="75" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>TRAELC</v>
       </c>
       <c r="AK208" s="75" t="s">
@@ -12725,7 +12852,7 @@
     </row>
     <row r="209" spans="2:41" ht="13.8" x14ac:dyDescent="0.25">
       <c r="B209" s="1" t="str">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>T-TAX-PHEV40_DST31</v>
       </c>
       <c r="C209" s="1" t="str">
@@ -12820,11 +12947,11 @@
         <v>0.5</v>
       </c>
       <c r="AI209" s="75" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>T-TAX-PHEV40_DST31</v>
       </c>
       <c r="AJ209" s="75" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>TRAELC</v>
       </c>
       <c r="AK209" s="75" t="s">
@@ -12931,11 +13058,11 @@
         <v>0.5</v>
       </c>
       <c r="AI210" s="75" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>T-LGT-PHEV_DST61</v>
       </c>
       <c r="AJ210" s="75" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>TRAELC</v>
       </c>
       <c r="AK210" s="75" t="s">
@@ -13042,11 +13169,11 @@
         <v>0.5</v>
       </c>
       <c r="AI211" s="80" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>T-LGT-PHEV_NGB61</v>
       </c>
       <c r="AJ211" s="80" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
         <v>TRAELC</v>
       </c>
       <c r="AK211" s="80" t="s">
@@ -13311,107 +13438,107 @@
         <v>IE</v>
       </c>
       <c r="G218" s="24" t="str">
-        <f t="shared" ref="G218:AF218" si="24">G194</f>
+        <f t="shared" ref="G218:AF218" si="29">G194</f>
         <v>IE-CW</v>
       </c>
       <c r="H218" s="24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>IE-D</v>
       </c>
       <c r="I218" s="24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>IE-KE</v>
       </c>
       <c r="J218" s="24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>IE-KK</v>
       </c>
       <c r="K218" s="24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>IE-LS</v>
       </c>
       <c r="L218" s="24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>IE-LD</v>
       </c>
       <c r="M218" s="24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>IE-LH</v>
       </c>
       <c r="N218" s="24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>IE-MH</v>
       </c>
       <c r="O218" s="24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>IE-OY</v>
       </c>
       <c r="P218" s="24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>IE-WH</v>
       </c>
       <c r="Q218" s="24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>IE-WX</v>
       </c>
       <c r="R218" s="24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>IE-WW</v>
       </c>
       <c r="S218" s="24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>IE-CE</v>
       </c>
       <c r="T218" s="24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>IE-CO</v>
       </c>
       <c r="U218" s="24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>IE-KY</v>
       </c>
       <c r="V218" s="24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>IE-LK</v>
       </c>
       <c r="W218" s="24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>IE-TA</v>
       </c>
       <c r="X218" s="24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>IE-WD</v>
       </c>
       <c r="Y218" s="24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>IE-G</v>
       </c>
       <c r="Z218" s="24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>IE-LM</v>
       </c>
       <c r="AA218" s="24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>IE-MO</v>
       </c>
       <c r="AB218" s="24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>IE-RN</v>
       </c>
       <c r="AC218" s="24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>IE-SO</v>
       </c>
       <c r="AD218" s="24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>IE-CN</v>
       </c>
       <c r="AE218" s="24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>IE-DL</v>
       </c>
       <c r="AF218" s="24" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>IE-MN</v>
       </c>
     </row>
@@ -13438,103 +13565,103 @@
         <v>0.04</v>
       </c>
       <c r="H219" s="77">
-        <f t="shared" ref="H219:AF219" si="25">G219</f>
+        <f t="shared" ref="H219:AF219" si="30">G219</f>
         <v>0.04</v>
       </c>
       <c r="I219" s="77">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.04</v>
       </c>
       <c r="J219" s="77">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.04</v>
       </c>
       <c r="K219" s="77">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.04</v>
       </c>
       <c r="L219" s="77">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.04</v>
       </c>
       <c r="M219" s="77">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.04</v>
       </c>
       <c r="N219" s="77">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.04</v>
       </c>
       <c r="O219" s="77">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.04</v>
       </c>
       <c r="P219" s="77">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.04</v>
       </c>
       <c r="Q219" s="77">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.04</v>
       </c>
       <c r="R219" s="77">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.04</v>
       </c>
       <c r="S219" s="77">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.04</v>
       </c>
       <c r="T219" s="77">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.04</v>
       </c>
       <c r="U219" s="77">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.04</v>
       </c>
       <c r="V219" s="77">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.04</v>
       </c>
       <c r="W219" s="77">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.04</v>
       </c>
       <c r="X219" s="77">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.04</v>
       </c>
       <c r="Y219" s="77">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.04</v>
       </c>
       <c r="Z219" s="77">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.04</v>
       </c>
       <c r="AA219" s="77">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.04</v>
       </c>
       <c r="AB219" s="77">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.04</v>
       </c>
       <c r="AC219" s="77">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.04</v>
       </c>
       <c r="AD219" s="77">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.04</v>
       </c>
       <c r="AE219" s="77">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.04</v>
       </c>
       <c r="AF219" s="77">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.04</v>
       </c>
     </row>
@@ -13561,103 +13688,103 @@
         <v>0.5</v>
       </c>
       <c r="H220" s="77">
-        <f t="shared" ref="H220:AF220" si="26">G220</f>
+        <f t="shared" ref="H220:AF220" si="31">G220</f>
         <v>0.5</v>
       </c>
       <c r="I220" s="77">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="J220" s="77">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="K220" s="77">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="L220" s="77">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="M220" s="77">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="N220" s="77">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="O220" s="77">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="P220" s="77">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="Q220" s="77">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="R220" s="77">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="S220" s="77">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="T220" s="77">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="U220" s="77">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="V220" s="77">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="W220" s="77">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="X220" s="77">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="Y220" s="77">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="Z220" s="77">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="AA220" s="77">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="AB220" s="77">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="AC220" s="77">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="AD220" s="77">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="AE220" s="77">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="AF220" s="77">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
     </row>
@@ -13684,103 +13811,103 @@
         <v>5</v>
       </c>
       <c r="H221" s="84">
-        <f t="shared" ref="H221:AF221" si="27">G221</f>
+        <f t="shared" ref="H221:AF221" si="32">G221</f>
         <v>5</v>
       </c>
       <c r="I221" s="84">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
       <c r="J221" s="84">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
       <c r="K221" s="84">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
       <c r="L221" s="84">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
       <c r="M221" s="84">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
       <c r="N221" s="84">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
       <c r="O221" s="84">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
       <c r="P221" s="84">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
       <c r="Q221" s="84">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
       <c r="R221" s="84">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
       <c r="S221" s="84">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
       <c r="T221" s="84">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
       <c r="U221" s="84">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
       <c r="V221" s="84">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
       <c r="W221" s="84">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
       <c r="X221" s="84">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
       <c r="Y221" s="84">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
       <c r="Z221" s="84">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
       <c r="AA221" s="84">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
       <c r="AB221" s="84">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
       <c r="AC221" s="84">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
       <c r="AD221" s="84">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
       <c r="AE221" s="84">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
       <c r="AF221" s="84">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
     </row>
@@ -13807,109 +13934,109 @@
         <v>0.04</v>
       </c>
       <c r="H222" s="58">
-        <f t="shared" ref="H222:AF224" si="28">G222</f>
+        <f t="shared" ref="H222:AF224" si="33">G222</f>
         <v>0.04</v>
       </c>
       <c r="I222" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.04</v>
       </c>
       <c r="J222" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.04</v>
       </c>
       <c r="K222" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.04</v>
       </c>
       <c r="L222" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.04</v>
       </c>
       <c r="M222" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.04</v>
       </c>
       <c r="N222" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.04</v>
       </c>
       <c r="O222" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.04</v>
       </c>
       <c r="P222" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.04</v>
       </c>
       <c r="Q222" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.04</v>
       </c>
       <c r="R222" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.04</v>
       </c>
       <c r="S222" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.04</v>
       </c>
       <c r="T222" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.04</v>
       </c>
       <c r="U222" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.04</v>
       </c>
       <c r="V222" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.04</v>
       </c>
       <c r="W222" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.04</v>
       </c>
       <c r="X222" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.04</v>
       </c>
       <c r="Y222" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.04</v>
       </c>
       <c r="Z222" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.04</v>
       </c>
       <c r="AA222" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.04</v>
       </c>
       <c r="AB222" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.04</v>
       </c>
       <c r="AC222" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.04</v>
       </c>
       <c r="AD222" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.04</v>
       </c>
       <c r="AE222" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.04</v>
       </c>
       <c r="AF222" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.04</v>
       </c>
     </row>
     <row r="223" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B223" s="86" t="str">
-        <f t="shared" ref="B223:B224" si="29">B222</f>
+        <f t="shared" ref="B223:B224" si="34">B222</f>
         <v>T-OTH_NEW</v>
       </c>
       <c r="C223" s="87" t="str">
@@ -13926,113 +14053,113 @@
         <v>0.2</v>
       </c>
       <c r="G223" s="58">
-        <f t="shared" ref="G223:V224" si="30">F223</f>
+        <f t="shared" ref="G223:V224" si="35">F223</f>
         <v>0.2</v>
       </c>
       <c r="H223" s="58">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>0.2</v>
       </c>
       <c r="I223" s="58">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>0.2</v>
       </c>
       <c r="J223" s="58">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>0.2</v>
       </c>
       <c r="K223" s="58">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>0.2</v>
       </c>
       <c r="L223" s="58">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>0.2</v>
       </c>
       <c r="M223" s="58">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>0.2</v>
       </c>
       <c r="N223" s="58">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>0.2</v>
       </c>
       <c r="O223" s="58">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>0.2</v>
       </c>
       <c r="P223" s="58">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>0.2</v>
       </c>
       <c r="Q223" s="58">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>0.2</v>
       </c>
       <c r="R223" s="58">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>0.2</v>
       </c>
       <c r="S223" s="58">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>0.2</v>
       </c>
       <c r="T223" s="58">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>0.2</v>
       </c>
       <c r="U223" s="58">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>0.2</v>
       </c>
       <c r="V223" s="58">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>0.2</v>
       </c>
       <c r="W223" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.2</v>
       </c>
       <c r="X223" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.2</v>
       </c>
       <c r="Y223" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.2</v>
       </c>
       <c r="Z223" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.2</v>
       </c>
       <c r="AA223" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.2</v>
       </c>
       <c r="AB223" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.2</v>
       </c>
       <c r="AC223" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.2</v>
       </c>
       <c r="AD223" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.2</v>
       </c>
       <c r="AE223" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.2</v>
       </c>
       <c r="AF223" s="58">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.2</v>
       </c>
     </row>
     <row r="224" spans="2:41" x14ac:dyDescent="0.25">
       <c r="B224" s="86" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>T-OTH_NEW</v>
       </c>
       <c r="C224" s="92" t="str">
@@ -14049,107 +14176,107 @@
         <v>5</v>
       </c>
       <c r="G224" s="84">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>5</v>
       </c>
       <c r="H224" s="84">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="I224" s="84">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="J224" s="84">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="K224" s="84">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="L224" s="84">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="M224" s="84">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="N224" s="84">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="O224" s="84">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="P224" s="84">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="Q224" s="84">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="R224" s="84">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="S224" s="84">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="T224" s="84">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="U224" s="84">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="V224" s="84">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="W224" s="84">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="X224" s="84">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="Y224" s="84">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="Z224" s="84">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="AA224" s="84">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="AB224" s="84">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="AC224" s="84">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="AD224" s="84">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="AE224" s="84">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="AF224" s="84">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
     </row>
@@ -15228,7 +15355,7 @@
       <c r="Z265" s="1"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="13" type="noConversion"/>
+  <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
Modify Efficiency and load factor for new freight vehicles
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
+++ b/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6055BA0B-005A-4C7E-A8AD-46D78DA1C52D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA43409-E371-46E4-B895-08E5B8AFA694}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1448,10 +1448,17 @@
     <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="38" x14ac:knownFonts="1">
+  <fonts count="40" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1688,6 +1695,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="13">
     <fill>
@@ -1832,11 +1845,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="108">
+  <cellStyleXfs count="214">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1845,12 +1862,21 @@
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1877,6 +1903,8 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1886,26 +1914,50 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1941,56 +1993,123 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="23" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1999,255 +2118,361 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="26" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="27" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="26" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="27" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="26" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="27" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="9" fontId="18" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="41" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="21" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="41" fontId="27" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="26" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="19" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="41" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="41" fontId="28" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="27" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="22" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="8" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="8" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="8" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="35" fillId="0" borderId="0" xfId="12" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="12" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="8" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="8" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="8" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="8" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="36" fillId="0" borderId="0" xfId="12" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="12" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="8" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="12" borderId="1" xfId="53" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="37" fillId="11" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="37" fillId="12" borderId="4" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="12" borderId="0" xfId="53" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="11" borderId="0" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="12" borderId="1" xfId="53" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="38" fillId="11" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="38" fillId="12" borderId="4" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="12" borderId="0" xfId="53" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="11" borderId="0" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="12" borderId="4" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="12" borderId="4" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="37" fillId="12" borderId="1" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="11" borderId="0" xfId="53" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="37" fillId="12" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="12" borderId="1" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="38" fillId="12" borderId="1" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="11" borderId="0" xfId="53" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="38" fillId="12" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="12" borderId="1" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="12" borderId="4" xfId="53" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="12" borderId="0" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="12" borderId="4" xfId="53" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="12" borderId="0" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="53"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="53" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="2" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="53"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="53" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="2" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="0" xfId="53" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="5" borderId="2" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="4" borderId="0" xfId="53" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="2" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="108">
+  <cellStyles count="214">
     <cellStyle name="20% - Accent5" xfId="1" builtinId="46"/>
     <cellStyle name="20% - Accent5 2" xfId="7" xr:uid="{41FADB5D-774C-4581-9E04-795745F45B3A}"/>
     <cellStyle name="20% - Accent5 2 2" xfId="22" xr:uid="{9D85FBE9-8CBA-4BC4-A23E-71E72F7E6CC9}"/>
     <cellStyle name="20% - Accent5 2 2 2" xfId="77" xr:uid="{056F0309-84E5-4341-AF71-2EEBE7BF74FD}"/>
+    <cellStyle name="20% - Accent5 2 2 2 2" xfId="182" xr:uid="{F15C4DC7-EC48-407F-96A3-3CC4A53A0ED7}"/>
+    <cellStyle name="20% - Accent5 2 2 3" xfId="129" xr:uid="{747D9A38-2066-47A4-B4DB-0321AD8ED675}"/>
     <cellStyle name="20% - Accent5 2 3" xfId="35" xr:uid="{64A1DEB4-76C7-4D7E-B183-769228520DF6}"/>
     <cellStyle name="20% - Accent5 2 3 2" xfId="90" xr:uid="{0D0D6279-2017-4898-BAD5-6B558FB10637}"/>
+    <cellStyle name="20% - Accent5 2 3 2 2" xfId="195" xr:uid="{A57918F3-0541-4AE7-A008-24B794DBD6BA}"/>
+    <cellStyle name="20% - Accent5 2 3 3" xfId="142" xr:uid="{84384C81-7E3B-4CED-8965-E92625ACB23F}"/>
     <cellStyle name="20% - Accent5 2 4" xfId="48" xr:uid="{B6EB5E8B-FCFF-4F4E-8AB6-E3215DFC371B}"/>
     <cellStyle name="20% - Accent5 2 4 2" xfId="103" xr:uid="{30AF541E-196B-40C1-AC50-FC8192ADC0BE}"/>
+    <cellStyle name="20% - Accent5 2 4 2 2" xfId="208" xr:uid="{E1A90527-D767-4E40-A42F-1441A5209B93}"/>
+    <cellStyle name="20% - Accent5 2 4 3" xfId="155" xr:uid="{C01430D9-A083-4562-BDE8-FA155F38893A}"/>
     <cellStyle name="20% - Accent5 2 5" xfId="63" xr:uid="{E4942102-333A-4347-87C5-3BB3880A6AB3}"/>
+    <cellStyle name="20% - Accent5 2 5 2" xfId="169" xr:uid="{2A094B50-A181-4DC4-9E77-CC329BF5AD02}"/>
+    <cellStyle name="20% - Accent5 2 6" xfId="116" xr:uid="{11144059-BF5C-47A5-906B-F54FDE629215}"/>
     <cellStyle name="20% - Accent5 3" xfId="11" xr:uid="{42C3DA6A-E515-4F68-9D9F-3335D19CEA18}"/>
     <cellStyle name="20% - Accent5 3 2" xfId="26" xr:uid="{7ABCF359-2591-4C83-A95F-469CD11EC77F}"/>
     <cellStyle name="20% - Accent5 3 2 2" xfId="81" xr:uid="{AE2A66F3-A94C-4BED-A4C4-1DA3B2F7359C}"/>
+    <cellStyle name="20% - Accent5 3 2 2 2" xfId="186" xr:uid="{FB3BCC98-10A5-4328-8D99-ADB9FF0542A4}"/>
+    <cellStyle name="20% - Accent5 3 2 3" xfId="133" xr:uid="{1B89ABCD-870A-4506-B46D-838882985AA7}"/>
     <cellStyle name="20% - Accent5 3 3" xfId="39" xr:uid="{A4C767C1-51C3-47D5-A74C-587D3519900C}"/>
     <cellStyle name="20% - Accent5 3 3 2" xfId="94" xr:uid="{9F2AEC89-E3E1-456E-AFAB-746F7754295C}"/>
+    <cellStyle name="20% - Accent5 3 3 2 2" xfId="199" xr:uid="{33F4A8EC-24DE-486C-9439-4505BDC2142F}"/>
+    <cellStyle name="20% - Accent5 3 3 3" xfId="146" xr:uid="{4A445855-314A-41F5-B200-BE580F9BF77A}"/>
     <cellStyle name="20% - Accent5 3 4" xfId="52" xr:uid="{C90B685B-F75D-460B-BDFC-7D7533C48C33}"/>
     <cellStyle name="20% - Accent5 3 4 2" xfId="107" xr:uid="{138EC8A5-98DD-41B5-8AEA-B3E4F6DDC91C}"/>
+    <cellStyle name="20% - Accent5 3 4 2 2" xfId="212" xr:uid="{96CBC248-D81C-4E6F-93B1-59086153C386}"/>
+    <cellStyle name="20% - Accent5 3 4 3" xfId="159" xr:uid="{476E5B0D-5D23-41FC-9BD9-5877E4E80DCA}"/>
     <cellStyle name="20% - Accent5 3 5" xfId="67" xr:uid="{CB8D90FD-E342-4E4E-97ED-6566F0383DA8}"/>
+    <cellStyle name="20% - Accent5 3 5 2" xfId="173" xr:uid="{2DCD6ED4-3401-42A7-ADE2-91C5ADAAD83C}"/>
+    <cellStyle name="20% - Accent5 3 6" xfId="120" xr:uid="{142A7217-93B3-45E6-B2CF-A38D4C05FEF1}"/>
     <cellStyle name="20% - Accent5 4" xfId="15" xr:uid="{DC1DD871-6B98-4E25-8BE8-6A14C839CFCF}"/>
     <cellStyle name="20% - Accent5 4 2" xfId="71" xr:uid="{8A5ADE6F-838F-4859-A40E-05FF9B5ED05F}"/>
+    <cellStyle name="20% - Accent5 4 2 2" xfId="177" xr:uid="{1925C8DE-A583-4977-881C-7AA07FA5FC9E}"/>
+    <cellStyle name="20% - Accent5 4 3" xfId="124" xr:uid="{FFB271F5-1793-486C-AE40-E19C3CBDBEB0}"/>
     <cellStyle name="20% - Accent5 5" xfId="30" xr:uid="{0FAED7C7-EA67-4CB3-AE34-15128E10EBDD}"/>
     <cellStyle name="20% - Accent5 5 2" xfId="85" xr:uid="{FD83161D-F025-47DE-932C-C09CCF236B28}"/>
+    <cellStyle name="20% - Accent5 5 2 2" xfId="190" xr:uid="{43C13AD6-900F-461F-8F95-559594527B82}"/>
+    <cellStyle name="20% - Accent5 5 3" xfId="137" xr:uid="{26763EF3-AAB4-49FD-B2E9-8091E450A013}"/>
     <cellStyle name="20% - Accent5 6" xfId="43" xr:uid="{AED42CDA-BA61-497A-9B25-6EC421F7DD74}"/>
     <cellStyle name="20% - Accent5 6 2" xfId="98" xr:uid="{D3154FDA-750D-4526-89DE-A27FA32F362A}"/>
+    <cellStyle name="20% - Accent5 6 2 2" xfId="203" xr:uid="{74FAEAC9-9C79-4665-99DB-0CC3729BEA23}"/>
+    <cellStyle name="20% - Accent5 6 3" xfId="150" xr:uid="{CF11A72E-A3DC-4FF7-A592-68CCAD865D3F}"/>
     <cellStyle name="20% - Accent5 7" xfId="56" xr:uid="{DA7F47C0-FD1B-441F-935D-8AD7CC5C6E1D}"/>
+    <cellStyle name="20% - Accent5 7 2" xfId="164" xr:uid="{C40728DF-3CDC-47FE-BEBE-ED23A7DBC6E2}"/>
     <cellStyle name="Comma 2" xfId="5" xr:uid="{ED6C98B7-B2A1-4B47-AF8A-A39872245B39}"/>
     <cellStyle name="Comma 2 2" xfId="20" xr:uid="{B7AC5FAF-634D-41F9-85B3-9CDBB33D0333}"/>
     <cellStyle name="Comma 2 2 2" xfId="75" xr:uid="{8C001DC2-FE51-45BF-B6C7-A77CFC0D7B9C}"/>
+    <cellStyle name="Comma 2 2 2 2" xfId="180" xr:uid="{2FD74F75-ACE2-478F-98C1-12834DF9A133}"/>
+    <cellStyle name="Comma 2 2 3" xfId="127" xr:uid="{A447AB2E-39B0-4840-9ECB-835C36444D50}"/>
     <cellStyle name="Comma 2 3" xfId="33" xr:uid="{9A5060E8-4621-4D2E-8FA3-F2C0D822E9A4}"/>
     <cellStyle name="Comma 2 3 2" xfId="88" xr:uid="{E1923561-86EC-460D-BC19-5C07AEBF1D47}"/>
+    <cellStyle name="Comma 2 3 2 2" xfId="193" xr:uid="{01AFDCE0-A29E-47CE-B8CC-2ACAD8C38FC6}"/>
+    <cellStyle name="Comma 2 3 3" xfId="140" xr:uid="{02FF3435-B693-406B-B6FE-F28D0C11BBD8}"/>
     <cellStyle name="Comma 2 4" xfId="46" xr:uid="{640D3F39-7ADA-41F7-A824-1BFD8996D38B}"/>
     <cellStyle name="Comma 2 4 2" xfId="101" xr:uid="{E2D14C34-0F3F-44F3-A287-3464F22C7687}"/>
+    <cellStyle name="Comma 2 4 2 2" xfId="206" xr:uid="{F47C579F-3E2C-4535-A8D9-200B26DBC5DA}"/>
+    <cellStyle name="Comma 2 4 3" xfId="153" xr:uid="{1F0E6A60-17A2-4114-803E-D183E9058A58}"/>
     <cellStyle name="Comma 2 5" xfId="61" xr:uid="{243DF1CB-25DA-4BF4-8322-1D82C49CD531}"/>
+    <cellStyle name="Comma 2 5 2" xfId="167" xr:uid="{94630E3C-0678-42AA-8F03-1265C844C8FB}"/>
+    <cellStyle name="Comma 2 6" xfId="114" xr:uid="{27D0662D-D964-4C3E-948B-5A67D2F9F373}"/>
     <cellStyle name="Comma 3" xfId="9" xr:uid="{9BBE06F6-DF43-4386-A7EA-84770CBB1110}"/>
     <cellStyle name="Comma 3 2" xfId="24" xr:uid="{AB59C64B-085D-4C79-B275-6709641D5BB7}"/>
     <cellStyle name="Comma 3 2 2" xfId="79" xr:uid="{CD323AA4-22F9-4E99-9009-6D23DBE24110}"/>
+    <cellStyle name="Comma 3 2 2 2" xfId="184" xr:uid="{6BF0A02D-702E-459D-B813-A3CA51E0E1F9}"/>
+    <cellStyle name="Comma 3 2 3" xfId="131" xr:uid="{F3063D94-C775-4408-BEFE-84D8981CED7C}"/>
     <cellStyle name="Comma 3 3" xfId="37" xr:uid="{96E677B2-1E39-47F3-B561-DD4F13597381}"/>
     <cellStyle name="Comma 3 3 2" xfId="92" xr:uid="{0339C6BC-2315-4A35-972E-9C0115061548}"/>
+    <cellStyle name="Comma 3 3 2 2" xfId="197" xr:uid="{D347A85F-2F28-4CD9-B728-B92448649D10}"/>
+    <cellStyle name="Comma 3 3 3" xfId="144" xr:uid="{5E8F8B59-2437-4316-8FB6-F54DA82463FD}"/>
     <cellStyle name="Comma 3 4" xfId="50" xr:uid="{B86C2900-CA03-40CB-895D-AA126B40D038}"/>
     <cellStyle name="Comma 3 4 2" xfId="105" xr:uid="{2F1C02E0-F632-41D5-921C-A25FF8C789F7}"/>
+    <cellStyle name="Comma 3 4 2 2" xfId="210" xr:uid="{8EC804B6-67BA-44DE-9646-4BD589C60F7E}"/>
+    <cellStyle name="Comma 3 4 3" xfId="157" xr:uid="{514AEA27-53F6-4C07-9438-4707B85AC645}"/>
     <cellStyle name="Comma 3 5" xfId="65" xr:uid="{7CB782F8-2A35-46DD-9621-962ECDE1F2C7}"/>
+    <cellStyle name="Comma 3 5 2" xfId="171" xr:uid="{114D7B81-2D05-4116-8FEF-05B6544CFB4E}"/>
+    <cellStyle name="Comma 3 6" xfId="118" xr:uid="{59AB25DC-52EB-443B-A345-EEB07344637F}"/>
     <cellStyle name="Comma 4" xfId="13" xr:uid="{F10BAA2F-325D-48FE-B4DE-588412CF4783}"/>
     <cellStyle name="Comma 4 2" xfId="69" xr:uid="{B1AE5C0E-22F5-4478-9785-B9413DBF2438}"/>
+    <cellStyle name="Comma 4 2 2" xfId="175" xr:uid="{C01683A5-C27C-49A6-B395-A40C00ED172A}"/>
+    <cellStyle name="Comma 4 3" xfId="122" xr:uid="{F31725B9-E626-491E-AAAF-23C26A0AB515}"/>
     <cellStyle name="Comma 5" xfId="28" xr:uid="{A96DE9F5-7FB1-4FAB-B94D-B2EF920E5378}"/>
     <cellStyle name="Comma 5 2" xfId="83" xr:uid="{BBE1F8E9-1232-44B8-BCCF-1C0927C0783C}"/>
+    <cellStyle name="Comma 5 2 2" xfId="188" xr:uid="{ABB0A5E4-96DC-486B-8B31-6D9601EFDE31}"/>
+    <cellStyle name="Comma 5 3" xfId="135" xr:uid="{1F3E63D5-428E-400A-B0C1-16DB1C638C5B}"/>
     <cellStyle name="Comma 6" xfId="41" xr:uid="{F6AC73A4-766F-41AF-8546-1BD92C1A5DC3}"/>
     <cellStyle name="Comma 6 2" xfId="96" xr:uid="{77D1E22B-1913-4AD1-A0DD-3B9445C9B943}"/>
+    <cellStyle name="Comma 6 2 2" xfId="201" xr:uid="{C697C2DF-C17F-4553-B24A-957F8430F01E}"/>
+    <cellStyle name="Comma 6 3" xfId="148" xr:uid="{AEC0336C-48D4-428B-AA3B-C51D96186F10}"/>
     <cellStyle name="Comma 7" xfId="54" xr:uid="{94DEC19E-A6A7-4788-812E-6C5318BF22E8}"/>
+    <cellStyle name="Comma 7 2" xfId="162" xr:uid="{F18459FC-7540-4004-ADA7-32E985107525}"/>
+    <cellStyle name="Comma 8" xfId="110" xr:uid="{CE5F3CAC-02ED-403F-8BDB-50BCB276743E}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="53" xr:uid="{8BBE64AA-0071-44B5-A766-DD878DA19F08}"/>
+    <cellStyle name="Normal 10 2" xfId="161" xr:uid="{53431DF4-F434-4E58-8B64-6ACB4079A7DF}"/>
+    <cellStyle name="Normal 11" xfId="160" xr:uid="{06F42D7C-516D-4DB0-A9FE-B6423B71AAD8}"/>
+    <cellStyle name="Normal 12" xfId="109" xr:uid="{A0DDEDD4-62D6-4BB4-9F38-7DB5B8015081}"/>
+    <cellStyle name="Normal 13" xfId="108" xr:uid="{FA5BC1D4-F714-4C97-B6A6-8886159FB69C}"/>
+    <cellStyle name="Normal 13 2" xfId="213" xr:uid="{3F198362-F8B7-4613-B058-8756CBD31E94}"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{4F4ED162-C45F-4637-99B9-0DC288E0E26C}"/>
     <cellStyle name="Normal 2 2" xfId="18" xr:uid="{73520720-7CC8-4636-BEA4-4BA7AD8E3294}"/>
     <cellStyle name="Normal 2 2 2" xfId="73" xr:uid="{2CD71C79-1AA4-45A0-9788-9D2D6FAD34B2}"/>
+    <cellStyle name="Normal 2 2 2 2" xfId="178" xr:uid="{7E7CE0F8-BE26-4F38-923F-700901A1DA6B}"/>
+    <cellStyle name="Normal 2 2 3" xfId="125" xr:uid="{2AFC3B25-5274-4BE5-AF40-AFB32CA2152A}"/>
     <cellStyle name="Normal 2 3" xfId="31" xr:uid="{3DE8F047-C232-4A35-B429-F0537449F260}"/>
     <cellStyle name="Normal 2 3 2" xfId="86" xr:uid="{11AAA4BB-E8A9-4185-ADFA-83841C071238}"/>
+    <cellStyle name="Normal 2 3 2 2" xfId="191" xr:uid="{555E5143-5542-4F10-93AC-675A424DF628}"/>
+    <cellStyle name="Normal 2 3 3" xfId="138" xr:uid="{CD3C54C7-74E6-4120-BC63-E077FD94C7F1}"/>
     <cellStyle name="Normal 2 4" xfId="44" xr:uid="{4FF9CFE9-7E21-4A6B-A29A-1180095F3394}"/>
     <cellStyle name="Normal 2 4 2" xfId="99" xr:uid="{3320B5F5-33BD-4D66-8320-92478374F742}"/>
+    <cellStyle name="Normal 2 4 2 2" xfId="204" xr:uid="{EFF28F27-780E-499A-944A-DD50FE742FB2}"/>
+    <cellStyle name="Normal 2 4 3" xfId="151" xr:uid="{14701181-5D67-48F7-89EE-2E5A66EAD732}"/>
     <cellStyle name="Normal 2 5" xfId="59" xr:uid="{82B1CADE-454F-41BD-B69C-1C727AEACFA4}"/>
+    <cellStyle name="Normal 2 5 2" xfId="165" xr:uid="{AD3B439E-CA24-47F2-9D4B-3B06FC8B5FC2}"/>
+    <cellStyle name="Normal 2 6" xfId="112" xr:uid="{BCA5A7C5-CA87-43C5-B301-853508413108}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{6F56F0E9-E05C-4C30-B878-F9B9EA162652}"/>
     <cellStyle name="Normal 3 2" xfId="19" xr:uid="{A32771C3-61B9-4017-BCB7-A8447F558936}"/>
     <cellStyle name="Normal 3 2 2" xfId="74" xr:uid="{EB3EB93F-B77D-4BA5-9B37-4507D01FE212}"/>
+    <cellStyle name="Normal 3 2 2 2" xfId="179" xr:uid="{693168B0-96BE-47F2-B453-4306E6AE7CE8}"/>
+    <cellStyle name="Normal 3 2 3" xfId="126" xr:uid="{61161275-A351-4B23-8415-F39367DD8024}"/>
     <cellStyle name="Normal 3 3" xfId="32" xr:uid="{6D6D7D4C-E015-466A-A2A9-35851197F9B9}"/>
     <cellStyle name="Normal 3 3 2" xfId="87" xr:uid="{A09B1EDC-BC53-4A84-8A09-CD2B3E72AB92}"/>
+    <cellStyle name="Normal 3 3 2 2" xfId="192" xr:uid="{09930C38-6C2B-4EF3-9187-539467ADB60B}"/>
+    <cellStyle name="Normal 3 3 3" xfId="139" xr:uid="{D3BD1A57-CC9D-4CDF-A3B5-01F1AF1FC06F}"/>
     <cellStyle name="Normal 3 4" xfId="45" xr:uid="{3F2C4675-A6B6-4303-ADF3-7F5FDBCC1201}"/>
     <cellStyle name="Normal 3 4 2" xfId="100" xr:uid="{52A0E527-D628-412E-933C-8E8D41704332}"/>
+    <cellStyle name="Normal 3 4 2 2" xfId="205" xr:uid="{9F36FAE0-1145-4DB4-ADC6-CB3DE2BEEE9F}"/>
+    <cellStyle name="Normal 3 4 3" xfId="152" xr:uid="{795989F9-BCAF-47BD-8728-F8406BAF9D65}"/>
     <cellStyle name="Normal 3 5" xfId="60" xr:uid="{3B4793EE-2556-4444-B5B4-4962FF9A0B3A}"/>
+    <cellStyle name="Normal 3 5 2" xfId="166" xr:uid="{9A7B49F9-AB24-48A9-BF78-AC2ED43283A3}"/>
+    <cellStyle name="Normal 3 6" xfId="113" xr:uid="{1B5B4019-2C60-4C1C-9403-E6C70EA177AB}"/>
     <cellStyle name="Normal 4" xfId="8" xr:uid="{E0019DBD-0F4A-4352-B357-025C5C0BFAEC}"/>
     <cellStyle name="Normal 4 2" xfId="23" xr:uid="{10393A82-218B-43FD-AA73-2D1C9788B975}"/>
     <cellStyle name="Normal 4 2 2" xfId="78" xr:uid="{518A0805-EFF6-4BCF-A4BB-CAAB7F8F705D}"/>
+    <cellStyle name="Normal 4 2 2 2" xfId="183" xr:uid="{D62E6486-14CF-4FFD-9272-A8B3325C08A5}"/>
+    <cellStyle name="Normal 4 2 3" xfId="130" xr:uid="{2C009DF5-CBF1-4F94-90D7-738B2088C271}"/>
     <cellStyle name="Normal 4 3" xfId="36" xr:uid="{62A12A76-EC25-4B9B-9DE7-60E39637AA4D}"/>
     <cellStyle name="Normal 4 3 2" xfId="91" xr:uid="{EC7D6496-983A-4947-B588-F58C77B67828}"/>
+    <cellStyle name="Normal 4 3 2 2" xfId="196" xr:uid="{8A9F63B9-F301-4EFC-A27E-C4C6DBAD14B2}"/>
+    <cellStyle name="Normal 4 3 3" xfId="143" xr:uid="{A209E494-1E57-4511-9967-C6BB4CB69798}"/>
     <cellStyle name="Normal 4 4" xfId="49" xr:uid="{0D81F105-5652-4284-861E-275768C81364}"/>
     <cellStyle name="Normal 4 4 2" xfId="104" xr:uid="{2ED90C63-2832-484C-8BE6-4FE320068DCF}"/>
+    <cellStyle name="Normal 4 4 2 2" xfId="209" xr:uid="{DBBD8277-5ED3-406B-B252-BBC562C99C8F}"/>
+    <cellStyle name="Normal 4 4 3" xfId="156" xr:uid="{77BBDA96-C1B4-488B-A294-0EDF35D9022C}"/>
     <cellStyle name="Normal 4 5" xfId="64" xr:uid="{C01B067D-10D4-4312-A991-9BB0541632E1}"/>
+    <cellStyle name="Normal 4 5 2" xfId="170" xr:uid="{216A4D32-F34F-4D2E-9FAA-2ED46145C0B4}"/>
+    <cellStyle name="Normal 4 6" xfId="117" xr:uid="{48E6E147-FC1F-4C0C-8FE7-982FD956AD07}"/>
     <cellStyle name="Normal 5" xfId="16" xr:uid="{49545144-F3A9-4825-A6BA-5936F162C050}"/>
     <cellStyle name="Normal 5 2" xfId="72" xr:uid="{ADCDC5E4-A063-457A-A471-FEB0D7FB14D2}"/>
     <cellStyle name="Normal 6" xfId="12" xr:uid="{4EF6E554-0085-465F-A330-E88543107D27}"/>
     <cellStyle name="Normal 6 2" xfId="68" xr:uid="{16F122DE-5D56-4A1B-BB1C-A9AD62F8B2A1}"/>
+    <cellStyle name="Normal 6 2 2" xfId="174" xr:uid="{5CBC1DAA-AC29-4F13-9168-80B81077ABF7}"/>
+    <cellStyle name="Normal 6 3" xfId="121" xr:uid="{D2A38596-2B9B-4FFC-9085-3A9557F73DB5}"/>
     <cellStyle name="Normal 7" xfId="27" xr:uid="{2534D22A-6169-4D9A-B012-B7294C0AC758}"/>
     <cellStyle name="Normal 7 2" xfId="82" xr:uid="{A89A0637-FCF4-4BBE-973F-383CEA45A07D}"/>
+    <cellStyle name="Normal 7 2 2" xfId="187" xr:uid="{54FCB699-B6CD-4B8E-B5C7-29F0EA489663}"/>
+    <cellStyle name="Normal 7 3" xfId="134" xr:uid="{C1422B8C-C674-46F0-AB09-B49D4057DCEA}"/>
     <cellStyle name="Normal 8" xfId="40" xr:uid="{19F067A3-D80D-48FD-BF06-BF292EC8BB24}"/>
     <cellStyle name="Normal 8 2" xfId="95" xr:uid="{7AC36C7D-8CC4-4325-8C2B-FA3C713B7CF5}"/>
+    <cellStyle name="Normal 8 2 2" xfId="200" xr:uid="{6C397B7D-6E90-4109-A1F7-15EA72BFFF46}"/>
+    <cellStyle name="Normal 8 3" xfId="147" xr:uid="{9D1787CE-1718-4788-B651-58825DA7D955}"/>
     <cellStyle name="Normal 9" xfId="57" xr:uid="{CC04280B-7E40-41C0-B008-E89A699DBC6E}"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Percent 10" xfId="111" xr:uid="{1F4F8886-BC30-46CB-A926-4376A9109BBF}"/>
     <cellStyle name="Percent 2" xfId="6" xr:uid="{BC0C5A78-644A-4E8A-8133-E61F2E94C271}"/>
     <cellStyle name="Percent 2 2" xfId="21" xr:uid="{ABEFFD90-1C5B-44F4-94F2-8F5C545B6CE3}"/>
     <cellStyle name="Percent 2 2 2" xfId="76" xr:uid="{3BD6292D-5384-4692-B5F6-884298F64563}"/>
+    <cellStyle name="Percent 2 2 2 2" xfId="181" xr:uid="{46C8F6F1-24D5-4168-8158-FC0E4886AC1D}"/>
+    <cellStyle name="Percent 2 2 3" xfId="128" xr:uid="{36EE822D-4B3E-44B1-B029-B8B78867EF7A}"/>
     <cellStyle name="Percent 2 3" xfId="34" xr:uid="{F1235FEE-D3ED-46E3-8284-249567537760}"/>
     <cellStyle name="Percent 2 3 2" xfId="89" xr:uid="{243A6ED9-AAFA-49A8-9C9D-1F9201E74EE5}"/>
+    <cellStyle name="Percent 2 3 2 2" xfId="194" xr:uid="{43806F43-EF60-4BA2-92C0-5EFD1054D0EB}"/>
+    <cellStyle name="Percent 2 3 3" xfId="141" xr:uid="{671C13B9-D85F-49B6-8210-22AFF3720429}"/>
     <cellStyle name="Percent 2 4" xfId="47" xr:uid="{9B5DB1B9-289D-4910-A43A-3BB8D718BF50}"/>
     <cellStyle name="Percent 2 4 2" xfId="102" xr:uid="{72EADBC2-7F91-4039-B221-1AF9C08D12D9}"/>
+    <cellStyle name="Percent 2 4 2 2" xfId="207" xr:uid="{5AFE4152-FEC5-49A0-9D8D-D5FDA1723B5A}"/>
+    <cellStyle name="Percent 2 4 3" xfId="154" xr:uid="{A4294857-D78B-4B2B-8455-A9A7CCA9968E}"/>
     <cellStyle name="Percent 2 5" xfId="62" xr:uid="{99781A41-93CF-4EB0-92D0-C5CD68D53132}"/>
+    <cellStyle name="Percent 2 5 2" xfId="168" xr:uid="{433B7183-9537-4B65-A460-0F8F04644F1F}"/>
+    <cellStyle name="Percent 2 6" xfId="115" xr:uid="{AB1C876A-61E7-4015-A43C-086187C228D5}"/>
     <cellStyle name="Percent 3" xfId="10" xr:uid="{5A577D97-9D8D-44CD-94BE-F7C4D5E216D4}"/>
     <cellStyle name="Percent 3 2" xfId="25" xr:uid="{AA877386-D0A2-4CA8-9066-CA902896BC86}"/>
     <cellStyle name="Percent 3 2 2" xfId="80" xr:uid="{A88F4B8E-3D7E-46C4-935F-75A2D1DC2F86}"/>
+    <cellStyle name="Percent 3 2 2 2" xfId="185" xr:uid="{AA51F800-E197-4EBD-A00E-5ED6D281A99C}"/>
+    <cellStyle name="Percent 3 2 3" xfId="132" xr:uid="{AD596E79-6618-4E8C-9AAE-C8188B1A7654}"/>
     <cellStyle name="Percent 3 3" xfId="38" xr:uid="{2C62A5E3-4F5C-4053-B9EE-104D29570544}"/>
     <cellStyle name="Percent 3 3 2" xfId="93" xr:uid="{84DDFECE-69E2-4B0E-A09E-659E48A24F42}"/>
+    <cellStyle name="Percent 3 3 2 2" xfId="198" xr:uid="{D5138662-9B50-4909-B103-A9540759A334}"/>
+    <cellStyle name="Percent 3 3 3" xfId="145" xr:uid="{DB58C7EC-334E-4AE6-B68E-D68247DB256A}"/>
     <cellStyle name="Percent 3 4" xfId="51" xr:uid="{71214003-4755-4936-B69C-71301425DFDB}"/>
     <cellStyle name="Percent 3 4 2" xfId="106" xr:uid="{C8250550-A077-468C-AEF8-166BFF71412B}"/>
+    <cellStyle name="Percent 3 4 2 2" xfId="211" xr:uid="{6BCEDAED-9BA6-48C4-98D1-B239A2FBFB06}"/>
+    <cellStyle name="Percent 3 4 3" xfId="158" xr:uid="{E9A8A10A-09C4-40C8-8279-A039F46E57ED}"/>
     <cellStyle name="Percent 3 5" xfId="66" xr:uid="{90D550B4-A467-4B1F-8791-783C947825CE}"/>
+    <cellStyle name="Percent 3 5 2" xfId="172" xr:uid="{50881C98-C99E-4650-827C-766929596D85}"/>
+    <cellStyle name="Percent 3 6" xfId="119" xr:uid="{52DB9A23-2753-48D6-90A2-C68B5942AD40}"/>
     <cellStyle name="Percent 4" xfId="17" xr:uid="{766E512C-159B-4546-AE75-4E591D8E346F}"/>
     <cellStyle name="Percent 5" xfId="14" xr:uid="{761C96E9-6829-47E8-ABEF-BAFE0B7B7D1A}"/>
     <cellStyle name="Percent 5 2" xfId="70" xr:uid="{3753DDE5-24BA-4D95-9E8F-1428A4C09B68}"/>
+    <cellStyle name="Percent 5 2 2" xfId="176" xr:uid="{C789F3EB-F70E-407F-B666-32BF7BA046C9}"/>
+    <cellStyle name="Percent 5 3" xfId="123" xr:uid="{30D8A2A0-D19C-4CB4-A9B2-F1A31449CDBF}"/>
     <cellStyle name="Percent 6" xfId="29" xr:uid="{3C9E2FB6-4013-4108-851E-44B42960E338}"/>
     <cellStyle name="Percent 6 2" xfId="84" xr:uid="{A9529AA1-C733-45A5-9A59-8E9A9D926271}"/>
+    <cellStyle name="Percent 6 2 2" xfId="189" xr:uid="{DCA23980-98AC-43CA-941E-9708457EFE2C}"/>
+    <cellStyle name="Percent 6 3" xfId="136" xr:uid="{EABCDA63-DFA2-47E3-B194-D18A8290ED26}"/>
     <cellStyle name="Percent 7" xfId="42" xr:uid="{E615D24B-233E-4FC3-8466-3E474BB7156C}"/>
     <cellStyle name="Percent 7 2" xfId="97" xr:uid="{C8975516-84DD-418A-B968-A1AE0DCED118}"/>
+    <cellStyle name="Percent 7 2 2" xfId="202" xr:uid="{B240505D-1F90-4AB5-9ECC-FDF506CBA6F0}"/>
+    <cellStyle name="Percent 7 3" xfId="149" xr:uid="{C16F36D8-1935-485F-A488-481927ED7425}"/>
     <cellStyle name="Percent 8" xfId="58" xr:uid="{DAF5A91A-7863-44B8-B357-3AAC899BD8B2}"/>
     <cellStyle name="Percent 9" xfId="55" xr:uid="{05B3DA8B-8D4B-4546-93F0-A0F74AD24A02}"/>
+    <cellStyle name="Percent 9 2" xfId="163" xr:uid="{DE2C4031-335C-4ED2-9DB3-04920DD9A697}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -4053,7 +4278,7 @@
   <mergeCells count="1">
     <mergeCell ref="B38:C38"/>
   </mergeCells>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4063,8 +4288,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B3:AF305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="K208" sqref="K208"/>
+    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U153" sqref="U153:U158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -9142,14 +9367,14 @@
       <c r="E154" s="49">
         <v>2019</v>
       </c>
-      <c r="F154" s="50">
-        <v>0.32300000000000001</v>
-      </c>
-      <c r="G154" s="50">
-        <v>0.36099999999999999</v>
-      </c>
-      <c r="H154" s="50">
-        <v>0.39100000000000001</v>
+      <c r="F154" s="48">
+        <v>0.51000446210607897</v>
+      </c>
+      <c r="G154" s="48">
+        <v>0.57000498705973535</v>
+      </c>
+      <c r="H154" s="48">
+        <v>0.61737382254946405</v>
       </c>
       <c r="I154" s="50">
         <v>23.135000000000002</v>
@@ -9176,8 +9401,8 @@
       <c r="P154" s="50">
         <v>20.794499999999999</v>
       </c>
-      <c r="Q154" s="50">
-        <v>4.5493804447819669E-2</v>
+      <c r="Q154" s="1">
+        <v>3.6395043558255735E-2</v>
       </c>
       <c r="R154" s="49">
         <v>20</v>
@@ -9202,14 +9427,14 @@
       <c r="E155" s="49">
         <v>2019</v>
       </c>
-      <c r="F155" s="50">
-        <v>0.40300000000000002</v>
-      </c>
-      <c r="G155" s="50">
-        <v>0.45500000000000002</v>
-      </c>
-      <c r="H155" s="50">
-        <v>0.48699999999999999</v>
+      <c r="F155" s="48">
+        <v>0.63632135674535562</v>
+      </c>
+      <c r="G155" s="48">
+        <v>0.71842733826088534</v>
+      </c>
+      <c r="H155" s="48">
+        <v>0.76895409611659593</v>
       </c>
       <c r="I155" s="50">
         <v>26.946999999999999</v>
@@ -9236,9 +9461,8 @@
       <c r="P155" s="50">
         <v>20.794499999999999</v>
       </c>
-      <c r="Q155" s="50">
-        <f>Q154</f>
-        <v>4.5493804447819669E-2</v>
+      <c r="Q155" s="1">
+        <v>3.6395043558255735E-2</v>
       </c>
       <c r="R155" s="49">
         <v>20</v>
@@ -9263,14 +9487,14 @@
       <c r="E156" s="49">
         <v>2019</v>
       </c>
-      <c r="F156" s="50">
-        <v>0.56699999999999995</v>
-      </c>
-      <c r="G156" s="50">
-        <v>0.66100000000000003</v>
-      </c>
-      <c r="H156" s="50">
-        <v>0.73099999999999998</v>
+      <c r="F156" s="48">
+        <v>0.89527099075587235</v>
+      </c>
+      <c r="G156" s="48">
+        <v>1.0436933419570225</v>
+      </c>
+      <c r="H156" s="48">
+        <v>1.1542206247663893</v>
       </c>
       <c r="I156" s="50">
         <v>33.524000000000001</v>
@@ -9297,9 +9521,8 @@
       <c r="P156" s="50">
         <v>20.794499999999999</v>
       </c>
-      <c r="Q156" s="50">
-        <f t="shared" ref="Q156:Q160" si="8">Q155</f>
-        <v>4.5493804447819669E-2</v>
+      <c r="Q156" s="1">
+        <v>3.6395043558255735E-2</v>
       </c>
       <c r="R156" s="49">
         <v>20</v>
@@ -9307,6 +9530,7 @@
       <c r="S156" s="49">
         <v>1E-3</v>
       </c>
+      <c r="U156" s="1"/>
     </row>
     <row r="157" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B157" s="1" t="str">
@@ -9324,14 +9548,14 @@
       <c r="E157" s="49">
         <v>2019</v>
       </c>
-      <c r="F157" s="50">
-        <v>0.22800000000000001</v>
-      </c>
-      <c r="G157" s="50">
-        <v>0.23699999999999999</v>
-      </c>
-      <c r="H157" s="50">
-        <v>0.27</v>
+      <c r="F157" s="48">
+        <v>0.36000314972193814</v>
+      </c>
+      <c r="G157" s="48">
+        <v>0.37421380036885671</v>
+      </c>
+      <c r="H157" s="48">
+        <v>0.42631951940755836</v>
       </c>
       <c r="I157" s="50">
         <v>28.097999999999999</v>
@@ -9358,9 +9582,8 @@
       <c r="P157" s="50">
         <v>20.794499999999999</v>
       </c>
-      <c r="Q157" s="50">
-        <f t="shared" si="8"/>
-        <v>4.5493804447819669E-2</v>
+      <c r="Q157" s="1">
+        <v>3.6395043558255735E-2</v>
       </c>
       <c r="R157" s="49">
         <v>20</v>
@@ -9385,14 +9608,14 @@
       <c r="E158" s="49">
         <v>2019</v>
       </c>
-      <c r="F158" s="50">
-        <v>0.46300000000000002</v>
-      </c>
-      <c r="G158" s="50">
-        <v>0.496</v>
-      </c>
-      <c r="H158" s="50">
-        <v>0.56699999999999995</v>
+      <c r="F158" s="48">
+        <v>0.73105902772481302</v>
+      </c>
+      <c r="G158" s="48">
+        <v>0.78316474676351455</v>
+      </c>
+      <c r="H158" s="48">
+        <v>0.89527099075587235</v>
       </c>
       <c r="I158" s="50">
         <v>36.548000000000002</v>
@@ -9419,9 +9642,8 @@
       <c r="P158" s="50">
         <v>20.794499999999999</v>
       </c>
-      <c r="Q158" s="50">
-        <f t="shared" si="8"/>
-        <v>4.5493804447819669E-2</v>
+      <c r="Q158" s="1">
+        <v>3.6395043558255735E-2</v>
       </c>
       <c r="R158" s="49">
         <v>20</v>
@@ -9446,14 +9668,14 @@
       <c r="E159" s="49">
         <v>2019</v>
       </c>
-      <c r="F159" s="50">
-        <v>0.53400000000000003</v>
-      </c>
-      <c r="G159" s="50">
-        <v>0.60399999999999998</v>
-      </c>
-      <c r="H159" s="50">
-        <v>0.64600000000000002</v>
+      <c r="F159" s="48">
+        <v>0.84316527171717093</v>
+      </c>
+      <c r="G159" s="48">
+        <v>0.95369255452653778</v>
+      </c>
+      <c r="H159" s="48">
+        <v>1.0200089242121579</v>
       </c>
       <c r="I159" s="50">
         <v>56.146000000000001</v>
@@ -9480,9 +9702,8 @@
       <c r="P159" s="50">
         <v>20.794499999999999</v>
       </c>
-      <c r="Q159" s="50">
-        <f t="shared" si="8"/>
-        <v>4.5493804447819669E-2</v>
+      <c r="Q159" s="1">
+        <v>3.6395043558255735E-2</v>
       </c>
       <c r="R159" s="49">
         <v>20</v>
@@ -9508,14 +9729,14 @@
       <c r="E160" s="49">
         <v>2019</v>
       </c>
-      <c r="F160" s="50">
-        <v>0.92600000000000005</v>
-      </c>
-      <c r="G160" s="50">
-        <v>1.111</v>
-      </c>
-      <c r="H160" s="50">
-        <v>1.2629999999999999</v>
+      <c r="F160" s="48">
+        <v>1.462118055449626</v>
+      </c>
+      <c r="G160" s="48">
+        <v>1.7542258743029528</v>
+      </c>
+      <c r="H160" s="48">
+        <v>1.9942279741175781</v>
       </c>
       <c r="I160" s="50">
         <v>32.17</v>
@@ -9542,9 +9763,8 @@
       <c r="P160" s="50">
         <v>20.794499999999999</v>
       </c>
-      <c r="Q160" s="50">
-        <f t="shared" si="8"/>
-        <v>4.5493804447819669E-2</v>
+      <c r="Q160" s="1">
+        <v>3.6395043558255735E-2</v>
       </c>
       <c r="R160" s="49">
         <v>20</v>
@@ -9580,7 +9800,7 @@
     </row>
     <row r="162" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B162" s="1" t="str">
-        <f t="shared" ref="B162:B168" si="9">D68</f>
+        <f t="shared" ref="B162:B168" si="8">D68</f>
         <v>T-MGT-ICE_DST71</v>
       </c>
       <c r="C162" s="1" t="str">
@@ -9592,47 +9812,44 @@
         <v>TRAF</v>
       </c>
       <c r="E162" s="1">
-        <f t="shared" ref="E162:J162" si="10">E170</f>
+        <f t="shared" ref="E162:J162" si="9">E170</f>
         <v>2019</v>
       </c>
-      <c r="F162" s="1">
-        <f t="shared" si="10"/>
-        <v>0.121</v>
-      </c>
-      <c r="G162" s="1">
-        <f t="shared" si="10"/>
-        <v>0.13200000000000001</v>
-      </c>
-      <c r="H162" s="1">
-        <f t="shared" si="10"/>
-        <v>0.157</v>
+      <c r="F162" s="48">
+        <v>2.2955699033471548E-2</v>
+      </c>
+      <c r="G162" s="48">
+        <v>2.5042580763787146E-2</v>
+      </c>
+      <c r="H162" s="48">
+        <v>2.9785493787231682E-2</v>
       </c>
       <c r="I162" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>95.69</v>
       </c>
       <c r="J162" s="1">
-        <f t="shared" si="10"/>
+        <f t="shared" si="9"/>
         <v>100.95</v>
       </c>
       <c r="K162" s="48">
-        <f t="shared" ref="K162:K168" si="11">J162-((J162-L162)/4)</f>
+        <f t="shared" ref="K162:K168" si="10">J162-((J162-L162)/4)</f>
         <v>100.95</v>
       </c>
       <c r="L162" s="1">
-        <f t="shared" ref="L162:O168" si="12">L170</f>
+        <f t="shared" ref="L162:O168" si="11">L170</f>
         <v>100.95</v>
       </c>
       <c r="M162" s="48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>2.1157042474212369</v>
       </c>
       <c r="N162" s="48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>2.1689507539373367</v>
       </c>
       <c r="O162" s="48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>2.1689507539373367</v>
       </c>
       <c r="P162" s="48">
@@ -9645,13 +9862,13 @@
         <v>20</v>
       </c>
       <c r="S162" s="1">
-        <f t="shared" ref="S162:S168" si="13">S170</f>
+        <f t="shared" ref="S162:S168" si="12">S170</f>
         <v>1E-3</v>
       </c>
     </row>
     <row r="163" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B163" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>T-MGT-HEV_DST71</v>
       </c>
       <c r="C163" s="1" t="str">
@@ -9663,27 +9880,24 @@
         <v>TRAF</v>
       </c>
       <c r="E163" s="1">
-        <f t="shared" ref="C163:J168" si="14">E171</f>
+        <f t="shared" ref="C163:J168" si="13">E171</f>
         <v>2019</v>
       </c>
-      <c r="F163" s="1">
-        <f t="shared" si="14"/>
-        <v>0.17299999999999999</v>
-      </c>
-      <c r="G163" s="1">
-        <f t="shared" si="14"/>
-        <v>0.189</v>
-      </c>
-      <c r="H163" s="1">
-        <f t="shared" si="14"/>
-        <v>0.224</v>
+      <c r="F163" s="48">
+        <v>3.2820958122236184E-2</v>
+      </c>
+      <c r="G163" s="48">
+        <v>3.5856422457240689E-2</v>
+      </c>
+      <c r="H163" s="48">
+        <v>4.2496500690063034E-2</v>
       </c>
       <c r="I163" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>124.73</v>
       </c>
       <c r="J163" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>125.12</v>
       </c>
       <c r="K163" s="48">
@@ -9691,19 +9905,19 @@
         <v>123.88250000000001</v>
       </c>
       <c r="L163" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>120.17</v>
       </c>
       <c r="M163" s="48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>3.5721072259038325</v>
       </c>
       <c r="N163" s="48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>3.0618061936318557</v>
       </c>
       <c r="O163" s="48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>2.3858458293310703</v>
       </c>
       <c r="P163" s="48">
@@ -9717,85 +9931,82 @@
         <v>20</v>
       </c>
       <c r="S163" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1E-3</v>
       </c>
     </row>
     <row r="164" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B164" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>T-MGT-FCV_HYD71</v>
       </c>
       <c r="C164" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>TRAHYD</v>
       </c>
       <c r="D164" s="1" t="str">
-        <f t="shared" ref="D164:D168" si="15">D163</f>
+        <f t="shared" ref="D164:D168" si="14">D163</f>
         <v>TRAF</v>
       </c>
       <c r="E164" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>2019</v>
       </c>
-      <c r="F164" s="1">
-        <f t="shared" si="14"/>
-        <v>0.20100000000000001</v>
-      </c>
-      <c r="G164" s="1">
-        <f t="shared" si="14"/>
-        <v>0.22</v>
-      </c>
-      <c r="H164" s="1">
-        <f t="shared" si="14"/>
-        <v>0.26200000000000001</v>
+      <c r="F164" s="48">
+        <v>3.8133020708494066E-2</v>
+      </c>
+      <c r="G164" s="48">
+        <v>4.1737634606311913E-2</v>
+      </c>
+      <c r="H164" s="48">
+        <v>4.9705728485698729E-2</v>
       </c>
       <c r="I164" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>345.67</v>
       </c>
       <c r="J164" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>222.22</v>
       </c>
       <c r="K164" s="48">
+        <f t="shared" si="10"/>
+        <v>195.70750000000001</v>
+      </c>
+      <c r="L164" s="1">
         <f t="shared" si="11"/>
-        <v>195.70750000000001</v>
-      </c>
-      <c r="L164" s="1">
-        <f t="shared" si="12"/>
         <v>116.17</v>
       </c>
       <c r="M164" s="48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>3.5721072259038325</v>
       </c>
       <c r="N164" s="48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>3.0618061936318557</v>
       </c>
       <c r="O164" s="48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>2.3858458293310703</v>
       </c>
       <c r="P164" s="48">
         <v>29.397500000000001</v>
       </c>
       <c r="Q164" s="50">
-        <f t="shared" ref="Q164:Q168" si="16">Q163</f>
+        <f t="shared" ref="Q164:Q168" si="15">Q163</f>
         <v>3.592571901094749</v>
       </c>
       <c r="R164" s="1">
         <v>20</v>
       </c>
       <c r="S164" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1E-3</v>
       </c>
     </row>
     <row r="165" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B165" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>T-MGT-ICE_NGB71</v>
       </c>
       <c r="C165" s="1" t="str">
@@ -9803,71 +10014,68 @@
         <v>TRACNG,TRABNG</v>
       </c>
       <c r="D165" s="1" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>TRAF</v>
       </c>
       <c r="E165" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>2019</v>
       </c>
-      <c r="F165" s="1">
-        <f t="shared" si="14"/>
-        <v>0.11799999999999999</v>
-      </c>
-      <c r="G165" s="1">
-        <f t="shared" si="14"/>
-        <v>0.14099999999999999</v>
-      </c>
-      <c r="H165" s="1">
-        <f t="shared" si="14"/>
-        <v>0.155</v>
+      <c r="F165" s="48">
+        <v>2.2386549470658205E-2</v>
+      </c>
+      <c r="G165" s="48">
+        <v>2.6750029452227177E-2</v>
+      </c>
+      <c r="H165" s="48">
+        <v>2.9406060745356118E-2</v>
       </c>
       <c r="I165" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>115.69</v>
       </c>
       <c r="J165" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>120.95</v>
       </c>
       <c r="K165" s="48">
+        <f t="shared" si="10"/>
+        <v>120.95</v>
+      </c>
+      <c r="L165" s="1">
         <f t="shared" si="11"/>
         <v>120.95</v>
       </c>
-      <c r="L165" s="1">
-        <f t="shared" si="12"/>
-        <v>120.95</v>
-      </c>
       <c r="M165" s="48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>5.0989820625747049</v>
       </c>
       <c r="N165" s="48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>3.5538821890369761</v>
       </c>
       <c r="O165" s="48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>2.3292245236828353</v>
       </c>
       <c r="P165" s="48">
         <v>29.397500000000001</v>
       </c>
       <c r="Q165" s="50">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>3.592571901094749</v>
       </c>
       <c r="R165" s="1">
         <v>20</v>
       </c>
       <c r="S165" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1E-3</v>
       </c>
     </row>
     <row r="166" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B166" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>T-MGT-HEV_NGB71</v>
       </c>
       <c r="C166" s="1" t="str">
@@ -9875,209 +10083,200 @@
         <v>TRACNG,TRABNG</v>
       </c>
       <c r="D166" s="1" t="str">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>TRAF</v>
       </c>
       <c r="E166" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>2019</v>
       </c>
-      <c r="F166" s="1">
-        <f t="shared" si="14"/>
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="G166" s="1">
-        <f t="shared" si="14"/>
-        <v>0.20100000000000001</v>
-      </c>
-      <c r="H166" s="1">
-        <f t="shared" si="14"/>
-        <v>0.222</v>
+      <c r="F166" s="48">
+        <v>3.1872375517547277E-2</v>
+      </c>
+      <c r="G166" s="48">
+        <v>3.8133020708494066E-2</v>
+      </c>
+      <c r="H166" s="48">
+        <v>4.211706764818747E-2</v>
       </c>
       <c r="I166" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>144.72999999999999</v>
       </c>
       <c r="J166" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>145.12</v>
       </c>
       <c r="K166" s="48">
+        <f t="shared" si="10"/>
+        <v>143.88249999999999</v>
+      </c>
+      <c r="L166" s="1">
         <f t="shared" si="11"/>
-        <v>143.88249999999999</v>
-      </c>
-      <c r="L166" s="1">
-        <f t="shared" si="12"/>
         <v>140.16999999999999</v>
       </c>
       <c r="M166" s="48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>5.0989820625747049</v>
       </c>
       <c r="N166" s="48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>3.5538821890369761</v>
       </c>
       <c r="O166" s="48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>2.3292245236828353</v>
       </c>
       <c r="P166" s="48">
         <v>29.397500000000001</v>
       </c>
       <c r="Q166" s="50">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>3.592571901094749</v>
       </c>
       <c r="R166" s="1">
         <v>20</v>
       </c>
       <c r="S166" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1E-3</v>
       </c>
     </row>
     <row r="167" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B167" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>T-MGT-ICE_LNG71</v>
       </c>
       <c r="C167" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>TRALNG</v>
+      </c>
+      <c r="D167" s="1" t="str">
         <f t="shared" si="14"/>
-        <v>TRALNG</v>
-      </c>
-      <c r="D167" s="1" t="str">
-        <f t="shared" si="15"/>
         <v>TRAF</v>
       </c>
       <c r="E167" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>2019</v>
       </c>
-      <c r="F167" s="1">
-        <f t="shared" si="14"/>
-        <v>0.11799999999999999</v>
-      </c>
-      <c r="G167" s="1">
-        <f t="shared" si="14"/>
-        <v>0.14099999999999999</v>
-      </c>
-      <c r="H167" s="1">
-        <f t="shared" si="14"/>
-        <v>0.155</v>
+      <c r="F167" s="48">
+        <v>2.2386549470658205E-2</v>
+      </c>
+      <c r="G167" s="48">
+        <v>2.6750029452227177E-2</v>
+      </c>
+      <c r="H167" s="48">
+        <v>2.9406060745356118E-2</v>
       </c>
       <c r="I167" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>130.68600000000001</v>
       </c>
       <c r="J167" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>128.75800000000001</v>
       </c>
       <c r="K167" s="48">
+        <f t="shared" si="10"/>
+        <v>128.11425</v>
+      </c>
+      <c r="L167" s="1">
         <f t="shared" si="11"/>
-        <v>128.11425</v>
-      </c>
-      <c r="L167" s="1">
-        <f t="shared" si="12"/>
         <v>126.18300000000001</v>
       </c>
       <c r="M167" s="48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>5.0989820625747049</v>
       </c>
       <c r="N167" s="48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>3.5538821890369761</v>
       </c>
       <c r="O167" s="48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>2.3292245236828353</v>
       </c>
       <c r="P167" s="48">
         <v>29.397500000000001</v>
       </c>
       <c r="Q167" s="50">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>3.592571901094749</v>
       </c>
       <c r="R167" s="1">
         <v>20</v>
       </c>
       <c r="S167" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1E-3</v>
       </c>
     </row>
     <row r="168" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B168" s="1" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="8"/>
         <v>T-MGT-BEV_ELC71</v>
       </c>
       <c r="C168" s="1" t="str">
+        <f t="shared" si="13"/>
+        <v>TRAELC</v>
+      </c>
+      <c r="D168" s="1" t="str">
         <f t="shared" si="14"/>
-        <v>TRAELC</v>
-      </c>
-      <c r="D168" s="1" t="str">
-        <f t="shared" si="15"/>
         <v>TRAF</v>
       </c>
       <c r="E168" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>2019</v>
       </c>
-      <c r="F168" s="1">
-        <f t="shared" si="14"/>
-        <v>0.34699999999999998</v>
-      </c>
-      <c r="G168" s="1">
-        <f t="shared" si="14"/>
-        <v>0.34699999999999998</v>
-      </c>
-      <c r="H168" s="1">
-        <f t="shared" si="14"/>
-        <v>0.34699999999999998</v>
+      <c r="F168" s="48">
+        <v>6.5831632765410139E-2</v>
+      </c>
+      <c r="G168" s="48">
+        <v>6.5831632765410139E-2</v>
+      </c>
+      <c r="H168" s="48">
+        <v>6.5831632765410139E-2</v>
       </c>
       <c r="I168" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>345.67</v>
       </c>
       <c r="J168" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>274.11</v>
       </c>
       <c r="K168" s="48">
+        <f t="shared" si="10"/>
+        <v>234.625</v>
+      </c>
+      <c r="L168" s="1">
         <f t="shared" si="11"/>
-        <v>234.625</v>
-      </c>
-      <c r="L168" s="1">
-        <f t="shared" si="12"/>
         <v>116.17</v>
       </c>
       <c r="M168" s="48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>3.5721072259038325</v>
       </c>
       <c r="N168" s="48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>3.0618061936318557</v>
       </c>
       <c r="O168" s="48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="11"/>
         <v>2.3858458293310703</v>
       </c>
       <c r="P168" s="48">
         <v>29.397500000000001</v>
       </c>
       <c r="Q168" s="50">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>3.592571901094749</v>
       </c>
       <c r="R168" s="1">
         <v>20</v>
       </c>
       <c r="S168" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="12"/>
         <v>1E-3</v>
       </c>
     </row>
@@ -10105,7 +10304,7 @@
     </row>
     <row r="170" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B170" s="1" t="str">
-        <f t="shared" ref="B170:B176" si="17">D76</f>
+        <f t="shared" ref="B170:B176" si="16">D76</f>
         <v>T-HGT-ICE_DST81</v>
       </c>
       <c r="C170" s="1" t="str">
@@ -10119,14 +10318,14 @@
       <c r="E170" s="49">
         <v>2019</v>
       </c>
-      <c r="F170" s="50">
-        <v>0.121</v>
-      </c>
-      <c r="G170" s="50">
-        <v>0.13200000000000001</v>
-      </c>
-      <c r="H170" s="50">
-        <v>0.157</v>
+      <c r="F170" s="48">
+        <v>2.2955699033471548E-2</v>
+      </c>
+      <c r="G170" s="48">
+        <v>2.5042580763787146E-2</v>
+      </c>
+      <c r="H170" s="48">
+        <v>2.9785493787231682E-2</v>
       </c>
       <c r="I170" s="50">
         <v>95.69</v>
@@ -10135,7 +10334,7 @@
         <v>100.95</v>
       </c>
       <c r="K170" s="48">
-        <f t="shared" ref="K170:K176" si="18">J170-((J170-L170)/4)</f>
+        <f t="shared" ref="K170:K176" si="17">J170-((J170-L170)/4)</f>
         <v>100.95</v>
       </c>
       <c r="L170" s="50">
@@ -10166,7 +10365,7 @@
     </row>
     <row r="171" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B171" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>T-HGT-HEV_DST81</v>
       </c>
       <c r="C171" s="1" t="str">
@@ -10180,14 +10379,14 @@
       <c r="E171" s="49">
         <v>2019</v>
       </c>
-      <c r="F171" s="50">
-        <v>0.17299999999999999</v>
-      </c>
-      <c r="G171" s="50">
-        <v>0.189</v>
-      </c>
-      <c r="H171" s="50">
-        <v>0.224</v>
+      <c r="F171" s="48">
+        <v>3.2820958122236184E-2</v>
+      </c>
+      <c r="G171" s="48">
+        <v>3.5856422457240689E-2</v>
+      </c>
+      <c r="H171" s="48">
+        <v>4.2496500690063034E-2</v>
       </c>
       <c r="I171" s="50">
         <v>124.73</v>
@@ -10196,7 +10395,7 @@
         <v>125.12</v>
       </c>
       <c r="K171" s="48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>123.88250000000001</v>
       </c>
       <c r="L171" s="50">
@@ -10228,7 +10427,7 @@
     </row>
     <row r="172" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B172" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>T-HGT-FCV_HYD81</v>
       </c>
       <c r="C172" s="1" t="str">
@@ -10236,20 +10435,20 @@
         <v>TRAHYD</v>
       </c>
       <c r="D172" s="49" t="str">
-        <f t="shared" ref="D172:D176" si="19">D171</f>
+        <f t="shared" ref="D172:D176" si="18">D171</f>
         <v>TRAF</v>
       </c>
       <c r="E172" s="49">
         <v>2019</v>
       </c>
-      <c r="F172" s="50">
-        <v>0.20100000000000001</v>
-      </c>
-      <c r="G172" s="50">
-        <v>0.22</v>
-      </c>
-      <c r="H172" s="50">
-        <v>0.26200000000000001</v>
+      <c r="F172" s="48">
+        <v>3.8133020708494066E-2</v>
+      </c>
+      <c r="G172" s="48">
+        <v>4.1737634606311913E-2</v>
+      </c>
+      <c r="H172" s="48">
+        <v>4.9705728485698729E-2</v>
       </c>
       <c r="I172" s="50">
         <v>345.67</v>
@@ -10258,7 +10457,7 @@
         <v>222.22</v>
       </c>
       <c r="K172" s="48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>195.70750000000001</v>
       </c>
       <c r="L172" s="50">
@@ -10277,7 +10476,7 @@
         <v>50.915999999999997</v>
       </c>
       <c r="Q172" s="50">
-        <f t="shared" ref="Q172:Q176" si="20">Q171</f>
+        <f t="shared" ref="Q172:Q176" si="19">Q171</f>
         <v>9.2231504438872829</v>
       </c>
       <c r="R172" s="49">
@@ -10290,7 +10489,7 @@
     </row>
     <row r="173" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B173" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>T-HGT-ICE_NGB81</v>
       </c>
       <c r="C173" s="1" t="str">
@@ -10298,20 +10497,20 @@
         <v>TRACNG,TRABNG</v>
       </c>
       <c r="D173" s="49" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>TRAF</v>
       </c>
       <c r="E173" s="49">
         <v>2019</v>
       </c>
-      <c r="F173" s="50">
-        <v>0.11799999999999999</v>
-      </c>
-      <c r="G173" s="50">
-        <v>0.14099999999999999</v>
-      </c>
-      <c r="H173" s="50">
-        <v>0.155</v>
+      <c r="F173" s="48">
+        <v>2.2386549470658205E-2</v>
+      </c>
+      <c r="G173" s="48">
+        <v>2.6750029452227177E-2</v>
+      </c>
+      <c r="H173" s="48">
+        <v>2.9406060745356118E-2</v>
       </c>
       <c r="I173" s="50">
         <v>115.69</v>
@@ -10320,7 +10519,7 @@
         <v>120.95</v>
       </c>
       <c r="K173" s="48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>120.95</v>
       </c>
       <c r="L173" s="50">
@@ -10339,7 +10538,7 @@
         <v>50.915999999999997</v>
       </c>
       <c r="Q173" s="50">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>9.2231504438872829</v>
       </c>
       <c r="R173" s="49">
@@ -10352,7 +10551,7 @@
     </row>
     <row r="174" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B174" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>T-HGT-HEV_NGB81</v>
       </c>
       <c r="C174" s="1" t="str">
@@ -10360,20 +10559,20 @@
         <v>TRACNG,TRABNG</v>
       </c>
       <c r="D174" s="49" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>TRAF</v>
       </c>
       <c r="E174" s="49">
         <v>2019</v>
       </c>
-      <c r="F174" s="50">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="G174" s="50">
-        <v>0.20100000000000001</v>
-      </c>
-      <c r="H174" s="50">
-        <v>0.222</v>
+      <c r="F174" s="48">
+        <v>3.1872375517547277E-2</v>
+      </c>
+      <c r="G174" s="48">
+        <v>3.8133020708494066E-2</v>
+      </c>
+      <c r="H174" s="48">
+        <v>4.211706764818747E-2</v>
       </c>
       <c r="I174" s="50">
         <v>144.72999999999999</v>
@@ -10382,7 +10581,7 @@
         <v>145.12</v>
       </c>
       <c r="K174" s="48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>143.88249999999999</v>
       </c>
       <c r="L174" s="50">
@@ -10401,7 +10600,7 @@
         <v>50.915999999999997</v>
       </c>
       <c r="Q174" s="50">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>9.2231504438872829</v>
       </c>
       <c r="R174" s="49">
@@ -10413,7 +10612,7 @@
     </row>
     <row r="175" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B175" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>T-HGT-ICE_LNG81</v>
       </c>
       <c r="C175" s="1" t="str">
@@ -10421,20 +10620,20 @@
         <v>TRALNG</v>
       </c>
       <c r="D175" s="49" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>TRAF</v>
       </c>
       <c r="E175" s="49">
         <v>2019</v>
       </c>
-      <c r="F175" s="50">
-        <v>0.11799999999999999</v>
-      </c>
-      <c r="G175" s="50">
-        <v>0.14099999999999999</v>
-      </c>
-      <c r="H175" s="50">
-        <v>0.155</v>
+      <c r="F175" s="48">
+        <v>2.2386549470658205E-2</v>
+      </c>
+      <c r="G175" s="48">
+        <v>2.6750029452227177E-2</v>
+      </c>
+      <c r="H175" s="48">
+        <v>2.9406060745356118E-2</v>
       </c>
       <c r="I175" s="50">
         <v>130.68600000000001</v>
@@ -10443,7 +10642,7 @@
         <v>128.75800000000001</v>
       </c>
       <c r="K175" s="48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>128.11425</v>
       </c>
       <c r="L175" s="50">
@@ -10462,7 +10661,7 @@
         <v>50.915999999999997</v>
       </c>
       <c r="Q175" s="50">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>9.2231504438872829</v>
       </c>
       <c r="R175" s="49">
@@ -10474,7 +10673,7 @@
     </row>
     <row r="176" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B176" s="1" t="str">
-        <f t="shared" si="17"/>
+        <f t="shared" si="16"/>
         <v>T-HGT-BEV_ELC81</v>
       </c>
       <c r="C176" s="1" t="str">
@@ -10482,20 +10681,20 @@
         <v>TRAELC</v>
       </c>
       <c r="D176" s="49" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="18"/>
         <v>TRAF</v>
       </c>
       <c r="E176" s="49">
         <v>2019</v>
       </c>
-      <c r="F176" s="50">
-        <v>0.34699999999999998</v>
-      </c>
-      <c r="G176" s="50">
-        <v>0.34699999999999998</v>
-      </c>
-      <c r="H176" s="50">
-        <v>0.34699999999999998</v>
+      <c r="F176" s="48">
+        <v>6.5831632765410139E-2</v>
+      </c>
+      <c r="G176" s="48">
+        <v>6.5831632765410139E-2</v>
+      </c>
+      <c r="H176" s="48">
+        <v>6.5831632765410139E-2</v>
       </c>
       <c r="I176" s="50">
         <v>345.67</v>
@@ -10504,7 +10703,7 @@
         <v>274.11</v>
       </c>
       <c r="K176" s="48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="17"/>
         <v>234.625</v>
       </c>
       <c r="L176" s="50">
@@ -10523,7 +10722,7 @@
         <v>50.915999999999997</v>
       </c>
       <c r="Q176" s="50">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>9.2231504438872829</v>
       </c>
       <c r="R176" s="49">
@@ -10587,7 +10786,7 @@
         <v>469.60386878903267</v>
       </c>
       <c r="K178" s="48">
-        <f t="shared" ref="K178:K179" si="21">J178-((J178-L178)/4)</f>
+        <f t="shared" ref="K178:K179" si="20">J178-((J178-L178)/4)</f>
         <v>469.60386878903267</v>
       </c>
       <c r="L178" s="48">
@@ -10647,7 +10846,7 @@
         <v>438.88212036358203</v>
       </c>
       <c r="K179" s="48">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>438.88212036358203</v>
       </c>
       <c r="L179" s="48">
@@ -10788,7 +10987,7 @@
     </row>
     <row r="183" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B183" s="1" t="str">
-        <f t="shared" ref="B183:B184" si="22">D89</f>
+        <f t="shared" ref="B183:B184" si="21">D89</f>
         <v>T-NAV_NEW</v>
       </c>
       <c r="C183" s="1" t="str">
@@ -10817,7 +11016,7 @@
     </row>
     <row r="184" spans="2:26" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B184" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="21"/>
         <v>T-OTH_NEW</v>
       </c>
       <c r="C184" s="1" t="str">
@@ -12201,23 +12400,23 @@
         <v>TRAGSL</v>
       </c>
       <c r="D226" s="93" t="str">
-        <f t="shared" ref="D226:H226" si="23">D200</f>
+        <f t="shared" ref="D226:H226" si="22">D200</f>
         <v>UP</v>
       </c>
       <c r="E226" s="89">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>0.96784365458672328</v>
       </c>
       <c r="F226" s="89">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="G226" s="89">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="H226" s="83">
-        <f t="shared" si="23"/>
+        <f t="shared" si="22"/>
         <v>5</v>
       </c>
     </row>
@@ -12227,27 +12426,27 @@
         <v>T-TAX-ICE_GSL31</v>
       </c>
       <c r="C227" s="83" t="str">
-        <f t="shared" ref="C227:H251" si="24">C201</f>
+        <f t="shared" ref="C227:H251" si="23">C201</f>
         <v>TRAGSL</v>
       </c>
       <c r="D227" s="93" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>LO</v>
       </c>
       <c r="E227" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.96784365458672328</v>
       </c>
       <c r="F227" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.95</v>
       </c>
       <c r="G227" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.9</v>
       </c>
       <c r="H227" s="83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
     </row>
@@ -12257,27 +12456,27 @@
         <v>T-TAX-ICE_DST31</v>
       </c>
       <c r="C228" s="83" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>TRADST</v>
       </c>
       <c r="D228" s="93" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>UP</v>
       </c>
       <c r="E228" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.95903634682608185</v>
       </c>
       <c r="F228" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="G228" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="H228" s="83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
     </row>
@@ -12287,27 +12486,27 @@
         <v>T-TAX-ICE_DST31</v>
       </c>
       <c r="C229" s="83" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>TRADST</v>
       </c>
       <c r="D229" s="93" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>LO</v>
       </c>
       <c r="E229" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.95903634682608185</v>
       </c>
       <c r="F229" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.95</v>
       </c>
       <c r="G229" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.9</v>
       </c>
       <c r="H229" s="83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
     </row>
@@ -12317,27 +12516,27 @@
         <v>T-TAX-ICE_DF31</v>
       </c>
       <c r="C230" s="83" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>TRACNG</v>
       </c>
       <c r="D230" s="93" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>UP</v>
       </c>
       <c r="E230" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="F230" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="G230" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.8</v>
       </c>
       <c r="H230" s="83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
     </row>
@@ -12347,27 +12546,27 @@
         <v>T-TAX-ICE_DF31</v>
       </c>
       <c r="C231" s="83" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>TRACNG</v>
       </c>
       <c r="D231" s="93" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>LO</v>
       </c>
       <c r="E231" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.4</v>
       </c>
       <c r="F231" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.4</v>
       </c>
       <c r="G231" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.4</v>
       </c>
       <c r="H231" s="83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
     </row>
@@ -12377,27 +12576,27 @@
         <v>T-TAX-ICE_NGB31</v>
       </c>
       <c r="C232" s="83" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>TRACNG</v>
       </c>
       <c r="D232" s="93" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>UP</v>
       </c>
       <c r="E232" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="F232" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="G232" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="H232" s="83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
       <c r="J232" s="1"/>
@@ -12424,27 +12623,27 @@
         <v>T-TAX-ICE_NGB31</v>
       </c>
       <c r="C233" s="83" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>TRACNG</v>
       </c>
       <c r="D233" s="93" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>LO</v>
       </c>
       <c r="E233" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="F233" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="G233" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="H233" s="83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
       <c r="J233" s="1"/>
@@ -12471,27 +12670,27 @@
         <v>T-TAX-ICE_E8531</v>
       </c>
       <c r="C234" s="83" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>TRAETH</v>
       </c>
       <c r="D234" s="93" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>UP</v>
       </c>
       <c r="E234" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.85</v>
       </c>
       <c r="F234" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.85</v>
       </c>
       <c r="G234" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.85</v>
       </c>
       <c r="H234" s="83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
       <c r="J234" s="1"/>
@@ -12518,27 +12717,27 @@
         <v>T-TAX-ICE_E8531</v>
       </c>
       <c r="C235" s="83" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>TRAETH</v>
       </c>
       <c r="D235" s="93" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>LO</v>
       </c>
       <c r="E235" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="F235" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="G235" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="H235" s="83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
       <c r="J235" s="1"/>
@@ -12565,27 +12764,27 @@
         <v>T-TAX-HEV_GSL31</v>
       </c>
       <c r="C236" s="83" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>TRAGSL</v>
       </c>
       <c r="D236" s="93" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>UP</v>
       </c>
       <c r="E236" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.96784365458672328</v>
       </c>
       <c r="F236" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="G236" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="H236" s="83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
       <c r="J236" s="1"/>
@@ -12612,27 +12811,27 @@
         <v>T-TAX-HEV_GSL31</v>
       </c>
       <c r="C237" s="83" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>TRAGSL</v>
       </c>
       <c r="D237" s="93" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>LO</v>
       </c>
       <c r="E237" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.96784365458672328</v>
       </c>
       <c r="F237" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.95</v>
       </c>
       <c r="G237" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.9</v>
       </c>
       <c r="H237" s="83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
       <c r="J237" s="1"/>
@@ -12659,27 +12858,27 @@
         <v>T-TAX-HEV_DST31</v>
       </c>
       <c r="C238" s="83" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>TRADST</v>
       </c>
       <c r="D238" s="93" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>UP</v>
       </c>
       <c r="E238" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.95903634682608185</v>
       </c>
       <c r="F238" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="G238" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="H238" s="83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
     </row>
@@ -12689,27 +12888,27 @@
         <v>T-TAX-HEV_DST31</v>
       </c>
       <c r="C239" s="83" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>TRADST</v>
       </c>
       <c r="D239" s="93" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>LO</v>
       </c>
       <c r="E239" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.95903634682608185</v>
       </c>
       <c r="F239" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.95</v>
       </c>
       <c r="G239" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.9</v>
       </c>
       <c r="H239" s="83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
     </row>
@@ -12719,27 +12918,27 @@
         <v>T-TAX-PHEV10_GSL31</v>
       </c>
       <c r="C240" s="83" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>TRAELC</v>
       </c>
       <c r="D240" s="93" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>UP</v>
       </c>
       <c r="E240" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="F240" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.6</v>
       </c>
       <c r="G240" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.8</v>
       </c>
       <c r="H240" s="83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
     </row>
@@ -12749,27 +12948,27 @@
         <v>T-TAX-PHEV10_GSL31</v>
       </c>
       <c r="C241" s="83" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>TRAELC</v>
       </c>
       <c r="D241" s="93" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>LO</v>
       </c>
       <c r="E241" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.3</v>
       </c>
       <c r="F241" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.3</v>
       </c>
       <c r="G241" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.3</v>
       </c>
       <c r="H241" s="83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
     </row>
@@ -12779,27 +12978,27 @@
         <v>T-TAX-PHEV20_GSL31</v>
       </c>
       <c r="C242" s="83" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>TRAELC</v>
       </c>
       <c r="D242" s="93" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>UP</v>
       </c>
       <c r="E242" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="F242" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.6</v>
       </c>
       <c r="G242" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.8</v>
       </c>
       <c r="H242" s="83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
     </row>
@@ -12809,27 +13008,27 @@
         <v>T-TAX-PHEV20_GSL31</v>
       </c>
       <c r="C243" s="83" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>TRAELC</v>
       </c>
       <c r="D243" s="93" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>LO</v>
       </c>
       <c r="E243" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.3</v>
       </c>
       <c r="F243" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.3</v>
       </c>
       <c r="G243" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.3</v>
       </c>
       <c r="H243" s="83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
     </row>
@@ -12839,27 +13038,27 @@
         <v>T-TAX-PHEV40_GSL31</v>
       </c>
       <c r="C244" s="83" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>TRAELC</v>
       </c>
       <c r="D244" s="93" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>UP</v>
       </c>
       <c r="E244" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="F244" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.6</v>
       </c>
       <c r="G244" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.8</v>
       </c>
       <c r="H244" s="83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
     </row>
@@ -12869,27 +13068,27 @@
         <v>T-TAX-PHEV40_GSL31</v>
       </c>
       <c r="C245" s="83" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>TRAELC</v>
       </c>
       <c r="D245" s="93" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>LO</v>
       </c>
       <c r="E245" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.3</v>
       </c>
       <c r="F245" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.3</v>
       </c>
       <c r="G245" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.3</v>
       </c>
       <c r="H245" s="83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
     </row>
@@ -12899,27 +13098,27 @@
         <v>T-TAX-PHEV10_DST31</v>
       </c>
       <c r="C246" s="83" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>TRAELC</v>
       </c>
       <c r="D246" s="93" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>UP</v>
       </c>
       <c r="E246" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="F246" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.6</v>
       </c>
       <c r="G246" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.8</v>
       </c>
       <c r="H246" s="83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
     </row>
@@ -12929,27 +13128,27 @@
         <v>T-TAX-PHEV10_DST31</v>
       </c>
       <c r="C247" s="83" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>TRAELC</v>
       </c>
       <c r="D247" s="93" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>LO</v>
       </c>
       <c r="E247" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.3</v>
       </c>
       <c r="F247" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.3</v>
       </c>
       <c r="G247" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.3</v>
       </c>
       <c r="H247" s="83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
     </row>
@@ -12959,27 +13158,27 @@
         <v>T-TAX-PHEV20_DST31</v>
       </c>
       <c r="C248" s="83" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>TRAELC</v>
       </c>
       <c r="D248" s="93" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>UP</v>
       </c>
       <c r="E248" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="F248" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.6</v>
       </c>
       <c r="G248" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.8</v>
       </c>
       <c r="H248" s="83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
     </row>
@@ -12989,27 +13188,27 @@
         <v>T-TAX-PHEV20_DST31</v>
       </c>
       <c r="C249" s="83" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>TRAELC</v>
       </c>
       <c r="D249" s="93" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>LO</v>
       </c>
       <c r="E249" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.3</v>
       </c>
       <c r="F249" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.3</v>
       </c>
       <c r="G249" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.3</v>
       </c>
       <c r="H249" s="83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
     </row>
@@ -13019,27 +13218,27 @@
         <v>T-TAX-PHEV40_DST31</v>
       </c>
       <c r="C250" s="83" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>TRAELC</v>
       </c>
       <c r="D250" s="93" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>UP</v>
       </c>
       <c r="E250" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.5</v>
       </c>
       <c r="F250" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.6</v>
       </c>
       <c r="G250" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.8</v>
       </c>
       <c r="H250" s="83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
     </row>
@@ -13049,27 +13248,27 @@
         <v>T-TAX-PHEV40_DST31</v>
       </c>
       <c r="C251" s="83" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>TRAELC</v>
       </c>
       <c r="D251" s="93" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>LO</v>
       </c>
       <c r="E251" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.3</v>
       </c>
       <c r="F251" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.3</v>
       </c>
       <c r="G251" s="89">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>0.3</v>
       </c>
       <c r="H251" s="83">
-        <f t="shared" si="24"/>
+        <f t="shared" si="23"/>
         <v>5</v>
       </c>
     </row>
@@ -13083,7 +13282,7 @@
         <v>TRADST</v>
       </c>
       <c r="D252" s="84" t="str">
-        <f t="shared" ref="D252" si="25">D226</f>
+        <f t="shared" ref="D252" si="24">D226</f>
         <v>UP</v>
       </c>
       <c r="E252" s="81">
@@ -13109,7 +13308,7 @@
         <v>TRADST</v>
       </c>
       <c r="D253" s="84" t="str">
-        <f t="shared" ref="D253" si="26">D227</f>
+        <f t="shared" ref="D253" si="25">D227</f>
         <v>LO</v>
       </c>
       <c r="E253" s="81">
@@ -13135,7 +13334,7 @@
         <v>TRACNG</v>
       </c>
       <c r="D254" s="84" t="str">
-        <f t="shared" ref="D254" si="27">D228</f>
+        <f t="shared" ref="D254" si="26">D228</f>
         <v>UP</v>
       </c>
       <c r="E254" s="81">
@@ -13161,7 +13360,7 @@
         <v>TRACNG</v>
       </c>
       <c r="D255" s="84" t="str">
-        <f t="shared" ref="D255" si="28">D229</f>
+        <f t="shared" ref="D255" si="27">D229</f>
         <v>LO</v>
       </c>
       <c r="E255" s="81">
@@ -14265,7 +14464,7 @@
     </row>
     <row r="294" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B294" s="88" t="str">
-        <f t="shared" ref="B294:B298" si="29">B293</f>
+        <f t="shared" ref="B294:B298" si="28">B293</f>
         <v>T-OTH_NEW</v>
       </c>
       <c r="C294" s="88" t="str">
@@ -14290,7 +14489,7 @@
     </row>
     <row r="295" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B295" s="88" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>T-OTH_NEW</v>
       </c>
       <c r="C295" s="88" t="str">
@@ -14315,7 +14514,7 @@
     </row>
     <row r="296" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B296" s="88" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>T-OTH_NEW</v>
       </c>
       <c r="C296" s="88" t="str">
@@ -14340,7 +14539,7 @@
     </row>
     <row r="297" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B297" s="88" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>T-OTH_NEW</v>
       </c>
       <c r="C297" s="88" t="str">
@@ -14365,7 +14564,7 @@
     </row>
     <row r="298" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B298" s="88" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="28"/>
         <v>T-OTH_NEW</v>
       </c>
       <c r="C298" s="88" t="str">
@@ -14564,7 +14763,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="15" type="noConversion"/>
+  <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
Modify load factor for new light goods truck
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
+++ b/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA43409-E371-46E4-B895-08E5B8AFA694}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1C3F38-F835-4BB5-8B25-98F8EBB239CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4288,8 +4288,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B3:AF305"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U153" sqref="U153:U158"/>
+    <sheetView tabSelected="1" topLeftCell="G136" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q154" sqref="Q154:Q160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -9402,7 +9402,7 @@
         <v>20.794499999999999</v>
       </c>
       <c r="Q154" s="1">
-        <v>3.6395043558255735E-2</v>
+        <v>0.05</v>
       </c>
       <c r="R154" s="49">
         <v>20</v>
@@ -9462,7 +9462,7 @@
         <v>20.794499999999999</v>
       </c>
       <c r="Q155" s="1">
-        <v>3.6395043558255735E-2</v>
+        <v>0.05</v>
       </c>
       <c r="R155" s="49">
         <v>20</v>
@@ -9522,7 +9522,7 @@
         <v>20.794499999999999</v>
       </c>
       <c r="Q156" s="1">
-        <v>3.6395043558255735E-2</v>
+        <v>0.05</v>
       </c>
       <c r="R156" s="49">
         <v>20</v>
@@ -9583,7 +9583,7 @@
         <v>20.794499999999999</v>
       </c>
       <c r="Q157" s="1">
-        <v>3.6395043558255735E-2</v>
+        <v>0.05</v>
       </c>
       <c r="R157" s="49">
         <v>20</v>
@@ -9643,7 +9643,7 @@
         <v>20.794499999999999</v>
       </c>
       <c r="Q158" s="1">
-        <v>3.6395043558255735E-2</v>
+        <v>0.05</v>
       </c>
       <c r="R158" s="49">
         <v>20</v>
@@ -9703,7 +9703,7 @@
         <v>20.794499999999999</v>
       </c>
       <c r="Q159" s="1">
-        <v>3.6395043558255735E-2</v>
+        <v>0.05</v>
       </c>
       <c r="R159" s="49">
         <v>20</v>
@@ -9764,7 +9764,7 @@
         <v>20.794499999999999</v>
       </c>
       <c r="Q160" s="1">
-        <v>3.6395043558255735E-2</v>
+        <v>0.05</v>
       </c>
       <c r="R160" s="49">
         <v>20</v>

</xml_diff>

<commit_message>
Change START attribute from 2019 to 2030 for FCVs
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
+++ b/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9946D6A4-D3A4-4337-9B47-45444966B964}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37690913-803D-412B-AF1D-6091141DA213}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4288,14 +4288,14 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B3:AF302"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A176" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B191" sqref="B191"/>
+    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E181" sqref="E181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" customWidth="1"/>
     <col min="3" max="3" width="46.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.5546875" customWidth="1"/>
@@ -7517,7 +7517,7 @@
         <v>TRAPS,TRAPM,TRAPL</v>
       </c>
       <c r="E121" s="1">
-        <v>2019</v>
+        <v>2030</v>
       </c>
       <c r="F121" s="48">
         <v>0.66724203897835621</v>
@@ -7578,7 +7578,7 @@
         <v>TRAPS,TRAPM,TRAPL</v>
       </c>
       <c r="E122" s="1">
-        <v>2019</v>
+        <v>2030</v>
       </c>
       <c r="F122" s="48">
         <v>0.82180053029786837</v>
@@ -8697,7 +8697,7 @@
         <v>TRAPS,TRAPM,TRAPL</v>
       </c>
       <c r="E141" s="1">
-        <v>2019</v>
+        <v>2030</v>
       </c>
       <c r="F141" s="48">
         <v>0.66724203897835621</v>
@@ -8758,7 +8758,7 @@
         <v>TRAPS,TRAPM,TRAPL</v>
       </c>
       <c r="E142" s="1">
-        <v>2019</v>
+        <v>2030</v>
       </c>
       <c r="F142" s="48">
         <v>0.82180053029786837</v>
@@ -9081,7 +9081,7 @@
         <v>TRAPS,TRAPM,TRAPL</v>
       </c>
       <c r="E148" s="1">
-        <v>2019</v>
+        <v>2030</v>
       </c>
       <c r="F148" s="48">
         <v>0.19205070620555917</v>
@@ -9666,7 +9666,7 @@
         <v>TRAF</v>
       </c>
       <c r="E159" s="49">
-        <v>2019</v>
+        <v>2030</v>
       </c>
       <c r="F159" s="48">
         <v>0.84316527171717093</v>
@@ -9949,8 +9949,7 @@
         <v>TRAF</v>
       </c>
       <c r="E164" s="1">
-        <f t="shared" si="13"/>
-        <v>2019</v>
+        <v>2030</v>
       </c>
       <c r="F164" s="48">
         <v>3.8133020708494066E-2</v>
@@ -10439,7 +10438,7 @@
         <v>TRAF</v>
       </c>
       <c r="E172" s="49">
-        <v>2019</v>
+        <v>2030</v>
       </c>
       <c r="F172" s="48">
         <v>3.8133020708494066E-2</v>
@@ -10888,7 +10887,7 @@
         <v>TRAF</v>
       </c>
       <c r="E180" s="52">
-        <v>2019</v>
+        <v>2030</v>
       </c>
       <c r="F180" s="61">
         <v>1.1393475951168699E-2</v>

</xml_diff>

<commit_message>
Remove H2 and Electricity from Unespecified transport demand
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
+++ b/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37690913-803D-412B-AF1D-6091141DA213}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF2CBD9-004E-4FC7-ACA7-1D77C993191B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -187,7 +187,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="389">
   <si>
     <t>~FI_T</t>
   </si>
@@ -4286,17 +4286,17 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B3:AF302"/>
+  <dimension ref="B3:AF298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E181" sqref="E181"/>
+    <sheetView tabSelected="1" topLeftCell="A185" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C293" sqref="C293:H294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="24.44140625" customWidth="1"/>
-    <col min="3" max="3" width="46.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.5546875" customWidth="1"/>
     <col min="6" max="8" width="13.44140625" customWidth="1"/>
@@ -11019,8 +11019,8 @@
         <v>T-OTH_NEW</v>
       </c>
       <c r="C184" s="1" t="str">
-        <f>Commodities!B8&amp;","&amp;Commodities!B10&amp;","&amp;Commodities!B9&amp;","&amp;Commodities!B11&amp;","&amp;Commodities!B15&amp;","&amp;Commodities!B17</f>
-        <v>TRAGSL,TRAETH,TRADST,TRABDL,TRAELC,TRAHYD</v>
+        <f>Commodities!B8&amp;","&amp;Commodities!B10&amp;","&amp;Commodities!B9&amp;","&amp;Commodities!B11</f>
+        <v>TRAGSL,TRAETH,TRADST,TRABDL</v>
       </c>
       <c r="D184" s="1" t="str">
         <f>Commodities!B25</f>
@@ -14409,7 +14409,7 @@
     </row>
     <row r="291" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B291" s="88" t="str">
-        <f t="shared" ref="B291:B295" si="28">B290</f>
+        <f t="shared" ref="B291:B294" si="28">B290</f>
         <v>T-OTH_NEW</v>
       </c>
       <c r="C291" s="88" t="str">
@@ -14463,20 +14463,20 @@
         <v>T-OTH_NEW</v>
       </c>
       <c r="C293" s="88" t="str">
-        <f>Commodities!B10</f>
-        <v>TRAETH</v>
+        <f>Commodities!B11</f>
+        <v>TRABDL</v>
       </c>
       <c r="D293" s="84" t="s">
         <v>196</v>
       </c>
       <c r="E293" s="81">
-        <v>0</v>
+        <v>2.774549221160999E-2</v>
       </c>
       <c r="F293" s="81">
-        <v>0</v>
+        <v>2.774549221160999E-2</v>
       </c>
       <c r="G293" s="81">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="H293" s="88">
         <v>5</v>
@@ -14489,16 +14489,16 @@
       </c>
       <c r="C294" s="88" t="str">
         <f>C293</f>
-        <v>TRAETH</v>
+        <v>TRABDL</v>
       </c>
       <c r="D294" s="84" t="s">
         <v>356</v>
       </c>
       <c r="E294" s="81">
-        <v>0</v>
+        <v>2.774549221160999E-2</v>
       </c>
       <c r="F294" s="81">
-        <v>0</v>
+        <v>2.774549221160999E-2</v>
       </c>
       <c r="G294" s="81">
         <v>0</v>
@@ -14508,202 +14508,102 @@
       </c>
     </row>
     <row r="295" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B295" s="88" t="str">
-        <f t="shared" si="28"/>
-        <v>T-OTH_NEW</v>
-      </c>
-      <c r="C295" s="88" t="str">
-        <f>Commodities!B11</f>
-        <v>TRABDL</v>
-      </c>
-      <c r="D295" s="84" t="s">
-        <v>196</v>
-      </c>
-      <c r="E295" s="81">
-        <v>2.774549221160999E-2</v>
-      </c>
-      <c r="F295" s="81">
-        <v>2.774549221160999E-2</v>
-      </c>
-      <c r="G295" s="81">
-        <v>0.2</v>
-      </c>
-      <c r="H295" s="88">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="296" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B296" s="88" t="str">
-        <f>B295</f>
-        <v>T-OTH_NEW</v>
-      </c>
-      <c r="C296" s="88" t="str">
-        <f>C295</f>
-        <v>TRABDL</v>
-      </c>
-      <c r="D296" s="84" t="s">
-        <v>356</v>
-      </c>
-      <c r="E296" s="81">
-        <v>2.774549221160999E-2</v>
-      </c>
-      <c r="F296" s="81">
-        <v>2.774549221160999E-2</v>
-      </c>
-      <c r="G296" s="81">
-        <v>0</v>
-      </c>
-      <c r="H296" s="88">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="297" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B297" s="88" t="str">
-        <f>B296</f>
-        <v>T-OTH_NEW</v>
-      </c>
-      <c r="C297" s="88" t="str">
-        <f>Commodities!B15</f>
-        <v>TRAELC</v>
-      </c>
-      <c r="D297" s="84" t="s">
-        <v>196</v>
-      </c>
-      <c r="E297" s="81">
-        <v>0</v>
-      </c>
-      <c r="F297" s="81">
-        <v>0</v>
-      </c>
-      <c r="G297" s="81">
-        <v>0.3</v>
-      </c>
-      <c r="H297" s="88">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="298" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B298" s="88" t="str">
-        <f>B297</f>
-        <v>T-OTH_NEW</v>
-      </c>
-      <c r="C298" s="88" t="str">
-        <f>C297</f>
-        <v>TRAELC</v>
-      </c>
-      <c r="D298" s="84" t="s">
-        <v>356</v>
-      </c>
-      <c r="E298" s="81">
-        <v>0</v>
-      </c>
-      <c r="F298" s="81">
-        <v>0</v>
-      </c>
-      <c r="G298" s="81">
-        <v>0</v>
-      </c>
-      <c r="H298" s="88">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="299" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B299" s="83" t="str">
+      <c r="B295" s="83" t="str">
         <f>B186</f>
         <v>T-AVI_DOM_NEW</v>
       </c>
-      <c r="C299" s="91" t="str">
+      <c r="C295" s="91" t="str">
         <f>Commodities!B18</f>
         <v>TRAKER</v>
       </c>
-      <c r="D299" s="93" t="s">
+      <c r="D295" s="93" t="s">
         <v>196</v>
       </c>
-      <c r="E299" s="89">
+      <c r="E295" s="89">
         <v>1</v>
       </c>
-      <c r="F299" s="89">
+      <c r="F295" s="89">
         <v>1</v>
       </c>
-      <c r="G299" s="89">
+      <c r="G295" s="89">
         <v>1</v>
       </c>
-      <c r="H299" s="83">
+      <c r="H295" s="83">
         <v>5</v>
       </c>
     </row>
-    <row r="300" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B300" s="83" t="str">
-        <f>B299</f>
+    <row r="296" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B296" s="83" t="str">
+        <f>B295</f>
         <v>T-AVI_DOM_NEW</v>
       </c>
-      <c r="C300" s="91" t="str">
-        <f>C299</f>
+      <c r="C296" s="91" t="str">
+        <f>C295</f>
         <v>TRAKER</v>
       </c>
-      <c r="D300" s="93" t="s">
+      <c r="D296" s="93" t="s">
         <v>356</v>
       </c>
-      <c r="E300" s="89">
+      <c r="E296" s="89">
         <v>1</v>
       </c>
-      <c r="F300" s="89">
+      <c r="F296" s="89">
         <v>1</v>
       </c>
-      <c r="G300" s="89">
-        <v>0</v>
-      </c>
-      <c r="H300" s="83">
+      <c r="G296" s="89">
+        <v>0</v>
+      </c>
+      <c r="H296" s="83">
         <v>5</v>
       </c>
     </row>
-    <row r="301" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B301" s="83" t="str">
+    <row r="297" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B297" s="83" t="str">
         <f>B187</f>
         <v>T-AVI_INT_NEW</v>
       </c>
-      <c r="C301" s="91" t="str">
+      <c r="C297" s="91" t="str">
         <f>Commodities!B18</f>
         <v>TRAKER</v>
       </c>
-      <c r="D301" s="93" t="s">
+      <c r="D297" s="93" t="s">
         <v>196</v>
       </c>
-      <c r="E301" s="89">
+      <c r="E297" s="89">
         <v>1</v>
       </c>
-      <c r="F301" s="89">
+      <c r="F297" s="89">
         <v>1</v>
       </c>
-      <c r="G301" s="89">
+      <c r="G297" s="89">
         <v>1</v>
       </c>
-      <c r="H301" s="83">
+      <c r="H297" s="83">
         <v>5</v>
       </c>
     </row>
-    <row r="302" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B302" s="87" t="str">
-        <f>B301</f>
+    <row r="298" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B298" s="87" t="str">
+        <f>B297</f>
         <v>T-AVI_INT_NEW</v>
       </c>
-      <c r="C302" s="87" t="str">
-        <f>C301</f>
+      <c r="C298" s="87" t="str">
+        <f>C297</f>
         <v>TRAKER</v>
       </c>
-      <c r="D302" s="85" t="s">
+      <c r="D298" s="85" t="s">
         <v>356</v>
       </c>
-      <c r="E302" s="82">
+      <c r="E298" s="82">
         <v>1</v>
       </c>
-      <c r="F302" s="82">
+      <c r="F298" s="82">
         <v>1</v>
       </c>
-      <c r="G302" s="82">
-        <v>0</v>
-      </c>
-      <c r="H302" s="92">
+      <c r="G298" s="82">
+        <v>0</v>
+      </c>
+      <c r="H298" s="92">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modify seed value for UC growth rate and modify AF for private cars
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
+++ b/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D141A3D9-8B8D-4E35-AAEB-5A9B607D46CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FC4AE5-E9A6-4A43-B7A0-93E3B5508899}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1451,10 +1451,17 @@
     <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="39" x14ac:knownFonts="1">
+  <fonts count="40" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1678,6 +1685,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1696,6 +1704,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1842,11 +1851,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="214">
+  <cellStyleXfs count="270">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1855,12 +1868,21 @@
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1887,6 +1909,8 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1896,26 +1920,50 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1951,59 +1999,73 @@
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2057,56 +2119,59 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="13" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="12" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="24" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2115,359 +2180,415 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="27" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="28" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="27" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="28" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="27" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="28" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="9" fontId="19" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="41" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="22" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="41" fontId="28" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="27" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="20" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="41" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="23" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="41" fontId="29" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="28" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="23" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="8" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="8" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="8" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="8" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="8" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="8" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="8" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="8" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="12" borderId="1" xfId="53" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="37" fillId="11" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="37" fillId="12" borderId="4" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="12" borderId="0" xfId="53" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="11" borderId="0" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="12" borderId="1" xfId="53" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="38" fillId="11" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="38" fillId="12" borderId="4" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="12" borderId="0" xfId="53" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="11" borderId="0" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="12" borderId="4" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="12" borderId="4" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="37" fillId="12" borderId="1" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="11" borderId="0" xfId="53" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="37" fillId="12" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="12" borderId="1" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="38" fillId="12" borderId="1" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="11" borderId="0" xfId="53" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="38" fillId="12" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="12" borderId="1" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="12" borderId="4" xfId="53" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="37" fillId="12" borderId="0" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="12" borderId="4" xfId="53" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="12" borderId="0" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="53"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="53" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="2" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="53"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="53" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="2" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="4" borderId="0" xfId="53" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="2" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="37" fillId="4" borderId="0" xfId="53" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="2" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="214">
+  <cellStyles count="270">
     <cellStyle name="20% - Accent5" xfId="1" builtinId="46"/>
     <cellStyle name="20% - Accent5 2" xfId="7" xr:uid="{41FADB5D-774C-4581-9E04-795745F45B3A}"/>
     <cellStyle name="20% - Accent5 2 2" xfId="22" xr:uid="{9D85FBE9-8CBA-4BC4-A23E-71E72F7E6CC9}"/>
     <cellStyle name="20% - Accent5 2 2 2" xfId="77" xr:uid="{056F0309-84E5-4341-AF71-2EEBE7BF74FD}"/>
     <cellStyle name="20% - Accent5 2 2 2 2" xfId="182" xr:uid="{F15C4DC7-EC48-407F-96A3-3CC4A53A0ED7}"/>
     <cellStyle name="20% - Accent5 2 2 3" xfId="129" xr:uid="{747D9A38-2066-47A4-B4DB-0321AD8ED675}"/>
+    <cellStyle name="20% - Accent5 2 2 4" xfId="235" xr:uid="{CE1210E9-19B9-41ED-A18B-6C55332279A1}"/>
     <cellStyle name="20% - Accent5 2 3" xfId="35" xr:uid="{64A1DEB4-76C7-4D7E-B183-769228520DF6}"/>
     <cellStyle name="20% - Accent5 2 3 2" xfId="90" xr:uid="{0D0D6279-2017-4898-BAD5-6B558FB10637}"/>
     <cellStyle name="20% - Accent5 2 3 2 2" xfId="195" xr:uid="{A57918F3-0541-4AE7-A008-24B794DBD6BA}"/>
     <cellStyle name="20% - Accent5 2 3 3" xfId="142" xr:uid="{84384C81-7E3B-4CED-8965-E92625ACB23F}"/>
+    <cellStyle name="20% - Accent5 2 3 4" xfId="248" xr:uid="{86D0E375-4FA4-4867-9887-F94EDB157F1D}"/>
     <cellStyle name="20% - Accent5 2 4" xfId="48" xr:uid="{B6EB5E8B-FCFF-4F4E-8AB6-E3215DFC371B}"/>
     <cellStyle name="20% - Accent5 2 4 2" xfId="103" xr:uid="{30AF541E-196B-40C1-AC50-FC8192ADC0BE}"/>
     <cellStyle name="20% - Accent5 2 4 2 2" xfId="208" xr:uid="{E1A90527-D767-4E40-A42F-1441A5209B93}"/>
     <cellStyle name="20% - Accent5 2 4 3" xfId="155" xr:uid="{C01430D9-A083-4562-BDE8-FA155F38893A}"/>
+    <cellStyle name="20% - Accent5 2 4 4" xfId="261" xr:uid="{FA80F33D-C34C-4593-8A87-7736DBA93C52}"/>
     <cellStyle name="20% - Accent5 2 5" xfId="63" xr:uid="{E4942102-333A-4347-87C5-3BB3880A6AB3}"/>
     <cellStyle name="20% - Accent5 2 5 2" xfId="169" xr:uid="{2A094B50-A181-4DC4-9E77-CC329BF5AD02}"/>
     <cellStyle name="20% - Accent5 2 6" xfId="116" xr:uid="{11144059-BF5C-47A5-906B-F54FDE629215}"/>
+    <cellStyle name="20% - Accent5 2 7" xfId="222" xr:uid="{9287B719-51C1-40AA-A757-0A8815AFB4F1}"/>
     <cellStyle name="20% - Accent5 3" xfId="11" xr:uid="{42C3DA6A-E515-4F68-9D9F-3335D19CEA18}"/>
     <cellStyle name="20% - Accent5 3 2" xfId="26" xr:uid="{7ABCF359-2591-4C83-A95F-469CD11EC77F}"/>
     <cellStyle name="20% - Accent5 3 2 2" xfId="81" xr:uid="{AE2A66F3-A94C-4BED-A4C4-1DA3B2F7359C}"/>
     <cellStyle name="20% - Accent5 3 2 2 2" xfId="186" xr:uid="{FB3BCC98-10A5-4328-8D99-ADB9FF0542A4}"/>
     <cellStyle name="20% - Accent5 3 2 3" xfId="133" xr:uid="{1B89ABCD-870A-4506-B46D-838882985AA7}"/>
+    <cellStyle name="20% - Accent5 3 2 4" xfId="239" xr:uid="{EBBF523E-5FA4-4789-B9B7-72EE40FC1392}"/>
     <cellStyle name="20% - Accent5 3 3" xfId="39" xr:uid="{A4C767C1-51C3-47D5-A74C-587D3519900C}"/>
     <cellStyle name="20% - Accent5 3 3 2" xfId="94" xr:uid="{9F2AEC89-E3E1-456E-AFAB-746F7754295C}"/>
     <cellStyle name="20% - Accent5 3 3 2 2" xfId="199" xr:uid="{33F4A8EC-24DE-486C-9439-4505BDC2142F}"/>
     <cellStyle name="20% - Accent5 3 3 3" xfId="146" xr:uid="{4A445855-314A-41F5-B200-BE580F9BF77A}"/>
+    <cellStyle name="20% - Accent5 3 3 4" xfId="252" xr:uid="{60D29DAC-E224-4284-A9E6-D79AFFF2D93D}"/>
     <cellStyle name="20% - Accent5 3 4" xfId="52" xr:uid="{C90B685B-F75D-460B-BDFC-7D7533C48C33}"/>
     <cellStyle name="20% - Accent5 3 4 2" xfId="107" xr:uid="{138EC8A5-98DD-41B5-8AEA-B3E4F6DDC91C}"/>
     <cellStyle name="20% - Accent5 3 4 2 2" xfId="212" xr:uid="{96CBC248-D81C-4E6F-93B1-59086153C386}"/>
     <cellStyle name="20% - Accent5 3 4 3" xfId="159" xr:uid="{476E5B0D-5D23-41FC-9BD9-5877E4E80DCA}"/>
+    <cellStyle name="20% - Accent5 3 4 4" xfId="265" xr:uid="{F8E1F334-0846-41DF-875A-C69D3B1AFA22}"/>
     <cellStyle name="20% - Accent5 3 5" xfId="67" xr:uid="{CB8D90FD-E342-4E4E-97ED-6566F0383DA8}"/>
     <cellStyle name="20% - Accent5 3 5 2" xfId="173" xr:uid="{2DCD6ED4-3401-42A7-ADE2-91C5ADAAD83C}"/>
     <cellStyle name="20% - Accent5 3 6" xfId="120" xr:uid="{142A7217-93B3-45E6-B2CF-A38D4C05FEF1}"/>
+    <cellStyle name="20% - Accent5 3 7" xfId="226" xr:uid="{D7C5723F-DD0D-44DE-9B51-55534C371639}"/>
     <cellStyle name="20% - Accent5 4" xfId="15" xr:uid="{DC1DD871-6B98-4E25-8BE8-6A14C839CFCF}"/>
     <cellStyle name="20% - Accent5 4 2" xfId="71" xr:uid="{8A5ADE6F-838F-4859-A40E-05FF9B5ED05F}"/>
     <cellStyle name="20% - Accent5 4 2 2" xfId="177" xr:uid="{1925C8DE-A583-4977-881C-7AA07FA5FC9E}"/>
     <cellStyle name="20% - Accent5 4 3" xfId="124" xr:uid="{FFB271F5-1793-486C-AE40-E19C3CBDBEB0}"/>
+    <cellStyle name="20% - Accent5 4 4" xfId="230" xr:uid="{FF839AF2-023B-48FC-BBDB-C3147FEC4149}"/>
     <cellStyle name="20% - Accent5 5" xfId="30" xr:uid="{0FAED7C7-EA67-4CB3-AE34-15128E10EBDD}"/>
     <cellStyle name="20% - Accent5 5 2" xfId="85" xr:uid="{FD83161D-F025-47DE-932C-C09CCF236B28}"/>
     <cellStyle name="20% - Accent5 5 2 2" xfId="190" xr:uid="{43C13AD6-900F-461F-8F95-559594527B82}"/>
     <cellStyle name="20% - Accent5 5 3" xfId="137" xr:uid="{26763EF3-AAB4-49FD-B2E9-8091E450A013}"/>
+    <cellStyle name="20% - Accent5 5 4" xfId="243" xr:uid="{B575CA75-F59C-446E-B845-17D0401EA6F0}"/>
     <cellStyle name="20% - Accent5 6" xfId="43" xr:uid="{AED42CDA-BA61-497A-9B25-6EC421F7DD74}"/>
     <cellStyle name="20% - Accent5 6 2" xfId="98" xr:uid="{D3154FDA-750D-4526-89DE-A27FA32F362A}"/>
     <cellStyle name="20% - Accent5 6 2 2" xfId="203" xr:uid="{74FAEAC9-9C79-4665-99DB-0CC3729BEA23}"/>
     <cellStyle name="20% - Accent5 6 3" xfId="150" xr:uid="{CF11A72E-A3DC-4FF7-A592-68CCAD865D3F}"/>
+    <cellStyle name="20% - Accent5 6 4" xfId="256" xr:uid="{C59E9B5B-B5A1-405D-A5B1-D542C5419CA9}"/>
     <cellStyle name="20% - Accent5 7" xfId="56" xr:uid="{DA7F47C0-FD1B-441F-935D-8AD7CC5C6E1D}"/>
     <cellStyle name="20% - Accent5 7 2" xfId="164" xr:uid="{C40728DF-3CDC-47FE-BEBE-ED23A7DBC6E2}"/>
+    <cellStyle name="20% - Accent5 8" xfId="217" xr:uid="{D8460B42-F464-4127-9199-B0659E538829}"/>
     <cellStyle name="Comma 2" xfId="5" xr:uid="{ED6C98B7-B2A1-4B47-AF8A-A39872245B39}"/>
     <cellStyle name="Comma 2 2" xfId="20" xr:uid="{B7AC5FAF-634D-41F9-85B3-9CDBB33D0333}"/>
     <cellStyle name="Comma 2 2 2" xfId="75" xr:uid="{8C001DC2-FE51-45BF-B6C7-A77CFC0D7B9C}"/>
     <cellStyle name="Comma 2 2 2 2" xfId="180" xr:uid="{2FD74F75-ACE2-478F-98C1-12834DF9A133}"/>
     <cellStyle name="Comma 2 2 3" xfId="127" xr:uid="{A447AB2E-39B0-4840-9ECB-835C36444D50}"/>
+    <cellStyle name="Comma 2 2 4" xfId="233" xr:uid="{367E2FAB-0B92-4541-8530-9CD2534184D0}"/>
     <cellStyle name="Comma 2 3" xfId="33" xr:uid="{9A5060E8-4621-4D2E-8FA3-F2C0D822E9A4}"/>
     <cellStyle name="Comma 2 3 2" xfId="88" xr:uid="{E1923561-86EC-460D-BC19-5C07AEBF1D47}"/>
     <cellStyle name="Comma 2 3 2 2" xfId="193" xr:uid="{01AFDCE0-A29E-47CE-B8CC-2ACAD8C38FC6}"/>
     <cellStyle name="Comma 2 3 3" xfId="140" xr:uid="{02FF3435-B693-406B-B6FE-F28D0C11BBD8}"/>
+    <cellStyle name="Comma 2 3 4" xfId="246" xr:uid="{40A51F9E-8A3B-4069-A2FC-7FF1E7035FF0}"/>
     <cellStyle name="Comma 2 4" xfId="46" xr:uid="{640D3F39-7ADA-41F7-A824-1BFD8996D38B}"/>
     <cellStyle name="Comma 2 4 2" xfId="101" xr:uid="{E2D14C34-0F3F-44F3-A287-3464F22C7687}"/>
     <cellStyle name="Comma 2 4 2 2" xfId="206" xr:uid="{F47C579F-3E2C-4535-A8D9-200B26DBC5DA}"/>
     <cellStyle name="Comma 2 4 3" xfId="153" xr:uid="{1F0E6A60-17A2-4114-803E-D183E9058A58}"/>
+    <cellStyle name="Comma 2 4 4" xfId="259" xr:uid="{E198A73C-A3A3-4FE5-9916-FF95DDAF50D1}"/>
     <cellStyle name="Comma 2 5" xfId="61" xr:uid="{243DF1CB-25DA-4BF4-8322-1D82C49CD531}"/>
     <cellStyle name="Comma 2 5 2" xfId="167" xr:uid="{94630E3C-0678-42AA-8F03-1265C844C8FB}"/>
     <cellStyle name="Comma 2 6" xfId="114" xr:uid="{27D0662D-D964-4C3E-948B-5A67D2F9F373}"/>
+    <cellStyle name="Comma 2 7" xfId="220" xr:uid="{B8C31877-60DA-4F7B-98A2-DA6CB5D48E08}"/>
     <cellStyle name="Comma 3" xfId="9" xr:uid="{9BBE06F6-DF43-4386-A7EA-84770CBB1110}"/>
     <cellStyle name="Comma 3 2" xfId="24" xr:uid="{AB59C64B-085D-4C79-B275-6709641D5BB7}"/>
     <cellStyle name="Comma 3 2 2" xfId="79" xr:uid="{CD323AA4-22F9-4E99-9009-6D23DBE24110}"/>
     <cellStyle name="Comma 3 2 2 2" xfId="184" xr:uid="{6BF0A02D-702E-459D-B813-A3CA51E0E1F9}"/>
     <cellStyle name="Comma 3 2 3" xfId="131" xr:uid="{F3063D94-C775-4408-BEFE-84D8981CED7C}"/>
+    <cellStyle name="Comma 3 2 4" xfId="237" xr:uid="{4C54E911-A9D8-49EF-ACA3-9C4F2676792A}"/>
     <cellStyle name="Comma 3 3" xfId="37" xr:uid="{96E677B2-1E39-47F3-B561-DD4F13597381}"/>
     <cellStyle name="Comma 3 3 2" xfId="92" xr:uid="{0339C6BC-2315-4A35-972E-9C0115061548}"/>
     <cellStyle name="Comma 3 3 2 2" xfId="197" xr:uid="{D347A85F-2F28-4CD9-B728-B92448649D10}"/>
     <cellStyle name="Comma 3 3 3" xfId="144" xr:uid="{5E8F8B59-2437-4316-8FB6-F54DA82463FD}"/>
+    <cellStyle name="Comma 3 3 4" xfId="250" xr:uid="{8CDCC416-91FB-4F12-88F7-EF7F6A04D065}"/>
     <cellStyle name="Comma 3 4" xfId="50" xr:uid="{B86C2900-CA03-40CB-895D-AA126B40D038}"/>
     <cellStyle name="Comma 3 4 2" xfId="105" xr:uid="{2F1C02E0-F632-41D5-921C-A25FF8C789F7}"/>
     <cellStyle name="Comma 3 4 2 2" xfId="210" xr:uid="{8EC804B6-67BA-44DE-9646-4BD589C60F7E}"/>
     <cellStyle name="Comma 3 4 3" xfId="157" xr:uid="{514AEA27-53F6-4C07-9438-4707B85AC645}"/>
+    <cellStyle name="Comma 3 4 4" xfId="263" xr:uid="{B85C39A4-8FC7-46F1-AC83-AD7214FBDBE8}"/>
     <cellStyle name="Comma 3 5" xfId="65" xr:uid="{7CB782F8-2A35-46DD-9621-962ECDE1F2C7}"/>
     <cellStyle name="Comma 3 5 2" xfId="171" xr:uid="{114D7B81-2D05-4116-8FEF-05B6544CFB4E}"/>
     <cellStyle name="Comma 3 6" xfId="118" xr:uid="{59AB25DC-52EB-443B-A345-EEB07344637F}"/>
+    <cellStyle name="Comma 3 7" xfId="224" xr:uid="{0E836A5E-347D-4EFC-8547-01BD7A373E7B}"/>
     <cellStyle name="Comma 4" xfId="13" xr:uid="{F10BAA2F-325D-48FE-B4DE-588412CF4783}"/>
     <cellStyle name="Comma 4 2" xfId="69" xr:uid="{B1AE5C0E-22F5-4478-9785-B9413DBF2438}"/>
     <cellStyle name="Comma 4 2 2" xfId="175" xr:uid="{C01683A5-C27C-49A6-B395-A40C00ED172A}"/>
     <cellStyle name="Comma 4 3" xfId="122" xr:uid="{F31725B9-E626-491E-AAAF-23C26A0AB515}"/>
+    <cellStyle name="Comma 4 4" xfId="228" xr:uid="{5AF6FEE8-23F9-4832-AE3D-59CFF3C1B1AE}"/>
     <cellStyle name="Comma 5" xfId="28" xr:uid="{A96DE9F5-7FB1-4FAB-B94D-B2EF920E5378}"/>
     <cellStyle name="Comma 5 2" xfId="83" xr:uid="{BBE1F8E9-1232-44B8-BCCF-1C0927C0783C}"/>
     <cellStyle name="Comma 5 2 2" xfId="188" xr:uid="{ABB0A5E4-96DC-486B-8B31-6D9601EFDE31}"/>
     <cellStyle name="Comma 5 3" xfId="135" xr:uid="{1F3E63D5-428E-400A-B0C1-16DB1C638C5B}"/>
+    <cellStyle name="Comma 5 4" xfId="241" xr:uid="{8DD008BA-5C76-4F0D-A930-83DC08C3246D}"/>
     <cellStyle name="Comma 6" xfId="41" xr:uid="{F6AC73A4-766F-41AF-8546-1BD92C1A5DC3}"/>
     <cellStyle name="Comma 6 2" xfId="96" xr:uid="{77D1E22B-1913-4AD1-A0DD-3B9445C9B943}"/>
     <cellStyle name="Comma 6 2 2" xfId="201" xr:uid="{C697C2DF-C17F-4553-B24A-957F8430F01E}"/>
     <cellStyle name="Comma 6 3" xfId="148" xr:uid="{AEC0336C-48D4-428B-AA3B-C51D96186F10}"/>
+    <cellStyle name="Comma 6 4" xfId="254" xr:uid="{1F322274-4276-4087-A861-CD3B4298D698}"/>
     <cellStyle name="Comma 7" xfId="54" xr:uid="{94DEC19E-A6A7-4788-812E-6C5318BF22E8}"/>
     <cellStyle name="Comma 7 2" xfId="162" xr:uid="{F18459FC-7540-4004-ADA7-32E985107525}"/>
+    <cellStyle name="Comma 7 3" xfId="268" xr:uid="{1F58F8A6-C1A1-4A5C-874F-A0EF4EE2D86B}"/>
     <cellStyle name="Comma 8" xfId="110" xr:uid="{CE5F3CAC-02ED-403F-8BDB-50BCB276743E}"/>
+    <cellStyle name="Comma 9" xfId="215" xr:uid="{28FD967D-9FF9-4ACA-B55C-DBB68C4E278B}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="53" xr:uid="{8BBE64AA-0071-44B5-A766-DD878DA19F08}"/>
     <cellStyle name="Normal 10 2" xfId="161" xr:uid="{53431DF4-F434-4E58-8B64-6ACB4079A7DF}"/>
+    <cellStyle name="Normal 10 3" xfId="267" xr:uid="{DEA5C9D2-B36F-413A-8C23-8EA0CB44A0D7}"/>
     <cellStyle name="Normal 11" xfId="160" xr:uid="{06F42D7C-516D-4DB0-A9FE-B6423B71AAD8}"/>
+    <cellStyle name="Normal 11 2" xfId="266" xr:uid="{A5603D19-1341-4BE7-95D8-3783290EB46E}"/>
     <cellStyle name="Normal 12" xfId="109" xr:uid="{A0DDEDD4-62D6-4BB4-9F38-7DB5B8015081}"/>
     <cellStyle name="Normal 13" xfId="108" xr:uid="{FA5BC1D4-F714-4C97-B6A6-8886159FB69C}"/>
     <cellStyle name="Normal 13 2" xfId="213" xr:uid="{3F198362-F8B7-4613-B058-8756CBD31E94}"/>
+    <cellStyle name="Normal 14" xfId="214" xr:uid="{545AC839-A1E7-434C-82E6-6C89551CDECD}"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{4F4ED162-C45F-4637-99B9-0DC288E0E26C}"/>
     <cellStyle name="Normal 2 2" xfId="18" xr:uid="{73520720-7CC8-4636-BEA4-4BA7AD8E3294}"/>
     <cellStyle name="Normal 2 2 2" xfId="73" xr:uid="{2CD71C79-1AA4-45A0-9788-9D2D6FAD34B2}"/>
     <cellStyle name="Normal 2 2 2 2" xfId="178" xr:uid="{7E7CE0F8-BE26-4F38-923F-700901A1DA6B}"/>
     <cellStyle name="Normal 2 2 3" xfId="125" xr:uid="{2AFC3B25-5274-4BE5-AF40-AFB32CA2152A}"/>
+    <cellStyle name="Normal 2 2 4" xfId="231" xr:uid="{F78140EA-9ADE-420C-AB1C-C2239AEDAEC5}"/>
     <cellStyle name="Normal 2 3" xfId="31" xr:uid="{3DE8F047-C232-4A35-B429-F0537449F260}"/>
     <cellStyle name="Normal 2 3 2" xfId="86" xr:uid="{11AAA4BB-E8A9-4185-ADFA-83841C071238}"/>
     <cellStyle name="Normal 2 3 2 2" xfId="191" xr:uid="{555E5143-5542-4F10-93AC-675A424DF628}"/>
     <cellStyle name="Normal 2 3 3" xfId="138" xr:uid="{CD3C54C7-74E6-4120-BC63-E077FD94C7F1}"/>
+    <cellStyle name="Normal 2 3 4" xfId="244" xr:uid="{66544081-7B2A-4F95-AC72-AA4A29F10EBA}"/>
     <cellStyle name="Normal 2 4" xfId="44" xr:uid="{4FF9CFE9-7E21-4A6B-A29A-1180095F3394}"/>
     <cellStyle name="Normal 2 4 2" xfId="99" xr:uid="{3320B5F5-33BD-4D66-8320-92478374F742}"/>
     <cellStyle name="Normal 2 4 2 2" xfId="204" xr:uid="{EFF28F27-780E-499A-944A-DD50FE742FB2}"/>
     <cellStyle name="Normal 2 4 3" xfId="151" xr:uid="{14701181-5D67-48F7-89EE-2E5A66EAD732}"/>
+    <cellStyle name="Normal 2 4 4" xfId="257" xr:uid="{B62AA6B2-D417-410D-A713-B353CE019A62}"/>
     <cellStyle name="Normal 2 5" xfId="59" xr:uid="{82B1CADE-454F-41BD-B69C-1C727AEACFA4}"/>
     <cellStyle name="Normal 2 5 2" xfId="165" xr:uid="{AD3B439E-CA24-47F2-9D4B-3B06FC8B5FC2}"/>
     <cellStyle name="Normal 2 6" xfId="112" xr:uid="{BCA5A7C5-CA87-43C5-B301-853508413108}"/>
+    <cellStyle name="Normal 2 7" xfId="218" xr:uid="{73D7A759-A024-4A63-BB0D-FAAE8D8C0C13}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{6F56F0E9-E05C-4C30-B878-F9B9EA162652}"/>
     <cellStyle name="Normal 3 2" xfId="19" xr:uid="{A32771C3-61B9-4017-BCB7-A8447F558936}"/>
     <cellStyle name="Normal 3 2 2" xfId="74" xr:uid="{EB3EB93F-B77D-4BA5-9B37-4507D01FE212}"/>
     <cellStyle name="Normal 3 2 2 2" xfId="179" xr:uid="{693168B0-96BE-47F2-B453-4306E6AE7CE8}"/>
     <cellStyle name="Normal 3 2 3" xfId="126" xr:uid="{61161275-A351-4B23-8415-F39367DD8024}"/>
+    <cellStyle name="Normal 3 2 4" xfId="232" xr:uid="{569549EB-D286-459D-8093-9FD926AB2902}"/>
     <cellStyle name="Normal 3 3" xfId="32" xr:uid="{6D6D7D4C-E015-466A-A2A9-35851197F9B9}"/>
     <cellStyle name="Normal 3 3 2" xfId="87" xr:uid="{A09B1EDC-BC53-4A84-8A09-CD2B3E72AB92}"/>
     <cellStyle name="Normal 3 3 2 2" xfId="192" xr:uid="{09930C38-6C2B-4EF3-9187-539467ADB60B}"/>
     <cellStyle name="Normal 3 3 3" xfId="139" xr:uid="{D3BD1A57-CC9D-4CDF-A3B5-01F1AF1FC06F}"/>
+    <cellStyle name="Normal 3 3 4" xfId="245" xr:uid="{FF50D7D0-02DF-431D-911D-855E0B846B2B}"/>
     <cellStyle name="Normal 3 4" xfId="45" xr:uid="{3F2C4675-A6B6-4303-ADF3-7F5FDBCC1201}"/>
     <cellStyle name="Normal 3 4 2" xfId="100" xr:uid="{52A0E527-D628-412E-933C-8E8D41704332}"/>
     <cellStyle name="Normal 3 4 2 2" xfId="205" xr:uid="{9F36FAE0-1145-4DB4-ADC6-CB3DE2BEEE9F}"/>
     <cellStyle name="Normal 3 4 3" xfId="152" xr:uid="{795989F9-BCAF-47BD-8728-F8406BAF9D65}"/>
+    <cellStyle name="Normal 3 4 4" xfId="258" xr:uid="{08F717B3-FBD9-4790-8F4A-67CB09B4ADA4}"/>
     <cellStyle name="Normal 3 5" xfId="60" xr:uid="{3B4793EE-2556-4444-B5B4-4962FF9A0B3A}"/>
     <cellStyle name="Normal 3 5 2" xfId="166" xr:uid="{9A7B49F9-AB24-48A9-BF78-AC2ED43283A3}"/>
     <cellStyle name="Normal 3 6" xfId="113" xr:uid="{1B5B4019-2C60-4C1C-9403-E6C70EA177AB}"/>
+    <cellStyle name="Normal 3 7" xfId="219" xr:uid="{6C1DC434-74EF-40B6-A373-F77BE75535E1}"/>
     <cellStyle name="Normal 4" xfId="8" xr:uid="{E0019DBD-0F4A-4352-B357-025C5C0BFAEC}"/>
     <cellStyle name="Normal 4 2" xfId="23" xr:uid="{10393A82-218B-43FD-AA73-2D1C9788B975}"/>
     <cellStyle name="Normal 4 2 2" xfId="78" xr:uid="{518A0805-EFF6-4BCF-A4BB-CAAB7F8F705D}"/>
     <cellStyle name="Normal 4 2 2 2" xfId="183" xr:uid="{D62E6486-14CF-4FFD-9272-A8B3325C08A5}"/>
     <cellStyle name="Normal 4 2 3" xfId="130" xr:uid="{2C009DF5-CBF1-4F94-90D7-738B2088C271}"/>
+    <cellStyle name="Normal 4 2 4" xfId="236" xr:uid="{708BF027-E485-4D55-A7B1-77981C64D475}"/>
     <cellStyle name="Normal 4 3" xfId="36" xr:uid="{62A12A76-EC25-4B9B-9DE7-60E39637AA4D}"/>
     <cellStyle name="Normal 4 3 2" xfId="91" xr:uid="{EC7D6496-983A-4947-B588-F58C77B67828}"/>
     <cellStyle name="Normal 4 3 2 2" xfId="196" xr:uid="{8A9F63B9-F301-4EFC-A27E-C4C6DBAD14B2}"/>
     <cellStyle name="Normal 4 3 3" xfId="143" xr:uid="{A209E494-1E57-4511-9967-C6BB4CB69798}"/>
+    <cellStyle name="Normal 4 3 4" xfId="249" xr:uid="{FA30BEB4-615C-450A-B9B8-F12D0CF2FCE8}"/>
     <cellStyle name="Normal 4 4" xfId="49" xr:uid="{0D81F105-5652-4284-861E-275768C81364}"/>
     <cellStyle name="Normal 4 4 2" xfId="104" xr:uid="{2ED90C63-2832-484C-8BE6-4FE320068DCF}"/>
     <cellStyle name="Normal 4 4 2 2" xfId="209" xr:uid="{DBBD8277-5ED3-406B-B252-BBC562C99C8F}"/>
     <cellStyle name="Normal 4 4 3" xfId="156" xr:uid="{77BBDA96-C1B4-488B-A294-0EDF35D9022C}"/>
+    <cellStyle name="Normal 4 4 4" xfId="262" xr:uid="{AFDEC5B6-57BB-445D-B4A7-6A9EE4329688}"/>
     <cellStyle name="Normal 4 5" xfId="64" xr:uid="{C01B067D-10D4-4312-A991-9BB0541632E1}"/>
     <cellStyle name="Normal 4 5 2" xfId="170" xr:uid="{216A4D32-F34F-4D2E-9FAA-2ED46145C0B4}"/>
     <cellStyle name="Normal 4 6" xfId="117" xr:uid="{48E6E147-FC1F-4C0C-8FE7-982FD956AD07}"/>
+    <cellStyle name="Normal 4 7" xfId="223" xr:uid="{253636F2-12A7-4675-A469-245A845E4595}"/>
     <cellStyle name="Normal 5" xfId="16" xr:uid="{49545144-F3A9-4825-A6BA-5936F162C050}"/>
     <cellStyle name="Normal 5 2" xfId="72" xr:uid="{ADCDC5E4-A063-457A-A471-FEB0D7FB14D2}"/>
     <cellStyle name="Normal 6" xfId="12" xr:uid="{4EF6E554-0085-465F-A330-E88543107D27}"/>
     <cellStyle name="Normal 6 2" xfId="68" xr:uid="{16F122DE-5D56-4A1B-BB1C-A9AD62F8B2A1}"/>
     <cellStyle name="Normal 6 2 2" xfId="174" xr:uid="{5CBC1DAA-AC29-4F13-9168-80B81077ABF7}"/>
     <cellStyle name="Normal 6 3" xfId="121" xr:uid="{D2A38596-2B9B-4FFC-9085-3A9557F73DB5}"/>
+    <cellStyle name="Normal 6 4" xfId="227" xr:uid="{88F7DA31-5BC1-4B4C-8D25-C558B012D626}"/>
     <cellStyle name="Normal 7" xfId="27" xr:uid="{2534D22A-6169-4D9A-B012-B7294C0AC758}"/>
     <cellStyle name="Normal 7 2" xfId="82" xr:uid="{A89A0637-FCF4-4BBE-973F-383CEA45A07D}"/>
     <cellStyle name="Normal 7 2 2" xfId="187" xr:uid="{54FCB699-B6CD-4B8E-B5C7-29F0EA489663}"/>
     <cellStyle name="Normal 7 3" xfId="134" xr:uid="{C1422B8C-C674-46F0-AB09-B49D4057DCEA}"/>
+    <cellStyle name="Normal 7 4" xfId="240" xr:uid="{DA7AAFC3-BCA2-43FA-9DD1-E78DA2644532}"/>
     <cellStyle name="Normal 8" xfId="40" xr:uid="{19F067A3-D80D-48FD-BF06-BF292EC8BB24}"/>
     <cellStyle name="Normal 8 2" xfId="95" xr:uid="{7AC36C7D-8CC4-4325-8C2B-FA3C713B7CF5}"/>
     <cellStyle name="Normal 8 2 2" xfId="200" xr:uid="{6C397B7D-6E90-4109-A1F7-15EA72BFFF46}"/>
     <cellStyle name="Normal 8 3" xfId="147" xr:uid="{9D1787CE-1718-4788-B651-58825DA7D955}"/>
+    <cellStyle name="Normal 8 4" xfId="253" xr:uid="{CC292DD9-883A-4975-B4C2-06D126A667E0}"/>
     <cellStyle name="Normal 9" xfId="57" xr:uid="{CC04280B-7E40-41C0-B008-E89A699DBC6E}"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
     <cellStyle name="Percent 10" xfId="111" xr:uid="{1F4F8886-BC30-46CB-A926-4376A9109BBF}"/>
+    <cellStyle name="Percent 11" xfId="216" xr:uid="{20B0FEC6-3B8E-4377-885D-2C9836F5717F}"/>
     <cellStyle name="Percent 2" xfId="6" xr:uid="{BC0C5A78-644A-4E8A-8133-E61F2E94C271}"/>
     <cellStyle name="Percent 2 2" xfId="21" xr:uid="{ABEFFD90-1C5B-44F4-94F2-8F5C545B6CE3}"/>
     <cellStyle name="Percent 2 2 2" xfId="76" xr:uid="{3BD6292D-5384-4692-B5F6-884298F64563}"/>
     <cellStyle name="Percent 2 2 2 2" xfId="181" xr:uid="{46C8F6F1-24D5-4168-8158-FC0E4886AC1D}"/>
     <cellStyle name="Percent 2 2 3" xfId="128" xr:uid="{36EE822D-4B3E-44B1-B029-B8B78867EF7A}"/>
+    <cellStyle name="Percent 2 2 4" xfId="234" xr:uid="{0CA13914-BAF3-4AA0-85F3-7568A4EEEEE2}"/>
     <cellStyle name="Percent 2 3" xfId="34" xr:uid="{F1235FEE-D3ED-46E3-8284-249567537760}"/>
     <cellStyle name="Percent 2 3 2" xfId="89" xr:uid="{243A6ED9-AAFA-49A8-9C9D-1F9201E74EE5}"/>
     <cellStyle name="Percent 2 3 2 2" xfId="194" xr:uid="{43806F43-EF60-4BA2-92C0-5EFD1054D0EB}"/>
     <cellStyle name="Percent 2 3 3" xfId="141" xr:uid="{671C13B9-D85F-49B6-8210-22AFF3720429}"/>
+    <cellStyle name="Percent 2 3 4" xfId="247" xr:uid="{8BC2E223-46D9-427D-9BFD-11DD52F74FCA}"/>
     <cellStyle name="Percent 2 4" xfId="47" xr:uid="{9B5DB1B9-289D-4910-A43A-3BB8D718BF50}"/>
     <cellStyle name="Percent 2 4 2" xfId="102" xr:uid="{72EADBC2-7F91-4039-B221-1AF9C08D12D9}"/>
     <cellStyle name="Percent 2 4 2 2" xfId="207" xr:uid="{5AFE4152-FEC5-49A0-9D8D-D5FDA1723B5A}"/>
     <cellStyle name="Percent 2 4 3" xfId="154" xr:uid="{A4294857-D78B-4B2B-8455-A9A7CCA9968E}"/>
+    <cellStyle name="Percent 2 4 4" xfId="260" xr:uid="{D849EB05-FC46-4181-9A00-C16740BD46E4}"/>
     <cellStyle name="Percent 2 5" xfId="62" xr:uid="{99781A41-93CF-4EB0-92D0-C5CD68D53132}"/>
     <cellStyle name="Percent 2 5 2" xfId="168" xr:uid="{433B7183-9537-4B65-A460-0F8F04644F1F}"/>
     <cellStyle name="Percent 2 6" xfId="115" xr:uid="{AB1C876A-61E7-4015-A43C-086187C228D5}"/>
+    <cellStyle name="Percent 2 7" xfId="221" xr:uid="{9917628B-F1B8-45F8-9822-519C060E47DD}"/>
     <cellStyle name="Percent 3" xfId="10" xr:uid="{5A577D97-9D8D-44CD-94BE-F7C4D5E216D4}"/>
     <cellStyle name="Percent 3 2" xfId="25" xr:uid="{AA877386-D0A2-4CA8-9066-CA902896BC86}"/>
     <cellStyle name="Percent 3 2 2" xfId="80" xr:uid="{A88F4B8E-3D7E-46C4-935F-75A2D1DC2F86}"/>
     <cellStyle name="Percent 3 2 2 2" xfId="185" xr:uid="{AA51F800-E197-4EBD-A00E-5ED6D281A99C}"/>
     <cellStyle name="Percent 3 2 3" xfId="132" xr:uid="{AD596E79-6618-4E8C-9AAE-C8188B1A7654}"/>
+    <cellStyle name="Percent 3 2 4" xfId="238" xr:uid="{6A791A4E-30E7-4DAF-80A4-30B07C71C12D}"/>
     <cellStyle name="Percent 3 3" xfId="38" xr:uid="{2C62A5E3-4F5C-4053-B9EE-104D29570544}"/>
     <cellStyle name="Percent 3 3 2" xfId="93" xr:uid="{84DDFECE-69E2-4B0E-A09E-659E48A24F42}"/>
     <cellStyle name="Percent 3 3 2 2" xfId="198" xr:uid="{D5138662-9B50-4909-B103-A9540759A334}"/>
     <cellStyle name="Percent 3 3 3" xfId="145" xr:uid="{DB58C7EC-334E-4AE6-B68E-D68247DB256A}"/>
+    <cellStyle name="Percent 3 3 4" xfId="251" xr:uid="{A12609E8-0A12-4AAD-8254-DA8E3F899CF6}"/>
     <cellStyle name="Percent 3 4" xfId="51" xr:uid="{71214003-4755-4936-B69C-71301425DFDB}"/>
     <cellStyle name="Percent 3 4 2" xfId="106" xr:uid="{C8250550-A077-468C-AEF8-166BFF71412B}"/>
     <cellStyle name="Percent 3 4 2 2" xfId="211" xr:uid="{6BCEDAED-9BA6-48C4-98D1-B239A2FBFB06}"/>
     <cellStyle name="Percent 3 4 3" xfId="158" xr:uid="{E9A8A10A-09C4-40C8-8279-A039F46E57ED}"/>
+    <cellStyle name="Percent 3 4 4" xfId="264" xr:uid="{69803DEE-6772-497F-98FE-6555CE87CCB3}"/>
     <cellStyle name="Percent 3 5" xfId="66" xr:uid="{90D550B4-A467-4B1F-8791-783C947825CE}"/>
     <cellStyle name="Percent 3 5 2" xfId="172" xr:uid="{50881C98-C99E-4650-827C-766929596D85}"/>
     <cellStyle name="Percent 3 6" xfId="119" xr:uid="{52DB9A23-2753-48D6-90A2-C68B5942AD40}"/>
+    <cellStyle name="Percent 3 7" xfId="225" xr:uid="{9191CB26-0C88-4F1E-9E3D-2BE3D92646F8}"/>
     <cellStyle name="Percent 4" xfId="17" xr:uid="{766E512C-159B-4546-AE75-4E591D8E346F}"/>
     <cellStyle name="Percent 5" xfId="14" xr:uid="{761C96E9-6829-47E8-ABEF-BAFE0B7B7D1A}"/>
     <cellStyle name="Percent 5 2" xfId="70" xr:uid="{3753DDE5-24BA-4D95-9E8F-1428A4C09B68}"/>
     <cellStyle name="Percent 5 2 2" xfId="176" xr:uid="{C789F3EB-F70E-407F-B666-32BF7BA046C9}"/>
     <cellStyle name="Percent 5 3" xfId="123" xr:uid="{30D8A2A0-D19C-4CB4-A9B2-F1A31449CDBF}"/>
+    <cellStyle name="Percent 5 4" xfId="229" xr:uid="{264F99D8-879C-433A-B678-4BDB3137D58B}"/>
     <cellStyle name="Percent 6" xfId="29" xr:uid="{3C9E2FB6-4013-4108-851E-44B42960E338}"/>
     <cellStyle name="Percent 6 2" xfId="84" xr:uid="{A9529AA1-C733-45A5-9A59-8E9A9D926271}"/>
     <cellStyle name="Percent 6 2 2" xfId="189" xr:uid="{DCA23980-98AC-43CA-941E-9708457EFE2C}"/>
     <cellStyle name="Percent 6 3" xfId="136" xr:uid="{EABCDA63-DFA2-47E3-B194-D18A8290ED26}"/>
+    <cellStyle name="Percent 6 4" xfId="242" xr:uid="{BF05A554-C9DA-4EDB-8DB8-0DF36B087CE2}"/>
     <cellStyle name="Percent 7" xfId="42" xr:uid="{E615D24B-233E-4FC3-8466-3E474BB7156C}"/>
     <cellStyle name="Percent 7 2" xfId="97" xr:uid="{C8975516-84DD-418A-B968-A1AE0DCED118}"/>
     <cellStyle name="Percent 7 2 2" xfId="202" xr:uid="{B240505D-1F90-4AB5-9ECC-FDF506CBA6F0}"/>
     <cellStyle name="Percent 7 3" xfId="149" xr:uid="{C16F36D8-1935-485F-A488-481927ED7425}"/>
+    <cellStyle name="Percent 7 4" xfId="255" xr:uid="{B366D0BE-EE6A-4940-AA7E-7AEEA6EF2312}"/>
     <cellStyle name="Percent 8" xfId="58" xr:uid="{DAF5A91A-7863-44B8-B357-3AAC899BD8B2}"/>
     <cellStyle name="Percent 9" xfId="55" xr:uid="{05B3DA8B-8D4B-4546-93F0-A0F74AD24A02}"/>
     <cellStyle name="Percent 9 2" xfId="163" xr:uid="{DE2C4031-335C-4ED2-9DB3-04920DD9A697}"/>
+    <cellStyle name="Percent 9 3" xfId="269" xr:uid="{7BB585CD-A1EF-4BBB-B700-8A33B7BBB134}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -4273,7 +4394,7 @@
   <mergeCells count="1">
     <mergeCell ref="B38:C38"/>
   </mergeCells>
-  <phoneticPr fontId="13" type="noConversion"/>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4283,8 +4404,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B3:AF298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D86" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="O88" sqref="O88"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="R116" sqref="R116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6445,6 +6566,7 @@
       <c r="T102" s="1">
         <v>1E-3</v>
       </c>
+      <c r="V102" s="1"/>
       <c r="W102" s="1"/>
       <c r="X102" s="1"/>
       <c r="Y102" s="1"/>
@@ -6528,7 +6650,7 @@
         <v>1.0145072391774981</v>
       </c>
       <c r="Q104" s="48">
-        <v>20.617000000000001</v>
+        <v>12.82</v>
       </c>
       <c r="R104" s="48">
         <v>1.49</v>
@@ -6539,6 +6661,9 @@
       <c r="T104" s="1">
         <v>1E-3</v>
       </c>
+      <c r="V104" s="1"/>
+      <c r="W104" s="1"/>
+      <c r="X104" s="1"/>
     </row>
     <row r="105" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B105" s="1" t="str">
@@ -6595,8 +6720,7 @@
         <v>1.0915793541378127</v>
       </c>
       <c r="Q105" s="48">
-        <f>Q104</f>
-        <v>20.617000000000001</v>
+        <v>20.62</v>
       </c>
       <c r="R105" s="48">
         <v>1.49</v>
@@ -6607,6 +6731,9 @@
       <c r="T105" s="1">
         <v>1E-3</v>
       </c>
+      <c r="V105" s="1"/>
+      <c r="W105" s="1"/>
+      <c r="X105" s="1"/>
     </row>
     <row r="106" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B106" s="1" t="str">
@@ -6660,8 +6787,8 @@
         <v>1.0915793541378127</v>
       </c>
       <c r="Q106" s="48">
-        <f t="shared" ref="Q106:Q122" si="3">Q105</f>
-        <v>20.617000000000001</v>
+        <f>20.62</f>
+        <v>20.62</v>
       </c>
       <c r="R106" s="48">
         <v>1.49</v>
@@ -6672,6 +6799,9 @@
       <c r="T106" s="1">
         <v>1E-3</v>
       </c>
+      <c r="V106" s="1"/>
+      <c r="W106" s="1"/>
+      <c r="X106" s="1"/>
     </row>
     <row r="107" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B107" s="1" t="str">
@@ -6725,8 +6855,7 @@
         <v>1.2315500000000001</v>
       </c>
       <c r="Q107" s="48">
-        <f t="shared" si="3"/>
-        <v>20.617000000000001</v>
+        <v>12.82</v>
       </c>
       <c r="R107" s="48">
         <v>1.49</v>
@@ -6737,6 +6866,9 @@
       <c r="T107" s="1">
         <v>1E-3</v>
       </c>
+      <c r="V107" s="1"/>
+      <c r="W107" s="1"/>
+      <c r="X107" s="1"/>
     </row>
     <row r="108" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B108" s="1" t="str">
@@ -6790,8 +6922,7 @@
         <v>1.0145072391774981</v>
       </c>
       <c r="Q108" s="48">
-        <f t="shared" si="3"/>
-        <v>20.617000000000001</v>
+        <v>12.82</v>
       </c>
       <c r="R108" s="48">
         <v>1.49</v>
@@ -6802,6 +6933,9 @@
       <c r="T108" s="1">
         <v>1E-3</v>
       </c>
+      <c r="V108" s="1"/>
+      <c r="W108" s="1"/>
+      <c r="X108" s="1"/>
     </row>
     <row r="109" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B109" s="1" t="str">
@@ -6855,8 +6989,8 @@
         <v>1.0915793541378127</v>
       </c>
       <c r="Q109" s="48">
-        <f t="shared" si="3"/>
-        <v>20.617000000000001</v>
+        <f>Q106</f>
+        <v>20.62</v>
       </c>
       <c r="R109" s="48">
         <v>1.49</v>
@@ -6867,6 +7001,9 @@
       <c r="T109" s="1">
         <v>1E-3</v>
       </c>
+      <c r="V109" s="1"/>
+      <c r="W109" s="1"/>
+      <c r="X109" s="1"/>
     </row>
     <row r="110" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B110" s="1" t="str">
@@ -6920,8 +7057,8 @@
         <v>1.13845</v>
       </c>
       <c r="Q110" s="48">
-        <f t="shared" si="3"/>
-        <v>20.617000000000001</v>
+        <f>Q106</f>
+        <v>20.62</v>
       </c>
       <c r="R110" s="48">
         <v>1.49</v>
@@ -6932,6 +7069,9 @@
       <c r="T110" s="1">
         <v>1E-3</v>
       </c>
+      <c r="V110" s="1"/>
+      <c r="W110" s="1"/>
+      <c r="X110" s="1"/>
     </row>
     <row r="111" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B111" s="1" t="str">
@@ -6985,8 +7125,8 @@
         <v>1.22845</v>
       </c>
       <c r="Q111" s="48">
-        <f t="shared" si="3"/>
-        <v>20.617000000000001</v>
+        <f>Q110</f>
+        <v>20.62</v>
       </c>
       <c r="R111" s="48">
         <v>1.49</v>
@@ -6997,6 +7137,9 @@
       <c r="T111" s="1">
         <v>1E-3</v>
       </c>
+      <c r="V111" s="1"/>
+      <c r="W111" s="1"/>
+      <c r="X111" s="1"/>
     </row>
     <row r="112" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B112" s="1" t="str">
@@ -7050,8 +7193,8 @@
         <v>1.2685500000000003</v>
       </c>
       <c r="Q112" s="48">
-        <f t="shared" si="3"/>
-        <v>20.617000000000001</v>
+        <f>Q104</f>
+        <v>12.82</v>
       </c>
       <c r="R112" s="48">
         <v>1.49</v>
@@ -7062,8 +7205,11 @@
       <c r="T112" s="1">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="113" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="V112" s="1"/>
+      <c r="W112" s="1"/>
+      <c r="X112" s="1"/>
+    </row>
+    <row r="113" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B113" s="1" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-PHEV20_GSL21</v>
@@ -7115,8 +7261,8 @@
         <v>1.2685500000000003</v>
       </c>
       <c r="Q113" s="48">
-        <f t="shared" si="3"/>
-        <v>20.617000000000001</v>
+        <f>AVERAGE(Q112,Q114)</f>
+        <v>16.72</v>
       </c>
       <c r="R113" s="48">
         <v>1.49</v>
@@ -7127,8 +7273,11 @@
       <c r="T113" s="1">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="114" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="V113" s="1"/>
+      <c r="W113" s="1"/>
+      <c r="X113" s="1"/>
+    </row>
+    <row r="114" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B114" s="1" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-PHEV40_GSL21</v>
@@ -7180,8 +7329,8 @@
         <v>1.2685500000000003</v>
       </c>
       <c r="Q114" s="48">
-        <f t="shared" si="3"/>
-        <v>20.617000000000001</v>
+        <f>Q105</f>
+        <v>20.62</v>
       </c>
       <c r="R114" s="48">
         <v>1.49</v>
@@ -7192,8 +7341,11 @@
       <c r="T114" s="1">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="115" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="V114" s="1"/>
+      <c r="W114" s="1"/>
+      <c r="X114" s="1"/>
+    </row>
+    <row r="115" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B115" s="1" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-PHEV10_DST21</v>
@@ -7245,8 +7397,8 @@
         <v>1.3688500000000001</v>
       </c>
       <c r="Q115" s="48">
-        <f t="shared" si="3"/>
-        <v>20.617000000000001</v>
+        <f>Q112</f>
+        <v>12.82</v>
       </c>
       <c r="R115" s="48">
         <v>1.49</v>
@@ -7257,8 +7409,11 @@
       <c r="T115" s="1">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="116" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="V115" s="1"/>
+      <c r="W115" s="1"/>
+      <c r="X115" s="1"/>
+    </row>
+    <row r="116" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B116" s="1" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-PHEV20_DST21</v>
@@ -7310,8 +7465,8 @@
         <v>1.3688500000000001</v>
       </c>
       <c r="Q116" s="48">
-        <f t="shared" si="3"/>
-        <v>20.617000000000001</v>
+        <f t="shared" ref="Q116:Q117" si="3">Q113</f>
+        <v>16.72</v>
       </c>
       <c r="R116" s="48">
         <v>1.49</v>
@@ -7322,8 +7477,11 @@
       <c r="T116" s="1">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="117" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="V116" s="1"/>
+      <c r="W116" s="1"/>
+      <c r="X116" s="1"/>
+    </row>
+    <row r="117" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B117" s="1" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-PHEV40_DST21</v>
@@ -7376,7 +7534,7 @@
       </c>
       <c r="Q117" s="48">
         <f t="shared" si="3"/>
-        <v>20.617000000000001</v>
+        <v>20.62</v>
       </c>
       <c r="R117" s="48">
         <v>1.49</v>
@@ -7387,8 +7545,11 @@
       <c r="T117" s="1">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="118" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="V117" s="1"/>
+      <c r="W117" s="1"/>
+      <c r="X117" s="1"/>
+    </row>
+    <row r="118" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B118" s="1" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-BEV100_ELC21</v>
@@ -7440,8 +7601,8 @@
         <v>1.2323000000000002</v>
       </c>
       <c r="Q118" s="48">
-        <f t="shared" si="3"/>
-        <v>20.617000000000001</v>
+        <f>Q115</f>
+        <v>12.82</v>
       </c>
       <c r="R118" s="48">
         <v>1.49</v>
@@ -7452,8 +7613,11 @@
       <c r="T118" s="1">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="119" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="V118" s="1"/>
+      <c r="W118" s="1"/>
+      <c r="X118" s="1"/>
+    </row>
+    <row r="119" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B119" s="1" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-BEV150_ELC21</v>
@@ -7505,8 +7669,8 @@
         <v>1.2323000000000002</v>
       </c>
       <c r="Q119" s="48">
-        <f t="shared" si="3"/>
-        <v>20.617000000000001</v>
+        <f t="shared" ref="Q119:Q120" si="4">Q116</f>
+        <v>16.72</v>
       </c>
       <c r="R119" s="48">
         <v>1.49</v>
@@ -7517,8 +7681,11 @@
       <c r="T119" s="1">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="120" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="V119" s="1"/>
+      <c r="W119" s="1"/>
+      <c r="X119" s="1"/>
+    </row>
+    <row r="120" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B120" s="1" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-BEV250_ELC21</v>
@@ -7570,8 +7737,8 @@
         <v>1.2323000000000002</v>
       </c>
       <c r="Q120" s="48">
-        <f t="shared" si="3"/>
-        <v>20.617000000000001</v>
+        <f t="shared" si="4"/>
+        <v>20.62</v>
       </c>
       <c r="R120" s="48">
         <v>1.49</v>
@@ -7582,8 +7749,11 @@
       <c r="T120" s="1">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="121" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="V120" s="1"/>
+      <c r="W120" s="1"/>
+      <c r="X120" s="1"/>
+    </row>
+    <row r="121" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B121" s="1" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-ICE_HYD21</v>
@@ -7635,8 +7805,8 @@
         <v>1.2398000000000002</v>
       </c>
       <c r="Q121" s="48">
-        <f t="shared" si="3"/>
-        <v>20.617000000000001</v>
+        <f>Q106</f>
+        <v>20.62</v>
       </c>
       <c r="R121" s="48">
         <v>1.49</v>
@@ -7647,8 +7817,11 @@
       <c r="T121" s="1">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="122" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="V121" s="1"/>
+      <c r="W121" s="1"/>
+      <c r="X121" s="1"/>
+    </row>
+    <row r="122" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B122" s="1" t="str">
         <f t="shared" si="0"/>
         <v>T-CAR-FCV_HYD21</v>
@@ -7700,8 +7873,8 @@
         <v>1.2398000000000002</v>
       </c>
       <c r="Q122" s="48">
-        <f t="shared" si="3"/>
-        <v>20.617000000000001</v>
+        <f>Q106</f>
+        <v>20.62</v>
       </c>
       <c r="R122" s="48">
         <v>1.49</v>
@@ -7712,8 +7885,11 @@
       <c r="T122" s="1">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="123" spans="2:20" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="V122" s="1"/>
+      <c r="W122" s="1"/>
+      <c r="X122" s="1"/>
+    </row>
+    <row r="123" spans="2:24" s="1" customFormat="1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B123" s="27" t="s">
         <v>115</v>
       </c>
@@ -7736,9 +7912,9 @@
       <c r="S123" s="27"/>
       <c r="T123" s="27"/>
     </row>
-    <row r="124" spans="2:20" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B124" s="1" t="str">
-        <f t="shared" ref="B124:B142" si="4">D30</f>
+        <f t="shared" ref="B124:B142" si="5">D30</f>
         <v>T-TAX-ICE_GSL31</v>
       </c>
       <c r="C124" s="1" t="str">
@@ -7799,10 +7975,13 @@
       <c r="T124" s="1">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="125" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="V124" s="1"/>
+      <c r="W124" s="1"/>
+      <c r="X124" s="1"/>
+    </row>
+    <row r="125" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B125" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>T-TAX-ICE_DST31</v>
       </c>
       <c r="C125" s="1" t="str">
@@ -7829,7 +8008,7 @@
         <v>21.831587082756254</v>
       </c>
       <c r="J125" s="48">
-        <f t="shared" ref="J125:J142" si="5">AVERAGE(I125,K125)</f>
+        <f t="shared" ref="J125:J142" si="6">AVERAGE(I125,K125)</f>
         <v>21.831587082756254</v>
       </c>
       <c r="K125" s="48">
@@ -7864,10 +8043,13 @@
       <c r="T125" s="1">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="126" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="V125" s="1"/>
+      <c r="W125" s="1"/>
+      <c r="X125" s="1"/>
+    </row>
+    <row r="126" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B126" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>T-TAX-ICE_DF31</v>
       </c>
       <c r="C126" s="1" t="str">
@@ -7894,7 +8076,7 @@
         <v>21.831587082756254</v>
       </c>
       <c r="J126" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>21.831587082756254</v>
       </c>
       <c r="K126" s="48">
@@ -7917,7 +8099,7 @@
         <v>1.0915793541378127</v>
       </c>
       <c r="Q126" s="48">
-        <f t="shared" ref="Q126:Q142" si="6">Q125</f>
+        <f t="shared" ref="Q126:Q142" si="7">Q125</f>
         <v>39.93</v>
       </c>
       <c r="R126" s="48">
@@ -7929,10 +8111,13 @@
       <c r="T126" s="1">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="127" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="V126" s="1"/>
+      <c r="W126" s="1"/>
+      <c r="X126" s="1"/>
+    </row>
+    <row r="127" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B127" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>T-TAX-ICE_NGB31</v>
       </c>
       <c r="C127" s="1" t="str">
@@ -7959,7 +8144,7 @@
         <v>24.631</v>
       </c>
       <c r="J127" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>24.631</v>
       </c>
       <c r="K127" s="48">
@@ -7982,7 +8167,7 @@
         <v>1.2315500000000001</v>
       </c>
       <c r="Q127" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>39.93</v>
       </c>
       <c r="R127" s="48">
@@ -7994,10 +8179,13 @@
       <c r="T127" s="1">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="128" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="V127" s="1"/>
+      <c r="W127" s="1"/>
+      <c r="X127" s="1"/>
+    </row>
+    <row r="128" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B128" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>T-TAX-ICE_E8531</v>
       </c>
       <c r="C128" s="1" t="str">
@@ -8024,7 +8212,7 @@
         <v>20.290144783549959</v>
       </c>
       <c r="J128" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20.290144783549959</v>
       </c>
       <c r="K128" s="48">
@@ -8047,7 +8235,7 @@
         <v>1.0145072391774981</v>
       </c>
       <c r="Q128" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>39.93</v>
       </c>
       <c r="R128" s="48">
@@ -8059,10 +8247,13 @@
       <c r="T128" s="1">
         <v>1E-3</v>
       </c>
+      <c r="V128" s="1"/>
+      <c r="W128" s="1"/>
+      <c r="X128" s="1"/>
     </row>
     <row r="129" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B129" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>T-TAX-ICE_B10031</v>
       </c>
       <c r="C129" s="1" t="str">
@@ -8089,7 +8280,7 @@
         <v>21.831587082756254</v>
       </c>
       <c r="J129" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>21.831587082756254</v>
       </c>
       <c r="K129" s="48">
@@ -8112,7 +8303,7 @@
         <v>1.0915793541378127</v>
       </c>
       <c r="Q129" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>39.93</v>
       </c>
       <c r="R129" s="48">
@@ -8127,7 +8318,7 @@
     </row>
     <row r="130" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B130" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>T-TAX-HEV_GSL31</v>
       </c>
       <c r="C130" s="1" t="str">
@@ -8154,7 +8345,7 @@
         <v>23.751999999999999</v>
       </c>
       <c r="J130" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>23.613999999999997</v>
       </c>
       <c r="K130" s="48">
@@ -8177,7 +8368,7 @@
         <v>1.13845</v>
       </c>
       <c r="Q130" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>39.93</v>
       </c>
       <c r="R130" s="48">
@@ -8192,7 +8383,7 @@
     </row>
     <row r="131" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B131" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>T-TAX-HEV_DST31</v>
       </c>
       <c r="C131" s="1" t="str">
@@ -8219,7 +8410,7 @@
         <v>25.646000000000001</v>
       </c>
       <c r="J131" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>25.489000000000001</v>
       </c>
       <c r="K131" s="48">
@@ -8242,7 +8433,7 @@
         <v>1.22845</v>
       </c>
       <c r="Q131" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>39.93</v>
       </c>
       <c r="R131" s="48">
@@ -8257,7 +8448,7 @@
     </row>
     <row r="132" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B132" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>T-TAX-PHEV10_GSL31</v>
       </c>
       <c r="C132" s="1" t="str">
@@ -8284,7 +8475,7 @@
         <v>30.9495</v>
       </c>
       <c r="J132" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>28.889250000000001</v>
       </c>
       <c r="K132" s="48">
@@ -8307,7 +8498,7 @@
         <v>1.2685500000000003</v>
       </c>
       <c r="Q132" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>39.93</v>
       </c>
       <c r="R132" s="48">
@@ -8322,7 +8513,7 @@
     </row>
     <row r="133" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B133" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>T-TAX-PHEV20_GSL31</v>
       </c>
       <c r="C133" s="1" t="str">
@@ -8349,7 +8540,7 @@
         <v>30.9495</v>
       </c>
       <c r="J133" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>28.889250000000001</v>
       </c>
       <c r="K133" s="48">
@@ -8372,7 +8563,7 @@
         <v>1.2685500000000003</v>
       </c>
       <c r="Q133" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>39.93</v>
       </c>
       <c r="R133" s="48">
@@ -8387,7 +8578,7 @@
     </row>
     <row r="134" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B134" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>T-TAX-PHEV40_GSL31</v>
       </c>
       <c r="C134" s="1" t="str">
@@ -8414,7 +8605,7 @@
         <v>30.9495</v>
       </c>
       <c r="J134" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>28.889250000000001</v>
       </c>
       <c r="K134" s="48">
@@ -8437,7 +8628,7 @@
         <v>1.2685500000000003</v>
       </c>
       <c r="Q134" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>39.93</v>
       </c>
       <c r="R134" s="48">
@@ -8452,7 +8643,7 @@
     </row>
     <row r="135" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B135" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>T-TAX-PHEV10_DST31</v>
       </c>
       <c r="C135" s="1" t="str">
@@ -8479,7 +8670,7 @@
         <v>33.423499999999997</v>
       </c>
       <c r="J135" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>31.186749999999996</v>
       </c>
       <c r="K135" s="48">
@@ -8502,7 +8693,7 @@
         <v>1.3688500000000001</v>
       </c>
       <c r="Q135" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>39.93</v>
       </c>
       <c r="R135" s="48">
@@ -8517,7 +8708,7 @@
     </row>
     <row r="136" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B136" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>T-TAX-PHEV20_DST31</v>
       </c>
       <c r="C136" s="1" t="str">
@@ -8544,7 +8735,7 @@
         <v>33.423499999999997</v>
       </c>
       <c r="J136" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>31.186749999999996</v>
       </c>
       <c r="K136" s="48">
@@ -8567,7 +8758,7 @@
         <v>1.3688500000000001</v>
       </c>
       <c r="Q136" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>39.93</v>
       </c>
       <c r="R136" s="48">
@@ -8582,7 +8773,7 @@
     </row>
     <row r="137" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B137" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>T-TAX-PHEV40_DST31</v>
       </c>
       <c r="C137" s="1" t="str">
@@ -8609,7 +8800,7 @@
         <v>33.423499999999997</v>
       </c>
       <c r="J137" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>31.186749999999996</v>
       </c>
       <c r="K137" s="48">
@@ -8632,7 +8823,7 @@
         <v>1.3688500000000001</v>
       </c>
       <c r="Q137" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>39.93</v>
       </c>
       <c r="R137" s="48">
@@ -8647,7 +8838,7 @@
     </row>
     <row r="138" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B138" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>T-TAX-BEV100_ELC31</v>
       </c>
       <c r="C138" s="1" t="str">
@@ -8674,7 +8865,7 @@
         <v>32.970999999999997</v>
       </c>
       <c r="J138" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>30.275999999999996</v>
       </c>
       <c r="K138" s="48">
@@ -8697,7 +8888,7 @@
         <v>1.2323000000000002</v>
       </c>
       <c r="Q138" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>39.93</v>
       </c>
       <c r="R138" s="48">
@@ -8712,7 +8903,7 @@
     </row>
     <row r="139" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B139" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>T-TAX-BEV150_ELC31</v>
       </c>
       <c r="C139" s="1" t="str">
@@ -8739,7 +8930,7 @@
         <v>32.970999999999997</v>
       </c>
       <c r="J139" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>30.275999999999996</v>
       </c>
       <c r="K139" s="48">
@@ -8762,7 +8953,7 @@
         <v>1.2323000000000002</v>
       </c>
       <c r="Q139" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>39.93</v>
       </c>
       <c r="R139" s="48">
@@ -8777,7 +8968,7 @@
     </row>
     <row r="140" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B140" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>T-TAX-BEV250_ELC31</v>
       </c>
       <c r="C140" s="1" t="str">
@@ -8804,7 +8995,7 @@
         <v>32.970999999999997</v>
       </c>
       <c r="J140" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>30.275999999999996</v>
       </c>
       <c r="K140" s="48">
@@ -8827,7 +9018,7 @@
         <v>1.2323000000000002</v>
       </c>
       <c r="Q140" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>39.93</v>
       </c>
       <c r="R140" s="48">
@@ -8842,7 +9033,7 @@
     </row>
     <row r="141" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B141" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>T-TAX-ICE_HYD31</v>
       </c>
       <c r="C141" s="1" t="str">
@@ -8869,7 +9060,7 @@
         <v>60.819000000000003</v>
       </c>
       <c r="J141" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>46.0015</v>
       </c>
       <c r="K141" s="48">
@@ -8892,7 +9083,7 @@
         <v>1.2398000000000002</v>
       </c>
       <c r="Q141" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>39.93</v>
       </c>
       <c r="R141" s="48">
@@ -8907,7 +9098,7 @@
     </row>
     <row r="142" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B142" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>T-TAX-FCV_HYD31</v>
       </c>
       <c r="C142" s="1" t="str">
@@ -8934,7 +9125,7 @@
         <v>60.819000000000003</v>
       </c>
       <c r="J142" s="48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>46.0015</v>
       </c>
       <c r="K142" s="48">
@@ -8957,7 +9148,7 @@
         <v>1.2398000000000002</v>
       </c>
       <c r="Q142" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>39.93</v>
       </c>
       <c r="R142" s="48">
@@ -9086,14 +9277,14 @@
         <v>109.959</v>
       </c>
       <c r="J145" s="48">
-        <f t="shared" ref="J145:J148" si="7">AVERAGE(I145,K145)</f>
+        <f t="shared" ref="J145:J148" si="8">AVERAGE(I145,K145)</f>
         <v>111.762</v>
       </c>
       <c r="K145" s="48">
         <v>113.565</v>
       </c>
       <c r="L145" s="48">
-        <f t="shared" ref="L145:L160" si="8">K145-((K145-M145)/4)</f>
+        <f t="shared" ref="L145:L160" si="9">K145-((K145-M145)/4)</f>
         <v>113.565</v>
       </c>
       <c r="M145" s="48">
@@ -9150,14 +9341,14 @@
         <v>109.959</v>
       </c>
       <c r="J146" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>111.762</v>
       </c>
       <c r="K146" s="48">
         <v>113.565</v>
       </c>
       <c r="L146" s="48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>113.565</v>
       </c>
       <c r="M146" s="48">
@@ -9214,14 +9405,14 @@
         <v>397.21899999999999</v>
       </c>
       <c r="J147" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>323.60950000000003</v>
       </c>
       <c r="K147" s="48">
         <v>250</v>
       </c>
       <c r="L147" s="48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>220</v>
       </c>
       <c r="M147" s="48">
@@ -9278,14 +9469,14 @@
         <v>397.21899999999999</v>
       </c>
       <c r="J148" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>352.79750000000001</v>
       </c>
       <c r="K148" s="48">
         <v>308.37599999999998</v>
       </c>
       <c r="L148" s="48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>263.95425</v>
       </c>
       <c r="M148" s="48">
@@ -9372,7 +9563,7 @@
         <v>231.58335558726841</v>
       </c>
       <c r="L150" s="48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>231.58335558726841</v>
       </c>
       <c r="M150" s="48">
@@ -9429,14 +9620,14 @@
         <v>935.5223742338045</v>
       </c>
       <c r="J151" s="48">
-        <f t="shared" ref="J151:J152" si="9">AVERAGE(I151,K151)</f>
+        <f t="shared" ref="J151:J152" si="10">AVERAGE(I151,K151)</f>
         <v>935.5223742338045</v>
       </c>
       <c r="K151" s="48">
         <v>935.5223742338045</v>
       </c>
       <c r="L151" s="48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>935.5223742338045</v>
       </c>
       <c r="M151" s="48">
@@ -9493,14 +9684,14 @@
         <v>989.2715097553122</v>
       </c>
       <c r="J152" s="48">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>989.2715097553122</v>
       </c>
       <c r="K152" s="48">
         <v>989.2715097553122</v>
       </c>
       <c r="L152" s="48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>989.2715097553122</v>
       </c>
       <c r="M152" s="48">
@@ -9553,7 +9744,7 @@
     </row>
     <row r="154" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B154" s="1" t="str">
-        <f t="shared" ref="B154:B160" si="10">D60</f>
+        <f t="shared" ref="B154:B160" si="11">D60</f>
         <v>T-LGT-ICE_DST61</v>
       </c>
       <c r="C154" s="1" t="str">
@@ -9587,7 +9778,7 @@
         <v>24.664999999999999</v>
       </c>
       <c r="L154" s="48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>24.664999999999999</v>
       </c>
       <c r="M154" s="50">
@@ -9617,7 +9808,7 @@
     </row>
     <row r="155" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B155" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>T-LGT-HEV_DST61</v>
       </c>
       <c r="C155" s="1" t="str">
@@ -9644,14 +9835,14 @@
         <v>26.946999999999999</v>
       </c>
       <c r="J155" s="48">
-        <f t="shared" ref="J155:J160" si="11">AVERAGE(I155,K155)</f>
+        <f t="shared" ref="J155:J160" si="12">AVERAGE(I155,K155)</f>
         <v>27.027999999999999</v>
       </c>
       <c r="K155" s="50">
         <v>27.109000000000002</v>
       </c>
       <c r="L155" s="48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>26.498000000000001</v>
       </c>
       <c r="M155" s="50">
@@ -9681,7 +9872,7 @@
     </row>
     <row r="156" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B156" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>T-LGT-PHEV_DST61</v>
       </c>
       <c r="C156" s="1" t="str">
@@ -9689,7 +9880,7 @@
         <v>TRADST,TRAELC</v>
       </c>
       <c r="D156" s="49" t="str">
-        <f t="shared" ref="D156:D160" si="12">D155</f>
+        <f t="shared" ref="D156:D160" si="13">D155</f>
         <v>TRAF</v>
       </c>
       <c r="E156" s="49">
@@ -9708,14 +9899,14 @@
         <v>33.524000000000001</v>
       </c>
       <c r="J156" s="48">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>31.293500000000002</v>
       </c>
       <c r="K156" s="50">
         <v>29.062999999999999</v>
       </c>
       <c r="L156" s="48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>28.66825</v>
       </c>
       <c r="M156" s="50">
@@ -9745,7 +9936,7 @@
     </row>
     <row r="157" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B157" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>T-LGT-ICE_NGB61</v>
       </c>
       <c r="C157" s="1" t="str">
@@ -9753,7 +9944,7 @@
         <v>TRACNG,TRABNG</v>
       </c>
       <c r="D157" s="49" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>TRAF</v>
       </c>
       <c r="E157" s="49">
@@ -9772,14 +9963,14 @@
         <v>28.097999999999999</v>
       </c>
       <c r="J157" s="48">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>26.765499999999999</v>
       </c>
       <c r="K157" s="50">
         <v>25.433</v>
       </c>
       <c r="L157" s="48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>25.394750000000002</v>
       </c>
       <c r="M157" s="50">
@@ -9809,7 +10000,7 @@
     </row>
     <row r="158" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B158" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>T-LGT-PHEV_NGB61</v>
       </c>
       <c r="C158" s="1" t="str">
@@ -9817,7 +10008,7 @@
         <v>TRACNG,TRAELC</v>
       </c>
       <c r="D158" s="49" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>TRAF</v>
       </c>
       <c r="E158" s="49">
@@ -9836,14 +10027,14 @@
         <v>36.548000000000002</v>
       </c>
       <c r="J158" s="48">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>33.258000000000003</v>
       </c>
       <c r="K158" s="50">
         <v>29.968</v>
       </c>
       <c r="L158" s="48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>29.539249999999999</v>
       </c>
       <c r="M158" s="50">
@@ -9873,7 +10064,7 @@
     </row>
     <row r="159" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B159" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>T-LGT-FCV_HYD61</v>
       </c>
       <c r="C159" s="1" t="str">
@@ -9881,7 +10072,7 @@
         <v>TRAHYD</v>
       </c>
       <c r="D159" s="49" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>TRAF</v>
       </c>
       <c r="E159" s="49">
@@ -9900,14 +10091,14 @@
         <v>56.146000000000001</v>
       </c>
       <c r="J159" s="48">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>44.363</v>
       </c>
       <c r="K159" s="50">
         <v>32.58</v>
       </c>
       <c r="L159" s="48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>30.911749999999998</v>
       </c>
       <c r="M159" s="50">
@@ -9937,7 +10128,7 @@
     </row>
     <row r="160" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B160" s="1" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>T-LGT-BEV_ELC61</v>
       </c>
       <c r="C160" s="1" t="str">
@@ -9945,7 +10136,7 @@
         <v>TRAELC</v>
       </c>
       <c r="D160" s="49" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>TRAF</v>
       </c>
       <c r="E160" s="49">
@@ -9964,14 +10155,14 @@
         <v>32.17</v>
       </c>
       <c r="J160" s="48">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>30.351500000000001</v>
       </c>
       <c r="K160" s="50">
         <v>28.533000000000001</v>
       </c>
       <c r="L160" s="48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>27.774000000000001</v>
       </c>
       <c r="M160" s="50">
@@ -10025,7 +10216,7 @@
     </row>
     <row r="162" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B162" s="1" t="str">
-        <f t="shared" ref="B162:B168" si="13">D68</f>
+        <f t="shared" ref="B162:B168" si="14">D68</f>
         <v>T-MGT-ICE_DST71</v>
       </c>
       <c r="C162" s="1" t="str">
@@ -10037,7 +10228,7 @@
         <v>TRAF</v>
       </c>
       <c r="E162" s="1">
-        <f t="shared" ref="E162:J162" si="14">E170</f>
+        <f t="shared" ref="E162:I162" si="15">E170</f>
         <v>2019</v>
       </c>
       <c r="F162" s="48">
@@ -10050,7 +10241,7 @@
         <v>2.9785493787231682E-2</v>
       </c>
       <c r="I162" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>95.69</v>
       </c>
       <c r="J162" s="48">
@@ -10058,27 +10249,27 @@
         <v>98.32</v>
       </c>
       <c r="K162" s="1">
-        <f>K170</f>
+        <f t="shared" ref="K162:K168" si="16">K170</f>
         <v>100.95</v>
       </c>
       <c r="L162" s="48">
-        <f t="shared" ref="L162:L168" si="15">K162-((K162-M162)/4)</f>
+        <f t="shared" ref="L162:L168" si="17">K162-((K162-M162)/4)</f>
         <v>100.95</v>
       </c>
       <c r="M162" s="1">
-        <f t="shared" ref="M162:P168" si="16">M170</f>
+        <f t="shared" ref="M162:P168" si="18">M170</f>
         <v>100.95</v>
       </c>
       <c r="N162" s="48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>2.1157042474212369</v>
       </c>
       <c r="O162" s="48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>2.1689507539373367</v>
       </c>
       <c r="P162" s="48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>2.1689507539373367</v>
       </c>
       <c r="Q162" s="48">
@@ -10091,13 +10282,13 @@
         <v>20</v>
       </c>
       <c r="T162" s="1">
-        <f t="shared" ref="T162:T168" si="17">T170</f>
+        <f t="shared" ref="T162:T168" si="19">T170</f>
         <v>1E-3</v>
       </c>
     </row>
     <row r="163" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B163" s="1" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>T-MGT-HEV_DST71</v>
       </c>
       <c r="C163" s="1" t="str">
@@ -10109,7 +10300,7 @@
         <v>TRAF</v>
       </c>
       <c r="E163" s="1">
-        <f t="shared" ref="C163:J168" si="18">E171</f>
+        <f t="shared" ref="C163:I168" si="20">E171</f>
         <v>2019</v>
       </c>
       <c r="F163" s="48">
@@ -10122,15 +10313,15 @@
         <v>4.2496500690063034E-2</v>
       </c>
       <c r="I163" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>124.73</v>
       </c>
       <c r="J163" s="48">
-        <f t="shared" ref="J163:J168" si="19">AVERAGE(I163,K163)</f>
+        <f t="shared" ref="J163:J168" si="21">AVERAGE(I163,K163)</f>
         <v>124.92500000000001</v>
       </c>
       <c r="K163" s="1">
-        <f>K171</f>
+        <f t="shared" si="16"/>
         <v>125.12</v>
       </c>
       <c r="L163" s="48">
@@ -10138,19 +10329,19 @@
         <v>123.88250000000001</v>
       </c>
       <c r="M163" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>120.17</v>
       </c>
       <c r="N163" s="48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>3.5721072259038325</v>
       </c>
       <c r="O163" s="48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>3.0618061936318557</v>
       </c>
       <c r="P163" s="48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>2.3858458293310703</v>
       </c>
       <c r="Q163" s="48">
@@ -10164,21 +10355,21 @@
         <v>20</v>
       </c>
       <c r="T163" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1E-3</v>
       </c>
     </row>
     <row r="164" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B164" s="1" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>T-MGT-FCV_HYD71</v>
       </c>
       <c r="C164" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>TRAHYD</v>
       </c>
       <c r="D164" s="1" t="str">
-        <f t="shared" ref="D164:D168" si="20">D163</f>
+        <f t="shared" ref="D164:D168" si="22">D163</f>
         <v>TRAF</v>
       </c>
       <c r="E164" s="1">
@@ -10194,55 +10385,55 @@
         <v>4.9705728485698729E-2</v>
       </c>
       <c r="I164" s="1">
+        <f t="shared" si="20"/>
+        <v>345.67</v>
+      </c>
+      <c r="J164" s="48">
+        <f t="shared" si="21"/>
+        <v>283.94499999999999</v>
+      </c>
+      <c r="K164" s="1">
+        <f t="shared" si="16"/>
+        <v>222.22</v>
+      </c>
+      <c r="L164" s="48">
+        <f t="shared" si="17"/>
+        <v>195.70750000000001</v>
+      </c>
+      <c r="M164" s="1">
         <f t="shared" si="18"/>
-        <v>345.67</v>
-      </c>
-      <c r="J164" s="48">
-        <f t="shared" si="19"/>
-        <v>283.94499999999999</v>
-      </c>
-      <c r="K164" s="1">
-        <f>K172</f>
-        <v>222.22</v>
-      </c>
-      <c r="L164" s="48">
-        <f t="shared" si="15"/>
-        <v>195.70750000000001</v>
-      </c>
-      <c r="M164" s="1">
-        <f t="shared" si="16"/>
         <v>116.17</v>
       </c>
       <c r="N164" s="48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>3.5721072259038325</v>
       </c>
       <c r="O164" s="48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>3.0618061936318557</v>
       </c>
       <c r="P164" s="48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>2.3858458293310703</v>
       </c>
       <c r="Q164" s="48">
         <v>29.397500000000001</v>
       </c>
       <c r="R164" s="50">
-        <f t="shared" ref="R164:R168" si="21">R163</f>
+        <f t="shared" ref="R164:R168" si="23">R163</f>
         <v>3.592571901094749</v>
       </c>
       <c r="S164" s="1">
         <v>20</v>
       </c>
       <c r="T164" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1E-3</v>
       </c>
     </row>
     <row r="165" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B165" s="1" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>T-MGT-ICE_NGB71</v>
       </c>
       <c r="C165" s="1" t="str">
@@ -10250,11 +10441,11 @@
         <v>TRACNG,TRABNG</v>
       </c>
       <c r="D165" s="1" t="str">
+        <f t="shared" si="22"/>
+        <v>TRAF</v>
+      </c>
+      <c r="E165" s="1">
         <f t="shared" si="20"/>
-        <v>TRAF</v>
-      </c>
-      <c r="E165" s="1">
-        <f t="shared" si="18"/>
         <v>2019</v>
       </c>
       <c r="F165" s="48">
@@ -10267,55 +10458,55 @@
         <v>2.9406060745356118E-2</v>
       </c>
       <c r="I165" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>115.69</v>
       </c>
       <c r="J165" s="48">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>118.32</v>
       </c>
       <c r="K165" s="1">
-        <f>K173</f>
-        <v>120.95</v>
-      </c>
-      <c r="L165" s="48">
-        <f t="shared" si="15"/>
-        <v>120.95</v>
-      </c>
-      <c r="M165" s="1">
         <f t="shared" si="16"/>
         <v>120.95</v>
       </c>
+      <c r="L165" s="48">
+        <f t="shared" si="17"/>
+        <v>120.95</v>
+      </c>
+      <c r="M165" s="1">
+        <f t="shared" si="18"/>
+        <v>120.95</v>
+      </c>
       <c r="N165" s="48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>5.0989820625747049</v>
       </c>
       <c r="O165" s="48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>3.5538821890369761</v>
       </c>
       <c r="P165" s="48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>2.3292245236828353</v>
       </c>
       <c r="Q165" s="48">
         <v>29.397500000000001</v>
       </c>
       <c r="R165" s="50">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>3.592571901094749</v>
       </c>
       <c r="S165" s="1">
         <v>20</v>
       </c>
       <c r="T165" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1E-3</v>
       </c>
     </row>
     <row r="166" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B166" s="1" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>T-MGT-HEV_NGB71</v>
       </c>
       <c r="C166" s="1" t="str">
@@ -10323,11 +10514,11 @@
         <v>TRACNG,TRABNG</v>
       </c>
       <c r="D166" s="1" t="str">
+        <f t="shared" si="22"/>
+        <v>TRAF</v>
+      </c>
+      <c r="E166" s="1">
         <f t="shared" si="20"/>
-        <v>TRAF</v>
-      </c>
-      <c r="E166" s="1">
-        <f t="shared" si="18"/>
         <v>2019</v>
       </c>
       <c r="F166" s="48">
@@ -10340,67 +10531,67 @@
         <v>4.211706764818747E-2</v>
       </c>
       <c r="I166" s="1">
+        <f t="shared" si="20"/>
+        <v>144.72999999999999</v>
+      </c>
+      <c r="J166" s="48">
+        <f t="shared" si="21"/>
+        <v>144.92500000000001</v>
+      </c>
+      <c r="K166" s="1">
+        <f t="shared" si="16"/>
+        <v>145.12</v>
+      </c>
+      <c r="L166" s="48">
+        <f t="shared" si="17"/>
+        <v>143.88249999999999</v>
+      </c>
+      <c r="M166" s="1">
         <f t="shared" si="18"/>
-        <v>144.72999999999999</v>
-      </c>
-      <c r="J166" s="48">
-        <f t="shared" si="19"/>
-        <v>144.92500000000001</v>
-      </c>
-      <c r="K166" s="1">
-        <f>K174</f>
-        <v>145.12</v>
-      </c>
-      <c r="L166" s="48">
-        <f t="shared" si="15"/>
-        <v>143.88249999999999</v>
-      </c>
-      <c r="M166" s="1">
-        <f t="shared" si="16"/>
         <v>140.16999999999999</v>
       </c>
       <c r="N166" s="48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>5.0989820625747049</v>
       </c>
       <c r="O166" s="48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>3.5538821890369761</v>
       </c>
       <c r="P166" s="48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>2.3292245236828353</v>
       </c>
       <c r="Q166" s="48">
         <v>29.397500000000001</v>
       </c>
       <c r="R166" s="50">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>3.592571901094749</v>
       </c>
       <c r="S166" s="1">
         <v>20</v>
       </c>
       <c r="T166" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1E-3</v>
       </c>
     </row>
     <row r="167" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B167" s="1" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>T-MGT-ICE_LNG71</v>
       </c>
       <c r="C167" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>TRALNG</v>
       </c>
       <c r="D167" s="1" t="str">
+        <f t="shared" si="22"/>
+        <v>TRAF</v>
+      </c>
+      <c r="E167" s="1">
         <f t="shared" si="20"/>
-        <v>TRAF</v>
-      </c>
-      <c r="E167" s="1">
-        <f t="shared" si="18"/>
         <v>2019</v>
       </c>
       <c r="F167" s="48">
@@ -10413,67 +10604,67 @@
         <v>2.9406060745356118E-2</v>
       </c>
       <c r="I167" s="1">
+        <f t="shared" si="20"/>
+        <v>130.68600000000001</v>
+      </c>
+      <c r="J167" s="48">
+        <f t="shared" si="21"/>
+        <v>129.72200000000001</v>
+      </c>
+      <c r="K167" s="1">
+        <f t="shared" si="16"/>
+        <v>128.75800000000001</v>
+      </c>
+      <c r="L167" s="48">
+        <f t="shared" si="17"/>
+        <v>128.11425</v>
+      </c>
+      <c r="M167" s="1">
         <f t="shared" si="18"/>
-        <v>130.68600000000001</v>
-      </c>
-      <c r="J167" s="48">
-        <f t="shared" si="19"/>
-        <v>129.72200000000001</v>
-      </c>
-      <c r="K167" s="1">
-        <f>K175</f>
-        <v>128.75800000000001</v>
-      </c>
-      <c r="L167" s="48">
-        <f t="shared" si="15"/>
-        <v>128.11425</v>
-      </c>
-      <c r="M167" s="1">
-        <f t="shared" si="16"/>
         <v>126.18300000000001</v>
       </c>
       <c r="N167" s="48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>5.0989820625747049</v>
       </c>
       <c r="O167" s="48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>3.5538821890369761</v>
       </c>
       <c r="P167" s="48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>2.3292245236828353</v>
       </c>
       <c r="Q167" s="48">
         <v>29.397500000000001</v>
       </c>
       <c r="R167" s="50">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>3.592571901094749</v>
       </c>
       <c r="S167" s="1">
         <v>20</v>
       </c>
       <c r="T167" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1E-3</v>
       </c>
     </row>
     <row r="168" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B168" s="1" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>T-MGT-BEV_ELC71</v>
       </c>
       <c r="C168" s="1" t="str">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>TRAELC</v>
       </c>
       <c r="D168" s="1" t="str">
+        <f t="shared" si="22"/>
+        <v>TRAF</v>
+      </c>
+      <c r="E168" s="1">
         <f t="shared" si="20"/>
-        <v>TRAF</v>
-      </c>
-      <c r="E168" s="1">
-        <f t="shared" si="18"/>
         <v>2019</v>
       </c>
       <c r="F168" s="48">
@@ -10486,49 +10677,49 @@
         <v>6.5831632765410139E-2</v>
       </c>
       <c r="I168" s="1">
+        <f t="shared" si="20"/>
+        <v>345.67</v>
+      </c>
+      <c r="J168" s="48">
+        <f t="shared" si="21"/>
+        <v>309.89</v>
+      </c>
+      <c r="K168" s="1">
+        <f t="shared" si="16"/>
+        <v>274.11</v>
+      </c>
+      <c r="L168" s="48">
+        <f t="shared" si="17"/>
+        <v>234.625</v>
+      </c>
+      <c r="M168" s="1">
         <f t="shared" si="18"/>
-        <v>345.67</v>
-      </c>
-      <c r="J168" s="48">
-        <f t="shared" si="19"/>
-        <v>309.89</v>
-      </c>
-      <c r="K168" s="1">
-        <f>K176</f>
-        <v>274.11</v>
-      </c>
-      <c r="L168" s="48">
-        <f t="shared" si="15"/>
-        <v>234.625</v>
-      </c>
-      <c r="M168" s="1">
-        <f t="shared" si="16"/>
         <v>116.17</v>
       </c>
       <c r="N168" s="48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>3.5721072259038325</v>
       </c>
       <c r="O168" s="48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>3.0618061936318557</v>
       </c>
       <c r="P168" s="48">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>2.3858458293310703</v>
       </c>
       <c r="Q168" s="48">
         <v>29.397500000000001</v>
       </c>
       <c r="R168" s="50">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>3.592571901094749</v>
       </c>
       <c r="S168" s="1">
         <v>20</v>
       </c>
       <c r="T168" s="1">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>1E-3</v>
       </c>
     </row>
@@ -10557,7 +10748,7 @@
     </row>
     <row r="170" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B170" s="1" t="str">
-        <f t="shared" ref="B170:B176" si="22">D76</f>
+        <f t="shared" ref="B170:B176" si="24">D76</f>
         <v>T-HGT-ICE_DST81</v>
       </c>
       <c r="C170" s="1" t="str">
@@ -10591,7 +10782,7 @@
         <v>100.95</v>
       </c>
       <c r="L170" s="48">
-        <f t="shared" ref="L170:L176" si="23">K170-((K170-M170)/4)</f>
+        <f t="shared" ref="L170:L176" si="25">K170-((K170-M170)/4)</f>
         <v>100.95</v>
       </c>
       <c r="M170" s="50">
@@ -10622,7 +10813,7 @@
     </row>
     <row r="171" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B171" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>T-HGT-HEV_DST81</v>
       </c>
       <c r="C171" s="1" t="str">
@@ -10649,14 +10840,14 @@
         <v>124.73</v>
       </c>
       <c r="J171" s="48">
-        <f t="shared" ref="J171:J176" si="24">AVERAGE(I171,K171)</f>
+        <f t="shared" ref="J171:J176" si="26">AVERAGE(I171,K171)</f>
         <v>124.92500000000001</v>
       </c>
       <c r="K171" s="50">
         <v>125.12</v>
       </c>
       <c r="L171" s="48">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>123.88250000000001</v>
       </c>
       <c r="M171" s="50">
@@ -10688,7 +10879,7 @@
     </row>
     <row r="172" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B172" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>T-HGT-FCV_HYD81</v>
       </c>
       <c r="C172" s="1" t="str">
@@ -10696,7 +10887,7 @@
         <v>TRAHYD</v>
       </c>
       <c r="D172" s="49" t="str">
-        <f t="shared" ref="D172:D176" si="25">D171</f>
+        <f t="shared" ref="D172:D176" si="27">D171</f>
         <v>TRAF</v>
       </c>
       <c r="E172" s="49">
@@ -10715,14 +10906,14 @@
         <v>345.67</v>
       </c>
       <c r="J172" s="48">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>283.94499999999999</v>
       </c>
       <c r="K172" s="50">
         <v>222.22</v>
       </c>
       <c r="L172" s="48">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>195.70750000000001</v>
       </c>
       <c r="M172" s="50">
@@ -10741,7 +10932,7 @@
         <v>50.915999999999997</v>
       </c>
       <c r="R172" s="50">
-        <f t="shared" ref="R172:R176" si="26">R171</f>
+        <f t="shared" ref="R172:R176" si="28">R171</f>
         <v>9.2231504438872829</v>
       </c>
       <c r="S172" s="49">
@@ -10754,7 +10945,7 @@
     </row>
     <row r="173" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B173" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>T-HGT-ICE_NGB81</v>
       </c>
       <c r="C173" s="1" t="str">
@@ -10762,7 +10953,7 @@
         <v>TRACNG,TRABNG</v>
       </c>
       <c r="D173" s="49" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>TRAF</v>
       </c>
       <c r="E173" s="49">
@@ -10781,14 +10972,14 @@
         <v>115.69</v>
       </c>
       <c r="J173" s="48">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>118.32</v>
       </c>
       <c r="K173" s="50">
         <v>120.95</v>
       </c>
       <c r="L173" s="48">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>120.95</v>
       </c>
       <c r="M173" s="50">
@@ -10807,7 +10998,7 @@
         <v>50.915999999999997</v>
       </c>
       <c r="R173" s="50">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>9.2231504438872829</v>
       </c>
       <c r="S173" s="49">
@@ -10820,7 +11011,7 @@
     </row>
     <row r="174" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B174" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>T-HGT-HEV_NGB81</v>
       </c>
       <c r="C174" s="1" t="str">
@@ -10828,7 +11019,7 @@
         <v>TRACNG,TRABNG</v>
       </c>
       <c r="D174" s="49" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>TRAF</v>
       </c>
       <c r="E174" s="49">
@@ -10847,14 +11038,14 @@
         <v>144.72999999999999</v>
       </c>
       <c r="J174" s="48">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>144.92500000000001</v>
       </c>
       <c r="K174" s="50">
         <v>145.12</v>
       </c>
       <c r="L174" s="48">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>143.88249999999999</v>
       </c>
       <c r="M174" s="50">
@@ -10873,7 +11064,7 @@
         <v>50.915999999999997</v>
       </c>
       <c r="R174" s="50">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>9.2231504438872829</v>
       </c>
       <c r="S174" s="49">
@@ -10885,7 +11076,7 @@
     </row>
     <row r="175" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B175" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>T-HGT-ICE_LNG81</v>
       </c>
       <c r="C175" s="1" t="str">
@@ -10893,7 +11084,7 @@
         <v>TRALNG</v>
       </c>
       <c r="D175" s="49" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>TRAF</v>
       </c>
       <c r="E175" s="49">
@@ -10912,14 +11103,14 @@
         <v>130.68600000000001</v>
       </c>
       <c r="J175" s="48">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>129.72200000000001</v>
       </c>
       <c r="K175" s="50">
         <v>128.75800000000001</v>
       </c>
       <c r="L175" s="48">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>128.11425</v>
       </c>
       <c r="M175" s="50">
@@ -10938,7 +11129,7 @@
         <v>50.915999999999997</v>
       </c>
       <c r="R175" s="50">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>9.2231504438872829</v>
       </c>
       <c r="S175" s="49">
@@ -10950,7 +11141,7 @@
     </row>
     <row r="176" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B176" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>T-HGT-BEV_ELC81</v>
       </c>
       <c r="C176" s="1" t="str">
@@ -10958,7 +11149,7 @@
         <v>TRAELC</v>
       </c>
       <c r="D176" s="49" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>TRAF</v>
       </c>
       <c r="E176" s="49">
@@ -10977,14 +11168,14 @@
         <v>345.67</v>
       </c>
       <c r="J176" s="48">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>309.89</v>
       </c>
       <c r="K176" s="50">
         <v>274.11</v>
       </c>
       <c r="L176" s="48">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>234.625</v>
       </c>
       <c r="M176" s="50">
@@ -11003,7 +11194,7 @@
         <v>50.915999999999997</v>
       </c>
       <c r="R176" s="50">
-        <f t="shared" si="26"/>
+        <f t="shared" si="28"/>
         <v>9.2231504438872829</v>
       </c>
       <c r="S176" s="49">
@@ -11072,7 +11263,7 @@
         <v>469.60386878903267</v>
       </c>
       <c r="L178" s="48">
-        <f t="shared" ref="L178:L179" si="27">K178-((K178-M178)/4)</f>
+        <f t="shared" ref="L178:L179" si="29">K178-((K178-M178)/4)</f>
         <v>469.60386878903267</v>
       </c>
       <c r="M178" s="48">
@@ -11129,14 +11320,14 @@
         <v>438.88212036358203</v>
       </c>
       <c r="J179" s="48">
-        <f t="shared" ref="J179:J180" si="28">AVERAGE(I179,K179)</f>
+        <f t="shared" ref="J179:J180" si="30">AVERAGE(I179,K179)</f>
         <v>438.88212036358203</v>
       </c>
       <c r="K179" s="48">
         <v>438.88212036358203</v>
       </c>
       <c r="L179" s="48">
-        <f t="shared" si="27"/>
+        <f t="shared" si="29"/>
         <v>438.88212036358203</v>
       </c>
       <c r="M179" s="48">
@@ -11193,7 +11384,7 @@
         <v>682.10068176688696</v>
       </c>
       <c r="J180" s="48">
-        <f t="shared" si="28"/>
+        <f t="shared" si="30"/>
         <v>653.58396473256948</v>
       </c>
       <c r="K180" s="61">
@@ -11282,7 +11473,7 @@
     </row>
     <row r="183" spans="2:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B183" s="1" t="str">
-        <f t="shared" ref="B183:B184" si="29">D89</f>
+        <f t="shared" ref="B183:B184" si="31">D89</f>
         <v>T-NAV_NEW</v>
       </c>
       <c r="C183" s="1" t="str">
@@ -11311,7 +11502,7 @@
     </row>
     <row r="184" spans="2:32" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B184" s="1" t="str">
-        <f t="shared" si="29"/>
+        <f t="shared" si="31"/>
         <v>T-OTH_NEW</v>
       </c>
       <c r="C184" s="1" t="str">
@@ -12644,23 +12835,23 @@
         <v>TRAGSL</v>
       </c>
       <c r="D223" s="91" t="str">
-        <f t="shared" ref="D223:H223" si="30">D197</f>
+        <f t="shared" ref="D223:H223" si="32">D197</f>
         <v>UP</v>
       </c>
       <c r="E223" s="87">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>0.96784365458672328</v>
       </c>
       <c r="F223" s="87">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>1</v>
       </c>
       <c r="G223" s="87">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>1</v>
       </c>
       <c r="H223" s="81">
-        <f t="shared" si="30"/>
+        <f t="shared" si="32"/>
         <v>5</v>
       </c>
     </row>
@@ -12670,27 +12861,27 @@
         <v>T-TAX-ICE_GSL31</v>
       </c>
       <c r="C224" s="81" t="str">
-        <f t="shared" ref="C224:H248" si="31">C198</f>
+        <f t="shared" ref="C224:H248" si="33">C198</f>
         <v>TRAGSL</v>
       </c>
       <c r="D224" s="91" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>LO</v>
       </c>
       <c r="E224" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.96784365458672328</v>
       </c>
       <c r="F224" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.95</v>
       </c>
       <c r="G224" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.9</v>
       </c>
       <c r="H224" s="81">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
     </row>
@@ -12700,27 +12891,27 @@
         <v>T-TAX-ICE_DST31</v>
       </c>
       <c r="C225" s="81" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>TRADST</v>
       </c>
       <c r="D225" s="91" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>UP</v>
       </c>
       <c r="E225" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.95903634682608185</v>
       </c>
       <c r="F225" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="G225" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="H225" s="81">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
     </row>
@@ -12730,27 +12921,27 @@
         <v>T-TAX-ICE_DST31</v>
       </c>
       <c r="C226" s="81" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>TRADST</v>
       </c>
       <c r="D226" s="91" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>LO</v>
       </c>
       <c r="E226" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.95903634682608185</v>
       </c>
       <c r="F226" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.95</v>
       </c>
       <c r="G226" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.9</v>
       </c>
       <c r="H226" s="81">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
     </row>
@@ -12760,27 +12951,27 @@
         <v>T-TAX-ICE_DF31</v>
       </c>
       <c r="C227" s="81" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>TRACNG</v>
       </c>
       <c r="D227" s="91" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>UP</v>
       </c>
       <c r="E227" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.5</v>
       </c>
       <c r="F227" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.5</v>
       </c>
       <c r="G227" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.8</v>
       </c>
       <c r="H227" s="81">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
     </row>
@@ -12790,27 +12981,27 @@
         <v>T-TAX-ICE_DF31</v>
       </c>
       <c r="C228" s="81" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>TRACNG</v>
       </c>
       <c r="D228" s="91" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>LO</v>
       </c>
       <c r="E228" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.4</v>
       </c>
       <c r="F228" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.4</v>
       </c>
       <c r="G228" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.4</v>
       </c>
       <c r="H228" s="81">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
     </row>
@@ -12820,27 +13011,27 @@
         <v>T-TAX-ICE_NGB31</v>
       </c>
       <c r="C229" s="81" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>TRACNG</v>
       </c>
       <c r="D229" s="91" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>UP</v>
       </c>
       <c r="E229" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.5</v>
       </c>
       <c r="F229" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.5</v>
       </c>
       <c r="G229" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="H229" s="81">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="J229" s="1"/>
@@ -12867,27 +13058,27 @@
         <v>T-TAX-ICE_NGB31</v>
       </c>
       <c r="C230" s="81" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>TRACNG</v>
       </c>
       <c r="D230" s="91" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>LO</v>
       </c>
       <c r="E230" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.5</v>
       </c>
       <c r="F230" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.5</v>
       </c>
       <c r="G230" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="H230" s="81">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="J230" s="1"/>
@@ -12914,27 +13105,27 @@
         <v>T-TAX-ICE_E8531</v>
       </c>
       <c r="C231" s="81" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>TRAETH</v>
       </c>
       <c r="D231" s="91" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>UP</v>
       </c>
       <c r="E231" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.85</v>
       </c>
       <c r="F231" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.85</v>
       </c>
       <c r="G231" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.85</v>
       </c>
       <c r="H231" s="81">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="J231" s="1"/>
@@ -12961,27 +13152,27 @@
         <v>T-TAX-ICE_E8531</v>
       </c>
       <c r="C232" s="81" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>TRAETH</v>
       </c>
       <c r="D232" s="91" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>LO</v>
       </c>
       <c r="E232" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="F232" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="G232" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="H232" s="81">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="J232" s="1"/>
@@ -13008,27 +13199,27 @@
         <v>T-TAX-HEV_GSL31</v>
       </c>
       <c r="C233" s="81" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>TRAGSL</v>
       </c>
       <c r="D233" s="91" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>UP</v>
       </c>
       <c r="E233" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.96784365458672328</v>
       </c>
       <c r="F233" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="G233" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="H233" s="81">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="J233" s="1"/>
@@ -13055,27 +13246,27 @@
         <v>T-TAX-HEV_GSL31</v>
       </c>
       <c r="C234" s="81" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>TRAGSL</v>
       </c>
       <c r="D234" s="91" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>LO</v>
       </c>
       <c r="E234" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.96784365458672328</v>
       </c>
       <c r="F234" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.95</v>
       </c>
       <c r="G234" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.9</v>
       </c>
       <c r="H234" s="81">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
       <c r="J234" s="1"/>
@@ -13102,27 +13293,27 @@
         <v>T-TAX-HEV_DST31</v>
       </c>
       <c r="C235" s="81" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>TRADST</v>
       </c>
       <c r="D235" s="91" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>UP</v>
       </c>
       <c r="E235" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.95903634682608185</v>
       </c>
       <c r="F235" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="G235" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="H235" s="81">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
     </row>
@@ -13132,27 +13323,27 @@
         <v>T-TAX-HEV_DST31</v>
       </c>
       <c r="C236" s="81" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>TRADST</v>
       </c>
       <c r="D236" s="91" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>LO</v>
       </c>
       <c r="E236" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.95903634682608185</v>
       </c>
       <c r="F236" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.95</v>
       </c>
       <c r="G236" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.9</v>
       </c>
       <c r="H236" s="81">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
     </row>
@@ -13162,27 +13353,27 @@
         <v>T-TAX-PHEV10_GSL31</v>
       </c>
       <c r="C237" s="81" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>TRAELC</v>
       </c>
       <c r="D237" s="91" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>UP</v>
       </c>
       <c r="E237" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.5</v>
       </c>
       <c r="F237" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.6</v>
       </c>
       <c r="G237" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.8</v>
       </c>
       <c r="H237" s="81">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
     </row>
@@ -13192,27 +13383,27 @@
         <v>T-TAX-PHEV10_GSL31</v>
       </c>
       <c r="C238" s="81" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>TRAELC</v>
       </c>
       <c r="D238" s="91" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>LO</v>
       </c>
       <c r="E238" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.3</v>
       </c>
       <c r="F238" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.3</v>
       </c>
       <c r="G238" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.3</v>
       </c>
       <c r="H238" s="81">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
     </row>
@@ -13222,27 +13413,27 @@
         <v>T-TAX-PHEV20_GSL31</v>
       </c>
       <c r="C239" s="81" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>TRAELC</v>
       </c>
       <c r="D239" s="91" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>UP</v>
       </c>
       <c r="E239" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.5</v>
       </c>
       <c r="F239" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.6</v>
       </c>
       <c r="G239" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.8</v>
       </c>
       <c r="H239" s="81">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
     </row>
@@ -13252,27 +13443,27 @@
         <v>T-TAX-PHEV20_GSL31</v>
       </c>
       <c r="C240" s="81" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>TRAELC</v>
       </c>
       <c r="D240" s="91" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>LO</v>
       </c>
       <c r="E240" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.3</v>
       </c>
       <c r="F240" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.3</v>
       </c>
       <c r="G240" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.3</v>
       </c>
       <c r="H240" s="81">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
     </row>
@@ -13282,27 +13473,27 @@
         <v>T-TAX-PHEV40_GSL31</v>
       </c>
       <c r="C241" s="81" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>TRAELC</v>
       </c>
       <c r="D241" s="91" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>UP</v>
       </c>
       <c r="E241" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.5</v>
       </c>
       <c r="F241" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.6</v>
       </c>
       <c r="G241" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.8</v>
       </c>
       <c r="H241" s="81">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
     </row>
@@ -13312,27 +13503,27 @@
         <v>T-TAX-PHEV40_GSL31</v>
       </c>
       <c r="C242" s="81" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>TRAELC</v>
       </c>
       <c r="D242" s="91" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>LO</v>
       </c>
       <c r="E242" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.3</v>
       </c>
       <c r="F242" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.3</v>
       </c>
       <c r="G242" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.3</v>
       </c>
       <c r="H242" s="81">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
     </row>
@@ -13342,27 +13533,27 @@
         <v>T-TAX-PHEV10_DST31</v>
       </c>
       <c r="C243" s="81" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>TRAELC</v>
       </c>
       <c r="D243" s="91" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>UP</v>
       </c>
       <c r="E243" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.5</v>
       </c>
       <c r="F243" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.6</v>
       </c>
       <c r="G243" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.8</v>
       </c>
       <c r="H243" s="81">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
     </row>
@@ -13372,27 +13563,27 @@
         <v>T-TAX-PHEV10_DST31</v>
       </c>
       <c r="C244" s="81" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>TRAELC</v>
       </c>
       <c r="D244" s="91" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>LO</v>
       </c>
       <c r="E244" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.3</v>
       </c>
       <c r="F244" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.3</v>
       </c>
       <c r="G244" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.3</v>
       </c>
       <c r="H244" s="81">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
     </row>
@@ -13402,27 +13593,27 @@
         <v>T-TAX-PHEV20_DST31</v>
       </c>
       <c r="C245" s="81" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>TRAELC</v>
       </c>
       <c r="D245" s="91" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>UP</v>
       </c>
       <c r="E245" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.5</v>
       </c>
       <c r="F245" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.6</v>
       </c>
       <c r="G245" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.8</v>
       </c>
       <c r="H245" s="81">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
     </row>
@@ -13432,27 +13623,27 @@
         <v>T-TAX-PHEV20_DST31</v>
       </c>
       <c r="C246" s="81" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>TRAELC</v>
       </c>
       <c r="D246" s="91" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>LO</v>
       </c>
       <c r="E246" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.3</v>
       </c>
       <c r="F246" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.3</v>
       </c>
       <c r="G246" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.3</v>
       </c>
       <c r="H246" s="81">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
     </row>
@@ -13462,27 +13653,27 @@
         <v>T-TAX-PHEV40_DST31</v>
       </c>
       <c r="C247" s="81" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>TRAELC</v>
       </c>
       <c r="D247" s="91" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>UP</v>
       </c>
       <c r="E247" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.5</v>
       </c>
       <c r="F247" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.6</v>
       </c>
       <c r="G247" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.8</v>
       </c>
       <c r="H247" s="81">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
     </row>
@@ -13492,27 +13683,27 @@
         <v>T-TAX-PHEV40_DST31</v>
       </c>
       <c r="C248" s="81" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>TRAELC</v>
       </c>
       <c r="D248" s="91" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>LO</v>
       </c>
       <c r="E248" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.3</v>
       </c>
       <c r="F248" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.3</v>
       </c>
       <c r="G248" s="87">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>0.3</v>
       </c>
       <c r="H248" s="81">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>5</v>
       </c>
     </row>
@@ -13526,7 +13717,7 @@
         <v>TRADST</v>
       </c>
       <c r="D249" s="82" t="str">
-        <f t="shared" ref="D249" si="32">D223</f>
+        <f t="shared" ref="D249" si="34">D223</f>
         <v>UP</v>
       </c>
       <c r="E249" s="79">
@@ -13552,7 +13743,7 @@
         <v>TRADST</v>
       </c>
       <c r="D250" s="82" t="str">
-        <f t="shared" ref="D250" si="33">D224</f>
+        <f t="shared" ref="D250" si="35">D224</f>
         <v>LO</v>
       </c>
       <c r="E250" s="79">
@@ -13578,7 +13769,7 @@
         <v>TRACNG</v>
       </c>
       <c r="D251" s="82" t="str">
-        <f t="shared" ref="D251" si="34">D225</f>
+        <f t="shared" ref="D251" si="36">D225</f>
         <v>UP</v>
       </c>
       <c r="E251" s="79">
@@ -13604,7 +13795,7 @@
         <v>TRACNG</v>
       </c>
       <c r="D252" s="82" t="str">
-        <f t="shared" ref="D252" si="35">D226</f>
+        <f t="shared" ref="D252" si="37">D226</f>
         <v>LO</v>
       </c>
       <c r="E252" s="79">
@@ -14708,7 +14899,7 @@
     </row>
     <row r="291" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B291" s="86" t="str">
-        <f t="shared" ref="B291:B294" si="36">B290</f>
+        <f t="shared" ref="B291:B294" si="38">B290</f>
         <v>T-OTH_NEW</v>
       </c>
       <c r="C291" s="86" t="str">
@@ -14733,7 +14924,7 @@
     </row>
     <row r="292" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B292" s="86" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>T-OTH_NEW</v>
       </c>
       <c r="C292" s="86" t="str">
@@ -14758,7 +14949,7 @@
     </row>
     <row r="293" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B293" s="86" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>T-OTH_NEW</v>
       </c>
       <c r="C293" s="86" t="str">
@@ -14783,7 +14974,7 @@
     </row>
     <row r="294" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B294" s="86" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>T-OTH_NEW</v>
       </c>
       <c r="C294" s="86" t="str">
@@ -14907,7 +15098,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="17" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
Add ACT_BND for biodiesel supply for 2030 (100 times the base-year) and change the maximum bio-diesel blend to 20% for ICEs
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
+++ b/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FC4AE5-E9A6-4A43-B7A0-93E3B5508899}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90254492-0B15-4175-AB52-B1A603C76143}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4404,8 +4404,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B3:AF298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="R116" sqref="R116"/>
+    <sheetView tabSelected="1" topLeftCell="A265" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J285" sqref="J285"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -12038,7 +12038,7 @@
         <v>0.95</v>
       </c>
       <c r="G200" s="79">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="H200" s="86">
         <v>5</v>
@@ -12436,7 +12436,7 @@
         <v>0.95</v>
       </c>
       <c r="G210" s="79">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="H210" s="86">
         <v>5</v>
@@ -12937,8 +12937,8 @@
         <v>0.95</v>
       </c>
       <c r="G226" s="87">
-        <f t="shared" si="33"/>
-        <v>0.9</v>
+        <f>G200</f>
+        <v>0.8</v>
       </c>
       <c r="H226" s="81">
         <f t="shared" si="33"/>
@@ -13340,7 +13340,7 @@
       </c>
       <c r="G236" s="87">
         <f t="shared" si="33"/>
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="H236" s="81">
         <f t="shared" si="33"/>
@@ -13753,7 +13753,7 @@
         <v>0.95</v>
       </c>
       <c r="G250" s="79">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="H250" s="86">
         <v>5</v>
@@ -13939,7 +13939,7 @@
         <v>0.95</v>
       </c>
       <c r="G256" s="79">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="H256" s="86">
         <v>5</v>
@@ -14023,7 +14023,7 @@
         <v>0.95</v>
       </c>
       <c r="G258" s="79">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="H258" s="86">
         <v>5</v>
@@ -14257,7 +14257,7 @@
         <v>0.95</v>
       </c>
       <c r="G266" s="87">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="H266" s="81">
         <v>5</v>
@@ -14324,7 +14324,7 @@
         <v>0.95</v>
       </c>
       <c r="G268" s="87">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="H268" s="81">
         <v>5</v>
@@ -14491,7 +14491,7 @@
         <v>0.95</v>
       </c>
       <c r="G274" s="79">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="H274" s="86">
         <v>5</v>
@@ -14541,7 +14541,7 @@
         <v>0.95</v>
       </c>
       <c r="G276" s="79">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="H276" s="86">
         <v>5</v>

</xml_diff>

<commit_message>
Change START for heavy/medium electric  truck to 2025
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
+++ b/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Irish-TIMES-model\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90254492-0B15-4175-AB52-B1A603C76143}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{575768E3-5BA6-456A-8858-6826FDC1F181}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4404,8 +4404,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B3:AF298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A265" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J285" sqref="J285"/>
+    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E177" sqref="E177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -10664,8 +10664,8 @@
         <v>TRAF</v>
       </c>
       <c r="E168" s="1">
-        <f t="shared" si="20"/>
-        <v>2019</v>
+        <f>E176</f>
+        <v>2025</v>
       </c>
       <c r="F168" s="48">
         <v>6.5831632765410139E-2</v>
@@ -11153,7 +11153,7 @@
         <v>TRAF</v>
       </c>
       <c r="E176" s="49">
-        <v>2019</v>
+        <v>2025</v>
       </c>
       <c r="F176" s="48">
         <v>6.5831632765410139E-2</v>

</xml_diff>

<commit_message>
Update SubRES_TRA AF new cars
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
+++ b/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SubRES_TMPL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HannahD\Documents\GitHub\Irish-TIMES-model\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEDB45EC-5DB5-49FC-9671-B3C9575EDD19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF84600B-3192-4B33-AEAB-EA287513FF8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4530" yWindow="16050" windowWidth="19650" windowHeight="11070" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Commodities" sheetId="6" r:id="rId1"/>
@@ -35,10 +35,19 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={DD5752A7-7C11-45E4-A354-EAE94CA564A8}</author>
     <author>McDonagh, Shane</author>
   </authors>
   <commentList>
-    <comment ref="N158" authorId="0" shapeId="0" xr:uid="{B1EF7E76-3B15-41F9-828C-665E0AA36C10}">
+    <comment ref="Q104" authorId="0" shapeId="0" xr:uid="{DD5752A7-7C11-45E4-A354-EAE94CA564A8}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Changed to average 2018 vkm/car</t>
+      </text>
+    </comment>
+    <comment ref="N158" authorId="1" shapeId="0" xr:uid="{B1EF7E76-3B15-41F9-828C-665E0AA36C10}">
       <text>
         <r>
           <rPr>
@@ -62,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B173" authorId="0" shapeId="0" xr:uid="{D7F6B638-06DB-476A-9A7A-52F66837F5FA}">
+    <comment ref="B173" authorId="1" shapeId="0" xr:uid="{D7F6B638-06DB-476A-9A7A-52F66837F5FA}">
       <text>
         <r>
           <rPr>
@@ -86,7 +95,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B174" authorId="0" shapeId="0" xr:uid="{6D8EE3E3-F20A-4B40-AEF1-B0DBC49210F9}">
+    <comment ref="B174" authorId="1" shapeId="0" xr:uid="{6D8EE3E3-F20A-4B40-AEF1-B0DBC49210F9}">
       <text>
         <r>
           <rPr>
@@ -110,7 +119,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B175" authorId="0" shapeId="0" xr:uid="{F05AAF48-6722-4F63-9F4A-8F55BDFA5340}">
+    <comment ref="B175" authorId="1" shapeId="0" xr:uid="{F05AAF48-6722-4F63-9F4A-8F55BDFA5340}">
       <text>
         <r>
           <rPr>
@@ -134,7 +143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N175" authorId="0" shapeId="0" xr:uid="{94EFD0A5-4D87-471B-B4DE-580DE3E7310B}">
+    <comment ref="N175" authorId="1" shapeId="0" xr:uid="{94EFD0A5-4D87-471B-B4DE-580DE3E7310B}">
       <text>
         <r>
           <rPr>
@@ -158,7 +167,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B176" authorId="0" shapeId="0" xr:uid="{EB52D973-615A-43D8-8856-25EE78A9CC7E}">
+    <comment ref="B176" authorId="1" shapeId="0" xr:uid="{EB52D973-615A-43D8-8856-25EE78A9CC7E}">
       <text>
         <r>
           <rPr>
@@ -1451,7 +1460,7 @@
     <numFmt numFmtId="168" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="169" formatCode="_-* #,##0.000_-;\-* #,##0.000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="40" x14ac:knownFonts="1">
+  <fonts count="41" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1706,6 +1715,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="13">
@@ -2682,6 +2697,12 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Daly, Hannah E." id="{37EF901C-DE86-4021-A1F2-BBBCAC486477}" userId="S::h.daly@ucc.ie::524ee022-a37e-4c78-862e-198b12713a70" providerId="AD"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -3001,6 +3022,14 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="Q104" dT="2021-04-29T08:43:56.24" personId="{37EF901C-DE86-4021-A1F2-BBBCAC486477}" id="{DD5752A7-7C11-45E4-A354-EAE94CA564A8}">
+    <text>Changed to average 2018 vkm/car</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
@@ -4404,8 +4433,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B3:AF298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N149" sqref="N149"/>
+    <sheetView tabSelected="1" topLeftCell="F95" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q108" sqref="Q108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6650,7 +6679,7 @@
         <v>1.0145072391774981</v>
       </c>
       <c r="Q104" s="48">
-        <v>12.82</v>
+        <v>16.7</v>
       </c>
       <c r="R104" s="48">
         <v>1.49</v>
@@ -6720,7 +6749,7 @@
         <v>1.0915793541378127</v>
       </c>
       <c r="Q105" s="48">
-        <v>20.62</v>
+        <v>16.7</v>
       </c>
       <c r="R105" s="48">
         <v>1.49</v>
@@ -6787,8 +6816,7 @@
         <v>1.0915793541378127</v>
       </c>
       <c r="Q106" s="48">
-        <f>20.62</f>
-        <v>20.62</v>
+        <v>16.7</v>
       </c>
       <c r="R106" s="48">
         <v>1.49</v>
@@ -6855,7 +6883,7 @@
         <v>1.2315500000000001</v>
       </c>
       <c r="Q107" s="48">
-        <v>12.82</v>
+        <v>16.7</v>
       </c>
       <c r="R107" s="48">
         <v>1.49</v>
@@ -6922,7 +6950,7 @@
         <v>1.0145072391774981</v>
       </c>
       <c r="Q108" s="48">
-        <v>12.82</v>
+        <v>16.7</v>
       </c>
       <c r="R108" s="48">
         <v>1.49</v>
@@ -6989,8 +7017,7 @@
         <v>1.0915793541378127</v>
       </c>
       <c r="Q109" s="48">
-        <f>Q106</f>
-        <v>20.62</v>
+        <v>16.7</v>
       </c>
       <c r="R109" s="48">
         <v>1.49</v>
@@ -7057,8 +7084,7 @@
         <v>1.13845</v>
       </c>
       <c r="Q110" s="48">
-        <f>Q106</f>
-        <v>20.62</v>
+        <v>16.7</v>
       </c>
       <c r="R110" s="48">
         <v>1.49</v>
@@ -7125,8 +7151,7 @@
         <v>1.22845</v>
       </c>
       <c r="Q111" s="48">
-        <f>Q110</f>
-        <v>20.62</v>
+        <v>16.7</v>
       </c>
       <c r="R111" s="48">
         <v>1.49</v>
@@ -7193,8 +7218,7 @@
         <v>1.2685500000000003</v>
       </c>
       <c r="Q112" s="48">
-        <f>Q104</f>
-        <v>12.82</v>
+        <v>16.7</v>
       </c>
       <c r="R112" s="48">
         <v>1.49</v>
@@ -7261,8 +7285,7 @@
         <v>1.2685500000000003</v>
       </c>
       <c r="Q113" s="48">
-        <f>AVERAGE(Q112,Q114)</f>
-        <v>16.72</v>
+        <v>16.7</v>
       </c>
       <c r="R113" s="48">
         <v>1.49</v>
@@ -7329,8 +7352,7 @@
         <v>1.2685500000000003</v>
       </c>
       <c r="Q114" s="48">
-        <f>Q105</f>
-        <v>20.62</v>
+        <v>16.7</v>
       </c>
       <c r="R114" s="48">
         <v>1.49</v>
@@ -7397,8 +7419,7 @@
         <v>1.3688500000000001</v>
       </c>
       <c r="Q115" s="48">
-        <f>Q112</f>
-        <v>12.82</v>
+        <v>16.7</v>
       </c>
       <c r="R115" s="48">
         <v>1.49</v>
@@ -7465,8 +7486,7 @@
         <v>1.3688500000000001</v>
       </c>
       <c r="Q116" s="48">
-        <f t="shared" ref="Q116:Q117" si="3">Q113</f>
-        <v>16.72</v>
+        <v>16.7</v>
       </c>
       <c r="R116" s="48">
         <v>1.49</v>
@@ -7533,8 +7553,7 @@
         <v>1.3688500000000001</v>
       </c>
       <c r="Q117" s="48">
-        <f t="shared" si="3"/>
-        <v>20.62</v>
+        <v>16.7</v>
       </c>
       <c r="R117" s="48">
         <v>1.49</v>
@@ -7601,8 +7620,7 @@
         <v>1.2323000000000002</v>
       </c>
       <c r="Q118" s="48">
-        <f>Q115</f>
-        <v>12.82</v>
+        <v>16.7</v>
       </c>
       <c r="R118" s="48">
         <v>1.49</v>
@@ -7669,8 +7687,7 @@
         <v>1.2323000000000002</v>
       </c>
       <c r="Q119" s="48">
-        <f t="shared" ref="Q119:Q120" si="4">Q116</f>
-        <v>16.72</v>
+        <v>16.7</v>
       </c>
       <c r="R119" s="48">
         <v>1.49</v>
@@ -7737,8 +7754,7 @@
         <v>1.2323000000000002</v>
       </c>
       <c r="Q120" s="48">
-        <f t="shared" si="4"/>
-        <v>20.62</v>
+        <v>16.7</v>
       </c>
       <c r="R120" s="48">
         <v>1.49</v>
@@ -7805,8 +7821,7 @@
         <v>1.2398000000000002</v>
       </c>
       <c r="Q121" s="48">
-        <f>Q106</f>
-        <v>20.62</v>
+        <v>16.7</v>
       </c>
       <c r="R121" s="48">
         <v>1.49</v>
@@ -7873,8 +7888,7 @@
         <v>1.2398000000000002</v>
       </c>
       <c r="Q122" s="48">
-        <f>Q106</f>
-        <v>20.62</v>
+        <v>16.7</v>
       </c>
       <c r="R122" s="48">
         <v>1.49</v>
@@ -7914,7 +7928,7 @@
     </row>
     <row r="124" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B124" s="1" t="str">
-        <f t="shared" ref="B124:B142" si="5">D30</f>
+        <f t="shared" ref="B124:B142" si="3">D30</f>
         <v>T-TAX-ICE_GSL31</v>
       </c>
       <c r="C124" s="1" t="str">
@@ -7981,7 +7995,7 @@
     </row>
     <row r="125" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B125" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>T-TAX-ICE_DST31</v>
       </c>
       <c r="C125" s="1" t="str">
@@ -8008,7 +8022,7 @@
         <v>21.831587082756254</v>
       </c>
       <c r="J125" s="48">
-        <f t="shared" ref="J125:J142" si="6">AVERAGE(I125,K125)</f>
+        <f t="shared" ref="J125:J142" si="4">AVERAGE(I125,K125)</f>
         <v>21.831587082756254</v>
       </c>
       <c r="K125" s="48">
@@ -8049,7 +8063,7 @@
     </row>
     <row r="126" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B126" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>T-TAX-ICE_DF31</v>
       </c>
       <c r="C126" s="1" t="str">
@@ -8076,7 +8090,7 @@
         <v>21.831587082756254</v>
       </c>
       <c r="J126" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>21.831587082756254</v>
       </c>
       <c r="K126" s="48">
@@ -8099,7 +8113,7 @@
         <v>1.0915793541378127</v>
       </c>
       <c r="Q126" s="48">
-        <f t="shared" ref="Q126:Q142" si="7">Q125</f>
+        <f t="shared" ref="Q126:Q142" si="5">Q125</f>
         <v>39.93</v>
       </c>
       <c r="R126" s="48">
@@ -8117,7 +8131,7 @@
     </row>
     <row r="127" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B127" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>T-TAX-ICE_NGB31</v>
       </c>
       <c r="C127" s="1" t="str">
@@ -8144,7 +8158,7 @@
         <v>24.631</v>
       </c>
       <c r="J127" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>24.631</v>
       </c>
       <c r="K127" s="48">
@@ -8167,7 +8181,7 @@
         <v>1.2315500000000001</v>
       </c>
       <c r="Q127" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>39.93</v>
       </c>
       <c r="R127" s="48">
@@ -8185,7 +8199,7 @@
     </row>
     <row r="128" spans="2:24" x14ac:dyDescent="0.2">
       <c r="B128" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>T-TAX-ICE_E8531</v>
       </c>
       <c r="C128" s="1" t="str">
@@ -8212,7 +8226,7 @@
         <v>20.290144783549959</v>
       </c>
       <c r="J128" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>20.290144783549959</v>
       </c>
       <c r="K128" s="48">
@@ -8235,7 +8249,7 @@
         <v>1.0145072391774981</v>
       </c>
       <c r="Q128" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>39.93</v>
       </c>
       <c r="R128" s="48">
@@ -8253,7 +8267,7 @@
     </row>
     <row r="129" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B129" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>T-TAX-ICE_B10031</v>
       </c>
       <c r="C129" s="1" t="str">
@@ -8280,7 +8294,7 @@
         <v>21.831587082756254</v>
       </c>
       <c r="J129" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>21.831587082756254</v>
       </c>
       <c r="K129" s="48">
@@ -8303,7 +8317,7 @@
         <v>1.0915793541378127</v>
       </c>
       <c r="Q129" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>39.93</v>
       </c>
       <c r="R129" s="48">
@@ -8318,7 +8332,7 @@
     </row>
     <row r="130" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B130" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>T-TAX-HEV_GSL31</v>
       </c>
       <c r="C130" s="1" t="str">
@@ -8345,7 +8359,7 @@
         <v>23.751999999999999</v>
       </c>
       <c r="J130" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>23.613999999999997</v>
       </c>
       <c r="K130" s="48">
@@ -8368,7 +8382,7 @@
         <v>1.13845</v>
       </c>
       <c r="Q130" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>39.93</v>
       </c>
       <c r="R130" s="48">
@@ -8383,7 +8397,7 @@
     </row>
     <row r="131" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B131" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>T-TAX-HEV_DST31</v>
       </c>
       <c r="C131" s="1" t="str">
@@ -8410,7 +8424,7 @@
         <v>25.646000000000001</v>
       </c>
       <c r="J131" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>25.489000000000001</v>
       </c>
       <c r="K131" s="48">
@@ -8433,7 +8447,7 @@
         <v>1.22845</v>
       </c>
       <c r="Q131" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>39.93</v>
       </c>
       <c r="R131" s="48">
@@ -8448,7 +8462,7 @@
     </row>
     <row r="132" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B132" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>T-TAX-PHEV10_GSL31</v>
       </c>
       <c r="C132" s="1" t="str">
@@ -8475,7 +8489,7 @@
         <v>30.9495</v>
       </c>
       <c r="J132" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>28.889250000000001</v>
       </c>
       <c r="K132" s="48">
@@ -8498,7 +8512,7 @@
         <v>1.2685500000000003</v>
       </c>
       <c r="Q132" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>39.93</v>
       </c>
       <c r="R132" s="48">
@@ -8513,7 +8527,7 @@
     </row>
     <row r="133" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B133" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>T-TAX-PHEV20_GSL31</v>
       </c>
       <c r="C133" s="1" t="str">
@@ -8540,7 +8554,7 @@
         <v>30.9495</v>
       </c>
       <c r="J133" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>28.889250000000001</v>
       </c>
       <c r="K133" s="48">
@@ -8563,7 +8577,7 @@
         <v>1.2685500000000003</v>
       </c>
       <c r="Q133" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>39.93</v>
       </c>
       <c r="R133" s="48">
@@ -8578,7 +8592,7 @@
     </row>
     <row r="134" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B134" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>T-TAX-PHEV40_GSL31</v>
       </c>
       <c r="C134" s="1" t="str">
@@ -8605,7 +8619,7 @@
         <v>30.9495</v>
       </c>
       <c r="J134" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>28.889250000000001</v>
       </c>
       <c r="K134" s="48">
@@ -8628,7 +8642,7 @@
         <v>1.2685500000000003</v>
       </c>
       <c r="Q134" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>39.93</v>
       </c>
       <c r="R134" s="48">
@@ -8643,7 +8657,7 @@
     </row>
     <row r="135" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B135" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>T-TAX-PHEV10_DST31</v>
       </c>
       <c r="C135" s="1" t="str">
@@ -8670,7 +8684,7 @@
         <v>33.423499999999997</v>
       </c>
       <c r="J135" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>31.186749999999996</v>
       </c>
       <c r="K135" s="48">
@@ -8693,7 +8707,7 @@
         <v>1.3688500000000001</v>
       </c>
       <c r="Q135" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>39.93</v>
       </c>
       <c r="R135" s="48">
@@ -8708,7 +8722,7 @@
     </row>
     <row r="136" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B136" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>T-TAX-PHEV20_DST31</v>
       </c>
       <c r="C136" s="1" t="str">
@@ -8735,7 +8749,7 @@
         <v>33.423499999999997</v>
       </c>
       <c r="J136" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>31.186749999999996</v>
       </c>
       <c r="K136" s="48">
@@ -8758,7 +8772,7 @@
         <v>1.3688500000000001</v>
       </c>
       <c r="Q136" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>39.93</v>
       </c>
       <c r="R136" s="48">
@@ -8773,7 +8787,7 @@
     </row>
     <row r="137" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B137" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>T-TAX-PHEV40_DST31</v>
       </c>
       <c r="C137" s="1" t="str">
@@ -8800,7 +8814,7 @@
         <v>33.423499999999997</v>
       </c>
       <c r="J137" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>31.186749999999996</v>
       </c>
       <c r="K137" s="48">
@@ -8823,7 +8837,7 @@
         <v>1.3688500000000001</v>
       </c>
       <c r="Q137" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>39.93</v>
       </c>
       <c r="R137" s="48">
@@ -8838,7 +8852,7 @@
     </row>
     <row r="138" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B138" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>T-TAX-BEV100_ELC31</v>
       </c>
       <c r="C138" s="1" t="str">
@@ -8865,7 +8879,7 @@
         <v>32.970999999999997</v>
       </c>
       <c r="J138" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>30.275999999999996</v>
       </c>
       <c r="K138" s="48">
@@ -8888,7 +8902,7 @@
         <v>1.2323000000000002</v>
       </c>
       <c r="Q138" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>39.93</v>
       </c>
       <c r="R138" s="48">
@@ -8903,7 +8917,7 @@
     </row>
     <row r="139" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B139" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>T-TAX-BEV150_ELC31</v>
       </c>
       <c r="C139" s="1" t="str">
@@ -8930,7 +8944,7 @@
         <v>32.970999999999997</v>
       </c>
       <c r="J139" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>30.275999999999996</v>
       </c>
       <c r="K139" s="48">
@@ -8953,7 +8967,7 @@
         <v>1.2323000000000002</v>
       </c>
       <c r="Q139" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>39.93</v>
       </c>
       <c r="R139" s="48">
@@ -8968,7 +8982,7 @@
     </row>
     <row r="140" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B140" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>T-TAX-BEV250_ELC31</v>
       </c>
       <c r="C140" s="1" t="str">
@@ -8995,7 +9009,7 @@
         <v>32.970999999999997</v>
       </c>
       <c r="J140" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>30.275999999999996</v>
       </c>
       <c r="K140" s="48">
@@ -9018,7 +9032,7 @@
         <v>1.2323000000000002</v>
       </c>
       <c r="Q140" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>39.93</v>
       </c>
       <c r="R140" s="48">
@@ -9033,7 +9047,7 @@
     </row>
     <row r="141" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B141" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>T-TAX-ICE_HYD31</v>
       </c>
       <c r="C141" s="1" t="str">
@@ -9060,7 +9074,7 @@
         <v>60.819000000000003</v>
       </c>
       <c r="J141" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>46.0015</v>
       </c>
       <c r="K141" s="48">
@@ -9083,7 +9097,7 @@
         <v>1.2398000000000002</v>
       </c>
       <c r="Q141" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>39.93</v>
       </c>
       <c r="R141" s="48">
@@ -9098,7 +9112,7 @@
     </row>
     <row r="142" spans="2:20" x14ac:dyDescent="0.2">
       <c r="B142" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>T-TAX-FCV_HYD31</v>
       </c>
       <c r="C142" s="1" t="str">
@@ -9125,7 +9139,7 @@
         <v>60.819000000000003</v>
       </c>
       <c r="J142" s="48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>46.0015</v>
       </c>
       <c r="K142" s="48">
@@ -9148,7 +9162,7 @@
         <v>1.2398000000000002</v>
       </c>
       <c r="Q142" s="48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>39.93</v>
       </c>
       <c r="R142" s="48">
@@ -9277,14 +9291,14 @@
         <v>109.959</v>
       </c>
       <c r="J145" s="48">
-        <f t="shared" ref="J145:J148" si="8">AVERAGE(I145,K145)</f>
+        <f t="shared" ref="J145:J148" si="6">AVERAGE(I145,K145)</f>
         <v>111.762</v>
       </c>
       <c r="K145" s="48">
         <v>113.565</v>
       </c>
       <c r="L145" s="48">
-        <f t="shared" ref="L145:L160" si="9">K145-((K145-M145)/4)</f>
+        <f t="shared" ref="L145:L160" si="7">K145-((K145-M145)/4)</f>
         <v>113.565</v>
       </c>
       <c r="M145" s="48">
@@ -9341,14 +9355,14 @@
         <v>109.959</v>
       </c>
       <c r="J146" s="48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>111.762</v>
       </c>
       <c r="K146" s="48">
         <v>113.565</v>
       </c>
       <c r="L146" s="48">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>113.565</v>
       </c>
       <c r="M146" s="48">
@@ -9405,14 +9419,14 @@
         <v>397.21899999999999</v>
       </c>
       <c r="J147" s="48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>323.60950000000003</v>
       </c>
       <c r="K147" s="48">
         <v>250</v>
       </c>
       <c r="L147" s="48">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>220</v>
       </c>
       <c r="M147" s="48">
@@ -9469,14 +9483,14 @@
         <v>397.21899999999999</v>
       </c>
       <c r="J148" s="48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>352.79750000000001</v>
       </c>
       <c r="K148" s="48">
         <v>308.37599999999998</v>
       </c>
       <c r="L148" s="48">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>263.95425</v>
       </c>
       <c r="M148" s="48">
@@ -9563,7 +9577,7 @@
         <v>231.58335558726841</v>
       </c>
       <c r="L150" s="48">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>231.58335558726841</v>
       </c>
       <c r="M150" s="48">
@@ -9620,14 +9634,14 @@
         <v>935.5223742338045</v>
       </c>
       <c r="J151" s="48">
-        <f t="shared" ref="J151:J152" si="10">AVERAGE(I151,K151)</f>
+        <f t="shared" ref="J151:J152" si="8">AVERAGE(I151,K151)</f>
         <v>935.5223742338045</v>
       </c>
       <c r="K151" s="48">
         <v>935.5223742338045</v>
       </c>
       <c r="L151" s="48">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>935.5223742338045</v>
       </c>
       <c r="M151" s="48">
@@ -9684,14 +9698,14 @@
         <v>989.2715097553122</v>
       </c>
       <c r="J152" s="48">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>989.2715097553122</v>
       </c>
       <c r="K152" s="48">
         <v>989.2715097553122</v>
       </c>
       <c r="L152" s="48">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>989.2715097553122</v>
       </c>
       <c r="M152" s="48">
@@ -9744,7 +9758,7 @@
     </row>
     <row r="154" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B154" s="1" t="str">
-        <f t="shared" ref="B154:B160" si="11">D60</f>
+        <f t="shared" ref="B154:B160" si="9">D60</f>
         <v>T-LGT-ICE_DST61</v>
       </c>
       <c r="C154" s="1" t="str">
@@ -9778,7 +9792,7 @@
         <v>24.664999999999999</v>
       </c>
       <c r="L154" s="48">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>24.664999999999999</v>
       </c>
       <c r="M154" s="50">
@@ -9808,7 +9822,7 @@
     </row>
     <row r="155" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B155" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>T-LGT-HEV_DST61</v>
       </c>
       <c r="C155" s="1" t="str">
@@ -9835,14 +9849,14 @@
         <v>26.946999999999999</v>
       </c>
       <c r="J155" s="48">
-        <f t="shared" ref="J155:J160" si="12">AVERAGE(I155,K155)</f>
+        <f t="shared" ref="J155:J160" si="10">AVERAGE(I155,K155)</f>
         <v>27.027999999999999</v>
       </c>
       <c r="K155" s="50">
         <v>27.109000000000002</v>
       </c>
       <c r="L155" s="48">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>26.498000000000001</v>
       </c>
       <c r="M155" s="50">
@@ -9872,7 +9886,7 @@
     </row>
     <row r="156" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B156" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>T-LGT-PHEV_DST61</v>
       </c>
       <c r="C156" s="1" t="str">
@@ -9880,7 +9894,7 @@
         <v>TRADST,TRAELC</v>
       </c>
       <c r="D156" s="49" t="str">
-        <f t="shared" ref="D156:D160" si="13">D155</f>
+        <f t="shared" ref="D156:D160" si="11">D155</f>
         <v>TRAF</v>
       </c>
       <c r="E156" s="49">
@@ -9899,14 +9913,14 @@
         <v>33.524000000000001</v>
       </c>
       <c r="J156" s="48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>31.293500000000002</v>
       </c>
       <c r="K156" s="50">
         <v>29.062999999999999</v>
       </c>
       <c r="L156" s="48">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>28.66825</v>
       </c>
       <c r="M156" s="50">
@@ -9936,7 +9950,7 @@
     </row>
     <row r="157" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B157" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>T-LGT-ICE_NGB61</v>
       </c>
       <c r="C157" s="1" t="str">
@@ -9944,7 +9958,7 @@
         <v>TRACNG,TRABNG</v>
       </c>
       <c r="D157" s="49" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>TRAF</v>
       </c>
       <c r="E157" s="49">
@@ -9963,14 +9977,14 @@
         <v>28.097999999999999</v>
       </c>
       <c r="J157" s="48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>26.765499999999999</v>
       </c>
       <c r="K157" s="50">
         <v>25.433</v>
       </c>
       <c r="L157" s="48">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>25.394750000000002</v>
       </c>
       <c r="M157" s="50">
@@ -10000,7 +10014,7 @@
     </row>
     <row r="158" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B158" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>T-LGT-PHEV_NGB61</v>
       </c>
       <c r="C158" s="1" t="str">
@@ -10008,7 +10022,7 @@
         <v>TRACNG,TRAELC</v>
       </c>
       <c r="D158" s="49" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>TRAF</v>
       </c>
       <c r="E158" s="49">
@@ -10027,14 +10041,14 @@
         <v>36.548000000000002</v>
       </c>
       <c r="J158" s="48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>33.258000000000003</v>
       </c>
       <c r="K158" s="50">
         <v>29.968</v>
       </c>
       <c r="L158" s="48">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>29.539249999999999</v>
       </c>
       <c r="M158" s="50">
@@ -10064,7 +10078,7 @@
     </row>
     <row r="159" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B159" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>T-LGT-FCV_HYD61</v>
       </c>
       <c r="C159" s="1" t="str">
@@ -10072,7 +10086,7 @@
         <v>TRAH2</v>
       </c>
       <c r="D159" s="49" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>TRAF</v>
       </c>
       <c r="E159" s="49">
@@ -10091,14 +10105,14 @@
         <v>56.146000000000001</v>
       </c>
       <c r="J159" s="48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>44.363</v>
       </c>
       <c r="K159" s="50">
         <v>32.58</v>
       </c>
       <c r="L159" s="48">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>30.911749999999998</v>
       </c>
       <c r="M159" s="50">
@@ -10128,7 +10142,7 @@
     </row>
     <row r="160" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B160" s="1" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>T-LGT-BEV_ELC61</v>
       </c>
       <c r="C160" s="1" t="str">
@@ -10136,7 +10150,7 @@
         <v>TRAELC</v>
       </c>
       <c r="D160" s="49" t="str">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>TRAF</v>
       </c>
       <c r="E160" s="49">
@@ -10155,14 +10169,14 @@
         <v>32.17</v>
       </c>
       <c r="J160" s="48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>30.351500000000001</v>
       </c>
       <c r="K160" s="50">
         <v>28.533000000000001</v>
       </c>
       <c r="L160" s="48">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>27.774000000000001</v>
       </c>
       <c r="M160" s="50">
@@ -10216,7 +10230,7 @@
     </row>
     <row r="162" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B162" s="1" t="str">
-        <f t="shared" ref="B162:B168" si="14">D68</f>
+        <f t="shared" ref="B162:B168" si="12">D68</f>
         <v>T-MGT-ICE_DST71</v>
       </c>
       <c r="C162" s="1" t="str">
@@ -10228,7 +10242,7 @@
         <v>TRAF</v>
       </c>
       <c r="E162" s="1">
-        <f t="shared" ref="E162:I162" si="15">E170</f>
+        <f t="shared" ref="E162:I162" si="13">E170</f>
         <v>2019</v>
       </c>
       <c r="F162" s="48">
@@ -10241,7 +10255,7 @@
         <v>2.9785493787231682E-2</v>
       </c>
       <c r="I162" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>95.69</v>
       </c>
       <c r="J162" s="48">
@@ -10249,27 +10263,27 @@
         <v>98.32</v>
       </c>
       <c r="K162" s="1">
-        <f t="shared" ref="K162:K168" si="16">K170</f>
+        <f t="shared" ref="K162:K168" si="14">K170</f>
         <v>100.95</v>
       </c>
       <c r="L162" s="48">
-        <f t="shared" ref="L162:L168" si="17">K162-((K162-M162)/4)</f>
+        <f t="shared" ref="L162:L168" si="15">K162-((K162-M162)/4)</f>
         <v>100.95</v>
       </c>
       <c r="M162" s="1">
-        <f t="shared" ref="M162:P168" si="18">M170</f>
+        <f t="shared" ref="M162:P168" si="16">M170</f>
         <v>100.95</v>
       </c>
       <c r="N162" s="48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>2.1157042474212369</v>
       </c>
       <c r="O162" s="48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>2.1689507539373367</v>
       </c>
       <c r="P162" s="48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>2.1689507539373367</v>
       </c>
       <c r="Q162" s="48">
@@ -10282,13 +10296,13 @@
         <v>20</v>
       </c>
       <c r="T162" s="1">
-        <f t="shared" ref="T162:T168" si="19">T170</f>
+        <f t="shared" ref="T162:T168" si="17">T170</f>
         <v>1E-3</v>
       </c>
     </row>
     <row r="163" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B163" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>T-MGT-HEV_DST71</v>
       </c>
       <c r="C163" s="1" t="str">
@@ -10300,7 +10314,7 @@
         <v>TRAF</v>
       </c>
       <c r="E163" s="1">
-        <f t="shared" ref="C163:I168" si="20">E171</f>
+        <f t="shared" ref="C163:I168" si="18">E171</f>
         <v>2019</v>
       </c>
       <c r="F163" s="48">
@@ -10313,15 +10327,15 @@
         <v>4.2496500690063034E-2</v>
       </c>
       <c r="I163" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>124.73</v>
       </c>
       <c r="J163" s="48">
-        <f t="shared" ref="J163:J168" si="21">AVERAGE(I163,K163)</f>
+        <f t="shared" ref="J163:J168" si="19">AVERAGE(I163,K163)</f>
         <v>124.92500000000001</v>
       </c>
       <c r="K163" s="1">
-        <f t="shared" si="16"/>
+        <f t="shared" si="14"/>
         <v>125.12</v>
       </c>
       <c r="L163" s="48">
@@ -10329,19 +10343,19 @@
         <v>123.88250000000001</v>
       </c>
       <c r="M163" s="1">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>120.17</v>
       </c>
       <c r="N163" s="48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>3.5721072259038325</v>
       </c>
       <c r="O163" s="48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>3.0618061936318557</v>
       </c>
       <c r="P163" s="48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>2.3858458293310703</v>
       </c>
       <c r="Q163" s="48">
@@ -10355,21 +10369,21 @@
         <v>20</v>
       </c>
       <c r="T163" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>1E-3</v>
       </c>
     </row>
     <row r="164" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B164" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>T-MGT-FCV_HYD71</v>
       </c>
       <c r="C164" s="1" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>TRAH2</v>
       </c>
       <c r="D164" s="1" t="str">
-        <f t="shared" ref="D164:D168" si="22">D163</f>
+        <f t="shared" ref="D164:D168" si="20">D163</f>
         <v>TRAF</v>
       </c>
       <c r="E164" s="1">
@@ -10385,55 +10399,55 @@
         <v>4.9705728485698729E-2</v>
       </c>
       <c r="I164" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>345.67</v>
       </c>
       <c r="J164" s="48">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>283.94499999999999</v>
       </c>
       <c r="K164" s="1">
+        <f t="shared" si="14"/>
+        <v>222.22</v>
+      </c>
+      <c r="L164" s="48">
+        <f t="shared" si="15"/>
+        <v>195.70750000000001</v>
+      </c>
+      <c r="M164" s="1">
         <f t="shared" si="16"/>
-        <v>222.22</v>
-      </c>
-      <c r="L164" s="48">
-        <f t="shared" si="17"/>
-        <v>195.70750000000001</v>
-      </c>
-      <c r="M164" s="1">
-        <f t="shared" si="18"/>
         <v>116.17</v>
       </c>
       <c r="N164" s="48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>3.5721072259038325</v>
       </c>
       <c r="O164" s="48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>3.0618061936318557</v>
       </c>
       <c r="P164" s="48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>2.3858458293310703</v>
       </c>
       <c r="Q164" s="48">
         <v>29.397500000000001</v>
       </c>
       <c r="R164" s="50">
-        <f t="shared" ref="R164:R168" si="23">R163</f>
+        <f t="shared" ref="R164:R168" si="21">R163</f>
         <v>3.592571901094749</v>
       </c>
       <c r="S164" s="1">
         <v>20</v>
       </c>
       <c r="T164" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>1E-3</v>
       </c>
     </row>
     <row r="165" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B165" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>T-MGT-ICE_NGB71</v>
       </c>
       <c r="C165" s="1" t="str">
@@ -10441,11 +10455,11 @@
         <v>TRACNG,TRABNG</v>
       </c>
       <c r="D165" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>TRAF</v>
       </c>
       <c r="E165" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>2019</v>
       </c>
       <c r="F165" s="48">
@@ -10458,55 +10472,55 @@
         <v>2.9406060745356118E-2</v>
       </c>
       <c r="I165" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>115.69</v>
       </c>
       <c r="J165" s="48">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>118.32</v>
       </c>
       <c r="K165" s="1">
+        <f t="shared" si="14"/>
+        <v>120.95</v>
+      </c>
+      <c r="L165" s="48">
+        <f t="shared" si="15"/>
+        <v>120.95</v>
+      </c>
+      <c r="M165" s="1">
         <f t="shared" si="16"/>
         <v>120.95</v>
       </c>
-      <c r="L165" s="48">
-        <f t="shared" si="17"/>
-        <v>120.95</v>
-      </c>
-      <c r="M165" s="1">
-        <f t="shared" si="18"/>
-        <v>120.95</v>
-      </c>
       <c r="N165" s="48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>5.0989820625747049</v>
       </c>
       <c r="O165" s="48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>3.5538821890369761</v>
       </c>
       <c r="P165" s="48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>2.3292245236828353</v>
       </c>
       <c r="Q165" s="48">
         <v>29.397500000000001</v>
       </c>
       <c r="R165" s="50">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>3.592571901094749</v>
       </c>
       <c r="S165" s="1">
         <v>20</v>
       </c>
       <c r="T165" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>1E-3</v>
       </c>
     </row>
     <row r="166" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B166" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>T-MGT-HEV_NGB71</v>
       </c>
       <c r="C166" s="1" t="str">
@@ -10514,11 +10528,11 @@
         <v>TRACNG,TRABNG</v>
       </c>
       <c r="D166" s="1" t="str">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>TRAF</v>
       </c>
       <c r="E166" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>2019</v>
       </c>
       <c r="F166" s="48">
@@ -10531,67 +10545,67 @@
         <v>4.211706764818747E-2</v>
       </c>
       <c r="I166" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>144.72999999999999</v>
       </c>
       <c r="J166" s="48">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>144.92500000000001</v>
       </c>
       <c r="K166" s="1">
+        <f t="shared" si="14"/>
+        <v>145.12</v>
+      </c>
+      <c r="L166" s="48">
+        <f t="shared" si="15"/>
+        <v>143.88249999999999</v>
+      </c>
+      <c r="M166" s="1">
         <f t="shared" si="16"/>
-        <v>145.12</v>
-      </c>
-      <c r="L166" s="48">
-        <f t="shared" si="17"/>
-        <v>143.88249999999999</v>
-      </c>
-      <c r="M166" s="1">
-        <f t="shared" si="18"/>
         <v>140.16999999999999</v>
       </c>
       <c r="N166" s="48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>5.0989820625747049</v>
       </c>
       <c r="O166" s="48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>3.5538821890369761</v>
       </c>
       <c r="P166" s="48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>2.3292245236828353</v>
       </c>
       <c r="Q166" s="48">
         <v>29.397500000000001</v>
       </c>
       <c r="R166" s="50">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>3.592571901094749</v>
       </c>
       <c r="S166" s="1">
         <v>20</v>
       </c>
       <c r="T166" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>1E-3</v>
       </c>
     </row>
     <row r="167" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B167" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>T-MGT-ICE_LNG71</v>
       </c>
       <c r="C167" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>TRALNG</v>
+      </c>
+      <c r="D167" s="1" t="str">
         <f t="shared" si="20"/>
-        <v>TRALNG</v>
-      </c>
-      <c r="D167" s="1" t="str">
-        <f t="shared" si="22"/>
         <v>TRAF</v>
       </c>
       <c r="E167" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>2019</v>
       </c>
       <c r="F167" s="48">
@@ -10604,63 +10618,63 @@
         <v>2.9406060745356118E-2</v>
       </c>
       <c r="I167" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>130.68600000000001</v>
       </c>
       <c r="J167" s="48">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>129.72200000000001</v>
       </c>
       <c r="K167" s="1">
+        <f t="shared" si="14"/>
+        <v>128.75800000000001</v>
+      </c>
+      <c r="L167" s="48">
+        <f t="shared" si="15"/>
+        <v>128.11425</v>
+      </c>
+      <c r="M167" s="1">
         <f t="shared" si="16"/>
-        <v>128.75800000000001</v>
-      </c>
-      <c r="L167" s="48">
-        <f t="shared" si="17"/>
-        <v>128.11425</v>
-      </c>
-      <c r="M167" s="1">
-        <f t="shared" si="18"/>
         <v>126.18300000000001</v>
       </c>
       <c r="N167" s="48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>5.0989820625747049</v>
       </c>
       <c r="O167" s="48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>3.5538821890369761</v>
       </c>
       <c r="P167" s="48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>2.3292245236828353</v>
       </c>
       <c r="Q167" s="48">
         <v>29.397500000000001</v>
       </c>
       <c r="R167" s="50">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>3.592571901094749</v>
       </c>
       <c r="S167" s="1">
         <v>20</v>
       </c>
       <c r="T167" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>1E-3</v>
       </c>
     </row>
     <row r="168" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B168" s="1" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>T-MGT-BEV_ELC71</v>
       </c>
       <c r="C168" s="1" t="str">
+        <f t="shared" si="18"/>
+        <v>TRAELC</v>
+      </c>
+      <c r="D168" s="1" t="str">
         <f t="shared" si="20"/>
-        <v>TRAELC</v>
-      </c>
-      <c r="D168" s="1" t="str">
-        <f t="shared" si="22"/>
         <v>TRAF</v>
       </c>
       <c r="E168" s="1">
@@ -10677,49 +10691,49 @@
         <v>6.5831632765410139E-2</v>
       </c>
       <c r="I168" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="18"/>
         <v>345.67</v>
       </c>
       <c r="J168" s="48">
-        <f t="shared" si="21"/>
+        <f t="shared" si="19"/>
         <v>309.89</v>
       </c>
       <c r="K168" s="1">
+        <f t="shared" si="14"/>
+        <v>274.11</v>
+      </c>
+      <c r="L168" s="48">
+        <f t="shared" si="15"/>
+        <v>234.625</v>
+      </c>
+      <c r="M168" s="1">
         <f t="shared" si="16"/>
-        <v>274.11</v>
-      </c>
-      <c r="L168" s="48">
-        <f t="shared" si="17"/>
-        <v>234.625</v>
-      </c>
-      <c r="M168" s="1">
-        <f t="shared" si="18"/>
         <v>116.17</v>
       </c>
       <c r="N168" s="48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>3.5721072259038325</v>
       </c>
       <c r="O168" s="48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>3.0618061936318557</v>
       </c>
       <c r="P168" s="48">
-        <f t="shared" si="18"/>
+        <f t="shared" si="16"/>
         <v>2.3858458293310703</v>
       </c>
       <c r="Q168" s="48">
         <v>29.397500000000001</v>
       </c>
       <c r="R168" s="50">
-        <f t="shared" si="23"/>
+        <f t="shared" si="21"/>
         <v>3.592571901094749</v>
       </c>
       <c r="S168" s="1">
         <v>20</v>
       </c>
       <c r="T168" s="1">
-        <f t="shared" si="19"/>
+        <f t="shared" si="17"/>
         <v>1E-3</v>
       </c>
     </row>
@@ -10748,7 +10762,7 @@
     </row>
     <row r="170" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B170" s="1" t="str">
-        <f t="shared" ref="B170:B176" si="24">D76</f>
+        <f t="shared" ref="B170:B176" si="22">D76</f>
         <v>T-HGT-ICE_DST81</v>
       </c>
       <c r="C170" s="1" t="str">
@@ -10782,7 +10796,7 @@
         <v>100.95</v>
       </c>
       <c r="L170" s="48">
-        <f t="shared" ref="L170:L176" si="25">K170-((K170-M170)/4)</f>
+        <f t="shared" ref="L170:L176" si="23">K170-((K170-M170)/4)</f>
         <v>100.95</v>
       </c>
       <c r="M170" s="50">
@@ -10813,7 +10827,7 @@
     </row>
     <row r="171" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B171" s="1" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>T-HGT-HEV_DST81</v>
       </c>
       <c r="C171" s="1" t="str">
@@ -10840,14 +10854,14 @@
         <v>124.73</v>
       </c>
       <c r="J171" s="48">
-        <f t="shared" ref="J171:J176" si="26">AVERAGE(I171,K171)</f>
+        <f t="shared" ref="J171:J176" si="24">AVERAGE(I171,K171)</f>
         <v>124.92500000000001</v>
       </c>
       <c r="K171" s="50">
         <v>125.12</v>
       </c>
       <c r="L171" s="48">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>123.88250000000001</v>
       </c>
       <c r="M171" s="50">
@@ -10879,7 +10893,7 @@
     </row>
     <row r="172" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B172" s="1" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>T-HGT-FCV_HYD81</v>
       </c>
       <c r="C172" s="1" t="str">
@@ -10887,7 +10901,7 @@
         <v>TRAH2</v>
       </c>
       <c r="D172" s="49" t="str">
-        <f t="shared" ref="D172:D176" si="27">D171</f>
+        <f t="shared" ref="D172:D176" si="25">D171</f>
         <v>TRAF</v>
       </c>
       <c r="E172" s="49">
@@ -10906,14 +10920,14 @@
         <v>345.67</v>
       </c>
       <c r="J172" s="48">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>283.94499999999999</v>
       </c>
       <c r="K172" s="50">
         <v>222.22</v>
       </c>
       <c r="L172" s="48">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>195.70750000000001</v>
       </c>
       <c r="M172" s="50">
@@ -10932,7 +10946,7 @@
         <v>50.915999999999997</v>
       </c>
       <c r="R172" s="50">
-        <f t="shared" ref="R172:R176" si="28">R171</f>
+        <f t="shared" ref="R172:R176" si="26">R171</f>
         <v>9.2231504438872829</v>
       </c>
       <c r="S172" s="49">
@@ -10945,7 +10959,7 @@
     </row>
     <row r="173" spans="2:22" x14ac:dyDescent="0.2">
       <c r="B173" s="1" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>T-HGT-ICE_NGB81</v>
       </c>
       <c r="C173" s="1" t="str">
@@ -10953,7 +10967,7 @@
         <v>TRACNG,TRABNG</v>
       </c>
       <c r="D173" s="49" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>TRAF</v>
       </c>
       <c r="E173" s="49">
@@ -10972,14 +10986,14 @@
         <v>115.69</v>
       </c>
       <c r="J173" s="48">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>118.32</v>
       </c>
       <c r="K173" s="50">
         <v>120.95</v>
       </c>
       <c r="L173" s="48">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>120.95</v>
       </c>
       <c r="M173" s="50">
@@ -10998,7 +11012,7 @@
         <v>50.915999999999997</v>
       </c>
       <c r="R173" s="50">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>9.2231504438872829</v>
       </c>
       <c r="S173" s="49">
@@ -11011,7 +11025,7 @@
     </row>
     <row r="174" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B174" s="1" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>T-HGT-HEV_NGB81</v>
       </c>
       <c r="C174" s="1" t="str">
@@ -11019,7 +11033,7 @@
         <v>TRACNG,TRABNG</v>
       </c>
       <c r="D174" s="49" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>TRAF</v>
       </c>
       <c r="E174" s="49">
@@ -11038,14 +11052,14 @@
         <v>144.72999999999999</v>
       </c>
       <c r="J174" s="48">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>144.92500000000001</v>
       </c>
       <c r="K174" s="50">
         <v>145.12</v>
       </c>
       <c r="L174" s="48">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>143.88249999999999</v>
       </c>
       <c r="M174" s="50">
@@ -11064,7 +11078,7 @@
         <v>50.915999999999997</v>
       </c>
       <c r="R174" s="50">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>9.2231504438872829</v>
       </c>
       <c r="S174" s="49">
@@ -11076,7 +11090,7 @@
     </row>
     <row r="175" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B175" s="1" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>T-HGT-ICE_LNG81</v>
       </c>
       <c r="C175" s="1" t="str">
@@ -11084,7 +11098,7 @@
         <v>TRALNG</v>
       </c>
       <c r="D175" s="49" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>TRAF</v>
       </c>
       <c r="E175" s="49">
@@ -11103,14 +11117,14 @@
         <v>130.68600000000001</v>
       </c>
       <c r="J175" s="48">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>129.72200000000001</v>
       </c>
       <c r="K175" s="50">
         <v>128.75800000000001</v>
       </c>
       <c r="L175" s="48">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>128.11425</v>
       </c>
       <c r="M175" s="50">
@@ -11129,7 +11143,7 @@
         <v>50.915999999999997</v>
       </c>
       <c r="R175" s="50">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>9.2231504438872829</v>
       </c>
       <c r="S175" s="49">
@@ -11141,7 +11155,7 @@
     </row>
     <row r="176" spans="2:22" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B176" s="1" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="22"/>
         <v>T-HGT-BEV_ELC81</v>
       </c>
       <c r="C176" s="1" t="str">
@@ -11149,7 +11163,7 @@
         <v>TRAELC</v>
       </c>
       <c r="D176" s="49" t="str">
-        <f t="shared" si="27"/>
+        <f t="shared" si="25"/>
         <v>TRAF</v>
       </c>
       <c r="E176" s="49">
@@ -11168,14 +11182,14 @@
         <v>345.67</v>
       </c>
       <c r="J176" s="48">
-        <f t="shared" si="26"/>
+        <f t="shared" si="24"/>
         <v>309.89</v>
       </c>
       <c r="K176" s="50">
         <v>274.11</v>
       </c>
       <c r="L176" s="48">
-        <f t="shared" si="25"/>
+        <f t="shared" si="23"/>
         <v>234.625</v>
       </c>
       <c r="M176" s="50">
@@ -11194,7 +11208,7 @@
         <v>50.915999999999997</v>
       </c>
       <c r="R176" s="50">
-        <f t="shared" si="28"/>
+        <f t="shared" si="26"/>
         <v>9.2231504438872829</v>
       </c>
       <c r="S176" s="49">
@@ -11263,7 +11277,7 @@
         <v>469.60386878903267</v>
       </c>
       <c r="L178" s="48">
-        <f t="shared" ref="L178:L179" si="29">K178-((K178-M178)/4)</f>
+        <f t="shared" ref="L178:L179" si="27">K178-((K178-M178)/4)</f>
         <v>469.60386878903267</v>
       </c>
       <c r="M178" s="48">
@@ -11320,14 +11334,14 @@
         <v>438.88212036358203</v>
       </c>
       <c r="J179" s="48">
-        <f t="shared" ref="J179:J180" si="30">AVERAGE(I179,K179)</f>
+        <f t="shared" ref="J179:J180" si="28">AVERAGE(I179,K179)</f>
         <v>438.88212036358203</v>
       </c>
       <c r="K179" s="48">
         <v>438.88212036358203</v>
       </c>
       <c r="L179" s="48">
-        <f t="shared" si="29"/>
+        <f t="shared" si="27"/>
         <v>438.88212036358203</v>
       </c>
       <c r="M179" s="48">
@@ -11384,7 +11398,7 @@
         <v>682.10068176688696</v>
       </c>
       <c r="J180" s="48">
-        <f t="shared" si="30"/>
+        <f t="shared" si="28"/>
         <v>653.58396473256948</v>
       </c>
       <c r="K180" s="61">
@@ -11473,7 +11487,7 @@
     </row>
     <row r="183" spans="2:32" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B183" s="1" t="str">
-        <f t="shared" ref="B183:B184" si="31">D89</f>
+        <f t="shared" ref="B183:B184" si="29">D89</f>
         <v>T-NAV_NEW</v>
       </c>
       <c r="C183" s="1" t="str">
@@ -11502,7 +11516,7 @@
     </row>
     <row r="184" spans="2:32" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B184" s="1" t="str">
-        <f t="shared" si="31"/>
+        <f t="shared" si="29"/>
         <v>T-OTH_NEW</v>
       </c>
       <c r="C184" s="1" t="str">
@@ -12835,23 +12849,23 @@
         <v>TRAGSL</v>
       </c>
       <c r="D223" s="91" t="str">
-        <f t="shared" ref="D223:H223" si="32">D197</f>
+        <f t="shared" ref="D223:H223" si="30">D197</f>
         <v>UP</v>
       </c>
       <c r="E223" s="87">
-        <f t="shared" si="32"/>
+        <f t="shared" si="30"/>
         <v>0.96784365458672328</v>
       </c>
       <c r="F223" s="87">
-        <f t="shared" si="32"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="G223" s="87">
-        <f t="shared" si="32"/>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="H223" s="81">
-        <f t="shared" si="32"/>
+        <f t="shared" si="30"/>
         <v>5</v>
       </c>
     </row>
@@ -12861,27 +12875,27 @@
         <v>T-TAX-ICE_GSL31</v>
       </c>
       <c r="C224" s="81" t="str">
-        <f t="shared" ref="C224:H248" si="33">C198</f>
+        <f t="shared" ref="C224:H248" si="31">C198</f>
         <v>TRAGSL</v>
       </c>
       <c r="D224" s="91" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>LO</v>
       </c>
       <c r="E224" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.96784365458672328</v>
       </c>
       <c r="F224" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.95</v>
       </c>
       <c r="G224" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.9</v>
       </c>
       <c r="H224" s="81">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
     </row>
@@ -12891,27 +12905,27 @@
         <v>T-TAX-ICE_DST31</v>
       </c>
       <c r="C225" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>TRADST</v>
       </c>
       <c r="D225" s="91" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>UP</v>
       </c>
       <c r="E225" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.95903634682608185</v>
       </c>
       <c r="F225" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>1</v>
       </c>
       <c r="G225" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>1</v>
       </c>
       <c r="H225" s="81">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
     </row>
@@ -12921,19 +12935,19 @@
         <v>T-TAX-ICE_DST31</v>
       </c>
       <c r="C226" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>TRADST</v>
       </c>
       <c r="D226" s="91" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>LO</v>
       </c>
       <c r="E226" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.95903634682608185</v>
       </c>
       <c r="F226" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.95</v>
       </c>
       <c r="G226" s="87">
@@ -12941,7 +12955,7 @@
         <v>0.8</v>
       </c>
       <c r="H226" s="81">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
     </row>
@@ -12951,27 +12965,27 @@
         <v>T-TAX-ICE_DF31</v>
       </c>
       <c r="C227" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>TRACNG</v>
       </c>
       <c r="D227" s="91" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>UP</v>
       </c>
       <c r="E227" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="F227" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="G227" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.8</v>
       </c>
       <c r="H227" s="81">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
     </row>
@@ -12981,27 +12995,27 @@
         <v>T-TAX-ICE_DF31</v>
       </c>
       <c r="C228" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>TRACNG</v>
       </c>
       <c r="D228" s="91" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>LO</v>
       </c>
       <c r="E228" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.4</v>
       </c>
       <c r="F228" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.4</v>
       </c>
       <c r="G228" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.4</v>
       </c>
       <c r="H228" s="81">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
     </row>
@@ -13011,27 +13025,27 @@
         <v>T-TAX-ICE_NGB31</v>
       </c>
       <c r="C229" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>TRACNG</v>
       </c>
       <c r="D229" s="91" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>UP</v>
       </c>
       <c r="E229" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="F229" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="G229" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>1</v>
       </c>
       <c r="H229" s="81">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
       <c r="J229" s="1"/>
@@ -13058,27 +13072,27 @@
         <v>T-TAX-ICE_NGB31</v>
       </c>
       <c r="C230" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>TRACNG</v>
       </c>
       <c r="D230" s="91" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>LO</v>
       </c>
       <c r="E230" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="F230" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="G230" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="H230" s="81">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
       <c r="J230" s="1"/>
@@ -13105,27 +13119,27 @@
         <v>T-TAX-ICE_E8531</v>
       </c>
       <c r="C231" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>TRAETH</v>
       </c>
       <c r="D231" s="91" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>UP</v>
       </c>
       <c r="E231" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.85</v>
       </c>
       <c r="F231" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.85</v>
       </c>
       <c r="G231" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.85</v>
       </c>
       <c r="H231" s="81">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
       <c r="J231" s="1"/>
@@ -13152,27 +13166,27 @@
         <v>T-TAX-ICE_E8531</v>
       </c>
       <c r="C232" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>TRAETH</v>
       </c>
       <c r="D232" s="91" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>LO</v>
       </c>
       <c r="E232" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="F232" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="G232" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="H232" s="81">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
       <c r="J232" s="1"/>
@@ -13199,27 +13213,27 @@
         <v>T-TAX-HEV_GSL31</v>
       </c>
       <c r="C233" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>TRAGSL</v>
       </c>
       <c r="D233" s="91" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>UP</v>
       </c>
       <c r="E233" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.96784365458672328</v>
       </c>
       <c r="F233" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>1</v>
       </c>
       <c r="G233" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>1</v>
       </c>
       <c r="H233" s="81">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
       <c r="J233" s="1"/>
@@ -13246,27 +13260,27 @@
         <v>T-TAX-HEV_GSL31</v>
       </c>
       <c r="C234" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>TRAGSL</v>
       </c>
       <c r="D234" s="91" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>LO</v>
       </c>
       <c r="E234" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.96784365458672328</v>
       </c>
       <c r="F234" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.95</v>
       </c>
       <c r="G234" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.9</v>
       </c>
       <c r="H234" s="81">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
       <c r="J234" s="1"/>
@@ -13293,27 +13307,27 @@
         <v>T-TAX-HEV_DST31</v>
       </c>
       <c r="C235" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>TRADST</v>
       </c>
       <c r="D235" s="91" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>UP</v>
       </c>
       <c r="E235" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.95903634682608185</v>
       </c>
       <c r="F235" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>1</v>
       </c>
       <c r="G235" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>1</v>
       </c>
       <c r="H235" s="81">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
     </row>
@@ -13323,27 +13337,27 @@
         <v>T-TAX-HEV_DST31</v>
       </c>
       <c r="C236" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>TRADST</v>
       </c>
       <c r="D236" s="91" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>LO</v>
       </c>
       <c r="E236" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.95903634682608185</v>
       </c>
       <c r="F236" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.95</v>
       </c>
       <c r="G236" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.8</v>
       </c>
       <c r="H236" s="81">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
     </row>
@@ -13353,27 +13367,27 @@
         <v>T-TAX-PHEV10_GSL31</v>
       </c>
       <c r="C237" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>TRAELC</v>
       </c>
       <c r="D237" s="91" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>UP</v>
       </c>
       <c r="E237" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="F237" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.6</v>
       </c>
       <c r="G237" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.8</v>
       </c>
       <c r="H237" s="81">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
     </row>
@@ -13383,27 +13397,27 @@
         <v>T-TAX-PHEV10_GSL31</v>
       </c>
       <c r="C238" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>TRAELC</v>
       </c>
       <c r="D238" s="91" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>LO</v>
       </c>
       <c r="E238" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.3</v>
       </c>
       <c r="F238" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.3</v>
       </c>
       <c r="G238" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.3</v>
       </c>
       <c r="H238" s="81">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
     </row>
@@ -13413,27 +13427,27 @@
         <v>T-TAX-PHEV20_GSL31</v>
       </c>
       <c r="C239" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>TRAELC</v>
       </c>
       <c r="D239" s="91" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>UP</v>
       </c>
       <c r="E239" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="F239" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.6</v>
       </c>
       <c r="G239" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.8</v>
       </c>
       <c r="H239" s="81">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
     </row>
@@ -13443,27 +13457,27 @@
         <v>T-TAX-PHEV20_GSL31</v>
       </c>
       <c r="C240" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>TRAELC</v>
       </c>
       <c r="D240" s="91" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>LO</v>
       </c>
       <c r="E240" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.3</v>
       </c>
       <c r="F240" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.3</v>
       </c>
       <c r="G240" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.3</v>
       </c>
       <c r="H240" s="81">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
     </row>
@@ -13473,27 +13487,27 @@
         <v>T-TAX-PHEV40_GSL31</v>
       </c>
       <c r="C241" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>TRAELC</v>
       </c>
       <c r="D241" s="91" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>UP</v>
       </c>
       <c r="E241" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="F241" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.6</v>
       </c>
       <c r="G241" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.8</v>
       </c>
       <c r="H241" s="81">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
     </row>
@@ -13503,27 +13517,27 @@
         <v>T-TAX-PHEV40_GSL31</v>
       </c>
       <c r="C242" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>TRAELC</v>
       </c>
       <c r="D242" s="91" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>LO</v>
       </c>
       <c r="E242" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.3</v>
       </c>
       <c r="F242" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.3</v>
       </c>
       <c r="G242" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.3</v>
       </c>
       <c r="H242" s="81">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
     </row>
@@ -13533,27 +13547,27 @@
         <v>T-TAX-PHEV10_DST31</v>
       </c>
       <c r="C243" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>TRAELC</v>
       </c>
       <c r="D243" s="91" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>UP</v>
       </c>
       <c r="E243" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="F243" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.6</v>
       </c>
       <c r="G243" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.8</v>
       </c>
       <c r="H243" s="81">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
     </row>
@@ -13563,27 +13577,27 @@
         <v>T-TAX-PHEV10_DST31</v>
       </c>
       <c r="C244" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>TRAELC</v>
       </c>
       <c r="D244" s="91" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>LO</v>
       </c>
       <c r="E244" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.3</v>
       </c>
       <c r="F244" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.3</v>
       </c>
       <c r="G244" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.3</v>
       </c>
       <c r="H244" s="81">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
     </row>
@@ -13593,27 +13607,27 @@
         <v>T-TAX-PHEV20_DST31</v>
       </c>
       <c r="C245" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>TRAELC</v>
       </c>
       <c r="D245" s="91" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>UP</v>
       </c>
       <c r="E245" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="F245" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.6</v>
       </c>
       <c r="G245" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.8</v>
       </c>
       <c r="H245" s="81">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
     </row>
@@ -13623,27 +13637,27 @@
         <v>T-TAX-PHEV20_DST31</v>
       </c>
       <c r="C246" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>TRAELC</v>
       </c>
       <c r="D246" s="91" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>LO</v>
       </c>
       <c r="E246" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.3</v>
       </c>
       <c r="F246" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.3</v>
       </c>
       <c r="G246" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.3</v>
       </c>
       <c r="H246" s="81">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
     </row>
@@ -13653,27 +13667,27 @@
         <v>T-TAX-PHEV40_DST31</v>
       </c>
       <c r="C247" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>TRAELC</v>
       </c>
       <c r="D247" s="91" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>UP</v>
       </c>
       <c r="E247" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.5</v>
       </c>
       <c r="F247" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.6</v>
       </c>
       <c r="G247" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.8</v>
       </c>
       <c r="H247" s="81">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
     </row>
@@ -13683,27 +13697,27 @@
         <v>T-TAX-PHEV40_DST31</v>
       </c>
       <c r="C248" s="81" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>TRAELC</v>
       </c>
       <c r="D248" s="91" t="str">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>LO</v>
       </c>
       <c r="E248" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.3</v>
       </c>
       <c r="F248" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.3</v>
       </c>
       <c r="G248" s="87">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>0.3</v>
       </c>
       <c r="H248" s="81">
-        <f t="shared" si="33"/>
+        <f t="shared" si="31"/>
         <v>5</v>
       </c>
     </row>
@@ -13717,7 +13731,7 @@
         <v>TRADST</v>
       </c>
       <c r="D249" s="82" t="str">
-        <f t="shared" ref="D249" si="34">D223</f>
+        <f t="shared" ref="D249" si="32">D223</f>
         <v>UP</v>
       </c>
       <c r="E249" s="79">
@@ -13743,7 +13757,7 @@
         <v>TRADST</v>
       </c>
       <c r="D250" s="82" t="str">
-        <f t="shared" ref="D250" si="35">D224</f>
+        <f t="shared" ref="D250" si="33">D224</f>
         <v>LO</v>
       </c>
       <c r="E250" s="79">
@@ -13769,7 +13783,7 @@
         <v>TRACNG</v>
       </c>
       <c r="D251" s="82" t="str">
-        <f t="shared" ref="D251" si="36">D225</f>
+        <f t="shared" ref="D251" si="34">D225</f>
         <v>UP</v>
       </c>
       <c r="E251" s="79">
@@ -13795,7 +13809,7 @@
         <v>TRACNG</v>
       </c>
       <c r="D252" s="82" t="str">
-        <f t="shared" ref="D252" si="37">D226</f>
+        <f t="shared" ref="D252" si="35">D226</f>
         <v>LO</v>
       </c>
       <c r="E252" s="79">
@@ -14899,7 +14913,7 @@
     </row>
     <row r="291" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B291" s="86" t="str">
-        <f t="shared" ref="B291:B294" si="38">B290</f>
+        <f t="shared" ref="B291:B294" si="36">B290</f>
         <v>T-OTH_NEW</v>
       </c>
       <c r="C291" s="86" t="str">
@@ -14924,7 +14938,7 @@
     </row>
     <row r="292" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B292" s="86" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>T-OTH_NEW</v>
       </c>
       <c r="C292" s="86" t="str">
@@ -14949,7 +14963,7 @@
     </row>
     <row r="293" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B293" s="86" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>T-OTH_NEW</v>
       </c>
       <c r="C293" s="86" t="str">
@@ -14974,7 +14988,7 @@
     </row>
     <row r="294" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B294" s="86" t="str">
-        <f t="shared" si="38"/>
+        <f t="shared" si="36"/>
         <v>T-OTH_NEW</v>
       </c>
       <c r="C294" s="86" t="str">

</xml_diff>